<commit_message>
updated with 2020-03-30 data
</commit_message>
<xml_diff>
--- a/covid19 lockdown evaluation .xlsx
+++ b/covid19 lockdown evaluation .xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="45">
   <si>
     <t>Effects of the lockdown issued by governments</t>
   </si>
@@ -140,16 +140,16 @@
     <t>France</t>
   </si>
   <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
     <t>USA</t>
   </si>
   <si>
-    <t>UK</t>
-  </si>
-  <si>
     <t>Germany</t>
-  </si>
-  <si>
-    <t>Sweden</t>
   </si>
 </sst>
 </file>
@@ -329,10 +329,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q65"/>
+  <dimension ref="A1:Q77"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F66" activeCellId="0" sqref="F66"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -750,7 +750,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="7" t="n">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="D21" s="0"/>
       <c r="E21" s="8" t="s">
@@ -823,31 +823,31 @@
         <v>300</v>
       </c>
       <c r="D23" s="1" t="n">
-        <v>10779</v>
+        <v>11591</v>
       </c>
       <c r="E23" s="12" t="n">
         <f aca="false">D23/60.48</f>
-        <v>178.224206349206</v>
+        <v>191.650132275132</v>
       </c>
       <c r="F23" s="12" t="n">
-        <v>756</v>
+        <v>812</v>
       </c>
       <c r="G23" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H23" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$21,G23)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I23" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J23" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$21,I23)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K23" s="13" t="n">
-        <f aca="false">$B$21+1</f>
+        <f aca="false">$B$33+1</f>
         <v>43920</v>
       </c>
       <c r="L23" s="0"/>
@@ -865,31 +865,31 @@
         <v>230</v>
       </c>
       <c r="D24" s="1" t="n">
-        <v>6803</v>
+        <v>7716</v>
       </c>
       <c r="E24" s="12" t="n">
         <f aca="false">D24/46.75</f>
-        <v>145.51871657754</v>
+        <v>165.048128342246</v>
       </c>
       <c r="F24" s="12" t="n">
-        <v>821</v>
+        <v>913</v>
       </c>
       <c r="G24" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H24" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$21,G24)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I24" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J24" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$21,I24)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K24" s="13" t="n">
-        <f aca="false">$B$21+1</f>
+        <f aca="false">$B$33+1</f>
         <v>43920</v>
       </c>
       <c r="L24" s="0"/>
@@ -907,31 +907,31 @@
         <v>330</v>
       </c>
       <c r="D25" s="1" t="n">
-        <v>2606</v>
+        <v>3024</v>
       </c>
       <c r="E25" s="12" t="n">
         <f aca="false">D25/65.27</f>
-        <v>39.9264593228129</v>
+        <v>46.3306266278535</v>
       </c>
       <c r="F25" s="12" t="n">
-        <v>292</v>
+        <v>418</v>
       </c>
       <c r="G25" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H25" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$21,G25)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I25" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J25" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$21,I25)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K25" s="13" t="n">
-        <f aca="false">$B$21+1</f>
+        <f aca="false">$B$33+1</f>
         <v>43920</v>
       </c>
       <c r="L25" s="0"/>
@@ -946,35 +946,35 @@
         <v>41</v>
       </c>
       <c r="C26" s="12" t="n">
-        <v>1660</v>
-      </c>
-      <c r="D26" s="1" t="n">
-        <v>2583</v>
+        <v>50</v>
+      </c>
+      <c r="D26" s="12" t="n">
+        <v>146</v>
       </c>
       <c r="E26" s="12" t="n">
-        <f aca="false">D26/331</f>
-        <v>7.8036253776435</v>
+        <f aca="false">D26/10.36</f>
+        <v>14.0926640926641</v>
       </c>
       <c r="F26" s="12" t="n">
-        <v>363</v>
+        <v>36</v>
       </c>
       <c r="G26" s="13" t="n">
-        <v>43917</v>
+        <v>43915</v>
       </c>
       <c r="H26" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$21,G26)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I26" s="13" t="n">
         <f aca="false">$B$21+1</f>
-        <v>43920</v>
+        <v>43921</v>
       </c>
       <c r="J26" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$21,I26)</f>
         <v>-1</v>
       </c>
       <c r="K26" s="13" t="n">
-        <f aca="false">$B$21+1</f>
+        <f aca="false">$B$33+1</f>
         <v>43920</v>
       </c>
       <c r="L26" s="0"/>
@@ -992,32 +992,32 @@
         <v>330</v>
       </c>
       <c r="D27" s="1" t="n">
-        <v>1228</v>
+        <v>1408</v>
       </c>
       <c r="E27" s="12" t="n">
         <f aca="false">D27/67.79</f>
-        <v>18.1147661897035</v>
+        <v>20.770025077445</v>
       </c>
       <c r="F27" s="12" t="n">
-        <v>209</v>
+        <v>180</v>
       </c>
       <c r="G27" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H27" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$21,G27)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I27" s="13" t="n">
         <f aca="false">$B$21+1</f>
-        <v>43920</v>
+        <v>43921</v>
       </c>
       <c r="J27" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$21,I27)</f>
         <v>-1</v>
       </c>
       <c r="K27" s="13" t="n">
-        <f aca="false">$B$21+1</f>
+        <f aca="false">$B$33+1</f>
         <v>43920</v>
       </c>
       <c r="L27" s="0"/>
@@ -1032,35 +1032,34 @@
         <v>43</v>
       </c>
       <c r="C28" s="12" t="n">
-        <v>414</v>
+        <v>1660</v>
       </c>
       <c r="D28" s="1" t="n">
-        <v>541</v>
+        <v>3156</v>
       </c>
       <c r="E28" s="12" t="n">
-        <f aca="false">D28/83.784</f>
-        <v>6.457080110761</v>
+        <f aca="false">D28/331</f>
+        <v>9.53474320241692</v>
       </c>
       <c r="F28" s="12" t="n">
-        <v>108</v>
+        <v>573</v>
       </c>
       <c r="G28" s="13" t="n">
-        <v>43918</v>
+        <v>43917</v>
       </c>
       <c r="H28" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$21,G28)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I28" s="13" t="n">
-        <f aca="false">$B$21+1</f>
         <v>43920</v>
       </c>
       <c r="J28" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$21,I28)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="K28" s="13" t="n">
-        <f aca="false">$B$21+1</f>
+        <f aca="false">$B$33+1</f>
         <v>43920</v>
       </c>
       <c r="L28" s="0"/>
@@ -1075,35 +1074,35 @@
         <v>44</v>
       </c>
       <c r="C29" s="12" t="n">
-        <v>50</v>
-      </c>
-      <c r="D29" s="12" t="n">
-        <v>110</v>
+        <v>414</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <v>645</v>
       </c>
       <c r="E29" s="12" t="n">
-        <f aca="false">D29/10.36</f>
-        <v>10.6177606177606</v>
+        <f aca="false">D29/83.784</f>
+        <v>7.69836723002005</v>
       </c>
       <c r="F29" s="12" t="n">
-        <v>5</v>
+        <v>104</v>
       </c>
       <c r="G29" s="13" t="n">
-        <v>43915</v>
+        <v>43918</v>
       </c>
       <c r="H29" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$21,G29)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I29" s="13" t="n">
         <f aca="false">$B$21+1</f>
-        <v>43920</v>
+        <v>43921</v>
       </c>
       <c r="J29" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$21,I29)</f>
         <v>-1</v>
       </c>
       <c r="K29" s="13" t="n">
-        <f aca="false">$B$21+1</f>
+        <f aca="false">$B$33+1</f>
         <v>43920</v>
       </c>
       <c r="L29" s="0"/>
@@ -1170,15 +1169,13 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="7" t="n">
-        <v>43918</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>6</v>
-      </c>
+        <v>43919</v>
+      </c>
+      <c r="D33" s="0"/>
       <c r="E33" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F33" s="8"/>
+      <c r="F33" s="0"/>
       <c r="G33" s="8" t="s">
         <v>27</v>
       </c>
@@ -1206,8 +1203,8 @@
       <c r="C34" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="10" t="s">
-        <v>2</v>
+      <c r="D34" s="8" t="s">
+        <v>6</v>
       </c>
       <c r="E34" s="10" t="s">
         <v>32</v>
@@ -1245,32 +1242,32 @@
         <v>300</v>
       </c>
       <c r="D35" s="1" t="n">
-        <v>10023</v>
+        <v>10779</v>
       </c>
       <c r="E35" s="12" t="n">
         <f aca="false">D35/60.48</f>
-        <v>165.724206349206</v>
+        <v>178.224206349206</v>
       </c>
       <c r="F35" s="12" t="n">
-        <v>889</v>
+        <v>756</v>
       </c>
       <c r="G35" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H35" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$33,G35)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I35" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J35" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$45,I35)</f>
-        <v>15</v>
+        <f aca="false">_xlfn.DAYS($B$33,I35)</f>
+        <v>17</v>
       </c>
       <c r="K35" s="13" t="n">
         <f aca="false">$B$33+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L35" s="0"/>
       <c r="M35" s="0"/>
@@ -1287,32 +1284,32 @@
         <v>230</v>
       </c>
       <c r="D36" s="1" t="n">
-        <v>5982</v>
+        <v>6803</v>
       </c>
       <c r="E36" s="12" t="n">
         <f aca="false">D36/46.75</f>
-        <v>127.957219251337</v>
+        <v>145.51871657754</v>
       </c>
       <c r="F36" s="12" t="n">
-        <v>844</v>
+        <v>821</v>
       </c>
       <c r="G36" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H36" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$33,G36)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I36" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J36" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$45,I36)</f>
-        <v>4</v>
+        <f aca="false">_xlfn.DAYS($B$33,I36)</f>
+        <v>6</v>
       </c>
       <c r="K36" s="13" t="n">
         <f aca="false">$B$33+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L36" s="0"/>
       <c r="M36" s="0"/>
@@ -1329,32 +1326,32 @@
         <v>330</v>
       </c>
       <c r="D37" s="1" t="n">
-        <v>2314</v>
+        <v>2606</v>
       </c>
       <c r="E37" s="12" t="n">
         <f aca="false">D37/65.27</f>
-        <v>35.4527347939329</v>
+        <v>39.9264593228129</v>
       </c>
       <c r="F37" s="12" t="n">
-        <v>319</v>
+        <v>292</v>
       </c>
       <c r="G37" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H37" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$33,G37)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I37" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J37" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$45,I37)</f>
-        <v>3</v>
+        <f aca="false">_xlfn.DAYS($B$33,I37)</f>
+        <v>5</v>
       </c>
       <c r="K37" s="13" t="n">
         <f aca="false">$B$33+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L37" s="0"/>
       <c r="M37" s="0"/>
@@ -1365,31 +1362,31 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C38" s="12" t="n">
         <v>1660</v>
       </c>
       <c r="D38" s="1" t="n">
-        <v>2221</v>
+        <v>2583</v>
       </c>
       <c r="E38" s="12" t="n">
         <f aca="false">D38/331</f>
-        <v>6.70996978851964</v>
+        <v>7.8036253776435</v>
       </c>
       <c r="F38" s="12" t="n">
-        <v>525</v>
+        <v>363</v>
       </c>
       <c r="G38" s="13" t="n">
         <v>43917</v>
       </c>
       <c r="H38" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$33,G38)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I38" s="13" t="n">
         <f aca="false">$B$33+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="J38" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$33,I38)</f>
@@ -1397,7 +1394,7 @@
       </c>
       <c r="K38" s="13" t="n">
         <f aca="false">$B$33+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L38" s="0"/>
       <c r="M38" s="0"/>
@@ -1414,25 +1411,25 @@
         <v>330</v>
       </c>
       <c r="D39" s="1" t="n">
-        <v>1019</v>
+        <v>1228</v>
       </c>
       <c r="E39" s="12" t="n">
         <f aca="false">D39/67.79</f>
-        <v>15.0317155922702</v>
+        <v>18.1147661897035</v>
       </c>
       <c r="F39" s="12" t="n">
-        <v>260</v>
+        <v>209</v>
       </c>
       <c r="G39" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H39" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$33,G39)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I39" s="13" t="n">
         <f aca="false">$B$33+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="J39" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$33,I39)</f>
@@ -1440,7 +1437,7 @@
       </c>
       <c r="K39" s="13" t="n">
         <f aca="false">$B$33+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L39" s="0"/>
       <c r="M39" s="0"/>
@@ -1451,31 +1448,31 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C40" s="12" t="n">
         <v>414</v>
       </c>
       <c r="D40" s="1" t="n">
-        <v>433</v>
+        <v>541</v>
       </c>
       <c r="E40" s="12" t="n">
         <f aca="false">D40/83.784</f>
-        <v>5.16805117922276</v>
+        <v>6.457080110761</v>
       </c>
       <c r="F40" s="12" t="n">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="G40" s="13" t="n">
         <v>43918</v>
       </c>
       <c r="H40" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$33,G40)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I40" s="13" t="n">
         <f aca="false">$B$33+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="J40" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$33,I40)</f>
@@ -1483,7 +1480,7 @@
       </c>
       <c r="K40" s="13" t="n">
         <f aca="false">$B$33+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L40" s="0"/>
       <c r="M40" s="0"/>
@@ -1494,31 +1491,31 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="0" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C41" s="12" t="n">
         <v>50</v>
       </c>
       <c r="D41" s="12" t="n">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="E41" s="12" t="n">
         <f aca="false">D41/10.36</f>
-        <v>10.1351351351351</v>
+        <v>10.6177606177606</v>
       </c>
       <c r="F41" s="12" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G41" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H41" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$33,G41)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I41" s="13" t="n">
         <f aca="false">$B$33+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="J41" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$33,I41)</f>
@@ -1526,7 +1523,7 @@
       </c>
       <c r="K41" s="13" t="n">
         <f aca="false">$B$33+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L41" s="0"/>
       <c r="M41" s="0"/>
@@ -1536,13 +1533,16 @@
       <c r="Q41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="13"/>
-      <c r="I42" s="13"/>
-      <c r="K42" s="13"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="0"/>
+      <c r="E42" s="0"/>
+      <c r="F42" s="0"/>
+      <c r="G42" s="0"/>
+      <c r="H42" s="0"/>
+      <c r="I42" s="0"/>
+      <c r="J42" s="0"/>
+      <c r="K42" s="0"/>
       <c r="L42" s="0"/>
       <c r="M42" s="0"/>
       <c r="N42" s="0"/>
@@ -1587,11 +1587,10 @@
       <c r="P44" s="0"/>
       <c r="Q44" s="0"/>
     </row>
-    <row r="45" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="7" t="n">
-        <v>43917</v>
-      </c>
-      <c r="C45" s="0"/>
+        <v>43918</v>
+      </c>
       <c r="D45" s="8" t="s">
         <v>6</v>
       </c>
@@ -1614,10 +1613,14 @@
       <c r="K45" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L45" s="8"/>
+      <c r="L45" s="0"/>
+      <c r="M45" s="0"/>
+      <c r="N45" s="0"/>
+      <c r="O45" s="0"/>
+      <c r="P45" s="0"/>
+      <c r="Q45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="3"/>
       <c r="B46" s="9"/>
       <c r="C46" s="10" t="s">
         <v>31</v>
@@ -1646,7 +1649,7 @@
       <c r="K46" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="L46" s="8"/>
+      <c r="L46" s="0"/>
       <c r="M46" s="0"/>
       <c r="N46" s="0"/>
       <c r="O46" s="0"/>
@@ -1661,32 +1664,32 @@
         <v>300</v>
       </c>
       <c r="D47" s="1" t="n">
-        <v>9134</v>
+        <v>10023</v>
       </c>
       <c r="E47" s="12" t="n">
         <f aca="false">D47/60.48</f>
-        <v>151.025132275132</v>
+        <v>165.724206349206</v>
       </c>
       <c r="F47" s="12" t="n">
-        <v>919</v>
+        <v>889</v>
       </c>
       <c r="G47" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H47" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$45,G47)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I47" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J47" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$45,I47)</f>
+        <f aca="false">_xlfn.DAYS(B$57,I47)</f>
         <v>15</v>
       </c>
       <c r="K47" s="13" t="n">
         <f aca="false">$B$45+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L47" s="0"/>
       <c r="M47" s="0"/>
@@ -1703,32 +1706,32 @@
         <v>230</v>
       </c>
       <c r="D48" s="1" t="n">
-        <v>5138</v>
+        <v>5982</v>
       </c>
       <c r="E48" s="12" t="n">
         <f aca="false">D48/46.75</f>
-        <v>109.903743315508</v>
+        <v>127.957219251337</v>
       </c>
       <c r="F48" s="12" t="n">
-        <v>773</v>
+        <v>844</v>
       </c>
       <c r="G48" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H48" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$45,G48)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I48" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J48" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$45,I48)</f>
+        <f aca="false">_xlfn.DAYS(B$57,I48)</f>
         <v>4</v>
       </c>
       <c r="K48" s="13" t="n">
         <f aca="false">$B$45+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L48" s="0"/>
       <c r="M48" s="0"/>
@@ -1745,32 +1748,32 @@
         <v>330</v>
       </c>
       <c r="D49" s="1" t="n">
-        <v>1995</v>
+        <v>2314</v>
       </c>
       <c r="E49" s="12" t="n">
         <f aca="false">D49/65.27</f>
-        <v>30.5653439558756</v>
+        <v>35.4527347939329</v>
       </c>
       <c r="F49" s="12" t="n">
-        <v>299</v>
+        <v>319</v>
       </c>
       <c r="G49" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H49" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$45,G49)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I49" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J49" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$45,I49)</f>
+        <f aca="false">_xlfn.DAYS(B$57,I49)</f>
         <v>3</v>
       </c>
       <c r="K49" s="13" t="n">
         <f aca="false">$B$45+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L49" s="0"/>
       <c r="M49" s="0"/>
@@ -1781,40 +1784,39 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C50" s="12" t="n">
         <v>1660</v>
       </c>
       <c r="D50" s="1" t="n">
-        <v>1696</v>
+        <v>2221</v>
       </c>
       <c r="E50" s="12" t="n">
         <f aca="false">D50/331</f>
-        <v>5.12386706948641</v>
+        <v>6.70996978851964</v>
       </c>
       <c r="F50" s="12" t="n">
-        <v>400</v>
+        <v>525</v>
       </c>
       <c r="G50" s="13" t="n">
-        <f aca="false">$B$45</f>
         <v>43917</v>
       </c>
       <c r="H50" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$45,G50)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I50" s="13" t="n">
         <f aca="false">$B$45+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="J50" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$45,I50)</f>
+        <f aca="false">_xlfn.DAYS($B$45,I50)</f>
         <v>-1</v>
       </c>
       <c r="K50" s="13" t="n">
         <f aca="false">$B$45+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L50" s="0"/>
       <c r="M50" s="0"/>
@@ -1831,33 +1833,33 @@
         <v>330</v>
       </c>
       <c r="D51" s="1" t="n">
-        <v>759</v>
+        <v>1019</v>
       </c>
       <c r="E51" s="12" t="n">
         <f aca="false">D51/67.79</f>
-        <v>11.1963416433102</v>
+        <v>15.0317155922702</v>
       </c>
       <c r="F51" s="12" t="n">
-        <v>181</v>
+        <v>260</v>
       </c>
       <c r="G51" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H51" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$45,G51)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I51" s="13" t="n">
         <f aca="false">$B$45+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="J51" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$45,I51)</f>
+        <f aca="false">_xlfn.DAYS($B$45,I51)</f>
         <v>-1</v>
       </c>
       <c r="K51" s="13" t="n">
         <f aca="false">$B$45+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L51" s="0"/>
       <c r="M51" s="0"/>
@@ -1868,40 +1870,39 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C52" s="12" t="n">
         <v>414</v>
       </c>
       <c r="D52" s="1" t="n">
-        <v>351</v>
+        <v>433</v>
       </c>
       <c r="E52" s="12" t="n">
         <f aca="false">D52/83.784</f>
-        <v>4.18934402749928</v>
+        <v>5.16805117922276</v>
       </c>
       <c r="F52" s="12" t="n">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G52" s="13" t="n">
-        <f aca="false">$B$45+1</f>
         <v>43918</v>
       </c>
       <c r="H52" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$45,G52)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="I52" s="13" t="n">
         <f aca="false">$B$45+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="J52" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$45,I52)</f>
+        <f aca="false">_xlfn.DAYS($B$45,I52)</f>
         <v>-1</v>
       </c>
       <c r="K52" s="13" t="n">
         <f aca="false">$B$45+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L52" s="0"/>
       <c r="M52" s="0"/>
@@ -1912,7 +1913,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="0" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C53" s="12" t="n">
         <v>50</v>
@@ -1925,26 +1926,26 @@
         <v>10.1351351351351</v>
       </c>
       <c r="F53" s="12" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="G53" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H53" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$45,G53)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I53" s="13" t="n">
         <f aca="false">$B$45+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="J53" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$45,I53)</f>
+        <f aca="false">_xlfn.DAYS($B$45,I53)</f>
         <v>-1</v>
       </c>
       <c r="K53" s="13" t="n">
         <f aca="false">$B$45+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L53" s="0"/>
       <c r="M53" s="0"/>
@@ -1954,14 +1955,15 @@
       <c r="Q53" s="0"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D54" s="0"/>
-      <c r="E54" s="0"/>
-      <c r="F54" s="0"/>
-      <c r="G54" s="0"/>
+      <c r="C54" s="12"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="13"/>
       <c r="H54" s="0"/>
-      <c r="I54" s="0"/>
+      <c r="I54" s="13"/>
       <c r="J54" s="0"/>
-      <c r="K54" s="0"/>
+      <c r="K54" s="13"/>
       <c r="L54" s="0"/>
       <c r="M54" s="0"/>
       <c r="N54" s="0"/>
@@ -1970,6 +1972,8 @@
       <c r="Q54" s="0"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="4"/>
+      <c r="C55" s="5"/>
       <c r="D55" s="0"/>
       <c r="E55" s="0"/>
       <c r="F55" s="0"/>
@@ -2004,10 +2008,11 @@
       <c r="P56" s="0"/>
       <c r="Q56" s="0"/>
     </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="7" t="n">
-        <v>43916</v>
-      </c>
+        <v>43917</v>
+      </c>
+      <c r="C57" s="0"/>
       <c r="D57" s="8" t="s">
         <v>6</v>
       </c>
@@ -2030,17 +2035,13 @@
       <c r="K57" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L57" s="0"/>
-      <c r="M57" s="0"/>
-      <c r="N57" s="0"/>
-      <c r="O57" s="0"/>
-      <c r="P57" s="0"/>
-      <c r="Q57" s="0"/>
+      <c r="L57" s="8"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="3"/>
       <c r="B58" s="9"/>
       <c r="C58" s="10" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="D58" s="10" t="s">
         <v>2</v>
@@ -2066,7 +2067,7 @@
       <c r="K58" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="L58" s="0"/>
+      <c r="L58" s="8"/>
       <c r="M58" s="0"/>
       <c r="N58" s="0"/>
       <c r="O58" s="0"/>
@@ -2081,32 +2082,32 @@
         <v>300</v>
       </c>
       <c r="D59" s="1" t="n">
-        <v>8215</v>
+        <v>9134</v>
       </c>
       <c r="E59" s="12" t="n">
         <f aca="false">D59/60.48</f>
-        <v>135.830026455026</v>
+        <v>151.025132275132</v>
       </c>
       <c r="F59" s="12" t="n">
-        <v>712</v>
+        <v>919</v>
       </c>
       <c r="G59" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H59" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$57,G59)</f>
-        <v>16</v>
+        <f aca="false">_xlfn.DAYS($B$57,G59)</f>
+        <v>17</v>
       </c>
       <c r="I59" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J59" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$57,I59)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K59" s="13" t="n">
-        <f aca="false">B$57+1</f>
-        <v>43917</v>
+        <f aca="false">$B$57+1</f>
+        <v>43918</v>
       </c>
       <c r="L59" s="0"/>
       <c r="M59" s="0"/>
@@ -2123,32 +2124,32 @@
         <v>230</v>
       </c>
       <c r="D60" s="1" t="n">
-        <v>4365</v>
+        <v>5138</v>
       </c>
       <c r="E60" s="12" t="n">
         <f aca="false">D60/46.75</f>
-        <v>93.3689839572193</v>
+        <v>109.903743315508</v>
       </c>
       <c r="F60" s="12" t="n">
-        <v>718</v>
+        <v>773</v>
       </c>
       <c r="G60" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H60" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$57,G60)</f>
-        <v>9</v>
+        <f aca="false">_xlfn.DAYS($B$57,G60)</f>
+        <v>10</v>
       </c>
       <c r="I60" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J60" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$57,I60)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K60" s="13" t="n">
-        <f aca="false">B$57+1</f>
-        <v>43917</v>
+        <f aca="false">$B$57+1</f>
+        <v>43918</v>
       </c>
       <c r="L60" s="0"/>
       <c r="M60" s="0"/>
@@ -2165,32 +2166,32 @@
         <v>330</v>
       </c>
       <c r="D61" s="1" t="n">
-        <v>1696</v>
+        <v>1995</v>
       </c>
       <c r="E61" s="12" t="n">
         <f aca="false">D61/65.27</f>
-        <v>25.9843726060978</v>
+        <v>30.5653439558756</v>
       </c>
       <c r="F61" s="12" t="n">
-        <v>365</v>
+        <v>299</v>
       </c>
       <c r="G61" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H61" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$57,G61)</f>
-        <v>4</v>
+        <f aca="false">_xlfn.DAYS($B$57,G61)</f>
+        <v>5</v>
       </c>
       <c r="I61" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J61" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$57,I61)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K61" s="13" t="n">
-        <f aca="false">B$57+1</f>
-        <v>43917</v>
+        <f aca="false">$B$57+1</f>
+        <v>43918</v>
       </c>
       <c r="L61" s="0"/>
       <c r="M61" s="0"/>
@@ -2201,39 +2202,40 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C62" s="12" t="n">
         <v>1660</v>
       </c>
       <c r="D62" s="1" t="n">
-        <v>1295</v>
+        <v>1696</v>
       </c>
       <c r="E62" s="12" t="n">
         <f aca="false">D62/331</f>
-        <v>3.91238670694864</v>
+        <v>5.12386706948641</v>
       </c>
       <c r="F62" s="12" t="n">
-        <v>268</v>
+        <v>400</v>
       </c>
       <c r="G62" s="13" t="n">
+        <f aca="false">$B$57</f>
         <v>43917</v>
       </c>
       <c r="H62" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$57,G62)</f>
+        <f aca="false">_xlfn.DAYS($B$57,G62)</f>
+        <v>0</v>
+      </c>
+      <c r="I62" s="13" t="n">
+        <f aca="false">$B$57+1</f>
+        <v>43918</v>
+      </c>
+      <c r="J62" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$57,I62)</f>
         <v>-1</v>
       </c>
-      <c r="I62" s="13" t="n">
-        <f aca="false">B$57+1</f>
-        <v>43917</v>
-      </c>
-      <c r="J62" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$57,I62)</f>
-        <v>-1</v>
-      </c>
       <c r="K62" s="13" t="n">
-        <f aca="false">B$57+1</f>
-        <v>43917</v>
+        <f aca="false">$B$57+1</f>
+        <v>43918</v>
       </c>
       <c r="L62" s="0"/>
       <c r="M62" s="0"/>
@@ -2250,33 +2252,33 @@
         <v>330</v>
       </c>
       <c r="D63" s="1" t="n">
-        <v>578</v>
+        <v>759</v>
       </c>
       <c r="E63" s="12" t="n">
         <f aca="false">D63/67.79</f>
-        <v>8.52633131730344</v>
+        <v>11.1963416433102</v>
       </c>
       <c r="F63" s="12" t="n">
-        <v>115</v>
+        <v>181</v>
       </c>
       <c r="G63" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H63" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$57,G63)</f>
-        <v>0</v>
+        <f aca="false">_xlfn.DAYS($B$57,G63)</f>
+        <v>1</v>
       </c>
       <c r="I63" s="13" t="n">
-        <f aca="false">B$57+1</f>
-        <v>43917</v>
+        <f aca="false">$B$57+1</f>
+        <v>43918</v>
       </c>
       <c r="J63" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$57,I63)</f>
         <v>-1</v>
       </c>
       <c r="K63" s="13" t="n">
-        <f aca="false">B$57+1</f>
-        <v>43917</v>
+        <f aca="false">$B$57+1</f>
+        <v>43918</v>
       </c>
       <c r="L63" s="0"/>
       <c r="M63" s="0"/>
@@ -2287,39 +2289,40 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C64" s="12" t="n">
         <v>414</v>
       </c>
       <c r="D64" s="1" t="n">
-        <v>267</v>
+        <v>351</v>
       </c>
       <c r="E64" s="12" t="n">
         <f aca="false">D64/83.784</f>
-        <v>3.18676596963621</v>
+        <v>4.18934402749928</v>
       </c>
       <c r="F64" s="12" t="n">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="G64" s="13" t="n">
-        <v>43917</v>
+        <f aca="false">$B$57+1</f>
+        <v>43918</v>
       </c>
       <c r="H64" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$57,G64)</f>
+        <f aca="false">_xlfn.DAYS($B$57,G64)</f>
         <v>-1</v>
       </c>
       <c r="I64" s="13" t="n">
-        <f aca="false">B$57+1</f>
-        <v>43917</v>
+        <f aca="false">$B$57+1</f>
+        <v>43918</v>
       </c>
       <c r="J64" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$57,I64)</f>
         <v>-1</v>
       </c>
       <c r="K64" s="13" t="n">
-        <f aca="false">B$57+1</f>
-        <v>43917</v>
+        <f aca="false">$B$57+1</f>
+        <v>43918</v>
       </c>
       <c r="L64" s="0"/>
       <c r="M64" s="0"/>
@@ -2330,39 +2333,39 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="0" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C65" s="12" t="n">
         <v>50</v>
       </c>
       <c r="D65" s="12" t="n">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="E65" s="12" t="n">
         <f aca="false">D65/10.36</f>
-        <v>7.43243243243243</v>
+        <v>10.1351351351351</v>
       </c>
       <c r="F65" s="12" t="n">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="G65" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H65" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$57,G65)</f>
-        <v>1</v>
+        <f aca="false">_xlfn.DAYS($B$57,G65)</f>
+        <v>2</v>
       </c>
       <c r="I65" s="13" t="n">
-        <f aca="false">B$57+1</f>
-        <v>43917</v>
+        <f aca="false">$B$57+1</f>
+        <v>43918</v>
       </c>
       <c r="J65" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$57,I65)</f>
         <v>-1</v>
       </c>
       <c r="K65" s="13" t="n">
-        <f aca="false">B$57+1</f>
-        <v>43917</v>
+        <f aca="false">$B$57+1</f>
+        <v>43918</v>
       </c>
       <c r="L65" s="0"/>
       <c r="M65" s="0"/>
@@ -2370,6 +2373,424 @@
       <c r="O65" s="0"/>
       <c r="P65" s="0"/>
       <c r="Q65" s="0"/>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D66" s="0"/>
+      <c r="E66" s="0"/>
+      <c r="F66" s="0"/>
+      <c r="G66" s="0"/>
+      <c r="H66" s="0"/>
+      <c r="I66" s="0"/>
+      <c r="J66" s="0"/>
+      <c r="K66" s="0"/>
+      <c r="L66" s="0"/>
+      <c r="M66" s="0"/>
+      <c r="N66" s="0"/>
+      <c r="O66" s="0"/>
+      <c r="P66" s="0"/>
+      <c r="Q66" s="0"/>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D67" s="0"/>
+      <c r="E67" s="0"/>
+      <c r="F67" s="0"/>
+      <c r="G67" s="0"/>
+      <c r="H67" s="0"/>
+      <c r="I67" s="0"/>
+      <c r="J67" s="0"/>
+      <c r="K67" s="0"/>
+      <c r="L67" s="0"/>
+      <c r="M67" s="0"/>
+      <c r="N67" s="0"/>
+      <c r="O67" s="0"/>
+      <c r="P67" s="0"/>
+      <c r="Q67" s="0"/>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B68" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D68" s="0"/>
+      <c r="E68" s="0"/>
+      <c r="F68" s="0"/>
+      <c r="G68" s="0"/>
+      <c r="H68" s="0"/>
+      <c r="I68" s="0"/>
+      <c r="J68" s="0"/>
+      <c r="K68" s="0"/>
+      <c r="L68" s="0"/>
+      <c r="M68" s="0"/>
+      <c r="N68" s="0"/>
+      <c r="O68" s="0"/>
+      <c r="P68" s="0"/>
+      <c r="Q68" s="0"/>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B69" s="7" t="n">
+        <v>43916</v>
+      </c>
+      <c r="D69" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E69" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F69" s="8"/>
+      <c r="G69" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H69" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I69" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J69" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K69" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L69" s="0"/>
+      <c r="M69" s="0"/>
+      <c r="N69" s="0"/>
+      <c r="O69" s="0"/>
+      <c r="P69" s="0"/>
+      <c r="Q69" s="0"/>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B70" s="9"/>
+      <c r="C70" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D70" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E70" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F70" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G70" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H70" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="I70" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="J70" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="K70" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="L70" s="0"/>
+      <c r="M70" s="0"/>
+      <c r="N70" s="0"/>
+      <c r="O70" s="0"/>
+      <c r="P70" s="0"/>
+      <c r="Q70" s="0"/>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B71" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C71" s="12" t="n">
+        <v>300</v>
+      </c>
+      <c r="D71" s="1" t="n">
+        <v>8215</v>
+      </c>
+      <c r="E71" s="12" t="n">
+        <f aca="false">D71/60.48</f>
+        <v>135.830026455026</v>
+      </c>
+      <c r="F71" s="12" t="n">
+        <v>712</v>
+      </c>
+      <c r="G71" s="13" t="n">
+        <v>43900</v>
+      </c>
+      <c r="H71" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$69,G71)</f>
+        <v>16</v>
+      </c>
+      <c r="I71" s="13" t="n">
+        <v>43902</v>
+      </c>
+      <c r="J71" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$69,I71)</f>
+        <v>14</v>
+      </c>
+      <c r="K71" s="13" t="n">
+        <f aca="false">B$69+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L71" s="0"/>
+      <c r="M71" s="0"/>
+      <c r="N71" s="0"/>
+      <c r="O71" s="0"/>
+      <c r="P71" s="0"/>
+      <c r="Q71" s="0"/>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B72" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C72" s="12" t="n">
+        <v>230</v>
+      </c>
+      <c r="D72" s="1" t="n">
+        <v>4365</v>
+      </c>
+      <c r="E72" s="12" t="n">
+        <f aca="false">D72/46.75</f>
+        <v>93.3689839572193</v>
+      </c>
+      <c r="F72" s="12" t="n">
+        <v>718</v>
+      </c>
+      <c r="G72" s="13" t="n">
+        <v>43907</v>
+      </c>
+      <c r="H72" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$69,G72)</f>
+        <v>9</v>
+      </c>
+      <c r="I72" s="13" t="n">
+        <v>43913</v>
+      </c>
+      <c r="J72" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$69,I72)</f>
+        <v>3</v>
+      </c>
+      <c r="K72" s="13" t="n">
+        <f aca="false">B$69+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L72" s="0"/>
+      <c r="M72" s="0"/>
+      <c r="N72" s="0"/>
+      <c r="O72" s="0"/>
+      <c r="P72" s="0"/>
+      <c r="Q72" s="0"/>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B73" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C73" s="12" t="n">
+        <v>330</v>
+      </c>
+      <c r="D73" s="1" t="n">
+        <v>1696</v>
+      </c>
+      <c r="E73" s="12" t="n">
+        <f aca="false">D73/65.27</f>
+        <v>25.9843726060978</v>
+      </c>
+      <c r="F73" s="12" t="n">
+        <v>365</v>
+      </c>
+      <c r="G73" s="13" t="n">
+        <v>43912</v>
+      </c>
+      <c r="H73" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$69,G73)</f>
+        <v>4</v>
+      </c>
+      <c r="I73" s="13" t="n">
+        <v>43914</v>
+      </c>
+      <c r="J73" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$69,I73)</f>
+        <v>2</v>
+      </c>
+      <c r="K73" s="13" t="n">
+        <f aca="false">B$69+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L73" s="0"/>
+      <c r="M73" s="0"/>
+      <c r="N73" s="0"/>
+      <c r="O73" s="0"/>
+      <c r="P73" s="0"/>
+      <c r="Q73" s="0"/>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B74" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C74" s="12" t="n">
+        <v>1660</v>
+      </c>
+      <c r="D74" s="1" t="n">
+        <v>1295</v>
+      </c>
+      <c r="E74" s="12" t="n">
+        <f aca="false">D74/331</f>
+        <v>3.91238670694864</v>
+      </c>
+      <c r="F74" s="12" t="n">
+        <v>268</v>
+      </c>
+      <c r="G74" s="13" t="n">
+        <v>43917</v>
+      </c>
+      <c r="H74" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$69,G74)</f>
+        <v>-1</v>
+      </c>
+      <c r="I74" s="13" t="n">
+        <f aca="false">B$69+1</f>
+        <v>43917</v>
+      </c>
+      <c r="J74" s="1" t="n">
+        <f aca="false">_xlfn.DAYS($B$69,I74)</f>
+        <v>-1</v>
+      </c>
+      <c r="K74" s="13" t="n">
+        <f aca="false">B$69+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L74" s="0"/>
+      <c r="M74" s="0"/>
+      <c r="N74" s="0"/>
+      <c r="O74" s="0"/>
+      <c r="P74" s="0"/>
+      <c r="Q74" s="0"/>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B75" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C75" s="12" t="n">
+        <v>330</v>
+      </c>
+      <c r="D75" s="1" t="n">
+        <v>578</v>
+      </c>
+      <c r="E75" s="12" t="n">
+        <f aca="false">D75/67.79</f>
+        <v>8.52633131730344</v>
+      </c>
+      <c r="F75" s="12" t="n">
+        <v>115</v>
+      </c>
+      <c r="G75" s="13" t="n">
+        <v>43916</v>
+      </c>
+      <c r="H75" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$69,G75)</f>
+        <v>0</v>
+      </c>
+      <c r="I75" s="13" t="n">
+        <f aca="false">B$69+1</f>
+        <v>43917</v>
+      </c>
+      <c r="J75" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$69,I75)</f>
+        <v>-1</v>
+      </c>
+      <c r="K75" s="13" t="n">
+        <f aca="false">B$69+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L75" s="0"/>
+      <c r="M75" s="0"/>
+      <c r="N75" s="0"/>
+      <c r="O75" s="0"/>
+      <c r="P75" s="0"/>
+      <c r="Q75" s="0"/>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B76" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C76" s="12" t="n">
+        <v>414</v>
+      </c>
+      <c r="D76" s="1" t="n">
+        <v>267</v>
+      </c>
+      <c r="E76" s="12" t="n">
+        <f aca="false">D76/83.784</f>
+        <v>3.18676596963621</v>
+      </c>
+      <c r="F76" s="12" t="n">
+        <v>61</v>
+      </c>
+      <c r="G76" s="13" t="n">
+        <v>43917</v>
+      </c>
+      <c r="H76" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$69,G76)</f>
+        <v>-1</v>
+      </c>
+      <c r="I76" s="13" t="n">
+        <f aca="false">B$69+1</f>
+        <v>43917</v>
+      </c>
+      <c r="J76" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$69,I76)</f>
+        <v>-1</v>
+      </c>
+      <c r="K76" s="13" t="n">
+        <f aca="false">B$69+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L76" s="0"/>
+      <c r="M76" s="0"/>
+      <c r="N76" s="0"/>
+      <c r="O76" s="0"/>
+      <c r="P76" s="0"/>
+      <c r="Q76" s="0"/>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B77" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C77" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="D77" s="12" t="n">
+        <v>77</v>
+      </c>
+      <c r="E77" s="12" t="n">
+        <f aca="false">D77/10.36</f>
+        <v>7.43243243243243</v>
+      </c>
+      <c r="F77" s="12" t="n">
+        <v>15</v>
+      </c>
+      <c r="G77" s="13" t="n">
+        <v>43915</v>
+      </c>
+      <c r="H77" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$69,G77)</f>
+        <v>1</v>
+      </c>
+      <c r="I77" s="13" t="n">
+        <f aca="false">B$69+1</f>
+        <v>43917</v>
+      </c>
+      <c r="J77" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$69,I77)</f>
+        <v>-1</v>
+      </c>
+      <c r="K77" s="13" t="n">
+        <f aca="false">B$69+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L77" s="0"/>
+      <c r="M77" s="0"/>
+      <c r="N77" s="0"/>
+      <c r="O77" s="0"/>
+      <c r="P77" s="0"/>
+      <c r="Q77" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
updated with 2020-03-31 data
</commit_message>
<xml_diff>
--- a/covid19 lockdown evaluation .xlsx
+++ b/covid19 lockdown evaluation .xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="49">
   <si>
     <t>Effects of the lockdown issued by governments</t>
   </si>
@@ -56,7 +56,7 @@
     <t>start of crisis</t>
   </si>
   <si>
-    <t>: init day, that is the day of more than 5 deaths per million peaople</t>
+    <t>: init day, that is the day of more than 5 deaths per million people inhabitants</t>
   </si>
   <si>
     <t>Days from start</t>
@@ -83,6 +83,12 @@
     <t>: days of maximum for daily deaths</t>
   </si>
   <si>
+    <t>Crisis duration</t>
+  </si>
+  <si>
+    <t>: # of days from init to end of crisis (eventually, crisi duration as of today)</t>
+  </si>
+  <si>
     <t>NOTE:</t>
   </si>
   <si>
@@ -110,6 +116,9 @@
     <t>End of</t>
   </si>
   <si>
+    <t>Crisis</t>
+  </si>
+  <si>
     <t>Start num</t>
   </si>
   <si>
@@ -129,6 +138,9 @@
   </si>
   <si>
     <t>lockdown</t>
+  </si>
+  <si>
+    <t>duration</t>
   </si>
   <si>
     <t>Italy</t>
@@ -329,15 +341,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q77"/>
+  <dimension ref="A1:Q90"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="1.94387755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="1" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.1938775510204"/>
     <col collapsed="false" hidden="false" max="17" min="7" style="1" width="11.5204081632653"/>
@@ -635,7 +648,12 @@
       <c r="Q14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="4"/>
+      <c r="B15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>23</v>
+      </c>
       <c r="D15" s="0"/>
       <c r="E15" s="0"/>
       <c r="F15" s="0"/>
@@ -652,12 +670,7 @@
       <c r="Q15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>23</v>
-      </c>
+      <c r="B16" s="4"/>
       <c r="D16" s="0"/>
       <c r="E16" s="0"/>
       <c r="F16" s="0"/>
@@ -674,9 +687,11 @@
       <c r="Q16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="4"/>
-      <c r="C17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>24</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="D17" s="0"/>
       <c r="E17" s="0"/>
@@ -695,7 +710,9 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="4"/>
-      <c r="C18" s="5"/>
+      <c r="C18" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="D18" s="0"/>
       <c r="E18" s="0"/>
       <c r="F18" s="0"/>
@@ -730,9 +747,8 @@
       <c r="Q19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="5"/>
       <c r="D20" s="0"/>
       <c r="E20" s="0"/>
       <c r="F20" s="0"/>
@@ -749,29 +765,17 @@
       <c r="Q20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="7" t="n">
-        <v>43920</v>
+      <c r="B21" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="D21" s="0"/>
-      <c r="E21" s="8" t="s">
-        <v>26</v>
-      </c>
+      <c r="E21" s="0"/>
       <c r="F21" s="0"/>
-      <c r="G21" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H21" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="I21" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="J21" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="K21" s="8" t="s">
-        <v>30</v>
-      </c>
+      <c r="G21" s="0"/>
+      <c r="H21" s="0"/>
+      <c r="I21" s="0"/>
+      <c r="J21" s="0"/>
+      <c r="K21" s="0"/>
       <c r="L21" s="0"/>
       <c r="M21" s="0"/>
       <c r="N21" s="0"/>
@@ -780,35 +784,32 @@
       <c r="Q21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="9"/>
-      <c r="C22" s="10" t="s">
+      <c r="B22" s="7" t="n">
+        <v>43921</v>
+      </c>
+      <c r="D22" s="0"/>
+      <c r="E22" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F22" s="0"/>
+      <c r="G22" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I22" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E22" s="10" t="s">
+      <c r="J22" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K22" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="L22" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="G22" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H22" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="I22" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="J22" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="K22" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="L22" s="0"/>
       <c r="M22" s="0"/>
       <c r="N22" s="0"/>
       <c r="O22" s="0"/>
@@ -816,41 +817,37 @@
       <c r="Q22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="9"/>
+      <c r="C23" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H23" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="12" t="n">
-        <v>300</v>
-      </c>
-      <c r="D23" s="1" t="n">
-        <v>11591</v>
-      </c>
-      <c r="E23" s="12" t="n">
-        <f aca="false">D23/60.48</f>
-        <v>191.650132275132</v>
-      </c>
-      <c r="F23" s="12" t="n">
-        <v>812</v>
-      </c>
-      <c r="G23" s="13" t="n">
-        <v>43900</v>
-      </c>
-      <c r="H23" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$21,G23)</f>
-        <v>20</v>
-      </c>
-      <c r="I23" s="13" t="n">
-        <v>43902</v>
-      </c>
-      <c r="J23" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$21,I23)</f>
-        <v>18</v>
-      </c>
-      <c r="K23" s="13" t="n">
-        <f aca="false">$B$33+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L23" s="0"/>
+      <c r="I23" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="J23" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K23" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L23" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="M23" s="0"/>
       <c r="N23" s="0"/>
       <c r="O23" s="0"/>
@@ -859,40 +856,43 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C24" s="12" t="n">
-        <v>230</v>
+        <v>300</v>
       </c>
       <c r="D24" s="1" t="n">
-        <v>7716</v>
+        <v>12428</v>
       </c>
       <c r="E24" s="12" t="n">
-        <f aca="false">D24/46.75</f>
-        <v>165.048128342246</v>
+        <f aca="false">D24/60.48</f>
+        <v>205.489417989418</v>
       </c>
       <c r="F24" s="12" t="n">
-        <v>913</v>
+        <v>837</v>
       </c>
       <c r="G24" s="13" t="n">
-        <v>43907</v>
+        <v>43900</v>
       </c>
       <c r="H24" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$21,G24)</f>
-        <v>13</v>
+        <f aca="false">_xlfn.DAYS($B$22,G24)</f>
+        <v>21</v>
       </c>
       <c r="I24" s="13" t="n">
-        <v>43913</v>
+        <v>43902</v>
       </c>
       <c r="J24" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$21,I24)</f>
-        <v>7</v>
+        <f aca="false">_xlfn.DAYS($B$22,I24)</f>
+        <v>19</v>
       </c>
       <c r="K24" s="13" t="n">
-        <f aca="false">$B$33+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L24" s="0"/>
+        <f aca="false">$B$22+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L24" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K24,G24)</f>
+        <v>22</v>
+      </c>
       <c r="M24" s="0"/>
       <c r="N24" s="0"/>
       <c r="O24" s="0"/>
@@ -901,40 +901,43 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C25" s="12" t="n">
-        <v>330</v>
+        <v>230</v>
       </c>
       <c r="D25" s="1" t="n">
-        <v>3024</v>
+        <v>8464</v>
       </c>
       <c r="E25" s="12" t="n">
-        <f aca="false">D25/65.27</f>
-        <v>46.3306266278535</v>
+        <f aca="false">D25/46.75</f>
+        <v>181.048128342246</v>
       </c>
       <c r="F25" s="12" t="n">
-        <v>418</v>
+        <v>748</v>
       </c>
       <c r="G25" s="13" t="n">
-        <v>43912</v>
+        <v>43907</v>
       </c>
       <c r="H25" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$21,G25)</f>
+        <f aca="false">_xlfn.DAYS($B$22,G25)</f>
+        <v>14</v>
+      </c>
+      <c r="I25" s="13" t="n">
+        <v>43913</v>
+      </c>
+      <c r="J25" s="1" t="n">
+        <f aca="false">_xlfn.DAYS($B$22,I25)</f>
         <v>8</v>
       </c>
-      <c r="I25" s="13" t="n">
-        <v>43914</v>
-      </c>
-      <c r="J25" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$21,I25)</f>
-        <v>6</v>
-      </c>
       <c r="K25" s="13" t="n">
-        <f aca="false">$B$33+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L25" s="0"/>
+        <f aca="false">$B$22+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L25" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K25,G25)</f>
+        <v>15</v>
+      </c>
       <c r="M25" s="0"/>
       <c r="N25" s="0"/>
       <c r="O25" s="0"/>
@@ -943,41 +946,43 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C26" s="12" t="n">
-        <v>50</v>
-      </c>
-      <c r="D26" s="12" t="n">
-        <v>146</v>
+        <v>330</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <v>3523</v>
       </c>
       <c r="E26" s="12" t="n">
-        <f aca="false">D26/10.36</f>
-        <v>14.0926640926641</v>
+        <f aca="false">D26/65.27</f>
+        <v>53.9757928604259</v>
       </c>
       <c r="F26" s="12" t="n">
-        <v>36</v>
+        <v>499</v>
       </c>
       <c r="G26" s="13" t="n">
-        <v>43915</v>
+        <v>43912</v>
       </c>
       <c r="H26" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$21,G26)</f>
-        <v>5</v>
+        <f aca="false">_xlfn.DAYS($B$22,G26)</f>
+        <v>9</v>
       </c>
       <c r="I26" s="13" t="n">
-        <f aca="false">$B$21+1</f>
-        <v>43921</v>
+        <v>43914</v>
       </c>
       <c r="J26" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$21,I26)</f>
-        <v>-1</v>
+        <f aca="false">_xlfn.DAYS($B$22,I26)</f>
+        <v>7</v>
       </c>
       <c r="K26" s="13" t="n">
-        <f aca="false">$B$33+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L26" s="0"/>
+        <f aca="false">$B$22+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L26" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K26,G26)</f>
+        <v>10</v>
+      </c>
       <c r="M26" s="0"/>
       <c r="N26" s="0"/>
       <c r="O26" s="0"/>
@@ -986,41 +991,44 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C27" s="12" t="n">
-        <v>330</v>
-      </c>
-      <c r="D27" s="1" t="n">
-        <v>1408</v>
+        <v>50</v>
+      </c>
+      <c r="D27" s="12" t="n">
+        <v>180</v>
       </c>
       <c r="E27" s="12" t="n">
-        <f aca="false">D27/67.79</f>
-        <v>20.770025077445</v>
+        <f aca="false">D27/10.36</f>
+        <v>17.3745173745174</v>
       </c>
       <c r="F27" s="12" t="n">
-        <v>180</v>
+        <v>34</v>
       </c>
       <c r="G27" s="13" t="n">
-        <v>43916</v>
+        <v>43915</v>
       </c>
       <c r="H27" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$21,G27)</f>
-        <v>4</v>
+        <f aca="false">_xlfn.DAYS($B$22,G27)</f>
+        <v>6</v>
       </c>
       <c r="I27" s="13" t="n">
-        <f aca="false">$B$21+1</f>
-        <v>43921</v>
+        <f aca="false">$B$22+1</f>
+        <v>43922</v>
       </c>
       <c r="J27" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$21,I27)</f>
+        <f aca="false">_xlfn.DAYS($B$22,I27)</f>
         <v>-1</v>
       </c>
       <c r="K27" s="13" t="n">
-        <f aca="false">$B$33+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L27" s="0"/>
+        <f aca="false">$B$22+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L27" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K27,G27)</f>
+        <v>7</v>
+      </c>
       <c r="M27" s="0"/>
       <c r="N27" s="0"/>
       <c r="O27" s="0"/>
@@ -1029,40 +1037,44 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C28" s="12" t="n">
-        <v>1660</v>
+        <v>330</v>
       </c>
       <c r="D28" s="1" t="n">
-        <v>3156</v>
+        <v>1789</v>
       </c>
       <c r="E28" s="12" t="n">
-        <f aca="false">D28/331</f>
-        <v>9.53474320241692</v>
+        <f aca="false">D28/67.79</f>
+        <v>26.390323056498</v>
       </c>
       <c r="F28" s="12" t="n">
-        <v>573</v>
+        <v>381</v>
       </c>
       <c r="G28" s="13" t="n">
-        <v>43917</v>
+        <v>43916</v>
       </c>
       <c r="H28" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$21,G28)</f>
-        <v>3</v>
+        <f aca="false">_xlfn.DAYS($B$22,G28)</f>
+        <v>5</v>
       </c>
       <c r="I28" s="13" t="n">
-        <v>43920</v>
+        <f aca="false">$B$22+1</f>
+        <v>43922</v>
       </c>
       <c r="J28" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$21,I28)</f>
-        <v>0</v>
+        <f aca="false">_xlfn.DAYS($B$22,I28)</f>
+        <v>-1</v>
       </c>
       <c r="K28" s="13" t="n">
-        <f aca="false">$B$33+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L28" s="0"/>
+        <f aca="false">$B$22+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L28" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K28,G28)</f>
+        <v>6</v>
+      </c>
       <c r="M28" s="0"/>
       <c r="N28" s="0"/>
       <c r="O28" s="0"/>
@@ -1071,41 +1083,44 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C29" s="12" t="n">
-        <v>414</v>
+        <v>1660</v>
       </c>
       <c r="D29" s="1" t="n">
-        <v>645</v>
+        <v>4053</v>
       </c>
       <c r="E29" s="12" t="n">
-        <f aca="false">D29/83.784</f>
-        <v>7.69836723002005</v>
+        <f aca="false">D29/331</f>
+        <v>12.2447129909366</v>
       </c>
       <c r="F29" s="12" t="n">
-        <v>104</v>
+        <v>912</v>
       </c>
       <c r="G29" s="13" t="n">
-        <v>43918</v>
+        <v>43917</v>
       </c>
       <c r="H29" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$21,G29)</f>
-        <v>2</v>
+        <f aca="false">_xlfn.DAYS($B$22,G29)</f>
+        <v>4</v>
       </c>
       <c r="I29" s="13" t="n">
-        <f aca="false">$B$21+1</f>
-        <v>43921</v>
+        <f aca="false">$B$22+1</f>
+        <v>43922</v>
       </c>
       <c r="J29" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$21,I29)</f>
+        <f aca="false">_xlfn.DAYS($B$22,I29)</f>
         <v>-1</v>
       </c>
       <c r="K29" s="13" t="n">
-        <f aca="false">$B$33+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L29" s="0"/>
+        <f aca="false">$B$22+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L29" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K29,G29)</f>
+        <v>5</v>
+      </c>
       <c r="M29" s="0"/>
       <c r="N29" s="0"/>
       <c r="O29" s="0"/>
@@ -1113,17 +1128,45 @@
       <c r="Q29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="4"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="0"/>
-      <c r="E30" s="0"/>
-      <c r="F30" s="0"/>
-      <c r="G30" s="0"/>
-      <c r="H30" s="0"/>
-      <c r="I30" s="0"/>
-      <c r="J30" s="0"/>
-      <c r="K30" s="0"/>
-      <c r="L30" s="0"/>
+      <c r="B30" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" s="12" t="n">
+        <v>414</v>
+      </c>
+      <c r="D30" s="1" t="n">
+        <v>775</v>
+      </c>
+      <c r="E30" s="12" t="n">
+        <f aca="false">D30/83.784</f>
+        <v>9.24997612909386</v>
+      </c>
+      <c r="F30" s="12" t="n">
+        <v>130</v>
+      </c>
+      <c r="G30" s="13" t="n">
+        <v>43918</v>
+      </c>
+      <c r="H30" s="1" t="n">
+        <f aca="false">_xlfn.DAYS($B$22,G30)</f>
+        <v>3</v>
+      </c>
+      <c r="I30" s="13" t="n">
+        <f aca="false">$B$22+1</f>
+        <v>43922</v>
+      </c>
+      <c r="J30" s="1" t="n">
+        <f aca="false">_xlfn.DAYS($B$22,I30)</f>
+        <v>-1</v>
+      </c>
+      <c r="K30" s="13" t="n">
+        <f aca="false">$B$22+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L30" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K30,G30)</f>
+        <v>4</v>
+      </c>
       <c r="M30" s="0"/>
       <c r="N30" s="0"/>
       <c r="O30" s="0"/>
@@ -1131,16 +1174,15 @@
       <c r="Q30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="4"/>
-      <c r="C31" s="5"/>
+      <c r="C31" s="12"/>
       <c r="D31" s="0"/>
-      <c r="E31" s="0"/>
-      <c r="F31" s="0"/>
-      <c r="G31" s="0"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="13"/>
       <c r="H31" s="0"/>
-      <c r="I31" s="0"/>
+      <c r="I31" s="13"/>
       <c r="J31" s="0"/>
-      <c r="K31" s="0"/>
+      <c r="K31" s="13"/>
       <c r="L31" s="0"/>
       <c r="M31" s="0"/>
       <c r="N31" s="0"/>
@@ -1149,17 +1191,15 @@
       <c r="Q31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="C32" s="12"/>
       <c r="D32" s="0"/>
-      <c r="E32" s="0"/>
-      <c r="F32" s="0"/>
-      <c r="G32" s="0"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="13"/>
       <c r="H32" s="0"/>
-      <c r="I32" s="0"/>
+      <c r="I32" s="13"/>
       <c r="J32" s="0"/>
-      <c r="K32" s="0"/>
+      <c r="K32" s="13"/>
       <c r="L32" s="0"/>
       <c r="M32" s="0"/>
       <c r="N32" s="0"/>
@@ -1168,29 +1208,17 @@
       <c r="Q32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="7" t="n">
-        <v>43919</v>
+      <c r="B33" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="D33" s="0"/>
-      <c r="E33" s="8" t="s">
-        <v>26</v>
-      </c>
+      <c r="E33" s="0"/>
       <c r="F33" s="0"/>
-      <c r="G33" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H33" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="I33" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="J33" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="K33" s="8" t="s">
-        <v>30</v>
-      </c>
+      <c r="G33" s="0"/>
+      <c r="H33" s="0"/>
+      <c r="I33" s="0"/>
+      <c r="J33" s="0"/>
+      <c r="K33" s="0"/>
       <c r="L33" s="0"/>
       <c r="M33" s="0"/>
       <c r="N33" s="0"/>
@@ -1199,33 +1227,28 @@
       <c r="Q33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="9"/>
-      <c r="C34" s="10" t="s">
+      <c r="B34" s="7" t="n">
+        <v>43920</v>
+      </c>
+      <c r="D34" s="0"/>
+      <c r="E34" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F34" s="0"/>
+      <c r="G34" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I34" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E34" s="10" t="s">
+      <c r="J34" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K34" s="8" t="s">
         <v>32</v>
-      </c>
-      <c r="F34" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G34" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H34" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="I34" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="J34" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="K34" s="8" t="s">
-        <v>34</v>
       </c>
       <c r="L34" s="0"/>
       <c r="M34" s="0"/>
@@ -1235,39 +1258,33 @@
       <c r="Q34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="0" t="s">
+      <c r="B35" s="9"/>
+      <c r="C35" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H35" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="12" t="n">
-        <v>300</v>
-      </c>
-      <c r="D35" s="1" t="n">
-        <v>10779</v>
-      </c>
-      <c r="E35" s="12" t="n">
-        <f aca="false">D35/60.48</f>
-        <v>178.224206349206</v>
-      </c>
-      <c r="F35" s="12" t="n">
-        <v>756</v>
-      </c>
-      <c r="G35" s="13" t="n">
-        <v>43900</v>
-      </c>
-      <c r="H35" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$33,G35)</f>
-        <v>19</v>
-      </c>
-      <c r="I35" s="13" t="n">
-        <v>43902</v>
-      </c>
-      <c r="J35" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$33,I35)</f>
-        <v>17</v>
-      </c>
-      <c r="K35" s="13" t="n">
-        <f aca="false">$B$33+1</f>
-        <v>43920</v>
+      <c r="I35" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="J35" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K35" s="8" t="s">
+        <v>37</v>
       </c>
       <c r="L35" s="0"/>
       <c r="M35" s="0"/>
@@ -1278,37 +1295,37 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C36" s="12" t="n">
-        <v>230</v>
+        <v>300</v>
       </c>
       <c r="D36" s="1" t="n">
-        <v>6803</v>
+        <v>11591</v>
       </c>
       <c r="E36" s="12" t="n">
-        <f aca="false">D36/46.75</f>
-        <v>145.51871657754</v>
+        <f aca="false">D36/60.48</f>
+        <v>191.650132275132</v>
       </c>
       <c r="F36" s="12" t="n">
-        <v>821</v>
+        <v>812</v>
       </c>
       <c r="G36" s="13" t="n">
-        <v>43907</v>
+        <v>43900</v>
       </c>
       <c r="H36" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$33,G36)</f>
-        <v>12</v>
+        <f aca="false">_xlfn.DAYS($B$34,G36)</f>
+        <v>20</v>
       </c>
       <c r="I36" s="13" t="n">
-        <v>43913</v>
+        <v>43902</v>
       </c>
       <c r="J36" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$33,I36)</f>
-        <v>6</v>
+        <f aca="false">_xlfn.DAYS($B$34,I36)</f>
+        <v>18</v>
       </c>
       <c r="K36" s="13" t="n">
-        <f aca="false">$B$33+1</f>
+        <f aca="false">$B$46+1</f>
         <v>43920</v>
       </c>
       <c r="L36" s="0"/>
@@ -1320,37 +1337,37 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C37" s="12" t="n">
-        <v>330</v>
+        <v>230</v>
       </c>
       <c r="D37" s="1" t="n">
-        <v>2606</v>
+        <v>7716</v>
       </c>
       <c r="E37" s="12" t="n">
-        <f aca="false">D37/65.27</f>
-        <v>39.9264593228129</v>
+        <f aca="false">D37/46.75</f>
+        <v>165.048128342246</v>
       </c>
       <c r="F37" s="12" t="n">
-        <v>292</v>
+        <v>913</v>
       </c>
       <c r="G37" s="13" t="n">
-        <v>43912</v>
+        <v>43907</v>
       </c>
       <c r="H37" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$33,G37)</f>
+        <f aca="false">_xlfn.DAYS($B$34,G37)</f>
+        <v>13</v>
+      </c>
+      <c r="I37" s="13" t="n">
+        <v>43913</v>
+      </c>
+      <c r="J37" s="1" t="n">
+        <f aca="false">_xlfn.DAYS($B$34,I37)</f>
         <v>7</v>
       </c>
-      <c r="I37" s="13" t="n">
-        <v>43914</v>
-      </c>
-      <c r="J37" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$33,I37)</f>
-        <v>5</v>
-      </c>
       <c r="K37" s="13" t="n">
-        <f aca="false">$B$33+1</f>
+        <f aca="false">$B$46+1</f>
         <v>43920</v>
       </c>
       <c r="L37" s="0"/>
@@ -1362,38 +1379,37 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C38" s="12" t="n">
-        <v>1660</v>
+        <v>330</v>
       </c>
       <c r="D38" s="1" t="n">
-        <v>2583</v>
+        <v>3024</v>
       </c>
       <c r="E38" s="12" t="n">
-        <f aca="false">D38/331</f>
-        <v>7.8036253776435</v>
+        <f aca="false">D38/65.27</f>
+        <v>46.3306266278535</v>
       </c>
       <c r="F38" s="12" t="n">
-        <v>363</v>
+        <v>418</v>
       </c>
       <c r="G38" s="13" t="n">
-        <v>43917</v>
+        <v>43912</v>
       </c>
       <c r="H38" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$33,G38)</f>
-        <v>2</v>
+        <f aca="false">_xlfn.DAYS($B$34,G38)</f>
+        <v>8</v>
       </c>
       <c r="I38" s="13" t="n">
-        <f aca="false">$B$33+1</f>
-        <v>43920</v>
+        <v>43914</v>
       </c>
       <c r="J38" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$33,I38)</f>
-        <v>-1</v>
+        <f aca="false">_xlfn.DAYS($B$34,I38)</f>
+        <v>6</v>
       </c>
       <c r="K38" s="13" t="n">
-        <f aca="false">$B$33+1</f>
+        <f aca="false">$B$46+1</f>
         <v>43920</v>
       </c>
       <c r="L38" s="0"/>
@@ -1405,38 +1421,38 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C39" s="12" t="n">
-        <v>330</v>
-      </c>
-      <c r="D39" s="1" t="n">
-        <v>1228</v>
+        <v>50</v>
+      </c>
+      <c r="D39" s="12" t="n">
+        <v>146</v>
       </c>
       <c r="E39" s="12" t="n">
-        <f aca="false">D39/67.79</f>
-        <v>18.1147661897035</v>
+        <f aca="false">D39/10.36</f>
+        <v>14.0926640926641</v>
       </c>
       <c r="F39" s="12" t="n">
-        <v>209</v>
+        <v>36</v>
       </c>
       <c r="G39" s="13" t="n">
-        <v>43916</v>
+        <v>43915</v>
       </c>
       <c r="H39" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$33,G39)</f>
-        <v>3</v>
+        <f aca="false">_xlfn.DAYS($B$34,G39)</f>
+        <v>5</v>
       </c>
       <c r="I39" s="13" t="n">
-        <f aca="false">$B$33+1</f>
-        <v>43920</v>
+        <f aca="false">$B$34+1</f>
+        <v>43921</v>
       </c>
       <c r="J39" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$33,I39)</f>
+        <f aca="false">_xlfn.DAYS($B$34,I39)</f>
         <v>-1</v>
       </c>
       <c r="K39" s="13" t="n">
-        <f aca="false">$B$33+1</f>
+        <f aca="false">$B$46+1</f>
         <v>43920</v>
       </c>
       <c r="L39" s="0"/>
@@ -1448,38 +1464,38 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C40" s="12" t="n">
-        <v>414</v>
+        <v>330</v>
       </c>
       <c r="D40" s="1" t="n">
-        <v>541</v>
+        <v>1408</v>
       </c>
       <c r="E40" s="12" t="n">
-        <f aca="false">D40/83.784</f>
-        <v>6.457080110761</v>
+        <f aca="false">D40/67.79</f>
+        <v>20.770025077445</v>
       </c>
       <c r="F40" s="12" t="n">
-        <v>108</v>
+        <v>180</v>
       </c>
       <c r="G40" s="13" t="n">
-        <v>43918</v>
+        <v>43916</v>
       </c>
       <c r="H40" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$33,G40)</f>
-        <v>1</v>
+        <f aca="false">_xlfn.DAYS($B$34,G40)</f>
+        <v>4</v>
       </c>
       <c r="I40" s="13" t="n">
-        <f aca="false">$B$33+1</f>
-        <v>43920</v>
+        <f aca="false">$B$34+1</f>
+        <v>43921</v>
       </c>
       <c r="J40" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$33,I40)</f>
+        <f aca="false">_xlfn.DAYS($B$34,I40)</f>
         <v>-1</v>
       </c>
       <c r="K40" s="13" t="n">
-        <f aca="false">$B$33+1</f>
+        <f aca="false">$B$46+1</f>
         <v>43920</v>
       </c>
       <c r="L40" s="0"/>
@@ -1491,38 +1507,37 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="0" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C41" s="12" t="n">
-        <v>50</v>
-      </c>
-      <c r="D41" s="12" t="n">
-        <v>110</v>
+        <v>1660</v>
+      </c>
+      <c r="D41" s="1" t="n">
+        <v>3141</v>
       </c>
       <c r="E41" s="12" t="n">
-        <f aca="false">D41/10.36</f>
-        <v>10.6177606177606</v>
+        <f aca="false">D41/331</f>
+        <v>9.48942598187311</v>
       </c>
       <c r="F41" s="12" t="n">
-        <v>5</v>
+        <v>573</v>
       </c>
       <c r="G41" s="13" t="n">
-        <v>43915</v>
+        <v>43917</v>
       </c>
       <c r="H41" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$33,G41)</f>
-        <v>4</v>
+        <f aca="false">_xlfn.DAYS($B$34,G41)</f>
+        <v>3</v>
       </c>
       <c r="I41" s="13" t="n">
-        <f aca="false">$B$33+1</f>
         <v>43920</v>
       </c>
       <c r="J41" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$33,I41)</f>
-        <v>-1</v>
+        <f aca="false">_xlfn.DAYS($B$34,I41)</f>
+        <v>0</v>
       </c>
       <c r="K41" s="13" t="n">
-        <f aca="false">$B$33+1</f>
+        <f aca="false">$B$46+1</f>
         <v>43920</v>
       </c>
       <c r="L41" s="0"/>
@@ -1533,16 +1548,41 @@
       <c r="Q41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="4"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="0"/>
-      <c r="E42" s="0"/>
-      <c r="F42" s="0"/>
-      <c r="G42" s="0"/>
-      <c r="H42" s="0"/>
-      <c r="I42" s="0"/>
-      <c r="J42" s="0"/>
-      <c r="K42" s="0"/>
+      <c r="B42" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42" s="12" t="n">
+        <v>414</v>
+      </c>
+      <c r="D42" s="1" t="n">
+        <v>645</v>
+      </c>
+      <c r="E42" s="12" t="n">
+        <f aca="false">D42/83.784</f>
+        <v>7.69836723002005</v>
+      </c>
+      <c r="F42" s="12" t="n">
+        <v>104</v>
+      </c>
+      <c r="G42" s="13" t="n">
+        <v>43918</v>
+      </c>
+      <c r="H42" s="1" t="n">
+        <f aca="false">_xlfn.DAYS($B$34,G42)</f>
+        <v>2</v>
+      </c>
+      <c r="I42" s="13" t="n">
+        <f aca="false">$B$34+1</f>
+        <v>43921</v>
+      </c>
+      <c r="J42" s="1" t="n">
+        <f aca="false">_xlfn.DAYS($B$34,I42)</f>
+        <v>-1</v>
+      </c>
+      <c r="K42" s="13" t="n">
+        <f aca="false">$B$46+1</f>
+        <v>43920</v>
+      </c>
       <c r="L42" s="0"/>
       <c r="M42" s="0"/>
       <c r="N42" s="0"/>
@@ -1569,9 +1609,8 @@
       <c r="Q43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="B44" s="4"/>
+      <c r="C44" s="5"/>
       <c r="D44" s="0"/>
       <c r="E44" s="0"/>
       <c r="F44" s="0"/>
@@ -1588,31 +1627,17 @@
       <c r="Q44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="7" t="n">
-        <v>43918</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E45" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F45" s="8"/>
-      <c r="G45" s="8" t="s">
+      <c r="B45" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H45" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="I45" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="J45" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="K45" s="8" t="s">
-        <v>30</v>
-      </c>
+      <c r="D45" s="0"/>
+      <c r="E45" s="0"/>
+      <c r="F45" s="0"/>
+      <c r="G45" s="0"/>
+      <c r="H45" s="0"/>
+      <c r="I45" s="0"/>
+      <c r="J45" s="0"/>
+      <c r="K45" s="0"/>
       <c r="L45" s="0"/>
       <c r="M45" s="0"/>
       <c r="N45" s="0"/>
@@ -1621,33 +1646,28 @@
       <c r="Q45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="9"/>
-      <c r="C46" s="10" t="s">
+      <c r="B46" s="7" t="n">
+        <v>43919</v>
+      </c>
+      <c r="D46" s="0"/>
+      <c r="E46" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F46" s="0"/>
+      <c r="G46" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H46" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I46" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D46" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E46" s="10" t="s">
+      <c r="J46" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K46" s="8" t="s">
         <v>32</v>
-      </c>
-      <c r="F46" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G46" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H46" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="I46" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="J46" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="K46" s="8" t="s">
-        <v>34</v>
       </c>
       <c r="L46" s="0"/>
       <c r="M46" s="0"/>
@@ -1657,39 +1677,33 @@
       <c r="Q46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="0" t="s">
+      <c r="B47" s="9"/>
+      <c r="C47" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F47" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G47" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H47" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C47" s="12" t="n">
-        <v>300</v>
-      </c>
-      <c r="D47" s="1" t="n">
-        <v>10023</v>
-      </c>
-      <c r="E47" s="12" t="n">
-        <f aca="false">D47/60.48</f>
-        <v>165.724206349206</v>
-      </c>
-      <c r="F47" s="12" t="n">
-        <v>889</v>
-      </c>
-      <c r="G47" s="13" t="n">
-        <v>43900</v>
-      </c>
-      <c r="H47" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$45,G47)</f>
-        <v>18</v>
-      </c>
-      <c r="I47" s="13" t="n">
-        <v>43902</v>
-      </c>
-      <c r="J47" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$57,I47)</f>
-        <v>15</v>
-      </c>
-      <c r="K47" s="13" t="n">
-        <f aca="false">$B$45+1</f>
-        <v>43919</v>
+      <c r="I47" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="J47" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K47" s="8" t="s">
+        <v>37</v>
       </c>
       <c r="L47" s="0"/>
       <c r="M47" s="0"/>
@@ -1700,38 +1714,38 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C48" s="12" t="n">
-        <v>230</v>
+        <v>300</v>
       </c>
       <c r="D48" s="1" t="n">
-        <v>5982</v>
+        <v>10779</v>
       </c>
       <c r="E48" s="12" t="n">
-        <f aca="false">D48/46.75</f>
-        <v>127.957219251337</v>
+        <f aca="false">D48/60.48</f>
+        <v>178.224206349206</v>
       </c>
       <c r="F48" s="12" t="n">
-        <v>844</v>
+        <v>756</v>
       </c>
       <c r="G48" s="13" t="n">
-        <v>43907</v>
+        <v>43900</v>
       </c>
       <c r="H48" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$45,G48)</f>
-        <v>11</v>
+        <f aca="false">_xlfn.DAYS($B$46,G48)</f>
+        <v>19</v>
       </c>
       <c r="I48" s="13" t="n">
-        <v>43913</v>
+        <v>43902</v>
       </c>
       <c r="J48" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$57,I48)</f>
-        <v>4</v>
+        <f aca="false">_xlfn.DAYS($B$46,I48)</f>
+        <v>17</v>
       </c>
       <c r="K48" s="13" t="n">
-        <f aca="false">$B$45+1</f>
-        <v>43919</v>
+        <f aca="false">$B$46+1</f>
+        <v>43920</v>
       </c>
       <c r="L48" s="0"/>
       <c r="M48" s="0"/>
@@ -1742,38 +1756,38 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C49" s="12" t="n">
-        <v>330</v>
+        <v>230</v>
       </c>
       <c r="D49" s="1" t="n">
-        <v>2314</v>
+        <v>6803</v>
       </c>
       <c r="E49" s="12" t="n">
-        <f aca="false">D49/65.27</f>
-        <v>35.4527347939329</v>
+        <f aca="false">D49/46.75</f>
+        <v>145.51871657754</v>
       </c>
       <c r="F49" s="12" t="n">
-        <v>319</v>
+        <v>821</v>
       </c>
       <c r="G49" s="13" t="n">
-        <v>43912</v>
+        <v>43907</v>
       </c>
       <c r="H49" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$45,G49)</f>
+        <f aca="false">_xlfn.DAYS($B$46,G49)</f>
+        <v>12</v>
+      </c>
+      <c r="I49" s="13" t="n">
+        <v>43913</v>
+      </c>
+      <c r="J49" s="1" t="n">
+        <f aca="false">_xlfn.DAYS($B$46,I49)</f>
         <v>6</v>
       </c>
-      <c r="I49" s="13" t="n">
-        <v>43914</v>
-      </c>
-      <c r="J49" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$57,I49)</f>
-        <v>3</v>
-      </c>
       <c r="K49" s="13" t="n">
-        <f aca="false">$B$45+1</f>
-        <v>43919</v>
+        <f aca="false">$B$46+1</f>
+        <v>43920</v>
       </c>
       <c r="L49" s="0"/>
       <c r="M49" s="0"/>
@@ -1784,39 +1798,38 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C50" s="12" t="n">
-        <v>1660</v>
+        <v>330</v>
       </c>
       <c r="D50" s="1" t="n">
-        <v>2221</v>
+        <v>2606</v>
       </c>
       <c r="E50" s="12" t="n">
-        <f aca="false">D50/331</f>
-        <v>6.70996978851964</v>
+        <f aca="false">D50/65.27</f>
+        <v>39.9264593228129</v>
       </c>
       <c r="F50" s="12" t="n">
-        <v>525</v>
+        <v>292</v>
       </c>
       <c r="G50" s="13" t="n">
-        <v>43917</v>
+        <v>43912</v>
       </c>
       <c r="H50" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$45,G50)</f>
-        <v>1</v>
+        <f aca="false">_xlfn.DAYS($B$46,G50)</f>
+        <v>7</v>
       </c>
       <c r="I50" s="13" t="n">
-        <f aca="false">$B$45+1</f>
-        <v>43919</v>
+        <v>43914</v>
       </c>
       <c r="J50" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$45,I50)</f>
-        <v>-1</v>
+        <f aca="false">_xlfn.DAYS($B$46,I50)</f>
+        <v>5</v>
       </c>
       <c r="K50" s="13" t="n">
-        <f aca="false">$B$45+1</f>
-        <v>43919</v>
+        <f aca="false">$B$46+1</f>
+        <v>43920</v>
       </c>
       <c r="L50" s="0"/>
       <c r="M50" s="0"/>
@@ -1827,39 +1840,39 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C51" s="12" t="n">
-        <v>330</v>
+        <v>1660</v>
       </c>
       <c r="D51" s="1" t="n">
-        <v>1019</v>
+        <v>2583</v>
       </c>
       <c r="E51" s="12" t="n">
-        <f aca="false">D51/67.79</f>
-        <v>15.0317155922702</v>
+        <f aca="false">D51/331</f>
+        <v>7.8036253776435</v>
       </c>
       <c r="F51" s="12" t="n">
-        <v>260</v>
+        <v>363</v>
       </c>
       <c r="G51" s="13" t="n">
-        <v>43916</v>
+        <v>43917</v>
       </c>
       <c r="H51" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$45,G51)</f>
+        <f aca="false">_xlfn.DAYS($B$46,G51)</f>
         <v>2</v>
       </c>
       <c r="I51" s="13" t="n">
-        <f aca="false">$B$45+1</f>
-        <v>43919</v>
+        <f aca="false">$B$46+1</f>
+        <v>43920</v>
       </c>
       <c r="J51" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$45,I51)</f>
+        <f aca="false">_xlfn.DAYS($B$46,I51)</f>
         <v>-1</v>
       </c>
       <c r="K51" s="13" t="n">
-        <f aca="false">$B$45+1</f>
-        <v>43919</v>
+        <f aca="false">$B$46+1</f>
+        <v>43920</v>
       </c>
       <c r="L51" s="0"/>
       <c r="M51" s="0"/>
@@ -1870,39 +1883,39 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C52" s="12" t="n">
-        <v>414</v>
+        <v>330</v>
       </c>
       <c r="D52" s="1" t="n">
-        <v>433</v>
+        <v>1228</v>
       </c>
       <c r="E52" s="12" t="n">
-        <f aca="false">D52/83.784</f>
-        <v>5.16805117922276</v>
+        <f aca="false">D52/67.79</f>
+        <v>18.1147661897035</v>
       </c>
       <c r="F52" s="12" t="n">
-        <v>82</v>
+        <v>209</v>
       </c>
       <c r="G52" s="13" t="n">
-        <v>43918</v>
+        <v>43916</v>
       </c>
       <c r="H52" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$45,G52)</f>
-        <v>0</v>
+        <f aca="false">_xlfn.DAYS($B$46,G52)</f>
+        <v>3</v>
       </c>
       <c r="I52" s="13" t="n">
-        <f aca="false">$B$45+1</f>
-        <v>43919</v>
+        <f aca="false">$B$46+1</f>
+        <v>43920</v>
       </c>
       <c r="J52" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$45,I52)</f>
+        <f aca="false">_xlfn.DAYS($B$46,I52)</f>
         <v>-1</v>
       </c>
       <c r="K52" s="13" t="n">
-        <f aca="false">$B$45+1</f>
-        <v>43919</v>
+        <f aca="false">$B$46+1</f>
+        <v>43920</v>
       </c>
       <c r="L52" s="0"/>
       <c r="M52" s="0"/>
@@ -1913,39 +1926,39 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="0" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C53" s="12" t="n">
-        <v>50</v>
-      </c>
-      <c r="D53" s="12" t="n">
-        <v>105</v>
+        <v>414</v>
+      </c>
+      <c r="D53" s="1" t="n">
+        <v>541</v>
       </c>
       <c r="E53" s="12" t="n">
-        <f aca="false">D53/10.36</f>
-        <v>10.1351351351351</v>
+        <f aca="false">D53/83.784</f>
+        <v>6.457080110761</v>
       </c>
       <c r="F53" s="12" t="n">
-        <v>0</v>
+        <v>108</v>
       </c>
       <c r="G53" s="13" t="n">
-        <v>43915</v>
+        <v>43918</v>
       </c>
       <c r="H53" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$45,G53)</f>
-        <v>3</v>
+        <f aca="false">_xlfn.DAYS($B$46,G53)</f>
+        <v>1</v>
       </c>
       <c r="I53" s="13" t="n">
-        <f aca="false">$B$45+1</f>
-        <v>43919</v>
+        <f aca="false">$B$46+1</f>
+        <v>43920</v>
       </c>
       <c r="J53" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$45,I53)</f>
+        <f aca="false">_xlfn.DAYS($B$46,I53)</f>
         <v>-1</v>
       </c>
       <c r="K53" s="13" t="n">
-        <f aca="false">$B$45+1</f>
-        <v>43919</v>
+        <f aca="false">$B$46+1</f>
+        <v>43920</v>
       </c>
       <c r="L53" s="0"/>
       <c r="M53" s="0"/>
@@ -1955,15 +1968,41 @@
       <c r="Q53" s="0"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C54" s="12"/>
-      <c r="D54" s="12"/>
-      <c r="E54" s="12"/>
-      <c r="F54" s="12"/>
-      <c r="G54" s="13"/>
-      <c r="H54" s="0"/>
-      <c r="I54" s="13"/>
-      <c r="J54" s="0"/>
-      <c r="K54" s="13"/>
+      <c r="B54" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C54" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="D54" s="12" t="n">
+        <v>110</v>
+      </c>
+      <c r="E54" s="12" t="n">
+        <f aca="false">D54/10.36</f>
+        <v>10.6177606177606</v>
+      </c>
+      <c r="F54" s="12" t="n">
+        <v>5</v>
+      </c>
+      <c r="G54" s="13" t="n">
+        <v>43915</v>
+      </c>
+      <c r="H54" s="1" t="n">
+        <f aca="false">_xlfn.DAYS($B$46,G54)</f>
+        <v>4</v>
+      </c>
+      <c r="I54" s="13" t="n">
+        <f aca="false">$B$46+1</f>
+        <v>43920</v>
+      </c>
+      <c r="J54" s="1" t="n">
+        <f aca="false">_xlfn.DAYS($B$46,I54)</f>
+        <v>-1</v>
+      </c>
+      <c r="K54" s="13" t="n">
+        <f aca="false">$B$46+1</f>
+        <v>43920</v>
+      </c>
       <c r="L54" s="0"/>
       <c r="M54" s="0"/>
       <c r="N54" s="0"/>
@@ -1990,9 +2029,8 @@
       <c r="Q55" s="0"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="B56" s="4"/>
+      <c r="C56" s="5"/>
       <c r="D56" s="0"/>
       <c r="E56" s="0"/>
       <c r="F56" s="0"/>
@@ -2008,66 +2046,52 @@
       <c r="P56" s="0"/>
       <c r="Q56" s="0"/>
     </row>
-    <row r="57" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="7" t="n">
-        <v>43917</v>
-      </c>
-      <c r="C57" s="0"/>
-      <c r="D57" s="8" t="s">
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D57" s="0"/>
+      <c r="E57" s="0"/>
+      <c r="F57" s="0"/>
+      <c r="G57" s="0"/>
+      <c r="H57" s="0"/>
+      <c r="I57" s="0"/>
+      <c r="J57" s="0"/>
+      <c r="K57" s="0"/>
+      <c r="L57" s="0"/>
+      <c r="M57" s="0"/>
+      <c r="N57" s="0"/>
+      <c r="O57" s="0"/>
+      <c r="P57" s="0"/>
+      <c r="Q57" s="0"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="7" t="n">
+        <v>43918</v>
+      </c>
+      <c r="D58" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E57" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F57" s="8"/>
-      <c r="G57" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H57" s="8" t="s">
+      <c r="E58" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="I57" s="8" t="s">
+      <c r="F58" s="8"/>
+      <c r="G58" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="J57" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="K57" s="8" t="s">
+      <c r="H58" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L57" s="8"/>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="3"/>
-      <c r="B58" s="9"/>
-      <c r="C58" s="10" t="s">
+      <c r="I58" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D58" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E58" s="10" t="s">
+      <c r="J58" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K58" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F58" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G58" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H58" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="I58" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="J58" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="K58" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="L58" s="8"/>
+      <c r="L58" s="0"/>
       <c r="M58" s="0"/>
       <c r="N58" s="0"/>
       <c r="O58" s="0"/>
@@ -2075,39 +2099,33 @@
       <c r="Q58" s="0"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="0" t="s">
+      <c r="B59" s="9"/>
+      <c r="C59" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D59" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E59" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F59" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G59" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H59" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C59" s="12" t="n">
-        <v>300</v>
-      </c>
-      <c r="D59" s="1" t="n">
-        <v>9134</v>
-      </c>
-      <c r="E59" s="12" t="n">
-        <f aca="false">D59/60.48</f>
-        <v>151.025132275132</v>
-      </c>
-      <c r="F59" s="12" t="n">
-        <v>919</v>
-      </c>
-      <c r="G59" s="13" t="n">
-        <v>43900</v>
-      </c>
-      <c r="H59" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$57,G59)</f>
-        <v>17</v>
-      </c>
-      <c r="I59" s="13" t="n">
-        <v>43902</v>
-      </c>
-      <c r="J59" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$57,I59)</f>
-        <v>15</v>
-      </c>
-      <c r="K59" s="13" t="n">
-        <f aca="false">$B$57+1</f>
-        <v>43918</v>
+      <c r="I59" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="J59" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K59" s="8" t="s">
+        <v>37</v>
       </c>
       <c r="L59" s="0"/>
       <c r="M59" s="0"/>
@@ -2118,38 +2136,38 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C60" s="12" t="n">
-        <v>230</v>
+        <v>300</v>
       </c>
       <c r="D60" s="1" t="n">
-        <v>5138</v>
+        <v>10023</v>
       </c>
       <c r="E60" s="12" t="n">
-        <f aca="false">D60/46.75</f>
-        <v>109.903743315508</v>
+        <f aca="false">D60/60.48</f>
+        <v>165.724206349206</v>
       </c>
       <c r="F60" s="12" t="n">
-        <v>773</v>
+        <v>889</v>
       </c>
       <c r="G60" s="13" t="n">
-        <v>43907</v>
+        <v>43900</v>
       </c>
       <c r="H60" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$57,G60)</f>
-        <v>10</v>
+        <f aca="false">_xlfn.DAYS($B$58,G60)</f>
+        <v>18</v>
       </c>
       <c r="I60" s="13" t="n">
-        <v>43913</v>
+        <v>43902</v>
       </c>
       <c r="J60" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$57,I60)</f>
-        <v>4</v>
+        <f aca="false">_xlfn.DAYS(B$70,I60)</f>
+        <v>15</v>
       </c>
       <c r="K60" s="13" t="n">
-        <f aca="false">$B$57+1</f>
-        <v>43918</v>
+        <f aca="false">$B$58+1</f>
+        <v>43919</v>
       </c>
       <c r="L60" s="0"/>
       <c r="M60" s="0"/>
@@ -2160,38 +2178,38 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C61" s="12" t="n">
-        <v>330</v>
+        <v>230</v>
       </c>
       <c r="D61" s="1" t="n">
-        <v>1995</v>
+        <v>5982</v>
       </c>
       <c r="E61" s="12" t="n">
-        <f aca="false">D61/65.27</f>
-        <v>30.5653439558756</v>
+        <f aca="false">D61/46.75</f>
+        <v>127.957219251337</v>
       </c>
       <c r="F61" s="12" t="n">
-        <v>299</v>
+        <v>844</v>
       </c>
       <c r="G61" s="13" t="n">
-        <v>43912</v>
+        <v>43907</v>
       </c>
       <c r="H61" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$57,G61)</f>
-        <v>5</v>
+        <f aca="false">_xlfn.DAYS($B$58,G61)</f>
+        <v>11</v>
       </c>
       <c r="I61" s="13" t="n">
-        <v>43914</v>
+        <v>43913</v>
       </c>
       <c r="J61" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$57,I61)</f>
-        <v>3</v>
+        <f aca="false">_xlfn.DAYS(B$70,I61)</f>
+        <v>4</v>
       </c>
       <c r="K61" s="13" t="n">
-        <f aca="false">$B$57+1</f>
-        <v>43918</v>
+        <f aca="false">$B$58+1</f>
+        <v>43919</v>
       </c>
       <c r="L61" s="0"/>
       <c r="M61" s="0"/>
@@ -2202,40 +2220,38 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C62" s="12" t="n">
-        <v>1660</v>
+        <v>330</v>
       </c>
       <c r="D62" s="1" t="n">
-        <v>1696</v>
+        <v>2314</v>
       </c>
       <c r="E62" s="12" t="n">
-        <f aca="false">D62/331</f>
-        <v>5.12386706948641</v>
+        <f aca="false">D62/65.27</f>
+        <v>35.4527347939329</v>
       </c>
       <c r="F62" s="12" t="n">
-        <v>400</v>
+        <v>319</v>
       </c>
       <c r="G62" s="13" t="n">
-        <f aca="false">$B$57</f>
-        <v>43917</v>
+        <v>43912</v>
       </c>
       <c r="H62" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$57,G62)</f>
-        <v>0</v>
+        <f aca="false">_xlfn.DAYS($B$58,G62)</f>
+        <v>6</v>
       </c>
       <c r="I62" s="13" t="n">
-        <f aca="false">$B$57+1</f>
-        <v>43918</v>
+        <v>43914</v>
       </c>
       <c r="J62" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$57,I62)</f>
-        <v>-1</v>
+        <f aca="false">_xlfn.DAYS(B$70,I62)</f>
+        <v>3</v>
       </c>
       <c r="K62" s="13" t="n">
-        <f aca="false">$B$57+1</f>
-        <v>43918</v>
+        <f aca="false">$B$58+1</f>
+        <v>43919</v>
       </c>
       <c r="L62" s="0"/>
       <c r="M62" s="0"/>
@@ -2246,39 +2262,39 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C63" s="12" t="n">
-        <v>330</v>
+        <v>1660</v>
       </c>
       <c r="D63" s="1" t="n">
-        <v>759</v>
+        <v>2221</v>
       </c>
       <c r="E63" s="12" t="n">
-        <f aca="false">D63/67.79</f>
-        <v>11.1963416433102</v>
+        <f aca="false">D63/331</f>
+        <v>6.70996978851964</v>
       </c>
       <c r="F63" s="12" t="n">
-        <v>181</v>
+        <v>525</v>
       </c>
       <c r="G63" s="13" t="n">
-        <v>43916</v>
+        <v>43917</v>
       </c>
       <c r="H63" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$57,G63)</f>
+        <f aca="false">_xlfn.DAYS($B$58,G63)</f>
         <v>1</v>
       </c>
       <c r="I63" s="13" t="n">
-        <f aca="false">$B$57+1</f>
-        <v>43918</v>
+        <f aca="false">$B$58+1</f>
+        <v>43919</v>
       </c>
       <c r="J63" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$57,I63)</f>
+        <f aca="false">_xlfn.DAYS($B$58,I63)</f>
         <v>-1</v>
       </c>
       <c r="K63" s="13" t="n">
-        <f aca="false">$B$57+1</f>
-        <v>43918</v>
+        <f aca="false">$B$58+1</f>
+        <v>43919</v>
       </c>
       <c r="L63" s="0"/>
       <c r="M63" s="0"/>
@@ -2289,40 +2305,39 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C64" s="12" t="n">
-        <v>414</v>
+        <v>330</v>
       </c>
       <c r="D64" s="1" t="n">
-        <v>351</v>
+        <v>1019</v>
       </c>
       <c r="E64" s="12" t="n">
-        <f aca="false">D64/83.784</f>
-        <v>4.18934402749928</v>
+        <f aca="false">D64/67.79</f>
+        <v>15.0317155922702</v>
       </c>
       <c r="F64" s="12" t="n">
-        <v>84</v>
+        <v>260</v>
       </c>
       <c r="G64" s="13" t="n">
-        <f aca="false">$B$57+1</f>
-        <v>43918</v>
+        <v>43916</v>
       </c>
       <c r="H64" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$57,G64)</f>
+        <f aca="false">_xlfn.DAYS($B$58,G64)</f>
+        <v>2</v>
+      </c>
+      <c r="I64" s="13" t="n">
+        <f aca="false">$B$58+1</f>
+        <v>43919</v>
+      </c>
+      <c r="J64" s="1" t="n">
+        <f aca="false">_xlfn.DAYS($B$58,I64)</f>
         <v>-1</v>
       </c>
-      <c r="I64" s="13" t="n">
-        <f aca="false">$B$57+1</f>
-        <v>43918</v>
-      </c>
-      <c r="J64" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$57,I64)</f>
-        <v>-1</v>
-      </c>
       <c r="K64" s="13" t="n">
-        <f aca="false">$B$57+1</f>
-        <v>43918</v>
+        <f aca="false">$B$58+1</f>
+        <v>43919</v>
       </c>
       <c r="L64" s="0"/>
       <c r="M64" s="0"/>
@@ -2333,39 +2348,39 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="0" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C65" s="12" t="n">
-        <v>50</v>
-      </c>
-      <c r="D65" s="12" t="n">
-        <v>105</v>
+        <v>414</v>
+      </c>
+      <c r="D65" s="1" t="n">
+        <v>433</v>
       </c>
       <c r="E65" s="12" t="n">
-        <f aca="false">D65/10.36</f>
-        <v>10.1351351351351</v>
+        <f aca="false">D65/83.784</f>
+        <v>5.16805117922276</v>
       </c>
       <c r="F65" s="12" t="n">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="G65" s="13" t="n">
-        <v>43915</v>
+        <v>43918</v>
       </c>
       <c r="H65" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$57,G65)</f>
-        <v>2</v>
+        <f aca="false">_xlfn.DAYS($B$58,G65)</f>
+        <v>0</v>
       </c>
       <c r="I65" s="13" t="n">
-        <f aca="false">$B$57+1</f>
-        <v>43918</v>
+        <f aca="false">$B$58+1</f>
+        <v>43919</v>
       </c>
       <c r="J65" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$57,I65)</f>
+        <f aca="false">_xlfn.DAYS($B$58,I65)</f>
         <v>-1</v>
       </c>
       <c r="K65" s="13" t="n">
-        <f aca="false">$B$57+1</f>
-        <v>43918</v>
+        <f aca="false">$B$58+1</f>
+        <v>43919</v>
       </c>
       <c r="L65" s="0"/>
       <c r="M65" s="0"/>
@@ -2375,14 +2390,41 @@
       <c r="Q65" s="0"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D66" s="0"/>
-      <c r="E66" s="0"/>
-      <c r="F66" s="0"/>
-      <c r="G66" s="0"/>
-      <c r="H66" s="0"/>
-      <c r="I66" s="0"/>
-      <c r="J66" s="0"/>
-      <c r="K66" s="0"/>
+      <c r="B66" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C66" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="D66" s="12" t="n">
+        <v>105</v>
+      </c>
+      <c r="E66" s="12" t="n">
+        <f aca="false">D66/10.36</f>
+        <v>10.1351351351351</v>
+      </c>
+      <c r="F66" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G66" s="13" t="n">
+        <v>43915</v>
+      </c>
+      <c r="H66" s="1" t="n">
+        <f aca="false">_xlfn.DAYS($B$58,G66)</f>
+        <v>3</v>
+      </c>
+      <c r="I66" s="13" t="n">
+        <f aca="false">$B$58+1</f>
+        <v>43919</v>
+      </c>
+      <c r="J66" s="1" t="n">
+        <f aca="false">_xlfn.DAYS($B$58,I66)</f>
+        <v>-1</v>
+      </c>
+      <c r="K66" s="13" t="n">
+        <f aca="false">$B$58+1</f>
+        <v>43919</v>
+      </c>
       <c r="L66" s="0"/>
       <c r="M66" s="0"/>
       <c r="N66" s="0"/>
@@ -2391,14 +2433,15 @@
       <c r="Q66" s="0"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D67" s="0"/>
-      <c r="E67" s="0"/>
-      <c r="F67" s="0"/>
-      <c r="G67" s="0"/>
+      <c r="C67" s="12"/>
+      <c r="D67" s="12"/>
+      <c r="E67" s="12"/>
+      <c r="F67" s="12"/>
+      <c r="G67" s="13"/>
       <c r="H67" s="0"/>
-      <c r="I67" s="0"/>
+      <c r="I67" s="13"/>
       <c r="J67" s="0"/>
-      <c r="K67" s="0"/>
+      <c r="K67" s="13"/>
       <c r="L67" s="0"/>
       <c r="M67" s="0"/>
       <c r="N67" s="0"/>
@@ -2407,9 +2450,8 @@
       <c r="Q67" s="0"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="B68" s="4"/>
+      <c r="C68" s="5"/>
       <c r="D68" s="0"/>
       <c r="E68" s="0"/>
       <c r="F68" s="0"/>
@@ -2426,31 +2468,17 @@
       <c r="Q68" s="0"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="7" t="n">
-        <v>43916</v>
-      </c>
-      <c r="D69" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E69" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F69" s="8"/>
-      <c r="G69" s="8" t="s">
+      <c r="B69" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H69" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="I69" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="J69" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="K69" s="8" t="s">
-        <v>30</v>
-      </c>
+      <c r="D69" s="0"/>
+      <c r="E69" s="0"/>
+      <c r="F69" s="0"/>
+      <c r="G69" s="0"/>
+      <c r="H69" s="0"/>
+      <c r="I69" s="0"/>
+      <c r="J69" s="0"/>
+      <c r="K69" s="0"/>
       <c r="L69" s="0"/>
       <c r="M69" s="0"/>
       <c r="N69" s="0"/>
@@ -2458,78 +2486,66 @@
       <c r="P69" s="0"/>
       <c r="Q69" s="0"/>
     </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="9"/>
-      <c r="C70" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D70" s="10" t="s">
+    <row r="70" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B70" s="7" t="n">
+        <v>43917</v>
+      </c>
+      <c r="C70" s="0"/>
+      <c r="D70" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E70" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F70" s="8"/>
+      <c r="G70" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H70" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I70" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="J70" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K70" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="L70" s="8"/>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="3"/>
+      <c r="B71" s="9"/>
+      <c r="C71" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D71" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E70" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="F70" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G70" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H70" s="8" t="s">
+      <c r="E71" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="I70" s="11" t="s">
+      <c r="F71" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="J70" s="8" t="s">
+      <c r="G71" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="K70" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="L70" s="0"/>
-      <c r="M70" s="0"/>
-      <c r="N70" s="0"/>
-      <c r="O70" s="0"/>
-      <c r="P70" s="0"/>
-      <c r="Q70" s="0"/>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="0" t="s">
+      <c r="H71" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C71" s="12" t="n">
-        <v>300</v>
-      </c>
-      <c r="D71" s="1" t="n">
-        <v>8215</v>
-      </c>
-      <c r="E71" s="12" t="n">
-        <f aca="false">D71/60.48</f>
-        <v>135.830026455026</v>
-      </c>
-      <c r="F71" s="12" t="n">
-        <v>712</v>
-      </c>
-      <c r="G71" s="13" t="n">
-        <v>43900</v>
-      </c>
-      <c r="H71" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$69,G71)</f>
-        <v>16</v>
-      </c>
-      <c r="I71" s="13" t="n">
-        <v>43902</v>
-      </c>
-      <c r="J71" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$69,I71)</f>
-        <v>14</v>
-      </c>
-      <c r="K71" s="13" t="n">
-        <f aca="false">B$69+1</f>
-        <v>43917</v>
-      </c>
-      <c r="L71" s="0"/>
+      <c r="I71" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="J71" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K71" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L71" s="8"/>
       <c r="M71" s="0"/>
       <c r="N71" s="0"/>
       <c r="O71" s="0"/>
@@ -2538,38 +2554,38 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C72" s="12" t="n">
-        <v>230</v>
+        <v>300</v>
       </c>
       <c r="D72" s="1" t="n">
-        <v>4365</v>
+        <v>9134</v>
       </c>
       <c r="E72" s="12" t="n">
-        <f aca="false">D72/46.75</f>
-        <v>93.3689839572193</v>
+        <f aca="false">D72/60.48</f>
+        <v>151.025132275132</v>
       </c>
       <c r="F72" s="12" t="n">
-        <v>718</v>
+        <v>919</v>
       </c>
       <c r="G72" s="13" t="n">
-        <v>43907</v>
+        <v>43900</v>
       </c>
       <c r="H72" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$69,G72)</f>
-        <v>9</v>
+        <f aca="false">_xlfn.DAYS($B$70,G72)</f>
+        <v>17</v>
       </c>
       <c r="I72" s="13" t="n">
-        <v>43913</v>
+        <v>43902</v>
       </c>
       <c r="J72" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$69,I72)</f>
-        <v>3</v>
+        <f aca="false">_xlfn.DAYS(B$70,I72)</f>
+        <v>15</v>
       </c>
       <c r="K72" s="13" t="n">
-        <f aca="false">B$69+1</f>
-        <v>43917</v>
+        <f aca="false">$B$70+1</f>
+        <v>43918</v>
       </c>
       <c r="L72" s="0"/>
       <c r="M72" s="0"/>
@@ -2580,38 +2596,38 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C73" s="12" t="n">
-        <v>330</v>
+        <v>230</v>
       </c>
       <c r="D73" s="1" t="n">
-        <v>1696</v>
+        <v>5138</v>
       </c>
       <c r="E73" s="12" t="n">
-        <f aca="false">D73/65.27</f>
-        <v>25.9843726060978</v>
+        <f aca="false">D73/46.75</f>
+        <v>109.903743315508</v>
       </c>
       <c r="F73" s="12" t="n">
-        <v>365</v>
+        <v>773</v>
       </c>
       <c r="G73" s="13" t="n">
-        <v>43912</v>
+        <v>43907</v>
       </c>
       <c r="H73" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$69,G73)</f>
+        <f aca="false">_xlfn.DAYS($B$70,G73)</f>
+        <v>10</v>
+      </c>
+      <c r="I73" s="13" t="n">
+        <v>43913</v>
+      </c>
+      <c r="J73" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$70,I73)</f>
         <v>4</v>
       </c>
-      <c r="I73" s="13" t="n">
-        <v>43914</v>
-      </c>
-      <c r="J73" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$69,I73)</f>
-        <v>2</v>
-      </c>
       <c r="K73" s="13" t="n">
-        <f aca="false">B$69+1</f>
-        <v>43917</v>
+        <f aca="false">$B$70+1</f>
+        <v>43918</v>
       </c>
       <c r="L73" s="0"/>
       <c r="M73" s="0"/>
@@ -2622,39 +2638,38 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C74" s="12" t="n">
-        <v>1660</v>
+        <v>330</v>
       </c>
       <c r="D74" s="1" t="n">
-        <v>1295</v>
+        <v>1995</v>
       </c>
       <c r="E74" s="12" t="n">
-        <f aca="false">D74/331</f>
-        <v>3.91238670694864</v>
+        <f aca="false">D74/65.27</f>
+        <v>30.5653439558756</v>
       </c>
       <c r="F74" s="12" t="n">
-        <v>268</v>
+        <v>299</v>
       </c>
       <c r="G74" s="13" t="n">
-        <v>43917</v>
+        <v>43912</v>
       </c>
       <c r="H74" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$69,G74)</f>
-        <v>-1</v>
+        <f aca="false">_xlfn.DAYS($B$70,G74)</f>
+        <v>5</v>
       </c>
       <c r="I74" s="13" t="n">
-        <f aca="false">B$69+1</f>
-        <v>43917</v>
+        <v>43914</v>
       </c>
       <c r="J74" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$69,I74)</f>
-        <v>-1</v>
+        <f aca="false">_xlfn.DAYS(B$70,I74)</f>
+        <v>3</v>
       </c>
       <c r="K74" s="13" t="n">
-        <f aca="false">B$69+1</f>
-        <v>43917</v>
+        <f aca="false">$B$70+1</f>
+        <v>43918</v>
       </c>
       <c r="L74" s="0"/>
       <c r="M74" s="0"/>
@@ -2665,39 +2680,40 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C75" s="12" t="n">
-        <v>330</v>
+        <v>1660</v>
       </c>
       <c r="D75" s="1" t="n">
-        <v>578</v>
+        <v>1696</v>
       </c>
       <c r="E75" s="12" t="n">
-        <f aca="false">D75/67.79</f>
-        <v>8.52633131730344</v>
+        <f aca="false">D75/331</f>
+        <v>5.12386706948641</v>
       </c>
       <c r="F75" s="12" t="n">
-        <v>115</v>
+        <v>400</v>
       </c>
       <c r="G75" s="13" t="n">
-        <v>43916</v>
+        <f aca="false">$B$70</f>
+        <v>43917</v>
       </c>
       <c r="H75" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$69,G75)</f>
+        <f aca="false">_xlfn.DAYS($B$70,G75)</f>
         <v>0</v>
       </c>
       <c r="I75" s="13" t="n">
-        <f aca="false">B$69+1</f>
-        <v>43917</v>
+        <f aca="false">$B$70+1</f>
+        <v>43918</v>
       </c>
       <c r="J75" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$69,I75)</f>
+        <f aca="false">_xlfn.DAYS(B$70,I75)</f>
         <v>-1</v>
       </c>
       <c r="K75" s="13" t="n">
-        <f aca="false">B$69+1</f>
-        <v>43917</v>
+        <f aca="false">$B$70+1</f>
+        <v>43918</v>
       </c>
       <c r="L75" s="0"/>
       <c r="M75" s="0"/>
@@ -2708,39 +2724,39 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C76" s="12" t="n">
-        <v>414</v>
+        <v>330</v>
       </c>
       <c r="D76" s="1" t="n">
-        <v>267</v>
+        <v>759</v>
       </c>
       <c r="E76" s="12" t="n">
-        <f aca="false">D76/83.784</f>
-        <v>3.18676596963621</v>
+        <f aca="false">D76/67.79</f>
+        <v>11.1963416433102</v>
       </c>
       <c r="F76" s="12" t="n">
-        <v>61</v>
+        <v>181</v>
       </c>
       <c r="G76" s="13" t="n">
-        <v>43917</v>
+        <v>43916</v>
       </c>
       <c r="H76" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$69,G76)</f>
+        <f aca="false">_xlfn.DAYS($B$70,G76)</f>
+        <v>1</v>
+      </c>
+      <c r="I76" s="13" t="n">
+        <f aca="false">$B$70+1</f>
+        <v>43918</v>
+      </c>
+      <c r="J76" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$70,I76)</f>
         <v>-1</v>
       </c>
-      <c r="I76" s="13" t="n">
-        <f aca="false">B$69+1</f>
-        <v>43917</v>
-      </c>
-      <c r="J76" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$69,I76)</f>
-        <v>-1</v>
-      </c>
       <c r="K76" s="13" t="n">
-        <f aca="false">B$69+1</f>
-        <v>43917</v>
+        <f aca="false">$B$70+1</f>
+        <v>43918</v>
       </c>
       <c r="L76" s="0"/>
       <c r="M76" s="0"/>
@@ -2751,39 +2767,40 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="0" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C77" s="12" t="n">
-        <v>50</v>
-      </c>
-      <c r="D77" s="12" t="n">
-        <v>77</v>
+        <v>414</v>
+      </c>
+      <c r="D77" s="1" t="n">
+        <v>351</v>
       </c>
       <c r="E77" s="12" t="n">
-        <f aca="false">D77/10.36</f>
-        <v>7.43243243243243</v>
+        <f aca="false">D77/83.784</f>
+        <v>4.18934402749928</v>
       </c>
       <c r="F77" s="12" t="n">
-        <v>15</v>
+        <v>84</v>
       </c>
       <c r="G77" s="13" t="n">
-        <v>43915</v>
+        <f aca="false">$B$70+1</f>
+        <v>43918</v>
       </c>
       <c r="H77" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$69,G77)</f>
-        <v>1</v>
+        <f aca="false">_xlfn.DAYS($B$70,G77)</f>
+        <v>-1</v>
       </c>
       <c r="I77" s="13" t="n">
-        <f aca="false">B$69+1</f>
-        <v>43917</v>
+        <f aca="false">$B$70+1</f>
+        <v>43918</v>
       </c>
       <c r="J77" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$69,I77)</f>
+        <f aca="false">_xlfn.DAYS(B$70,I77)</f>
         <v>-1</v>
       </c>
       <c r="K77" s="13" t="n">
-        <f aca="false">B$69+1</f>
-        <v>43917</v>
+        <f aca="false">$B$70+1</f>
+        <v>43918</v>
       </c>
       <c r="L77" s="0"/>
       <c r="M77" s="0"/>
@@ -2791,6 +2808,467 @@
       <c r="O77" s="0"/>
       <c r="P77" s="0"/>
       <c r="Q77" s="0"/>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B78" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C78" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="D78" s="12" t="n">
+        <v>105</v>
+      </c>
+      <c r="E78" s="12" t="n">
+        <f aca="false">D78/10.36</f>
+        <v>10.1351351351351</v>
+      </c>
+      <c r="F78" s="12" t="n">
+        <v>28</v>
+      </c>
+      <c r="G78" s="13" t="n">
+        <v>43915</v>
+      </c>
+      <c r="H78" s="1" t="n">
+        <f aca="false">_xlfn.DAYS($B$70,G78)</f>
+        <v>2</v>
+      </c>
+      <c r="I78" s="13" t="n">
+        <f aca="false">$B$70+1</f>
+        <v>43918</v>
+      </c>
+      <c r="J78" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$70,I78)</f>
+        <v>-1</v>
+      </c>
+      <c r="K78" s="13" t="n">
+        <f aca="false">$B$70+1</f>
+        <v>43918</v>
+      </c>
+      <c r="L78" s="0"/>
+      <c r="M78" s="0"/>
+      <c r="N78" s="0"/>
+      <c r="O78" s="0"/>
+      <c r="P78" s="0"/>
+      <c r="Q78" s="0"/>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D79" s="0"/>
+      <c r="E79" s="0"/>
+      <c r="F79" s="0"/>
+      <c r="G79" s="0"/>
+      <c r="H79" s="0"/>
+      <c r="I79" s="0"/>
+      <c r="J79" s="0"/>
+      <c r="K79" s="0"/>
+      <c r="L79" s="0"/>
+      <c r="M79" s="0"/>
+      <c r="N79" s="0"/>
+      <c r="O79" s="0"/>
+      <c r="P79" s="0"/>
+      <c r="Q79" s="0"/>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D80" s="0"/>
+      <c r="E80" s="0"/>
+      <c r="F80" s="0"/>
+      <c r="G80" s="0"/>
+      <c r="H80" s="0"/>
+      <c r="I80" s="0"/>
+      <c r="J80" s="0"/>
+      <c r="K80" s="0"/>
+      <c r="L80" s="0"/>
+      <c r="M80" s="0"/>
+      <c r="N80" s="0"/>
+      <c r="O80" s="0"/>
+      <c r="P80" s="0"/>
+      <c r="Q80" s="0"/>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B81" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D81" s="0"/>
+      <c r="E81" s="0"/>
+      <c r="F81" s="0"/>
+      <c r="G81" s="0"/>
+      <c r="H81" s="0"/>
+      <c r="I81" s="0"/>
+      <c r="J81" s="0"/>
+      <c r="K81" s="0"/>
+      <c r="L81" s="0"/>
+      <c r="M81" s="0"/>
+      <c r="N81" s="0"/>
+      <c r="O81" s="0"/>
+      <c r="P81" s="0"/>
+      <c r="Q81" s="0"/>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B82" s="7" t="n">
+        <v>43916</v>
+      </c>
+      <c r="D82" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E82" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F82" s="8"/>
+      <c r="G82" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H82" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I82" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="J82" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K82" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="L82" s="0"/>
+      <c r="M82" s="0"/>
+      <c r="N82" s="0"/>
+      <c r="O82" s="0"/>
+      <c r="P82" s="0"/>
+      <c r="Q82" s="0"/>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B83" s="9"/>
+      <c r="C83" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D83" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E83" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F83" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G83" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H83" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I83" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="J83" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K83" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L83" s="0"/>
+      <c r="M83" s="0"/>
+      <c r="N83" s="0"/>
+      <c r="O83" s="0"/>
+      <c r="P83" s="0"/>
+      <c r="Q83" s="0"/>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B84" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C84" s="12" t="n">
+        <v>300</v>
+      </c>
+      <c r="D84" s="1" t="n">
+        <v>8215</v>
+      </c>
+      <c r="E84" s="12" t="n">
+        <f aca="false">D84/60.48</f>
+        <v>135.830026455026</v>
+      </c>
+      <c r="F84" s="12" t="n">
+        <v>712</v>
+      </c>
+      <c r="G84" s="13" t="n">
+        <v>43900</v>
+      </c>
+      <c r="H84" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$82,G84)</f>
+        <v>16</v>
+      </c>
+      <c r="I84" s="13" t="n">
+        <v>43902</v>
+      </c>
+      <c r="J84" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$82,I84)</f>
+        <v>14</v>
+      </c>
+      <c r="K84" s="13" t="n">
+        <f aca="false">B$82+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L84" s="0"/>
+      <c r="M84" s="0"/>
+      <c r="N84" s="0"/>
+      <c r="O84" s="0"/>
+      <c r="P84" s="0"/>
+      <c r="Q84" s="0"/>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B85" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C85" s="12" t="n">
+        <v>230</v>
+      </c>
+      <c r="D85" s="1" t="n">
+        <v>4365</v>
+      </c>
+      <c r="E85" s="12" t="n">
+        <f aca="false">D85/46.75</f>
+        <v>93.3689839572193</v>
+      </c>
+      <c r="F85" s="12" t="n">
+        <v>718</v>
+      </c>
+      <c r="G85" s="13" t="n">
+        <v>43907</v>
+      </c>
+      <c r="H85" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$82,G85)</f>
+        <v>9</v>
+      </c>
+      <c r="I85" s="13" t="n">
+        <v>43913</v>
+      </c>
+      <c r="J85" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$82,I85)</f>
+        <v>3</v>
+      </c>
+      <c r="K85" s="13" t="n">
+        <f aca="false">B$82+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L85" s="0"/>
+      <c r="M85" s="0"/>
+      <c r="N85" s="0"/>
+      <c r="O85" s="0"/>
+      <c r="P85" s="0"/>
+      <c r="Q85" s="0"/>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B86" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C86" s="12" t="n">
+        <v>330</v>
+      </c>
+      <c r="D86" s="1" t="n">
+        <v>1696</v>
+      </c>
+      <c r="E86" s="12" t="n">
+        <f aca="false">D86/65.27</f>
+        <v>25.9843726060978</v>
+      </c>
+      <c r="F86" s="12" t="n">
+        <v>365</v>
+      </c>
+      <c r="G86" s="13" t="n">
+        <v>43912</v>
+      </c>
+      <c r="H86" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$82,G86)</f>
+        <v>4</v>
+      </c>
+      <c r="I86" s="13" t="n">
+        <v>43914</v>
+      </c>
+      <c r="J86" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$82,I86)</f>
+        <v>2</v>
+      </c>
+      <c r="K86" s="13" t="n">
+        <f aca="false">B$82+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L86" s="0"/>
+      <c r="M86" s="0"/>
+      <c r="N86" s="0"/>
+      <c r="O86" s="0"/>
+      <c r="P86" s="0"/>
+      <c r="Q86" s="0"/>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B87" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C87" s="12" t="n">
+        <v>1660</v>
+      </c>
+      <c r="D87" s="1" t="n">
+        <v>1295</v>
+      </c>
+      <c r="E87" s="12" t="n">
+        <f aca="false">D87/331</f>
+        <v>3.91238670694864</v>
+      </c>
+      <c r="F87" s="12" t="n">
+        <v>268</v>
+      </c>
+      <c r="G87" s="13" t="n">
+        <v>43917</v>
+      </c>
+      <c r="H87" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$82,G87)</f>
+        <v>-1</v>
+      </c>
+      <c r="I87" s="13" t="n">
+        <f aca="false">B$82+1</f>
+        <v>43917</v>
+      </c>
+      <c r="J87" s="1" t="n">
+        <f aca="false">_xlfn.DAYS($B$82,I87)</f>
+        <v>-1</v>
+      </c>
+      <c r="K87" s="13" t="n">
+        <f aca="false">B$82+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L87" s="0"/>
+      <c r="M87" s="0"/>
+      <c r="N87" s="0"/>
+      <c r="O87" s="0"/>
+      <c r="P87" s="0"/>
+      <c r="Q87" s="0"/>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B88" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C88" s="12" t="n">
+        <v>330</v>
+      </c>
+      <c r="D88" s="1" t="n">
+        <v>578</v>
+      </c>
+      <c r="E88" s="12" t="n">
+        <f aca="false">D88/67.79</f>
+        <v>8.52633131730344</v>
+      </c>
+      <c r="F88" s="12" t="n">
+        <v>115</v>
+      </c>
+      <c r="G88" s="13" t="n">
+        <v>43916</v>
+      </c>
+      <c r="H88" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$82,G88)</f>
+        <v>0</v>
+      </c>
+      <c r="I88" s="13" t="n">
+        <f aca="false">B$82+1</f>
+        <v>43917</v>
+      </c>
+      <c r="J88" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$82,I88)</f>
+        <v>-1</v>
+      </c>
+      <c r="K88" s="13" t="n">
+        <f aca="false">B$82+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L88" s="0"/>
+      <c r="M88" s="0"/>
+      <c r="N88" s="0"/>
+      <c r="O88" s="0"/>
+      <c r="P88" s="0"/>
+      <c r="Q88" s="0"/>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B89" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C89" s="12" t="n">
+        <v>414</v>
+      </c>
+      <c r="D89" s="1" t="n">
+        <v>267</v>
+      </c>
+      <c r="E89" s="12" t="n">
+        <f aca="false">D89/83.784</f>
+        <v>3.18676596963621</v>
+      </c>
+      <c r="F89" s="12" t="n">
+        <v>61</v>
+      </c>
+      <c r="G89" s="13" t="n">
+        <v>43917</v>
+      </c>
+      <c r="H89" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$82,G89)</f>
+        <v>-1</v>
+      </c>
+      <c r="I89" s="13" t="n">
+        <f aca="false">B$82+1</f>
+        <v>43917</v>
+      </c>
+      <c r="J89" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$82,I89)</f>
+        <v>-1</v>
+      </c>
+      <c r="K89" s="13" t="n">
+        <f aca="false">B$82+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L89" s="0"/>
+      <c r="M89" s="0"/>
+      <c r="N89" s="0"/>
+      <c r="O89" s="0"/>
+      <c r="P89" s="0"/>
+      <c r="Q89" s="0"/>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B90" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C90" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="D90" s="12" t="n">
+        <v>77</v>
+      </c>
+      <c r="E90" s="12" t="n">
+        <f aca="false">D90/10.36</f>
+        <v>7.43243243243243</v>
+      </c>
+      <c r="F90" s="12" t="n">
+        <v>15</v>
+      </c>
+      <c r="G90" s="13" t="n">
+        <v>43915</v>
+      </c>
+      <c r="H90" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$82,G90)</f>
+        <v>1</v>
+      </c>
+      <c r="I90" s="13" t="n">
+        <f aca="false">B$82+1</f>
+        <v>43917</v>
+      </c>
+      <c r="J90" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$82,I90)</f>
+        <v>-1</v>
+      </c>
+      <c r="K90" s="13" t="n">
+        <f aca="false">B$82+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L90" s="0"/>
+      <c r="M90" s="0"/>
+      <c r="N90" s="0"/>
+      <c r="O90" s="0"/>
+      <c r="P90" s="0"/>
+      <c r="Q90" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
updated with 2020-04-01 data
</commit_message>
<xml_diff>
--- a/covid19 lockdown evaluation .xlsx
+++ b/covid19 lockdown evaluation .xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="241" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="257" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="49">
   <si>
     <t>Effects of the lockdown issued by governments</t>
   </si>
@@ -341,10 +341,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q90"/>
+  <dimension ref="A1:Q102"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
+      <selection pane="topLeft" activeCell="N31" activeCellId="0" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -785,7 +785,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="7" t="n">
-        <v>43921</v>
+        <v>43922</v>
       </c>
       <c r="D22" s="0"/>
       <c r="E22" s="8" t="s">
@@ -876,22 +876,22 @@
       </c>
       <c r="H24" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,G24)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I24" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J24" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I24)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K24" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L24" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K24,G24)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M24" s="0"/>
       <c r="N24" s="0"/>
@@ -921,22 +921,22 @@
       </c>
       <c r="H25" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,G25)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I25" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J25" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I25)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K25" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L25" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K25,G25)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M25" s="0"/>
       <c r="N25" s="0"/>
@@ -966,22 +966,22 @@
       </c>
       <c r="H26" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,G26)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I26" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J26" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I26)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K26" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L26" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K26,G26)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M26" s="0"/>
       <c r="N26" s="0"/>
@@ -1011,11 +1011,11 @@
       </c>
       <c r="H27" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,G27)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I27" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="J27" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I27)</f>
@@ -1023,11 +1023,11 @@
       </c>
       <c r="K27" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L27" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K27,G27)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M27" s="0"/>
       <c r="N27" s="0"/>
@@ -1057,11 +1057,11 @@
       </c>
       <c r="H28" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,G28)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I28" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="J28" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I28)</f>
@@ -1069,11 +1069,11 @@
       </c>
       <c r="K28" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L28" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K28,G28)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M28" s="0"/>
       <c r="N28" s="0"/>
@@ -1103,11 +1103,11 @@
       </c>
       <c r="H29" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,G29)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I29" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="J29" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I29)</f>
@@ -1115,11 +1115,11 @@
       </c>
       <c r="K29" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L29" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K29,G29)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M29" s="0"/>
       <c r="N29" s="0"/>
@@ -1149,11 +1149,11 @@
       </c>
       <c r="H30" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,G30)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I30" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="J30" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I30)</f>
@@ -1161,11 +1161,11 @@
       </c>
       <c r="K30" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L30" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K30,G30)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M30" s="0"/>
       <c r="N30" s="0"/>
@@ -1174,15 +1174,16 @@
       <c r="Q30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="12"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="5"/>
       <c r="D31" s="0"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="13"/>
+      <c r="E31" s="0"/>
+      <c r="F31" s="0"/>
+      <c r="G31" s="0"/>
       <c r="H31" s="0"/>
-      <c r="I31" s="13"/>
+      <c r="I31" s="0"/>
       <c r="J31" s="0"/>
-      <c r="K31" s="13"/>
+      <c r="K31" s="0"/>
       <c r="L31" s="0"/>
       <c r="M31" s="0"/>
       <c r="N31" s="0"/>
@@ -1191,15 +1192,16 @@
       <c r="Q31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="12"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="5"/>
       <c r="D32" s="0"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="13"/>
+      <c r="E32" s="0"/>
+      <c r="F32" s="0"/>
+      <c r="G32" s="0"/>
       <c r="H32" s="0"/>
-      <c r="I32" s="13"/>
+      <c r="I32" s="0"/>
       <c r="J32" s="0"/>
-      <c r="K32" s="13"/>
+      <c r="K32" s="0"/>
       <c r="L32" s="0"/>
       <c r="M32" s="0"/>
       <c r="N32" s="0"/>
@@ -1228,7 +1230,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="7" t="n">
-        <v>43920</v>
+        <v>43921</v>
       </c>
       <c r="D34" s="0"/>
       <c r="E34" s="8" t="s">
@@ -1250,7 +1252,9 @@
       <c r="K34" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="L34" s="0"/>
+      <c r="L34" s="8" t="s">
+        <v>33</v>
+      </c>
       <c r="M34" s="0"/>
       <c r="N34" s="0"/>
       <c r="O34" s="0"/>
@@ -1286,7 +1290,9 @@
       <c r="K35" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L35" s="0"/>
+      <c r="L35" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="M35" s="0"/>
       <c r="N35" s="0"/>
       <c r="O35" s="0"/>
@@ -1301,34 +1307,37 @@
         <v>300</v>
       </c>
       <c r="D36" s="1" t="n">
-        <v>11591</v>
+        <v>12428</v>
       </c>
       <c r="E36" s="12" t="n">
         <f aca="false">D36/60.48</f>
-        <v>191.650132275132</v>
+        <v>205.489417989418</v>
       </c>
       <c r="F36" s="12" t="n">
-        <v>812</v>
+        <v>837</v>
       </c>
       <c r="G36" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H36" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,G36)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I36" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J36" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I36)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K36" s="13" t="n">
-        <f aca="false">$B$46+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L36" s="0"/>
+        <f aca="false">$B$34+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L36" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K36,G36)</f>
+        <v>22</v>
+      </c>
       <c r="M36" s="0"/>
       <c r="N36" s="0"/>
       <c r="O36" s="0"/>
@@ -1343,34 +1352,37 @@
         <v>230</v>
       </c>
       <c r="D37" s="1" t="n">
-        <v>7716</v>
+        <v>8464</v>
       </c>
       <c r="E37" s="12" t="n">
         <f aca="false">D37/46.75</f>
-        <v>165.048128342246</v>
+        <v>181.048128342246</v>
       </c>
       <c r="F37" s="12" t="n">
-        <v>913</v>
+        <v>748</v>
       </c>
       <c r="G37" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H37" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,G37)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I37" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J37" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I37)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K37" s="13" t="n">
-        <f aca="false">$B$46+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L37" s="0"/>
+        <f aca="false">$B$34+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L37" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K37,G37)</f>
+        <v>15</v>
+      </c>
       <c r="M37" s="0"/>
       <c r="N37" s="0"/>
       <c r="O37" s="0"/>
@@ -1385,34 +1397,37 @@
         <v>330</v>
       </c>
       <c r="D38" s="1" t="n">
-        <v>3024</v>
+        <v>3523</v>
       </c>
       <c r="E38" s="12" t="n">
         <f aca="false">D38/65.27</f>
-        <v>46.3306266278535</v>
+        <v>53.9757928604259</v>
       </c>
       <c r="F38" s="12" t="n">
-        <v>418</v>
+        <v>499</v>
       </c>
       <c r="G38" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H38" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,G38)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I38" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J38" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I38)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K38" s="13" t="n">
-        <f aca="false">$B$46+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L38" s="0"/>
+        <f aca="false">$B$34+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L38" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K38,G38)</f>
+        <v>10</v>
+      </c>
       <c r="M38" s="0"/>
       <c r="N38" s="0"/>
       <c r="O38" s="0"/>
@@ -1427,35 +1442,38 @@
         <v>50</v>
       </c>
       <c r="D39" s="12" t="n">
-        <v>146</v>
+        <v>180</v>
       </c>
       <c r="E39" s="12" t="n">
         <f aca="false">D39/10.36</f>
-        <v>14.0926640926641</v>
+        <v>17.3745173745174</v>
       </c>
       <c r="F39" s="12" t="n">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G39" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H39" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,G39)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I39" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43921</v>
+        <v>43922</v>
       </c>
       <c r="J39" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I39)</f>
         <v>-1</v>
       </c>
       <c r="K39" s="13" t="n">
-        <f aca="false">$B$46+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L39" s="0"/>
+        <f aca="false">$B$34+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L39" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K39,G39)</f>
+        <v>7</v>
+      </c>
       <c r="M39" s="0"/>
       <c r="N39" s="0"/>
       <c r="O39" s="0"/>
@@ -1470,35 +1488,38 @@
         <v>330</v>
       </c>
       <c r="D40" s="1" t="n">
-        <v>1408</v>
+        <v>1789</v>
       </c>
       <c r="E40" s="12" t="n">
         <f aca="false">D40/67.79</f>
-        <v>20.770025077445</v>
+        <v>26.390323056498</v>
       </c>
       <c r="F40" s="12" t="n">
-        <v>180</v>
+        <v>381</v>
       </c>
       <c r="G40" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H40" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,G40)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I40" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43921</v>
+        <v>43922</v>
       </c>
       <c r="J40" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I40)</f>
         <v>-1</v>
       </c>
       <c r="K40" s="13" t="n">
-        <f aca="false">$B$46+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L40" s="0"/>
+        <f aca="false">$B$34+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L40" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K40,G40)</f>
+        <v>6</v>
+      </c>
       <c r="M40" s="0"/>
       <c r="N40" s="0"/>
       <c r="O40" s="0"/>
@@ -1513,34 +1534,38 @@
         <v>1660</v>
       </c>
       <c r="D41" s="1" t="n">
-        <v>3141</v>
+        <v>4053</v>
       </c>
       <c r="E41" s="12" t="n">
         <f aca="false">D41/331</f>
-        <v>9.48942598187311</v>
+        <v>12.2447129909366</v>
       </c>
       <c r="F41" s="12" t="n">
-        <v>573</v>
+        <v>912</v>
       </c>
       <c r="G41" s="13" t="n">
         <v>43917</v>
       </c>
       <c r="H41" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,G41)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I41" s="13" t="n">
-        <v>43920</v>
+        <f aca="false">$B$34+1</f>
+        <v>43922</v>
       </c>
       <c r="J41" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I41)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="K41" s="13" t="n">
-        <f aca="false">$B$46+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L41" s="0"/>
+        <f aca="false">$B$34+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L41" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K41,G41)</f>
+        <v>5</v>
+      </c>
       <c r="M41" s="0"/>
       <c r="N41" s="0"/>
       <c r="O41" s="0"/>
@@ -1555,35 +1580,38 @@
         <v>414</v>
       </c>
       <c r="D42" s="1" t="n">
-        <v>645</v>
+        <v>775</v>
       </c>
       <c r="E42" s="12" t="n">
         <f aca="false">D42/83.784</f>
-        <v>7.69836723002005</v>
+        <v>9.24997612909386</v>
       </c>
       <c r="F42" s="12" t="n">
-        <v>104</v>
+        <v>130</v>
       </c>
       <c r="G42" s="13" t="n">
         <v>43918</v>
       </c>
       <c r="H42" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,G42)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I42" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43921</v>
+        <v>43922</v>
       </c>
       <c r="J42" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I42)</f>
         <v>-1</v>
       </c>
       <c r="K42" s="13" t="n">
-        <f aca="false">$B$46+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L42" s="0"/>
+        <f aca="false">$B$34+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L42" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K42,G42)</f>
+        <v>4</v>
+      </c>
       <c r="M42" s="0"/>
       <c r="N42" s="0"/>
       <c r="O42" s="0"/>
@@ -1591,16 +1619,15 @@
       <c r="Q42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="4"/>
-      <c r="C43" s="5"/>
+      <c r="C43" s="12"/>
       <c r="D43" s="0"/>
-      <c r="E43" s="0"/>
-      <c r="F43" s="0"/>
-      <c r="G43" s="0"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="13"/>
       <c r="H43" s="0"/>
-      <c r="I43" s="0"/>
+      <c r="I43" s="13"/>
       <c r="J43" s="0"/>
-      <c r="K43" s="0"/>
+      <c r="K43" s="13"/>
       <c r="L43" s="0"/>
       <c r="M43" s="0"/>
       <c r="N43" s="0"/>
@@ -1609,16 +1636,15 @@
       <c r="Q43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="4"/>
-      <c r="C44" s="5"/>
+      <c r="C44" s="12"/>
       <c r="D44" s="0"/>
-      <c r="E44" s="0"/>
-      <c r="F44" s="0"/>
-      <c r="G44" s="0"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="13"/>
       <c r="H44" s="0"/>
-      <c r="I44" s="0"/>
+      <c r="I44" s="13"/>
       <c r="J44" s="0"/>
-      <c r="K44" s="0"/>
+      <c r="K44" s="13"/>
       <c r="L44" s="0"/>
       <c r="M44" s="0"/>
       <c r="N44" s="0"/>
@@ -1647,7 +1673,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="7" t="n">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="D46" s="0"/>
       <c r="E46" s="8" t="s">
@@ -1720,31 +1746,31 @@
         <v>300</v>
       </c>
       <c r="D48" s="1" t="n">
-        <v>10779</v>
+        <v>11591</v>
       </c>
       <c r="E48" s="12" t="n">
         <f aca="false">D48/60.48</f>
-        <v>178.224206349206</v>
+        <v>191.650132275132</v>
       </c>
       <c r="F48" s="12" t="n">
-        <v>756</v>
+        <v>812</v>
       </c>
       <c r="G48" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H48" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,G48)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I48" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J48" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I48)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K48" s="13" t="n">
-        <f aca="false">$B$46+1</f>
+        <f aca="false">$B$58+1</f>
         <v>43920</v>
       </c>
       <c r="L48" s="0"/>
@@ -1762,31 +1788,31 @@
         <v>230</v>
       </c>
       <c r="D49" s="1" t="n">
-        <v>6803</v>
+        <v>7716</v>
       </c>
       <c r="E49" s="12" t="n">
         <f aca="false">D49/46.75</f>
-        <v>145.51871657754</v>
+        <v>165.048128342246</v>
       </c>
       <c r="F49" s="12" t="n">
-        <v>821</v>
+        <v>913</v>
       </c>
       <c r="G49" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H49" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,G49)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I49" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J49" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I49)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K49" s="13" t="n">
-        <f aca="false">$B$46+1</f>
+        <f aca="false">$B$58+1</f>
         <v>43920</v>
       </c>
       <c r="L49" s="0"/>
@@ -1804,31 +1830,31 @@
         <v>330</v>
       </c>
       <c r="D50" s="1" t="n">
-        <v>2606</v>
+        <v>3024</v>
       </c>
       <c r="E50" s="12" t="n">
         <f aca="false">D50/65.27</f>
-        <v>39.9264593228129</v>
+        <v>46.3306266278535</v>
       </c>
       <c r="F50" s="12" t="n">
-        <v>292</v>
+        <v>418</v>
       </c>
       <c r="G50" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H50" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,G50)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I50" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J50" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I50)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K50" s="13" t="n">
-        <f aca="false">$B$46+1</f>
+        <f aca="false">$B$58+1</f>
         <v>43920</v>
       </c>
       <c r="L50" s="0"/>
@@ -1840,38 +1866,38 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C51" s="12" t="n">
-        <v>1660</v>
-      </c>
-      <c r="D51" s="1" t="n">
-        <v>2583</v>
+        <v>50</v>
+      </c>
+      <c r="D51" s="12" t="n">
+        <v>146</v>
       </c>
       <c r="E51" s="12" t="n">
-        <f aca="false">D51/331</f>
-        <v>7.8036253776435</v>
+        <f aca="false">D51/10.36</f>
+        <v>14.0926640926641</v>
       </c>
       <c r="F51" s="12" t="n">
-        <v>363</v>
+        <v>36</v>
       </c>
       <c r="G51" s="13" t="n">
-        <v>43917</v>
+        <v>43915</v>
       </c>
       <c r="H51" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,G51)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I51" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43920</v>
+        <v>43921</v>
       </c>
       <c r="J51" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I51)</f>
         <v>-1</v>
       </c>
       <c r="K51" s="13" t="n">
-        <f aca="false">$B$46+1</f>
+        <f aca="false">$B$58+1</f>
         <v>43920</v>
       </c>
       <c r="L51" s="0"/>
@@ -1889,32 +1915,32 @@
         <v>330</v>
       </c>
       <c r="D52" s="1" t="n">
-        <v>1228</v>
+        <v>1408</v>
       </c>
       <c r="E52" s="12" t="n">
         <f aca="false">D52/67.79</f>
-        <v>18.1147661897035</v>
+        <v>20.770025077445</v>
       </c>
       <c r="F52" s="12" t="n">
-        <v>209</v>
+        <v>180</v>
       </c>
       <c r="G52" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H52" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,G52)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I52" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43920</v>
+        <v>43921</v>
       </c>
       <c r="J52" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I52)</f>
         <v>-1</v>
       </c>
       <c r="K52" s="13" t="n">
-        <f aca="false">$B$46+1</f>
+        <f aca="false">$B$58+1</f>
         <v>43920</v>
       </c>
       <c r="L52" s="0"/>
@@ -1926,38 +1952,37 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C53" s="12" t="n">
-        <v>414</v>
+        <v>1660</v>
       </c>
       <c r="D53" s="1" t="n">
-        <v>541</v>
+        <v>3141</v>
       </c>
       <c r="E53" s="12" t="n">
-        <f aca="false">D53/83.784</f>
-        <v>6.457080110761</v>
+        <f aca="false">D53/331</f>
+        <v>9.48942598187311</v>
       </c>
       <c r="F53" s="12" t="n">
-        <v>108</v>
+        <v>573</v>
       </c>
       <c r="G53" s="13" t="n">
-        <v>43918</v>
+        <v>43917</v>
       </c>
       <c r="H53" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,G53)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I53" s="13" t="n">
-        <f aca="false">$B$46+1</f>
         <v>43920</v>
       </c>
       <c r="J53" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I53)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="K53" s="13" t="n">
-        <f aca="false">$B$46+1</f>
+        <f aca="false">$B$58+1</f>
         <v>43920</v>
       </c>
       <c r="L53" s="0"/>
@@ -1969,38 +1994,38 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C54" s="12" t="n">
-        <v>50</v>
-      </c>
-      <c r="D54" s="12" t="n">
-        <v>110</v>
+        <v>414</v>
+      </c>
+      <c r="D54" s="1" t="n">
+        <v>645</v>
       </c>
       <c r="E54" s="12" t="n">
-        <f aca="false">D54/10.36</f>
-        <v>10.6177606177606</v>
+        <f aca="false">D54/83.784</f>
+        <v>7.69836723002005</v>
       </c>
       <c r="F54" s="12" t="n">
-        <v>5</v>
+        <v>104</v>
       </c>
       <c r="G54" s="13" t="n">
-        <v>43915</v>
+        <v>43918</v>
       </c>
       <c r="H54" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,G54)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I54" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43920</v>
+        <v>43921</v>
       </c>
       <c r="J54" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I54)</f>
         <v>-1</v>
       </c>
       <c r="K54" s="13" t="n">
-        <f aca="false">$B$46+1</f>
+        <f aca="false">$B$58+1</f>
         <v>43920</v>
       </c>
       <c r="L54" s="0"/>
@@ -2067,15 +2092,13 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="7" t="n">
-        <v>43918</v>
-      </c>
-      <c r="D58" s="8" t="s">
-        <v>6</v>
-      </c>
+        <v>43919</v>
+      </c>
+      <c r="D58" s="0"/>
       <c r="E58" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F58" s="8"/>
+      <c r="F58" s="0"/>
       <c r="G58" s="8" t="s">
         <v>29</v>
       </c>
@@ -2103,8 +2126,8 @@
       <c r="C59" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D59" s="10" t="s">
-        <v>2</v>
+      <c r="D59" s="8" t="s">
+        <v>6</v>
       </c>
       <c r="E59" s="10" t="s">
         <v>35</v>
@@ -2142,32 +2165,32 @@
         <v>300</v>
       </c>
       <c r="D60" s="1" t="n">
-        <v>10023</v>
+        <v>10779</v>
       </c>
       <c r="E60" s="12" t="n">
         <f aca="false">D60/60.48</f>
-        <v>165.724206349206</v>
+        <v>178.224206349206</v>
       </c>
       <c r="F60" s="12" t="n">
-        <v>889</v>
+        <v>756</v>
       </c>
       <c r="G60" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H60" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,G60)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I60" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J60" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$70,I60)</f>
-        <v>15</v>
+        <f aca="false">_xlfn.DAYS($B$58,I60)</f>
+        <v>17</v>
       </c>
       <c r="K60" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L60" s="0"/>
       <c r="M60" s="0"/>
@@ -2184,32 +2207,32 @@
         <v>230</v>
       </c>
       <c r="D61" s="1" t="n">
-        <v>5982</v>
+        <v>6803</v>
       </c>
       <c r="E61" s="12" t="n">
         <f aca="false">D61/46.75</f>
-        <v>127.957219251337</v>
+        <v>145.51871657754</v>
       </c>
       <c r="F61" s="12" t="n">
-        <v>844</v>
+        <v>821</v>
       </c>
       <c r="G61" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H61" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,G61)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I61" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J61" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$70,I61)</f>
-        <v>4</v>
+        <f aca="false">_xlfn.DAYS($B$58,I61)</f>
+        <v>6</v>
       </c>
       <c r="K61" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L61" s="0"/>
       <c r="M61" s="0"/>
@@ -2226,32 +2249,32 @@
         <v>330</v>
       </c>
       <c r="D62" s="1" t="n">
-        <v>2314</v>
+        <v>2606</v>
       </c>
       <c r="E62" s="12" t="n">
         <f aca="false">D62/65.27</f>
-        <v>35.4527347939329</v>
+        <v>39.9264593228129</v>
       </c>
       <c r="F62" s="12" t="n">
-        <v>319</v>
+        <v>292</v>
       </c>
       <c r="G62" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H62" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,G62)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I62" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J62" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$70,I62)</f>
-        <v>3</v>
+        <f aca="false">_xlfn.DAYS($B$58,I62)</f>
+        <v>5</v>
       </c>
       <c r="K62" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L62" s="0"/>
       <c r="M62" s="0"/>
@@ -2268,25 +2291,25 @@
         <v>1660</v>
       </c>
       <c r="D63" s="1" t="n">
-        <v>2221</v>
+        <v>2583</v>
       </c>
       <c r="E63" s="12" t="n">
         <f aca="false">D63/331</f>
-        <v>6.70996978851964</v>
+        <v>7.8036253776435</v>
       </c>
       <c r="F63" s="12" t="n">
-        <v>525</v>
+        <v>363</v>
       </c>
       <c r="G63" s="13" t="n">
         <v>43917</v>
       </c>
       <c r="H63" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,G63)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I63" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="J63" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I63)</f>
@@ -2294,7 +2317,7 @@
       </c>
       <c r="K63" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L63" s="0"/>
       <c r="M63" s="0"/>
@@ -2311,25 +2334,25 @@
         <v>330</v>
       </c>
       <c r="D64" s="1" t="n">
-        <v>1019</v>
+        <v>1228</v>
       </c>
       <c r="E64" s="12" t="n">
         <f aca="false">D64/67.79</f>
-        <v>15.0317155922702</v>
+        <v>18.1147661897035</v>
       </c>
       <c r="F64" s="12" t="n">
-        <v>260</v>
+        <v>209</v>
       </c>
       <c r="G64" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H64" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,G64)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I64" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="J64" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I64)</f>
@@ -2337,7 +2360,7 @@
       </c>
       <c r="K64" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L64" s="0"/>
       <c r="M64" s="0"/>
@@ -2354,25 +2377,25 @@
         <v>414</v>
       </c>
       <c r="D65" s="1" t="n">
-        <v>433</v>
+        <v>541</v>
       </c>
       <c r="E65" s="12" t="n">
         <f aca="false">D65/83.784</f>
-        <v>5.16805117922276</v>
+        <v>6.457080110761</v>
       </c>
       <c r="F65" s="12" t="n">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="G65" s="13" t="n">
         <v>43918</v>
       </c>
       <c r="H65" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,G65)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I65" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="J65" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I65)</f>
@@ -2380,7 +2403,7 @@
       </c>
       <c r="K65" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L65" s="0"/>
       <c r="M65" s="0"/>
@@ -2397,25 +2420,25 @@
         <v>50</v>
       </c>
       <c r="D66" s="12" t="n">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="E66" s="12" t="n">
         <f aca="false">D66/10.36</f>
-        <v>10.1351351351351</v>
+        <v>10.6177606177606</v>
       </c>
       <c r="F66" s="12" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G66" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H66" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,G66)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I66" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="J66" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I66)</f>
@@ -2423,7 +2446,7 @@
       </c>
       <c r="K66" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L66" s="0"/>
       <c r="M66" s="0"/>
@@ -2433,15 +2456,16 @@
       <c r="Q66" s="0"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C67" s="12"/>
-      <c r="D67" s="12"/>
-      <c r="E67" s="12"/>
-      <c r="F67" s="12"/>
-      <c r="G67" s="13"/>
+      <c r="B67" s="4"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="0"/>
+      <c r="E67" s="0"/>
+      <c r="F67" s="0"/>
+      <c r="G67" s="0"/>
       <c r="H67" s="0"/>
-      <c r="I67" s="13"/>
+      <c r="I67" s="0"/>
       <c r="J67" s="0"/>
-      <c r="K67" s="13"/>
+      <c r="K67" s="0"/>
       <c r="L67" s="0"/>
       <c r="M67" s="0"/>
       <c r="N67" s="0"/>
@@ -2486,11 +2510,10 @@
       <c r="P69" s="0"/>
       <c r="Q69" s="0"/>
     </row>
-    <row r="70" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="7" t="n">
-        <v>43917</v>
-      </c>
-      <c r="C70" s="0"/>
+        <v>43918</v>
+      </c>
       <c r="D70" s="8" t="s">
         <v>6</v>
       </c>
@@ -2513,10 +2536,14 @@
       <c r="K70" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="L70" s="8"/>
+      <c r="L70" s="0"/>
+      <c r="M70" s="0"/>
+      <c r="N70" s="0"/>
+      <c r="O70" s="0"/>
+      <c r="P70" s="0"/>
+      <c r="Q70" s="0"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="3"/>
       <c r="B71" s="9"/>
       <c r="C71" s="10" t="s">
         <v>34</v>
@@ -2545,7 +2572,7 @@
       <c r="K71" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L71" s="8"/>
+      <c r="L71" s="0"/>
       <c r="M71" s="0"/>
       <c r="N71" s="0"/>
       <c r="O71" s="0"/>
@@ -2560,32 +2587,32 @@
         <v>300</v>
       </c>
       <c r="D72" s="1" t="n">
-        <v>9134</v>
+        <v>10023</v>
       </c>
       <c r="E72" s="12" t="n">
         <f aca="false">D72/60.48</f>
-        <v>151.025132275132</v>
+        <v>165.724206349206</v>
       </c>
       <c r="F72" s="12" t="n">
-        <v>919</v>
+        <v>889</v>
       </c>
       <c r="G72" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H72" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,G72)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I72" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J72" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$70,I72)</f>
+        <f aca="false">_xlfn.DAYS(B$82,I72)</f>
         <v>15</v>
       </c>
       <c r="K72" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L72" s="0"/>
       <c r="M72" s="0"/>
@@ -2602,32 +2629,32 @@
         <v>230</v>
       </c>
       <c r="D73" s="1" t="n">
-        <v>5138</v>
+        <v>5982</v>
       </c>
       <c r="E73" s="12" t="n">
         <f aca="false">D73/46.75</f>
-        <v>109.903743315508</v>
+        <v>127.957219251337</v>
       </c>
       <c r="F73" s="12" t="n">
-        <v>773</v>
+        <v>844</v>
       </c>
       <c r="G73" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H73" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,G73)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I73" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J73" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$70,I73)</f>
+        <f aca="false">_xlfn.DAYS(B$82,I73)</f>
         <v>4</v>
       </c>
       <c r="K73" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L73" s="0"/>
       <c r="M73" s="0"/>
@@ -2644,32 +2671,32 @@
         <v>330</v>
       </c>
       <c r="D74" s="1" t="n">
-        <v>1995</v>
+        <v>2314</v>
       </c>
       <c r="E74" s="12" t="n">
         <f aca="false">D74/65.27</f>
-        <v>30.5653439558756</v>
+        <v>35.4527347939329</v>
       </c>
       <c r="F74" s="12" t="n">
-        <v>299</v>
+        <v>319</v>
       </c>
       <c r="G74" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H74" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,G74)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I74" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J74" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$70,I74)</f>
+        <f aca="false">_xlfn.DAYS(B$82,I74)</f>
         <v>3</v>
       </c>
       <c r="K74" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L74" s="0"/>
       <c r="M74" s="0"/>
@@ -2686,34 +2713,33 @@
         <v>1660</v>
       </c>
       <c r="D75" s="1" t="n">
-        <v>1696</v>
+        <v>2221</v>
       </c>
       <c r="E75" s="12" t="n">
         <f aca="false">D75/331</f>
-        <v>5.12386706948641</v>
+        <v>6.70996978851964</v>
       </c>
       <c r="F75" s="12" t="n">
-        <v>400</v>
+        <v>525</v>
       </c>
       <c r="G75" s="13" t="n">
-        <f aca="false">$B$70</f>
         <v>43917</v>
       </c>
       <c r="H75" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,G75)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I75" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="J75" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$70,I75)</f>
+        <f aca="false">_xlfn.DAYS($B$70,I75)</f>
         <v>-1</v>
       </c>
       <c r="K75" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L75" s="0"/>
       <c r="M75" s="0"/>
@@ -2730,33 +2756,33 @@
         <v>330</v>
       </c>
       <c r="D76" s="1" t="n">
-        <v>759</v>
+        <v>1019</v>
       </c>
       <c r="E76" s="12" t="n">
         <f aca="false">D76/67.79</f>
-        <v>11.1963416433102</v>
+        <v>15.0317155922702</v>
       </c>
       <c r="F76" s="12" t="n">
-        <v>181</v>
+        <v>260</v>
       </c>
       <c r="G76" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H76" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,G76)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I76" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="J76" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$70,I76)</f>
+        <f aca="false">_xlfn.DAYS($B$70,I76)</f>
         <v>-1</v>
       </c>
       <c r="K76" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L76" s="0"/>
       <c r="M76" s="0"/>
@@ -2773,34 +2799,33 @@
         <v>414</v>
       </c>
       <c r="D77" s="1" t="n">
-        <v>351</v>
+        <v>433</v>
       </c>
       <c r="E77" s="12" t="n">
         <f aca="false">D77/83.784</f>
-        <v>4.18934402749928</v>
+        <v>5.16805117922276</v>
       </c>
       <c r="F77" s="12" t="n">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G77" s="13" t="n">
-        <f aca="false">$B$70+1</f>
         <v>43918</v>
       </c>
       <c r="H77" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,G77)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="I77" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="J77" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$70,I77)</f>
+        <f aca="false">_xlfn.DAYS($B$70,I77)</f>
         <v>-1</v>
       </c>
       <c r="K77" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L77" s="0"/>
       <c r="M77" s="0"/>
@@ -2824,26 +2849,26 @@
         <v>10.1351351351351</v>
       </c>
       <c r="F78" s="12" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="G78" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H78" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,G78)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I78" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="J78" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$70,I78)</f>
+        <f aca="false">_xlfn.DAYS($B$70,I78)</f>
         <v>-1</v>
       </c>
       <c r="K78" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L78" s="0"/>
       <c r="M78" s="0"/>
@@ -2853,14 +2878,15 @@
       <c r="Q78" s="0"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D79" s="0"/>
-      <c r="E79" s="0"/>
-      <c r="F79" s="0"/>
-      <c r="G79" s="0"/>
+      <c r="C79" s="12"/>
+      <c r="D79" s="12"/>
+      <c r="E79" s="12"/>
+      <c r="F79" s="12"/>
+      <c r="G79" s="13"/>
       <c r="H79" s="0"/>
-      <c r="I79" s="0"/>
+      <c r="I79" s="13"/>
       <c r="J79" s="0"/>
-      <c r="K79" s="0"/>
+      <c r="K79" s="13"/>
       <c r="L79" s="0"/>
       <c r="M79" s="0"/>
       <c r="N79" s="0"/>
@@ -2869,6 +2895,8 @@
       <c r="Q79" s="0"/>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B80" s="4"/>
+      <c r="C80" s="5"/>
       <c r="D80" s="0"/>
       <c r="E80" s="0"/>
       <c r="F80" s="0"/>
@@ -2903,10 +2931,11 @@
       <c r="P81" s="0"/>
       <c r="Q81" s="0"/>
     </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="7" t="n">
-        <v>43916</v>
-      </c>
+        <v>43917</v>
+      </c>
+      <c r="C82" s="0"/>
       <c r="D82" s="8" t="s">
         <v>6</v>
       </c>
@@ -2929,17 +2958,13 @@
       <c r="K82" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="L82" s="0"/>
-      <c r="M82" s="0"/>
-      <c r="N82" s="0"/>
-      <c r="O82" s="0"/>
-      <c r="P82" s="0"/>
-      <c r="Q82" s="0"/>
+      <c r="L82" s="8"/>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="3"/>
       <c r="B83" s="9"/>
       <c r="C83" s="10" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="D83" s="10" t="s">
         <v>2</v>
@@ -2965,7 +2990,7 @@
       <c r="K83" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L83" s="0"/>
+      <c r="L83" s="8"/>
       <c r="M83" s="0"/>
       <c r="N83" s="0"/>
       <c r="O83" s="0"/>
@@ -2980,32 +3005,32 @@
         <v>300</v>
       </c>
       <c r="D84" s="1" t="n">
-        <v>8215</v>
+        <v>9134</v>
       </c>
       <c r="E84" s="12" t="n">
         <f aca="false">D84/60.48</f>
-        <v>135.830026455026</v>
+        <v>151.025132275132</v>
       </c>
       <c r="F84" s="12" t="n">
-        <v>712</v>
+        <v>919</v>
       </c>
       <c r="G84" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H84" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$82,G84)</f>
-        <v>16</v>
+        <f aca="false">_xlfn.DAYS($B$82,G84)</f>
+        <v>17</v>
       </c>
       <c r="I84" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J84" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$82,I84)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K84" s="13" t="n">
-        <f aca="false">B$82+1</f>
-        <v>43917</v>
+        <f aca="false">$B$82+1</f>
+        <v>43918</v>
       </c>
       <c r="L84" s="0"/>
       <c r="M84" s="0"/>
@@ -3022,32 +3047,32 @@
         <v>230</v>
       </c>
       <c r="D85" s="1" t="n">
-        <v>4365</v>
+        <v>5138</v>
       </c>
       <c r="E85" s="12" t="n">
         <f aca="false">D85/46.75</f>
-        <v>93.3689839572193</v>
+        <v>109.903743315508</v>
       </c>
       <c r="F85" s="12" t="n">
-        <v>718</v>
+        <v>773</v>
       </c>
       <c r="G85" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H85" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$82,G85)</f>
-        <v>9</v>
+        <f aca="false">_xlfn.DAYS($B$82,G85)</f>
+        <v>10</v>
       </c>
       <c r="I85" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J85" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$82,I85)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K85" s="13" t="n">
-        <f aca="false">B$82+1</f>
-        <v>43917</v>
+        <f aca="false">$B$82+1</f>
+        <v>43918</v>
       </c>
       <c r="L85" s="0"/>
       <c r="M85" s="0"/>
@@ -3064,32 +3089,32 @@
         <v>330</v>
       </c>
       <c r="D86" s="1" t="n">
-        <v>1696</v>
+        <v>1995</v>
       </c>
       <c r="E86" s="12" t="n">
         <f aca="false">D86/65.27</f>
-        <v>25.9843726060978</v>
+        <v>30.5653439558756</v>
       </c>
       <c r="F86" s="12" t="n">
-        <v>365</v>
+        <v>299</v>
       </c>
       <c r="G86" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H86" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$82,G86)</f>
-        <v>4</v>
+        <f aca="false">_xlfn.DAYS($B$82,G86)</f>
+        <v>5</v>
       </c>
       <c r="I86" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J86" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$82,I86)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K86" s="13" t="n">
-        <f aca="false">B$82+1</f>
-        <v>43917</v>
+        <f aca="false">$B$82+1</f>
+        <v>43918</v>
       </c>
       <c r="L86" s="0"/>
       <c r="M86" s="0"/>
@@ -3106,33 +3131,34 @@
         <v>1660</v>
       </c>
       <c r="D87" s="1" t="n">
-        <v>1295</v>
+        <v>1696</v>
       </c>
       <c r="E87" s="12" t="n">
         <f aca="false">D87/331</f>
-        <v>3.91238670694864</v>
+        <v>5.12386706948641</v>
       </c>
       <c r="F87" s="12" t="n">
-        <v>268</v>
+        <v>400</v>
       </c>
       <c r="G87" s="13" t="n">
+        <f aca="false">$B$82</f>
         <v>43917</v>
       </c>
       <c r="H87" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$82,G87)</f>
+        <f aca="false">_xlfn.DAYS($B$82,G87)</f>
+        <v>0</v>
+      </c>
+      <c r="I87" s="13" t="n">
+        <f aca="false">$B$82+1</f>
+        <v>43918</v>
+      </c>
+      <c r="J87" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$82,I87)</f>
         <v>-1</v>
       </c>
-      <c r="I87" s="13" t="n">
-        <f aca="false">B$82+1</f>
-        <v>43917</v>
-      </c>
-      <c r="J87" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$82,I87)</f>
-        <v>-1</v>
-      </c>
       <c r="K87" s="13" t="n">
-        <f aca="false">B$82+1</f>
-        <v>43917</v>
+        <f aca="false">$B$82+1</f>
+        <v>43918</v>
       </c>
       <c r="L87" s="0"/>
       <c r="M87" s="0"/>
@@ -3149,33 +3175,33 @@
         <v>330</v>
       </c>
       <c r="D88" s="1" t="n">
-        <v>578</v>
+        <v>759</v>
       </c>
       <c r="E88" s="12" t="n">
         <f aca="false">D88/67.79</f>
-        <v>8.52633131730344</v>
+        <v>11.1963416433102</v>
       </c>
       <c r="F88" s="12" t="n">
-        <v>115</v>
+        <v>181</v>
       </c>
       <c r="G88" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H88" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$82,G88)</f>
-        <v>0</v>
+        <f aca="false">_xlfn.DAYS($B$82,G88)</f>
+        <v>1</v>
       </c>
       <c r="I88" s="13" t="n">
-        <f aca="false">B$82+1</f>
-        <v>43917</v>
+        <f aca="false">$B$82+1</f>
+        <v>43918</v>
       </c>
       <c r="J88" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$82,I88)</f>
         <v>-1</v>
       </c>
       <c r="K88" s="13" t="n">
-        <f aca="false">B$82+1</f>
-        <v>43917</v>
+        <f aca="false">$B$82+1</f>
+        <v>43918</v>
       </c>
       <c r="L88" s="0"/>
       <c r="M88" s="0"/>
@@ -3192,33 +3218,34 @@
         <v>414</v>
       </c>
       <c r="D89" s="1" t="n">
-        <v>267</v>
+        <v>351</v>
       </c>
       <c r="E89" s="12" t="n">
         <f aca="false">D89/83.784</f>
-        <v>3.18676596963621</v>
+        <v>4.18934402749928</v>
       </c>
       <c r="F89" s="12" t="n">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="G89" s="13" t="n">
-        <v>43917</v>
+        <f aca="false">$B$82+1</f>
+        <v>43918</v>
       </c>
       <c r="H89" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$82,G89)</f>
+        <f aca="false">_xlfn.DAYS($B$82,G89)</f>
         <v>-1</v>
       </c>
       <c r="I89" s="13" t="n">
-        <f aca="false">B$82+1</f>
-        <v>43917</v>
+        <f aca="false">$B$82+1</f>
+        <v>43918</v>
       </c>
       <c r="J89" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$82,I89)</f>
         <v>-1</v>
       </c>
       <c r="K89" s="13" t="n">
-        <f aca="false">B$82+1</f>
-        <v>43917</v>
+        <f aca="false">$B$82+1</f>
+        <v>43918</v>
       </c>
       <c r="L89" s="0"/>
       <c r="M89" s="0"/>
@@ -3235,33 +3262,33 @@
         <v>50</v>
       </c>
       <c r="D90" s="12" t="n">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="E90" s="12" t="n">
         <f aca="false">D90/10.36</f>
-        <v>7.43243243243243</v>
+        <v>10.1351351351351</v>
       </c>
       <c r="F90" s="12" t="n">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="G90" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H90" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$82,G90)</f>
-        <v>1</v>
+        <f aca="false">_xlfn.DAYS($B$82,G90)</f>
+        <v>2</v>
       </c>
       <c r="I90" s="13" t="n">
-        <f aca="false">B$82+1</f>
-        <v>43917</v>
+        <f aca="false">$B$82+1</f>
+        <v>43918</v>
       </c>
       <c r="J90" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$82,I90)</f>
         <v>-1</v>
       </c>
       <c r="K90" s="13" t="n">
-        <f aca="false">B$82+1</f>
-        <v>43917</v>
+        <f aca="false">$B$82+1</f>
+        <v>43918</v>
       </c>
       <c r="L90" s="0"/>
       <c r="M90" s="0"/>
@@ -3269,6 +3296,424 @@
       <c r="O90" s="0"/>
       <c r="P90" s="0"/>
       <c r="Q90" s="0"/>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D91" s="0"/>
+      <c r="E91" s="0"/>
+      <c r="F91" s="0"/>
+      <c r="G91" s="0"/>
+      <c r="H91" s="0"/>
+      <c r="I91" s="0"/>
+      <c r="J91" s="0"/>
+      <c r="K91" s="0"/>
+      <c r="L91" s="0"/>
+      <c r="M91" s="0"/>
+      <c r="N91" s="0"/>
+      <c r="O91" s="0"/>
+      <c r="P91" s="0"/>
+      <c r="Q91" s="0"/>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D92" s="0"/>
+      <c r="E92" s="0"/>
+      <c r="F92" s="0"/>
+      <c r="G92" s="0"/>
+      <c r="H92" s="0"/>
+      <c r="I92" s="0"/>
+      <c r="J92" s="0"/>
+      <c r="K92" s="0"/>
+      <c r="L92" s="0"/>
+      <c r="M92" s="0"/>
+      <c r="N92" s="0"/>
+      <c r="O92" s="0"/>
+      <c r="P92" s="0"/>
+      <c r="Q92" s="0"/>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B93" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D93" s="0"/>
+      <c r="E93" s="0"/>
+      <c r="F93" s="0"/>
+      <c r="G93" s="0"/>
+      <c r="H93" s="0"/>
+      <c r="I93" s="0"/>
+      <c r="J93" s="0"/>
+      <c r="K93" s="0"/>
+      <c r="L93" s="0"/>
+      <c r="M93" s="0"/>
+      <c r="N93" s="0"/>
+      <c r="O93" s="0"/>
+      <c r="P93" s="0"/>
+      <c r="Q93" s="0"/>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B94" s="7" t="n">
+        <v>43916</v>
+      </c>
+      <c r="D94" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E94" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F94" s="8"/>
+      <c r="G94" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H94" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I94" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="J94" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K94" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="L94" s="0"/>
+      <c r="M94" s="0"/>
+      <c r="N94" s="0"/>
+      <c r="O94" s="0"/>
+      <c r="P94" s="0"/>
+      <c r="Q94" s="0"/>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B95" s="9"/>
+      <c r="C95" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D95" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E95" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F95" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G95" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H95" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I95" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="J95" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K95" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L95" s="0"/>
+      <c r="M95" s="0"/>
+      <c r="N95" s="0"/>
+      <c r="O95" s="0"/>
+      <c r="P95" s="0"/>
+      <c r="Q95" s="0"/>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B96" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C96" s="12" t="n">
+        <v>300</v>
+      </c>
+      <c r="D96" s="1" t="n">
+        <v>8215</v>
+      </c>
+      <c r="E96" s="12" t="n">
+        <f aca="false">D96/60.48</f>
+        <v>135.830026455026</v>
+      </c>
+      <c r="F96" s="12" t="n">
+        <v>712</v>
+      </c>
+      <c r="G96" s="13" t="n">
+        <v>43900</v>
+      </c>
+      <c r="H96" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$94,G96)</f>
+        <v>16</v>
+      </c>
+      <c r="I96" s="13" t="n">
+        <v>43902</v>
+      </c>
+      <c r="J96" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$94,I96)</f>
+        <v>14</v>
+      </c>
+      <c r="K96" s="13" t="n">
+        <f aca="false">B$94+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L96" s="0"/>
+      <c r="M96" s="0"/>
+      <c r="N96" s="0"/>
+      <c r="O96" s="0"/>
+      <c r="P96" s="0"/>
+      <c r="Q96" s="0"/>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B97" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C97" s="12" t="n">
+        <v>230</v>
+      </c>
+      <c r="D97" s="1" t="n">
+        <v>4365</v>
+      </c>
+      <c r="E97" s="12" t="n">
+        <f aca="false">D97/46.75</f>
+        <v>93.3689839572193</v>
+      </c>
+      <c r="F97" s="12" t="n">
+        <v>718</v>
+      </c>
+      <c r="G97" s="13" t="n">
+        <v>43907</v>
+      </c>
+      <c r="H97" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$94,G97)</f>
+        <v>9</v>
+      </c>
+      <c r="I97" s="13" t="n">
+        <v>43913</v>
+      </c>
+      <c r="J97" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$94,I97)</f>
+        <v>3</v>
+      </c>
+      <c r="K97" s="13" t="n">
+        <f aca="false">B$94+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L97" s="0"/>
+      <c r="M97" s="0"/>
+      <c r="N97" s="0"/>
+      <c r="O97" s="0"/>
+      <c r="P97" s="0"/>
+      <c r="Q97" s="0"/>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B98" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C98" s="12" t="n">
+        <v>330</v>
+      </c>
+      <c r="D98" s="1" t="n">
+        <v>1696</v>
+      </c>
+      <c r="E98" s="12" t="n">
+        <f aca="false">D98/65.27</f>
+        <v>25.9843726060978</v>
+      </c>
+      <c r="F98" s="12" t="n">
+        <v>365</v>
+      </c>
+      <c r="G98" s="13" t="n">
+        <v>43912</v>
+      </c>
+      <c r="H98" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$94,G98)</f>
+        <v>4</v>
+      </c>
+      <c r="I98" s="13" t="n">
+        <v>43914</v>
+      </c>
+      <c r="J98" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$94,I98)</f>
+        <v>2</v>
+      </c>
+      <c r="K98" s="13" t="n">
+        <f aca="false">B$94+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L98" s="0"/>
+      <c r="M98" s="0"/>
+      <c r="N98" s="0"/>
+      <c r="O98" s="0"/>
+      <c r="P98" s="0"/>
+      <c r="Q98" s="0"/>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B99" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C99" s="12" t="n">
+        <v>1660</v>
+      </c>
+      <c r="D99" s="1" t="n">
+        <v>1295</v>
+      </c>
+      <c r="E99" s="12" t="n">
+        <f aca="false">D99/331</f>
+        <v>3.91238670694864</v>
+      </c>
+      <c r="F99" s="12" t="n">
+        <v>268</v>
+      </c>
+      <c r="G99" s="13" t="n">
+        <v>43917</v>
+      </c>
+      <c r="H99" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$94,G99)</f>
+        <v>-1</v>
+      </c>
+      <c r="I99" s="13" t="n">
+        <f aca="false">B$94+1</f>
+        <v>43917</v>
+      </c>
+      <c r="J99" s="1" t="n">
+        <f aca="false">_xlfn.DAYS($B$94,I99)</f>
+        <v>-1</v>
+      </c>
+      <c r="K99" s="13" t="n">
+        <f aca="false">B$94+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L99" s="0"/>
+      <c r="M99" s="0"/>
+      <c r="N99" s="0"/>
+      <c r="O99" s="0"/>
+      <c r="P99" s="0"/>
+      <c r="Q99" s="0"/>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B100" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C100" s="12" t="n">
+        <v>330</v>
+      </c>
+      <c r="D100" s="1" t="n">
+        <v>578</v>
+      </c>
+      <c r="E100" s="12" t="n">
+        <f aca="false">D100/67.79</f>
+        <v>8.52633131730344</v>
+      </c>
+      <c r="F100" s="12" t="n">
+        <v>115</v>
+      </c>
+      <c r="G100" s="13" t="n">
+        <v>43916</v>
+      </c>
+      <c r="H100" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$94,G100)</f>
+        <v>0</v>
+      </c>
+      <c r="I100" s="13" t="n">
+        <f aca="false">B$94+1</f>
+        <v>43917</v>
+      </c>
+      <c r="J100" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$94,I100)</f>
+        <v>-1</v>
+      </c>
+      <c r="K100" s="13" t="n">
+        <f aca="false">B$94+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L100" s="0"/>
+      <c r="M100" s="0"/>
+      <c r="N100" s="0"/>
+      <c r="O100" s="0"/>
+      <c r="P100" s="0"/>
+      <c r="Q100" s="0"/>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B101" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C101" s="12" t="n">
+        <v>414</v>
+      </c>
+      <c r="D101" s="1" t="n">
+        <v>267</v>
+      </c>
+      <c r="E101" s="12" t="n">
+        <f aca="false">D101/83.784</f>
+        <v>3.18676596963621</v>
+      </c>
+      <c r="F101" s="12" t="n">
+        <v>61</v>
+      </c>
+      <c r="G101" s="13" t="n">
+        <v>43917</v>
+      </c>
+      <c r="H101" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$94,G101)</f>
+        <v>-1</v>
+      </c>
+      <c r="I101" s="13" t="n">
+        <f aca="false">B$94+1</f>
+        <v>43917</v>
+      </c>
+      <c r="J101" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$94,I101)</f>
+        <v>-1</v>
+      </c>
+      <c r="K101" s="13" t="n">
+        <f aca="false">B$94+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L101" s="0"/>
+      <c r="M101" s="0"/>
+      <c r="N101" s="0"/>
+      <c r="O101" s="0"/>
+      <c r="P101" s="0"/>
+      <c r="Q101" s="0"/>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B102" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C102" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="D102" s="12" t="n">
+        <v>77</v>
+      </c>
+      <c r="E102" s="12" t="n">
+        <f aca="false">D102/10.36</f>
+        <v>7.43243243243243</v>
+      </c>
+      <c r="F102" s="12" t="n">
+        <v>15</v>
+      </c>
+      <c r="G102" s="13" t="n">
+        <v>43915</v>
+      </c>
+      <c r="H102" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$94,G102)</f>
+        <v>1</v>
+      </c>
+      <c r="I102" s="13" t="n">
+        <f aca="false">B$94+1</f>
+        <v>43917</v>
+      </c>
+      <c r="J102" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$94,I102)</f>
+        <v>-1</v>
+      </c>
+      <c r="K102" s="13" t="n">
+        <f aca="false">B$94+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L102" s="0"/>
+      <c r="M102" s="0"/>
+      <c r="N102" s="0"/>
+      <c r="O102" s="0"/>
+      <c r="P102" s="0"/>
+      <c r="Q102" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
updated with 2020-04-02 available data
</commit_message>
<xml_diff>
--- a/covid19 lockdown evaluation .xlsx
+++ b/covid19 lockdown evaluation .xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="49">
   <si>
     <t>Effects of the lockdown issued by governments</t>
   </si>
@@ -341,9 +341,9 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q102"/>
+  <dimension ref="A1:Q114"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F31" activeCellId="0" sqref="F31"/>
     </sheetView>
   </sheetViews>
@@ -785,7 +785,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="7" t="n">
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="D22" s="0"/>
       <c r="E22" s="8" t="s">
@@ -862,36 +862,36 @@
         <v>300</v>
       </c>
       <c r="D24" s="1" t="n">
-        <v>13155</v>
+        <v>13915</v>
       </c>
       <c r="E24" s="12" t="n">
         <f aca="false">D24/60.48</f>
-        <v>217.509920634921</v>
+        <v>230.076058201058</v>
       </c>
       <c r="F24" s="12" t="n">
-        <v>727</v>
+        <v>760</v>
       </c>
       <c r="G24" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H24" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,G24)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I24" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J24" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I24)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K24" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="L24" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K24,G24)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M24" s="0"/>
       <c r="N24" s="0"/>
@@ -907,36 +907,36 @@
         <v>230</v>
       </c>
       <c r="D25" s="1" t="n">
-        <v>9387</v>
+        <v>10348</v>
       </c>
       <c r="E25" s="12" t="n">
         <f aca="false">D25/46.75</f>
-        <v>200.791443850267</v>
+        <v>221.347593582888</v>
       </c>
       <c r="F25" s="12" t="n">
-        <v>923</v>
+        <v>961</v>
       </c>
       <c r="G25" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H25" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,G25)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I25" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J25" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I25)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K25" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="L25" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K25,G25)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M25" s="0"/>
       <c r="N25" s="0"/>
@@ -952,36 +952,36 @@
         <v>330</v>
       </c>
       <c r="D26" s="1" t="n">
-        <v>4032</v>
+        <v>5387</v>
       </c>
       <c r="E26" s="12" t="n">
         <f aca="false">D26/65.27</f>
-        <v>61.7741688371381</v>
+        <v>82.5340891680711</v>
       </c>
       <c r="F26" s="12" t="n">
-        <v>509</v>
+        <v>1355</v>
       </c>
       <c r="G26" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H26" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,G26)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I26" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J26" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I26)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K26" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="L26" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K26,G26)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M26" s="0"/>
       <c r="N26" s="0"/>
@@ -997,25 +997,25 @@
         <v>50</v>
       </c>
       <c r="D27" s="12" t="n">
-        <v>239</v>
+        <v>308</v>
       </c>
       <c r="E27" s="12" t="n">
         <f aca="false">D27/10.36</f>
-        <v>23.0694980694981</v>
+        <v>29.7297297297297</v>
       </c>
       <c r="F27" s="12" t="n">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="G27" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H27" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,G27)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I27" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="J27" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I27)</f>
@@ -1023,11 +1023,11 @@
       </c>
       <c r="K27" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="L27" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K27,G27)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M27" s="0"/>
       <c r="N27" s="0"/>
@@ -1043,25 +1043,25 @@
         <v>330</v>
       </c>
       <c r="D28" s="1" t="n">
-        <v>2352</v>
+        <v>2921</v>
       </c>
       <c r="E28" s="12" t="n">
         <f aca="false">D28/67.79</f>
-        <v>34.695382799823</v>
+        <v>43.0889511727393</v>
       </c>
       <c r="F28" s="12" t="n">
-        <v>563</v>
+        <v>569</v>
       </c>
       <c r="G28" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H28" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,G28)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I28" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="J28" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I28)</f>
@@ -1069,11 +1069,11 @@
       </c>
       <c r="K28" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="L28" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K28,G28)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M28" s="0"/>
       <c r="N28" s="0"/>
@@ -1089,25 +1089,25 @@
         <v>1660</v>
       </c>
       <c r="D29" s="1" t="n">
-        <v>5102</v>
+        <v>6070</v>
       </c>
       <c r="E29" s="12" t="n">
         <f aca="false">D29/331</f>
-        <v>15.4138972809668</v>
+        <v>18.3383685800604</v>
       </c>
       <c r="F29" s="12" t="n">
-        <v>1049</v>
+        <v>968</v>
       </c>
       <c r="G29" s="13" t="n">
         <v>43917</v>
       </c>
       <c r="H29" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,G29)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I29" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="J29" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I29)</f>
@@ -1115,11 +1115,11 @@
       </c>
       <c r="K29" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="L29" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K29,G29)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M29" s="0"/>
       <c r="N29" s="0"/>
@@ -1135,25 +1135,25 @@
         <v>414</v>
       </c>
       <c r="D30" s="1" t="n">
-        <v>931</v>
+        <v>1107</v>
       </c>
       <c r="E30" s="12" t="n">
         <f aca="false">D30/83.784</f>
-        <v>11.1119068079824</v>
+        <v>13.212546548267</v>
       </c>
       <c r="F30" s="12" t="n">
-        <v>156</v>
+        <v>176</v>
       </c>
       <c r="G30" s="13" t="n">
         <v>43918</v>
       </c>
       <c r="H30" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,G30)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I30" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="J30" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I30)</f>
@@ -1161,11 +1161,11 @@
       </c>
       <c r="K30" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="L30" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K30,G30)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M30" s="0"/>
       <c r="N30" s="0"/>
@@ -1230,7 +1230,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="7" t="n">
-        <v>43921</v>
+        <v>43922</v>
       </c>
       <c r="D34" s="0"/>
       <c r="E34" s="8" t="s">
@@ -1307,36 +1307,36 @@
         <v>300</v>
       </c>
       <c r="D36" s="1" t="n">
-        <v>12428</v>
+        <v>13155</v>
       </c>
       <c r="E36" s="12" t="n">
         <f aca="false">D36/60.48</f>
-        <v>205.489417989418</v>
+        <v>217.509920634921</v>
       </c>
       <c r="F36" s="12" t="n">
-        <v>837</v>
+        <v>727</v>
       </c>
       <c r="G36" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H36" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,G36)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I36" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J36" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I36)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K36" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L36" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K36,G36)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M36" s="0"/>
       <c r="N36" s="0"/>
@@ -1352,36 +1352,36 @@
         <v>230</v>
       </c>
       <c r="D37" s="1" t="n">
-        <v>8464</v>
+        <v>9387</v>
       </c>
       <c r="E37" s="12" t="n">
         <f aca="false">D37/46.75</f>
-        <v>181.048128342246</v>
+        <v>200.791443850267</v>
       </c>
       <c r="F37" s="12" t="n">
-        <v>748</v>
+        <v>923</v>
       </c>
       <c r="G37" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H37" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,G37)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I37" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J37" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I37)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K37" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L37" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K37,G37)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M37" s="0"/>
       <c r="N37" s="0"/>
@@ -1397,36 +1397,36 @@
         <v>330</v>
       </c>
       <c r="D38" s="1" t="n">
-        <v>3523</v>
+        <v>4032</v>
       </c>
       <c r="E38" s="12" t="n">
         <f aca="false">D38/65.27</f>
-        <v>53.9757928604259</v>
+        <v>61.7741688371381</v>
       </c>
       <c r="F38" s="12" t="n">
-        <v>499</v>
+        <v>509</v>
       </c>
       <c r="G38" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H38" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,G38)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I38" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J38" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I38)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K38" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L38" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K38,G38)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M38" s="0"/>
       <c r="N38" s="0"/>
@@ -1442,25 +1442,25 @@
         <v>50</v>
       </c>
       <c r="D39" s="12" t="n">
-        <v>180</v>
+        <v>239</v>
       </c>
       <c r="E39" s="12" t="n">
         <f aca="false">D39/10.36</f>
-        <v>17.3745173745174</v>
+        <v>23.0694980694981</v>
       </c>
       <c r="F39" s="12" t="n">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="G39" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H39" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,G39)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I39" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="J39" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I39)</f>
@@ -1468,11 +1468,11 @@
       </c>
       <c r="K39" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L39" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K39,G39)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M39" s="0"/>
       <c r="N39" s="0"/>
@@ -1488,25 +1488,25 @@
         <v>330</v>
       </c>
       <c r="D40" s="1" t="n">
-        <v>1789</v>
+        <v>2352</v>
       </c>
       <c r="E40" s="12" t="n">
         <f aca="false">D40/67.79</f>
-        <v>26.390323056498</v>
+        <v>34.695382799823</v>
       </c>
       <c r="F40" s="12" t="n">
-        <v>381</v>
+        <v>563</v>
       </c>
       <c r="G40" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H40" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,G40)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I40" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="J40" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I40)</f>
@@ -1514,11 +1514,11 @@
       </c>
       <c r="K40" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L40" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K40,G40)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M40" s="0"/>
       <c r="N40" s="0"/>
@@ -1534,25 +1534,25 @@
         <v>1660</v>
       </c>
       <c r="D41" s="1" t="n">
-        <v>4053</v>
+        <v>5102</v>
       </c>
       <c r="E41" s="12" t="n">
         <f aca="false">D41/331</f>
-        <v>12.2447129909366</v>
+        <v>15.4138972809668</v>
       </c>
       <c r="F41" s="12" t="n">
-        <v>912</v>
+        <v>1049</v>
       </c>
       <c r="G41" s="13" t="n">
         <v>43917</v>
       </c>
       <c r="H41" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,G41)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I41" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="J41" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I41)</f>
@@ -1560,11 +1560,11 @@
       </c>
       <c r="K41" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L41" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K41,G41)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M41" s="0"/>
       <c r="N41" s="0"/>
@@ -1580,25 +1580,25 @@
         <v>414</v>
       </c>
       <c r="D42" s="1" t="n">
-        <v>775</v>
+        <v>931</v>
       </c>
       <c r="E42" s="12" t="n">
         <f aca="false">D42/83.784</f>
-        <v>9.24997612909386</v>
+        <v>11.1119068079824</v>
       </c>
       <c r="F42" s="12" t="n">
-        <v>130</v>
+        <v>156</v>
       </c>
       <c r="G42" s="13" t="n">
         <v>43918</v>
       </c>
       <c r="H42" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,G42)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I42" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="J42" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I42)</f>
@@ -1606,11 +1606,11 @@
       </c>
       <c r="K42" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L42" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K42,G42)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M42" s="0"/>
       <c r="N42" s="0"/>
@@ -1619,15 +1619,16 @@
       <c r="Q42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C43" s="12"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="5"/>
       <c r="D43" s="0"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="12"/>
-      <c r="G43" s="13"/>
+      <c r="E43" s="0"/>
+      <c r="F43" s="0"/>
+      <c r="G43" s="0"/>
       <c r="H43" s="0"/>
-      <c r="I43" s="13"/>
+      <c r="I43" s="0"/>
       <c r="J43" s="0"/>
-      <c r="K43" s="13"/>
+      <c r="K43" s="0"/>
       <c r="L43" s="0"/>
       <c r="M43" s="0"/>
       <c r="N43" s="0"/>
@@ -1636,15 +1637,16 @@
       <c r="Q43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C44" s="12"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="5"/>
       <c r="D44" s="0"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
-      <c r="G44" s="13"/>
+      <c r="E44" s="0"/>
+      <c r="F44" s="0"/>
+      <c r="G44" s="0"/>
       <c r="H44" s="0"/>
-      <c r="I44" s="13"/>
+      <c r="I44" s="0"/>
       <c r="J44" s="0"/>
-      <c r="K44" s="13"/>
+      <c r="K44" s="0"/>
       <c r="L44" s="0"/>
       <c r="M44" s="0"/>
       <c r="N44" s="0"/>
@@ -1673,7 +1675,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="7" t="n">
-        <v>43920</v>
+        <v>43921</v>
       </c>
       <c r="D46" s="0"/>
       <c r="E46" s="8" t="s">
@@ -1695,7 +1697,9 @@
       <c r="K46" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="L46" s="0"/>
+      <c r="L46" s="8" t="s">
+        <v>33</v>
+      </c>
       <c r="M46" s="0"/>
       <c r="N46" s="0"/>
       <c r="O46" s="0"/>
@@ -1731,7 +1735,9 @@
       <c r="K47" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L47" s="0"/>
+      <c r="L47" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="M47" s="0"/>
       <c r="N47" s="0"/>
       <c r="O47" s="0"/>
@@ -1746,34 +1752,37 @@
         <v>300</v>
       </c>
       <c r="D48" s="1" t="n">
-        <v>11591</v>
+        <v>12428</v>
       </c>
       <c r="E48" s="12" t="n">
         <f aca="false">D48/60.48</f>
-        <v>191.650132275132</v>
+        <v>205.489417989418</v>
       </c>
       <c r="F48" s="12" t="n">
-        <v>812</v>
+        <v>837</v>
       </c>
       <c r="G48" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H48" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,G48)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I48" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J48" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I48)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K48" s="13" t="n">
-        <f aca="false">$B$58+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L48" s="0"/>
+        <f aca="false">$B$46+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L48" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K48,G48)</f>
+        <v>22</v>
+      </c>
       <c r="M48" s="0"/>
       <c r="N48" s="0"/>
       <c r="O48" s="0"/>
@@ -1788,34 +1797,37 @@
         <v>230</v>
       </c>
       <c r="D49" s="1" t="n">
-        <v>7716</v>
+        <v>8464</v>
       </c>
       <c r="E49" s="12" t="n">
         <f aca="false">D49/46.75</f>
-        <v>165.048128342246</v>
+        <v>181.048128342246</v>
       </c>
       <c r="F49" s="12" t="n">
-        <v>913</v>
+        <v>748</v>
       </c>
       <c r="G49" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H49" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,G49)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I49" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J49" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I49)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K49" s="13" t="n">
-        <f aca="false">$B$58+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L49" s="0"/>
+        <f aca="false">$B$46+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L49" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K49,G49)</f>
+        <v>15</v>
+      </c>
       <c r="M49" s="0"/>
       <c r="N49" s="0"/>
       <c r="O49" s="0"/>
@@ -1830,34 +1842,37 @@
         <v>330</v>
       </c>
       <c r="D50" s="1" t="n">
-        <v>3024</v>
+        <v>3523</v>
       </c>
       <c r="E50" s="12" t="n">
         <f aca="false">D50/65.27</f>
-        <v>46.3306266278535</v>
+        <v>53.9757928604259</v>
       </c>
       <c r="F50" s="12" t="n">
-        <v>418</v>
+        <v>499</v>
       </c>
       <c r="G50" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H50" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,G50)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I50" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J50" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I50)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K50" s="13" t="n">
-        <f aca="false">$B$58+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L50" s="0"/>
+        <f aca="false">$B$46+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L50" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K50,G50)</f>
+        <v>10</v>
+      </c>
       <c r="M50" s="0"/>
       <c r="N50" s="0"/>
       <c r="O50" s="0"/>
@@ -1872,35 +1887,38 @@
         <v>50</v>
       </c>
       <c r="D51" s="12" t="n">
-        <v>146</v>
+        <v>180</v>
       </c>
       <c r="E51" s="12" t="n">
         <f aca="false">D51/10.36</f>
-        <v>14.0926640926641</v>
+        <v>17.3745173745174</v>
       </c>
       <c r="F51" s="12" t="n">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G51" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H51" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,G51)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I51" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43921</v>
+        <v>43922</v>
       </c>
       <c r="J51" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I51)</f>
         <v>-1</v>
       </c>
       <c r="K51" s="13" t="n">
-        <f aca="false">$B$58+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L51" s="0"/>
+        <f aca="false">$B$46+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L51" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K51,G51)</f>
+        <v>7</v>
+      </c>
       <c r="M51" s="0"/>
       <c r="N51" s="0"/>
       <c r="O51" s="0"/>
@@ -1915,35 +1933,38 @@
         <v>330</v>
       </c>
       <c r="D52" s="1" t="n">
-        <v>1408</v>
+        <v>1789</v>
       </c>
       <c r="E52" s="12" t="n">
         <f aca="false">D52/67.79</f>
-        <v>20.770025077445</v>
+        <v>26.390323056498</v>
       </c>
       <c r="F52" s="12" t="n">
-        <v>180</v>
+        <v>381</v>
       </c>
       <c r="G52" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H52" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,G52)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I52" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43921</v>
+        <v>43922</v>
       </c>
       <c r="J52" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I52)</f>
         <v>-1</v>
       </c>
       <c r="K52" s="13" t="n">
-        <f aca="false">$B$58+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L52" s="0"/>
+        <f aca="false">$B$46+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L52" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K52,G52)</f>
+        <v>6</v>
+      </c>
       <c r="M52" s="0"/>
       <c r="N52" s="0"/>
       <c r="O52" s="0"/>
@@ -1958,34 +1979,38 @@
         <v>1660</v>
       </c>
       <c r="D53" s="1" t="n">
-        <v>3141</v>
+        <v>4053</v>
       </c>
       <c r="E53" s="12" t="n">
         <f aca="false">D53/331</f>
-        <v>9.48942598187311</v>
+        <v>12.2447129909366</v>
       </c>
       <c r="F53" s="12" t="n">
-        <v>573</v>
+        <v>912</v>
       </c>
       <c r="G53" s="13" t="n">
         <v>43917</v>
       </c>
       <c r="H53" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,G53)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I53" s="13" t="n">
-        <v>43920</v>
+        <f aca="false">$B$46+1</f>
+        <v>43922</v>
       </c>
       <c r="J53" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I53)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="K53" s="13" t="n">
-        <f aca="false">$B$58+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L53" s="0"/>
+        <f aca="false">$B$46+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L53" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K53,G53)</f>
+        <v>5</v>
+      </c>
       <c r="M53" s="0"/>
       <c r="N53" s="0"/>
       <c r="O53" s="0"/>
@@ -2000,35 +2025,38 @@
         <v>414</v>
       </c>
       <c r="D54" s="1" t="n">
-        <v>645</v>
+        <v>775</v>
       </c>
       <c r="E54" s="12" t="n">
         <f aca="false">D54/83.784</f>
-        <v>7.69836723002005</v>
+        <v>9.24997612909386</v>
       </c>
       <c r="F54" s="12" t="n">
-        <v>104</v>
+        <v>130</v>
       </c>
       <c r="G54" s="13" t="n">
         <v>43918</v>
       </c>
       <c r="H54" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,G54)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I54" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43921</v>
+        <v>43922</v>
       </c>
       <c r="J54" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I54)</f>
         <v>-1</v>
       </c>
       <c r="K54" s="13" t="n">
-        <f aca="false">$B$58+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L54" s="0"/>
+        <f aca="false">$B$46+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L54" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K54,G54)</f>
+        <v>4</v>
+      </c>
       <c r="M54" s="0"/>
       <c r="N54" s="0"/>
       <c r="O54" s="0"/>
@@ -2036,16 +2064,15 @@
       <c r="Q54" s="0"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="4"/>
-      <c r="C55" s="5"/>
+      <c r="C55" s="12"/>
       <c r="D55" s="0"/>
-      <c r="E55" s="0"/>
-      <c r="F55" s="0"/>
-      <c r="G55" s="0"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="12"/>
+      <c r="G55" s="13"/>
       <c r="H55" s="0"/>
-      <c r="I55" s="0"/>
+      <c r="I55" s="13"/>
       <c r="J55" s="0"/>
-      <c r="K55" s="0"/>
+      <c r="K55" s="13"/>
       <c r="L55" s="0"/>
       <c r="M55" s="0"/>
       <c r="N55" s="0"/>
@@ -2054,16 +2081,15 @@
       <c r="Q55" s="0"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="4"/>
-      <c r="C56" s="5"/>
+      <c r="C56" s="12"/>
       <c r="D56" s="0"/>
-      <c r="E56" s="0"/>
-      <c r="F56" s="0"/>
-      <c r="G56" s="0"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="12"/>
+      <c r="G56" s="13"/>
       <c r="H56" s="0"/>
-      <c r="I56" s="0"/>
+      <c r="I56" s="13"/>
       <c r="J56" s="0"/>
-      <c r="K56" s="0"/>
+      <c r="K56" s="13"/>
       <c r="L56" s="0"/>
       <c r="M56" s="0"/>
       <c r="N56" s="0"/>
@@ -2092,7 +2118,7 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="7" t="n">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="D58" s="0"/>
       <c r="E58" s="8" t="s">
@@ -2165,31 +2191,31 @@
         <v>300</v>
       </c>
       <c r="D60" s="1" t="n">
-        <v>10779</v>
+        <v>11591</v>
       </c>
       <c r="E60" s="12" t="n">
         <f aca="false">D60/60.48</f>
-        <v>178.224206349206</v>
+        <v>191.650132275132</v>
       </c>
       <c r="F60" s="12" t="n">
-        <v>756</v>
+        <v>812</v>
       </c>
       <c r="G60" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H60" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,G60)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I60" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J60" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I60)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K60" s="13" t="n">
-        <f aca="false">$B$58+1</f>
+        <f aca="false">$B$70+1</f>
         <v>43920</v>
       </c>
       <c r="L60" s="0"/>
@@ -2207,31 +2233,31 @@
         <v>230</v>
       </c>
       <c r="D61" s="1" t="n">
-        <v>6803</v>
+        <v>7716</v>
       </c>
       <c r="E61" s="12" t="n">
         <f aca="false">D61/46.75</f>
-        <v>145.51871657754</v>
+        <v>165.048128342246</v>
       </c>
       <c r="F61" s="12" t="n">
-        <v>821</v>
+        <v>913</v>
       </c>
       <c r="G61" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H61" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,G61)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I61" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J61" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I61)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K61" s="13" t="n">
-        <f aca="false">$B$58+1</f>
+        <f aca="false">$B$70+1</f>
         <v>43920</v>
       </c>
       <c r="L61" s="0"/>
@@ -2249,31 +2275,31 @@
         <v>330</v>
       </c>
       <c r="D62" s="1" t="n">
-        <v>2606</v>
+        <v>3024</v>
       </c>
       <c r="E62" s="12" t="n">
         <f aca="false">D62/65.27</f>
-        <v>39.9264593228129</v>
+        <v>46.3306266278535</v>
       </c>
       <c r="F62" s="12" t="n">
-        <v>292</v>
+        <v>418</v>
       </c>
       <c r="G62" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H62" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,G62)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I62" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J62" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I62)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K62" s="13" t="n">
-        <f aca="false">$B$58+1</f>
+        <f aca="false">$B$70+1</f>
         <v>43920</v>
       </c>
       <c r="L62" s="0"/>
@@ -2285,38 +2311,38 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="0" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C63" s="12" t="n">
-        <v>1660</v>
-      </c>
-      <c r="D63" s="1" t="n">
-        <v>2583</v>
+        <v>50</v>
+      </c>
+      <c r="D63" s="12" t="n">
+        <v>146</v>
       </c>
       <c r="E63" s="12" t="n">
-        <f aca="false">D63/331</f>
-        <v>7.8036253776435</v>
+        <f aca="false">D63/10.36</f>
+        <v>14.0926640926641</v>
       </c>
       <c r="F63" s="12" t="n">
-        <v>363</v>
+        <v>36</v>
       </c>
       <c r="G63" s="13" t="n">
-        <v>43917</v>
+        <v>43915</v>
       </c>
       <c r="H63" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,G63)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I63" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43920</v>
+        <v>43921</v>
       </c>
       <c r="J63" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I63)</f>
         <v>-1</v>
       </c>
       <c r="K63" s="13" t="n">
-        <f aca="false">$B$58+1</f>
+        <f aca="false">$B$70+1</f>
         <v>43920</v>
       </c>
       <c r="L63" s="0"/>
@@ -2334,32 +2360,32 @@
         <v>330</v>
       </c>
       <c r="D64" s="1" t="n">
-        <v>1228</v>
+        <v>1408</v>
       </c>
       <c r="E64" s="12" t="n">
         <f aca="false">D64/67.79</f>
-        <v>18.1147661897035</v>
+        <v>20.770025077445</v>
       </c>
       <c r="F64" s="12" t="n">
-        <v>209</v>
+        <v>180</v>
       </c>
       <c r="G64" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H64" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,G64)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I64" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43920</v>
+        <v>43921</v>
       </c>
       <c r="J64" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I64)</f>
         <v>-1</v>
       </c>
       <c r="K64" s="13" t="n">
-        <f aca="false">$B$58+1</f>
+        <f aca="false">$B$70+1</f>
         <v>43920</v>
       </c>
       <c r="L64" s="0"/>
@@ -2371,38 +2397,37 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C65" s="12" t="n">
-        <v>414</v>
+        <v>1660</v>
       </c>
       <c r="D65" s="1" t="n">
-        <v>541</v>
+        <v>3141</v>
       </c>
       <c r="E65" s="12" t="n">
-        <f aca="false">D65/83.784</f>
-        <v>6.457080110761</v>
+        <f aca="false">D65/331</f>
+        <v>9.48942598187311</v>
       </c>
       <c r="F65" s="12" t="n">
-        <v>108</v>
+        <v>573</v>
       </c>
       <c r="G65" s="13" t="n">
-        <v>43918</v>
+        <v>43917</v>
       </c>
       <c r="H65" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,G65)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I65" s="13" t="n">
-        <f aca="false">$B$58+1</f>
         <v>43920</v>
       </c>
       <c r="J65" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I65)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="K65" s="13" t="n">
-        <f aca="false">$B$58+1</f>
+        <f aca="false">$B$70+1</f>
         <v>43920</v>
       </c>
       <c r="L65" s="0"/>
@@ -2414,38 +2439,38 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C66" s="12" t="n">
-        <v>50</v>
-      </c>
-      <c r="D66" s="12" t="n">
-        <v>110</v>
+        <v>414</v>
+      </c>
+      <c r="D66" s="1" t="n">
+        <v>645</v>
       </c>
       <c r="E66" s="12" t="n">
-        <f aca="false">D66/10.36</f>
-        <v>10.6177606177606</v>
+        <f aca="false">D66/83.784</f>
+        <v>7.69836723002005</v>
       </c>
       <c r="F66" s="12" t="n">
-        <v>5</v>
+        <v>104</v>
       </c>
       <c r="G66" s="13" t="n">
-        <v>43915</v>
+        <v>43918</v>
       </c>
       <c r="H66" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,G66)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I66" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43920</v>
+        <v>43921</v>
       </c>
       <c r="J66" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I66)</f>
         <v>-1</v>
       </c>
       <c r="K66" s="13" t="n">
-        <f aca="false">$B$58+1</f>
+        <f aca="false">$B$70+1</f>
         <v>43920</v>
       </c>
       <c r="L66" s="0"/>
@@ -2512,15 +2537,13 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="7" t="n">
-        <v>43918</v>
-      </c>
-      <c r="D70" s="8" t="s">
-        <v>6</v>
-      </c>
+        <v>43919</v>
+      </c>
+      <c r="D70" s="0"/>
       <c r="E70" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F70" s="8"/>
+      <c r="F70" s="0"/>
       <c r="G70" s="8" t="s">
         <v>29</v>
       </c>
@@ -2548,8 +2571,8 @@
       <c r="C71" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D71" s="10" t="s">
-        <v>2</v>
+      <c r="D71" s="8" t="s">
+        <v>6</v>
       </c>
       <c r="E71" s="10" t="s">
         <v>35</v>
@@ -2587,32 +2610,32 @@
         <v>300</v>
       </c>
       <c r="D72" s="1" t="n">
-        <v>10023</v>
+        <v>10779</v>
       </c>
       <c r="E72" s="12" t="n">
         <f aca="false">D72/60.48</f>
-        <v>165.724206349206</v>
+        <v>178.224206349206</v>
       </c>
       <c r="F72" s="12" t="n">
-        <v>889</v>
+        <v>756</v>
       </c>
       <c r="G72" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H72" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,G72)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I72" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J72" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$82,I72)</f>
-        <v>15</v>
+        <f aca="false">_xlfn.DAYS($B$70,I72)</f>
+        <v>17</v>
       </c>
       <c r="K72" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L72" s="0"/>
       <c r="M72" s="0"/>
@@ -2629,32 +2652,32 @@
         <v>230</v>
       </c>
       <c r="D73" s="1" t="n">
-        <v>5982</v>
+        <v>6803</v>
       </c>
       <c r="E73" s="12" t="n">
         <f aca="false">D73/46.75</f>
-        <v>127.957219251337</v>
+        <v>145.51871657754</v>
       </c>
       <c r="F73" s="12" t="n">
-        <v>844</v>
+        <v>821</v>
       </c>
       <c r="G73" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H73" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,G73)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I73" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J73" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$82,I73)</f>
-        <v>4</v>
+        <f aca="false">_xlfn.DAYS($B$70,I73)</f>
+        <v>6</v>
       </c>
       <c r="K73" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L73" s="0"/>
       <c r="M73" s="0"/>
@@ -2671,32 +2694,32 @@
         <v>330</v>
       </c>
       <c r="D74" s="1" t="n">
-        <v>2314</v>
+        <v>2606</v>
       </c>
       <c r="E74" s="12" t="n">
         <f aca="false">D74/65.27</f>
-        <v>35.4527347939329</v>
+        <v>39.9264593228129</v>
       </c>
       <c r="F74" s="12" t="n">
-        <v>319</v>
+        <v>292</v>
       </c>
       <c r="G74" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H74" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,G74)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I74" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J74" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$82,I74)</f>
-        <v>3</v>
+        <f aca="false">_xlfn.DAYS($B$70,I74)</f>
+        <v>5</v>
       </c>
       <c r="K74" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L74" s="0"/>
       <c r="M74" s="0"/>
@@ -2713,25 +2736,25 @@
         <v>1660</v>
       </c>
       <c r="D75" s="1" t="n">
-        <v>2221</v>
+        <v>2583</v>
       </c>
       <c r="E75" s="12" t="n">
         <f aca="false">D75/331</f>
-        <v>6.70996978851964</v>
+        <v>7.8036253776435</v>
       </c>
       <c r="F75" s="12" t="n">
-        <v>525</v>
+        <v>363</v>
       </c>
       <c r="G75" s="13" t="n">
         <v>43917</v>
       </c>
       <c r="H75" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,G75)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I75" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="J75" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,I75)</f>
@@ -2739,7 +2762,7 @@
       </c>
       <c r="K75" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L75" s="0"/>
       <c r="M75" s="0"/>
@@ -2756,25 +2779,25 @@
         <v>330</v>
       </c>
       <c r="D76" s="1" t="n">
-        <v>1019</v>
+        <v>1228</v>
       </c>
       <c r="E76" s="12" t="n">
         <f aca="false">D76/67.79</f>
-        <v>15.0317155922702</v>
+        <v>18.1147661897035</v>
       </c>
       <c r="F76" s="12" t="n">
-        <v>260</v>
+        <v>209</v>
       </c>
       <c r="G76" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H76" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,G76)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I76" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="J76" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,I76)</f>
@@ -2782,7 +2805,7 @@
       </c>
       <c r="K76" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L76" s="0"/>
       <c r="M76" s="0"/>
@@ -2799,25 +2822,25 @@
         <v>414</v>
       </c>
       <c r="D77" s="1" t="n">
-        <v>433</v>
+        <v>541</v>
       </c>
       <c r="E77" s="12" t="n">
         <f aca="false">D77/83.784</f>
-        <v>5.16805117922276</v>
+        <v>6.457080110761</v>
       </c>
       <c r="F77" s="12" t="n">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="G77" s="13" t="n">
         <v>43918</v>
       </c>
       <c r="H77" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,G77)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I77" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="J77" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,I77)</f>
@@ -2825,7 +2848,7 @@
       </c>
       <c r="K77" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L77" s="0"/>
       <c r="M77" s="0"/>
@@ -2842,25 +2865,25 @@
         <v>50</v>
       </c>
       <c r="D78" s="12" t="n">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="E78" s="12" t="n">
         <f aca="false">D78/10.36</f>
-        <v>10.1351351351351</v>
+        <v>10.6177606177606</v>
       </c>
       <c r="F78" s="12" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G78" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H78" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,G78)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I78" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="J78" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,I78)</f>
@@ -2868,7 +2891,7 @@
       </c>
       <c r="K78" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L78" s="0"/>
       <c r="M78" s="0"/>
@@ -2878,15 +2901,16 @@
       <c r="Q78" s="0"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C79" s="12"/>
-      <c r="D79" s="12"/>
-      <c r="E79" s="12"/>
-      <c r="F79" s="12"/>
-      <c r="G79" s="13"/>
+      <c r="B79" s="4"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="0"/>
+      <c r="E79" s="0"/>
+      <c r="F79" s="0"/>
+      <c r="G79" s="0"/>
       <c r="H79" s="0"/>
-      <c r="I79" s="13"/>
+      <c r="I79" s="0"/>
       <c r="J79" s="0"/>
-      <c r="K79" s="13"/>
+      <c r="K79" s="0"/>
       <c r="L79" s="0"/>
       <c r="M79" s="0"/>
       <c r="N79" s="0"/>
@@ -2931,11 +2955,10 @@
       <c r="P81" s="0"/>
       <c r="Q81" s="0"/>
     </row>
-    <row r="82" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="7" t="n">
-        <v>43917</v>
-      </c>
-      <c r="C82" s="0"/>
+        <v>43918</v>
+      </c>
       <c r="D82" s="8" t="s">
         <v>6</v>
       </c>
@@ -2958,10 +2981,14 @@
       <c r="K82" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="L82" s="8"/>
+      <c r="L82" s="0"/>
+      <c r="M82" s="0"/>
+      <c r="N82" s="0"/>
+      <c r="O82" s="0"/>
+      <c r="P82" s="0"/>
+      <c r="Q82" s="0"/>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="3"/>
       <c r="B83" s="9"/>
       <c r="C83" s="10" t="s">
         <v>34</v>
@@ -2990,7 +3017,7 @@
       <c r="K83" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L83" s="8"/>
+      <c r="L83" s="0"/>
       <c r="M83" s="0"/>
       <c r="N83" s="0"/>
       <c r="O83" s="0"/>
@@ -3005,32 +3032,32 @@
         <v>300</v>
       </c>
       <c r="D84" s="1" t="n">
-        <v>9134</v>
+        <v>10023</v>
       </c>
       <c r="E84" s="12" t="n">
         <f aca="false">D84/60.48</f>
-        <v>151.025132275132</v>
+        <v>165.724206349206</v>
       </c>
       <c r="F84" s="12" t="n">
-        <v>919</v>
+        <v>889</v>
       </c>
       <c r="G84" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H84" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,G84)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I84" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J84" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$82,I84)</f>
+        <f aca="false">_xlfn.DAYS(B$94,I84)</f>
         <v>15</v>
       </c>
       <c r="K84" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L84" s="0"/>
       <c r="M84" s="0"/>
@@ -3047,32 +3074,32 @@
         <v>230</v>
       </c>
       <c r="D85" s="1" t="n">
-        <v>5138</v>
+        <v>5982</v>
       </c>
       <c r="E85" s="12" t="n">
         <f aca="false">D85/46.75</f>
-        <v>109.903743315508</v>
+        <v>127.957219251337</v>
       </c>
       <c r="F85" s="12" t="n">
-        <v>773</v>
+        <v>844</v>
       </c>
       <c r="G85" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H85" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,G85)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I85" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J85" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$82,I85)</f>
+        <f aca="false">_xlfn.DAYS(B$94,I85)</f>
         <v>4</v>
       </c>
       <c r="K85" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L85" s="0"/>
       <c r="M85" s="0"/>
@@ -3089,32 +3116,32 @@
         <v>330</v>
       </c>
       <c r="D86" s="1" t="n">
-        <v>1995</v>
+        <v>2314</v>
       </c>
       <c r="E86" s="12" t="n">
         <f aca="false">D86/65.27</f>
-        <v>30.5653439558756</v>
+        <v>35.4527347939329</v>
       </c>
       <c r="F86" s="12" t="n">
-        <v>299</v>
+        <v>319</v>
       </c>
       <c r="G86" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H86" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,G86)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I86" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J86" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$82,I86)</f>
+        <f aca="false">_xlfn.DAYS(B$94,I86)</f>
         <v>3</v>
       </c>
       <c r="K86" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L86" s="0"/>
       <c r="M86" s="0"/>
@@ -3131,34 +3158,33 @@
         <v>1660</v>
       </c>
       <c r="D87" s="1" t="n">
-        <v>1696</v>
+        <v>2221</v>
       </c>
       <c r="E87" s="12" t="n">
         <f aca="false">D87/331</f>
-        <v>5.12386706948641</v>
+        <v>6.70996978851964</v>
       </c>
       <c r="F87" s="12" t="n">
-        <v>400</v>
+        <v>525</v>
       </c>
       <c r="G87" s="13" t="n">
-        <f aca="false">$B$82</f>
         <v>43917</v>
       </c>
       <c r="H87" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,G87)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I87" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="J87" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$82,I87)</f>
+        <f aca="false">_xlfn.DAYS($B$82,I87)</f>
         <v>-1</v>
       </c>
       <c r="K87" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L87" s="0"/>
       <c r="M87" s="0"/>
@@ -3175,33 +3201,33 @@
         <v>330</v>
       </c>
       <c r="D88" s="1" t="n">
-        <v>759</v>
+        <v>1019</v>
       </c>
       <c r="E88" s="12" t="n">
         <f aca="false">D88/67.79</f>
-        <v>11.1963416433102</v>
+        <v>15.0317155922702</v>
       </c>
       <c r="F88" s="12" t="n">
-        <v>181</v>
+        <v>260</v>
       </c>
       <c r="G88" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H88" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,G88)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I88" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="J88" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$82,I88)</f>
+        <f aca="false">_xlfn.DAYS($B$82,I88)</f>
         <v>-1</v>
       </c>
       <c r="K88" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L88" s="0"/>
       <c r="M88" s="0"/>
@@ -3218,34 +3244,33 @@
         <v>414</v>
       </c>
       <c r="D89" s="1" t="n">
-        <v>351</v>
+        <v>433</v>
       </c>
       <c r="E89" s="12" t="n">
         <f aca="false">D89/83.784</f>
-        <v>4.18934402749928</v>
+        <v>5.16805117922276</v>
       </c>
       <c r="F89" s="12" t="n">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G89" s="13" t="n">
-        <f aca="false">$B$82+1</f>
         <v>43918</v>
       </c>
       <c r="H89" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,G89)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="I89" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="J89" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$82,I89)</f>
+        <f aca="false">_xlfn.DAYS($B$82,I89)</f>
         <v>-1</v>
       </c>
       <c r="K89" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L89" s="0"/>
       <c r="M89" s="0"/>
@@ -3269,26 +3294,26 @@
         <v>10.1351351351351</v>
       </c>
       <c r="F90" s="12" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="G90" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H90" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,G90)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I90" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="J90" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$82,I90)</f>
+        <f aca="false">_xlfn.DAYS($B$82,I90)</f>
         <v>-1</v>
       </c>
       <c r="K90" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L90" s="0"/>
       <c r="M90" s="0"/>
@@ -3298,14 +3323,15 @@
       <c r="Q90" s="0"/>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D91" s="0"/>
-      <c r="E91" s="0"/>
-      <c r="F91" s="0"/>
-      <c r="G91" s="0"/>
+      <c r="C91" s="12"/>
+      <c r="D91" s="12"/>
+      <c r="E91" s="12"/>
+      <c r="F91" s="12"/>
+      <c r="G91" s="13"/>
       <c r="H91" s="0"/>
-      <c r="I91" s="0"/>
+      <c r="I91" s="13"/>
       <c r="J91" s="0"/>
-      <c r="K91" s="0"/>
+      <c r="K91" s="13"/>
       <c r="L91" s="0"/>
       <c r="M91" s="0"/>
       <c r="N91" s="0"/>
@@ -3314,6 +3340,8 @@
       <c r="Q91" s="0"/>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B92" s="4"/>
+      <c r="C92" s="5"/>
       <c r="D92" s="0"/>
       <c r="E92" s="0"/>
       <c r="F92" s="0"/>
@@ -3348,10 +3376,11 @@
       <c r="P93" s="0"/>
       <c r="Q93" s="0"/>
     </row>
-    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="7" t="n">
-        <v>43916</v>
-      </c>
+        <v>43917</v>
+      </c>
+      <c r="C94" s="0"/>
       <c r="D94" s="8" t="s">
         <v>6</v>
       </c>
@@ -3374,17 +3403,13 @@
       <c r="K94" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="L94" s="0"/>
-      <c r="M94" s="0"/>
-      <c r="N94" s="0"/>
-      <c r="O94" s="0"/>
-      <c r="P94" s="0"/>
-      <c r="Q94" s="0"/>
+      <c r="L94" s="8"/>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="3"/>
       <c r="B95" s="9"/>
       <c r="C95" s="10" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="D95" s="10" t="s">
         <v>2</v>
@@ -3410,7 +3435,7 @@
       <c r="K95" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L95" s="0"/>
+      <c r="L95" s="8"/>
       <c r="M95" s="0"/>
       <c r="N95" s="0"/>
       <c r="O95" s="0"/>
@@ -3425,32 +3450,32 @@
         <v>300</v>
       </c>
       <c r="D96" s="1" t="n">
-        <v>8215</v>
+        <v>9134</v>
       </c>
       <c r="E96" s="12" t="n">
         <f aca="false">D96/60.48</f>
-        <v>135.830026455026</v>
+        <v>151.025132275132</v>
       </c>
       <c r="F96" s="12" t="n">
-        <v>712</v>
+        <v>919</v>
       </c>
       <c r="G96" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H96" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$94,G96)</f>
-        <v>16</v>
+        <f aca="false">_xlfn.DAYS($B$94,G96)</f>
+        <v>17</v>
       </c>
       <c r="I96" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J96" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$94,I96)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K96" s="13" t="n">
-        <f aca="false">B$94+1</f>
-        <v>43917</v>
+        <f aca="false">$B$94+1</f>
+        <v>43918</v>
       </c>
       <c r="L96" s="0"/>
       <c r="M96" s="0"/>
@@ -3467,32 +3492,32 @@
         <v>230</v>
       </c>
       <c r="D97" s="1" t="n">
-        <v>4365</v>
+        <v>5138</v>
       </c>
       <c r="E97" s="12" t="n">
         <f aca="false">D97/46.75</f>
-        <v>93.3689839572193</v>
+        <v>109.903743315508</v>
       </c>
       <c r="F97" s="12" t="n">
-        <v>718</v>
+        <v>773</v>
       </c>
       <c r="G97" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H97" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$94,G97)</f>
-        <v>9</v>
+        <f aca="false">_xlfn.DAYS($B$94,G97)</f>
+        <v>10</v>
       </c>
       <c r="I97" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J97" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$94,I97)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K97" s="13" t="n">
-        <f aca="false">B$94+1</f>
-        <v>43917</v>
+        <f aca="false">$B$94+1</f>
+        <v>43918</v>
       </c>
       <c r="L97" s="0"/>
       <c r="M97" s="0"/>
@@ -3509,32 +3534,32 @@
         <v>330</v>
       </c>
       <c r="D98" s="1" t="n">
-        <v>1696</v>
+        <v>1995</v>
       </c>
       <c r="E98" s="12" t="n">
         <f aca="false">D98/65.27</f>
-        <v>25.9843726060978</v>
+        <v>30.5653439558756</v>
       </c>
       <c r="F98" s="12" t="n">
-        <v>365</v>
+        <v>299</v>
       </c>
       <c r="G98" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H98" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$94,G98)</f>
-        <v>4</v>
+        <f aca="false">_xlfn.DAYS($B$94,G98)</f>
+        <v>5</v>
       </c>
       <c r="I98" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J98" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$94,I98)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K98" s="13" t="n">
-        <f aca="false">B$94+1</f>
-        <v>43917</v>
+        <f aca="false">$B$94+1</f>
+        <v>43918</v>
       </c>
       <c r="L98" s="0"/>
       <c r="M98" s="0"/>
@@ -3551,33 +3576,34 @@
         <v>1660</v>
       </c>
       <c r="D99" s="1" t="n">
-        <v>1295</v>
+        <v>1696</v>
       </c>
       <c r="E99" s="12" t="n">
         <f aca="false">D99/331</f>
-        <v>3.91238670694864</v>
+        <v>5.12386706948641</v>
       </c>
       <c r="F99" s="12" t="n">
-        <v>268</v>
+        <v>400</v>
       </c>
       <c r="G99" s="13" t="n">
+        <f aca="false">$B$94</f>
         <v>43917</v>
       </c>
       <c r="H99" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$94,G99)</f>
+        <f aca="false">_xlfn.DAYS($B$94,G99)</f>
+        <v>0</v>
+      </c>
+      <c r="I99" s="13" t="n">
+        <f aca="false">$B$94+1</f>
+        <v>43918</v>
+      </c>
+      <c r="J99" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$94,I99)</f>
         <v>-1</v>
       </c>
-      <c r="I99" s="13" t="n">
-        <f aca="false">B$94+1</f>
-        <v>43917</v>
-      </c>
-      <c r="J99" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$94,I99)</f>
-        <v>-1</v>
-      </c>
       <c r="K99" s="13" t="n">
-        <f aca="false">B$94+1</f>
-        <v>43917</v>
+        <f aca="false">$B$94+1</f>
+        <v>43918</v>
       </c>
       <c r="L99" s="0"/>
       <c r="M99" s="0"/>
@@ -3594,33 +3620,33 @@
         <v>330</v>
       </c>
       <c r="D100" s="1" t="n">
-        <v>578</v>
+        <v>759</v>
       </c>
       <c r="E100" s="12" t="n">
         <f aca="false">D100/67.79</f>
-        <v>8.52633131730344</v>
+        <v>11.1963416433102</v>
       </c>
       <c r="F100" s="12" t="n">
-        <v>115</v>
+        <v>181</v>
       </c>
       <c r="G100" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H100" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$94,G100)</f>
-        <v>0</v>
+        <f aca="false">_xlfn.DAYS($B$94,G100)</f>
+        <v>1</v>
       </c>
       <c r="I100" s="13" t="n">
-        <f aca="false">B$94+1</f>
-        <v>43917</v>
+        <f aca="false">$B$94+1</f>
+        <v>43918</v>
       </c>
       <c r="J100" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$94,I100)</f>
         <v>-1</v>
       </c>
       <c r="K100" s="13" t="n">
-        <f aca="false">B$94+1</f>
-        <v>43917</v>
+        <f aca="false">$B$94+1</f>
+        <v>43918</v>
       </c>
       <c r="L100" s="0"/>
       <c r="M100" s="0"/>
@@ -3637,33 +3663,34 @@
         <v>414</v>
       </c>
       <c r="D101" s="1" t="n">
-        <v>267</v>
+        <v>351</v>
       </c>
       <c r="E101" s="12" t="n">
         <f aca="false">D101/83.784</f>
-        <v>3.18676596963621</v>
+        <v>4.18934402749928</v>
       </c>
       <c r="F101" s="12" t="n">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="G101" s="13" t="n">
-        <v>43917</v>
+        <f aca="false">$B$94+1</f>
+        <v>43918</v>
       </c>
       <c r="H101" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$94,G101)</f>
+        <f aca="false">_xlfn.DAYS($B$94,G101)</f>
         <v>-1</v>
       </c>
       <c r="I101" s="13" t="n">
-        <f aca="false">B$94+1</f>
-        <v>43917</v>
+        <f aca="false">$B$94+1</f>
+        <v>43918</v>
       </c>
       <c r="J101" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$94,I101)</f>
         <v>-1</v>
       </c>
       <c r="K101" s="13" t="n">
-        <f aca="false">B$94+1</f>
-        <v>43917</v>
+        <f aca="false">$B$94+1</f>
+        <v>43918</v>
       </c>
       <c r="L101" s="0"/>
       <c r="M101" s="0"/>
@@ -3680,33 +3707,33 @@
         <v>50</v>
       </c>
       <c r="D102" s="12" t="n">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="E102" s="12" t="n">
         <f aca="false">D102/10.36</f>
-        <v>7.43243243243243</v>
+        <v>10.1351351351351</v>
       </c>
       <c r="F102" s="12" t="n">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="G102" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H102" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$94,G102)</f>
-        <v>1</v>
+        <f aca="false">_xlfn.DAYS($B$94,G102)</f>
+        <v>2</v>
       </c>
       <c r="I102" s="13" t="n">
-        <f aca="false">B$94+1</f>
-        <v>43917</v>
+        <f aca="false">$B$94+1</f>
+        <v>43918</v>
       </c>
       <c r="J102" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$94,I102)</f>
         <v>-1</v>
       </c>
       <c r="K102" s="13" t="n">
-        <f aca="false">B$94+1</f>
-        <v>43917</v>
+        <f aca="false">$B$94+1</f>
+        <v>43918</v>
       </c>
       <c r="L102" s="0"/>
       <c r="M102" s="0"/>
@@ -3714,6 +3741,424 @@
       <c r="O102" s="0"/>
       <c r="P102" s="0"/>
       <c r="Q102" s="0"/>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D103" s="0"/>
+      <c r="E103" s="0"/>
+      <c r="F103" s="0"/>
+      <c r="G103" s="0"/>
+      <c r="H103" s="0"/>
+      <c r="I103" s="0"/>
+      <c r="J103" s="0"/>
+      <c r="K103" s="0"/>
+      <c r="L103" s="0"/>
+      <c r="M103" s="0"/>
+      <c r="N103" s="0"/>
+      <c r="O103" s="0"/>
+      <c r="P103" s="0"/>
+      <c r="Q103" s="0"/>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D104" s="0"/>
+      <c r="E104" s="0"/>
+      <c r="F104" s="0"/>
+      <c r="G104" s="0"/>
+      <c r="H104" s="0"/>
+      <c r="I104" s="0"/>
+      <c r="J104" s="0"/>
+      <c r="K104" s="0"/>
+      <c r="L104" s="0"/>
+      <c r="M104" s="0"/>
+      <c r="N104" s="0"/>
+      <c r="O104" s="0"/>
+      <c r="P104" s="0"/>
+      <c r="Q104" s="0"/>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B105" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D105" s="0"/>
+      <c r="E105" s="0"/>
+      <c r="F105" s="0"/>
+      <c r="G105" s="0"/>
+      <c r="H105" s="0"/>
+      <c r="I105" s="0"/>
+      <c r="J105" s="0"/>
+      <c r="K105" s="0"/>
+      <c r="L105" s="0"/>
+      <c r="M105" s="0"/>
+      <c r="N105" s="0"/>
+      <c r="O105" s="0"/>
+      <c r="P105" s="0"/>
+      <c r="Q105" s="0"/>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B106" s="7" t="n">
+        <v>43916</v>
+      </c>
+      <c r="D106" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E106" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F106" s="8"/>
+      <c r="G106" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H106" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I106" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="J106" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K106" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="L106" s="0"/>
+      <c r="M106" s="0"/>
+      <c r="N106" s="0"/>
+      <c r="O106" s="0"/>
+      <c r="P106" s="0"/>
+      <c r="Q106" s="0"/>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B107" s="9"/>
+      <c r="C107" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D107" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E107" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F107" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G107" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H107" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I107" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="J107" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K107" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L107" s="0"/>
+      <c r="M107" s="0"/>
+      <c r="N107" s="0"/>
+      <c r="O107" s="0"/>
+      <c r="P107" s="0"/>
+      <c r="Q107" s="0"/>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B108" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C108" s="12" t="n">
+        <v>300</v>
+      </c>
+      <c r="D108" s="1" t="n">
+        <v>8215</v>
+      </c>
+      <c r="E108" s="12" t="n">
+        <f aca="false">D108/60.48</f>
+        <v>135.830026455026</v>
+      </c>
+      <c r="F108" s="12" t="n">
+        <v>712</v>
+      </c>
+      <c r="G108" s="13" t="n">
+        <v>43900</v>
+      </c>
+      <c r="H108" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$106,G108)</f>
+        <v>16</v>
+      </c>
+      <c r="I108" s="13" t="n">
+        <v>43902</v>
+      </c>
+      <c r="J108" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$106,I108)</f>
+        <v>14</v>
+      </c>
+      <c r="K108" s="13" t="n">
+        <f aca="false">B$106+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L108" s="0"/>
+      <c r="M108" s="0"/>
+      <c r="N108" s="0"/>
+      <c r="O108" s="0"/>
+      <c r="P108" s="0"/>
+      <c r="Q108" s="0"/>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B109" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C109" s="12" t="n">
+        <v>230</v>
+      </c>
+      <c r="D109" s="1" t="n">
+        <v>4365</v>
+      </c>
+      <c r="E109" s="12" t="n">
+        <f aca="false">D109/46.75</f>
+        <v>93.3689839572193</v>
+      </c>
+      <c r="F109" s="12" t="n">
+        <v>718</v>
+      </c>
+      <c r="G109" s="13" t="n">
+        <v>43907</v>
+      </c>
+      <c r="H109" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$106,G109)</f>
+        <v>9</v>
+      </c>
+      <c r="I109" s="13" t="n">
+        <v>43913</v>
+      </c>
+      <c r="J109" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$106,I109)</f>
+        <v>3</v>
+      </c>
+      <c r="K109" s="13" t="n">
+        <f aca="false">B$106+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L109" s="0"/>
+      <c r="M109" s="0"/>
+      <c r="N109" s="0"/>
+      <c r="O109" s="0"/>
+      <c r="P109" s="0"/>
+      <c r="Q109" s="0"/>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B110" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C110" s="12" t="n">
+        <v>330</v>
+      </c>
+      <c r="D110" s="1" t="n">
+        <v>1696</v>
+      </c>
+      <c r="E110" s="12" t="n">
+        <f aca="false">D110/65.27</f>
+        <v>25.9843726060978</v>
+      </c>
+      <c r="F110" s="12" t="n">
+        <v>365</v>
+      </c>
+      <c r="G110" s="13" t="n">
+        <v>43912</v>
+      </c>
+      <c r="H110" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$106,G110)</f>
+        <v>4</v>
+      </c>
+      <c r="I110" s="13" t="n">
+        <v>43914</v>
+      </c>
+      <c r="J110" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$106,I110)</f>
+        <v>2</v>
+      </c>
+      <c r="K110" s="13" t="n">
+        <f aca="false">B$106+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L110" s="0"/>
+      <c r="M110" s="0"/>
+      <c r="N110" s="0"/>
+      <c r="O110" s="0"/>
+      <c r="P110" s="0"/>
+      <c r="Q110" s="0"/>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B111" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C111" s="12" t="n">
+        <v>1660</v>
+      </c>
+      <c r="D111" s="1" t="n">
+        <v>1295</v>
+      </c>
+      <c r="E111" s="12" t="n">
+        <f aca="false">D111/331</f>
+        <v>3.91238670694864</v>
+      </c>
+      <c r="F111" s="12" t="n">
+        <v>268</v>
+      </c>
+      <c r="G111" s="13" t="n">
+        <v>43917</v>
+      </c>
+      <c r="H111" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$106,G111)</f>
+        <v>-1</v>
+      </c>
+      <c r="I111" s="13" t="n">
+        <f aca="false">B$106+1</f>
+        <v>43917</v>
+      </c>
+      <c r="J111" s="1" t="n">
+        <f aca="false">_xlfn.DAYS($B$106,I111)</f>
+        <v>-1</v>
+      </c>
+      <c r="K111" s="13" t="n">
+        <f aca="false">B$106+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L111" s="0"/>
+      <c r="M111" s="0"/>
+      <c r="N111" s="0"/>
+      <c r="O111" s="0"/>
+      <c r="P111" s="0"/>
+      <c r="Q111" s="0"/>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B112" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C112" s="12" t="n">
+        <v>330</v>
+      </c>
+      <c r="D112" s="1" t="n">
+        <v>578</v>
+      </c>
+      <c r="E112" s="12" t="n">
+        <f aca="false">D112/67.79</f>
+        <v>8.52633131730344</v>
+      </c>
+      <c r="F112" s="12" t="n">
+        <v>115</v>
+      </c>
+      <c r="G112" s="13" t="n">
+        <v>43916</v>
+      </c>
+      <c r="H112" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$106,G112)</f>
+        <v>0</v>
+      </c>
+      <c r="I112" s="13" t="n">
+        <f aca="false">B$106+1</f>
+        <v>43917</v>
+      </c>
+      <c r="J112" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$106,I112)</f>
+        <v>-1</v>
+      </c>
+      <c r="K112" s="13" t="n">
+        <f aca="false">B$106+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L112" s="0"/>
+      <c r="M112" s="0"/>
+      <c r="N112" s="0"/>
+      <c r="O112" s="0"/>
+      <c r="P112" s="0"/>
+      <c r="Q112" s="0"/>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B113" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C113" s="12" t="n">
+        <v>414</v>
+      </c>
+      <c r="D113" s="1" t="n">
+        <v>267</v>
+      </c>
+      <c r="E113" s="12" t="n">
+        <f aca="false">D113/83.784</f>
+        <v>3.18676596963621</v>
+      </c>
+      <c r="F113" s="12" t="n">
+        <v>61</v>
+      </c>
+      <c r="G113" s="13" t="n">
+        <v>43917</v>
+      </c>
+      <c r="H113" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$106,G113)</f>
+        <v>-1</v>
+      </c>
+      <c r="I113" s="13" t="n">
+        <f aca="false">B$106+1</f>
+        <v>43917</v>
+      </c>
+      <c r="J113" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$106,I113)</f>
+        <v>-1</v>
+      </c>
+      <c r="K113" s="13" t="n">
+        <f aca="false">B$106+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L113" s="0"/>
+      <c r="M113" s="0"/>
+      <c r="N113" s="0"/>
+      <c r="O113" s="0"/>
+      <c r="P113" s="0"/>
+      <c r="Q113" s="0"/>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B114" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C114" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="D114" s="12" t="n">
+        <v>77</v>
+      </c>
+      <c r="E114" s="12" t="n">
+        <f aca="false">D114/10.36</f>
+        <v>7.43243243243243</v>
+      </c>
+      <c r="F114" s="12" t="n">
+        <v>15</v>
+      </c>
+      <c r="G114" s="13" t="n">
+        <v>43915</v>
+      </c>
+      <c r="H114" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$106,G114)</f>
+        <v>1</v>
+      </c>
+      <c r="I114" s="13" t="n">
+        <f aca="false">B$106+1</f>
+        <v>43917</v>
+      </c>
+      <c r="J114" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$106,I114)</f>
+        <v>-1</v>
+      </c>
+      <c r="K114" s="13" t="n">
+        <f aca="false">B$106+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L114" s="0"/>
+      <c r="M114" s="0"/>
+      <c r="N114" s="0"/>
+      <c r="O114" s="0"/>
+      <c r="P114" s="0"/>
+      <c r="Q114" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
updated with 2020-04-03 available data
</commit_message>
<xml_diff>
--- a/covid19 lockdown evaluation .xlsx
+++ b/covid19 lockdown evaluation .xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="257" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="279" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="49">
   <si>
     <t>Effects of the lockdown issued by governments</t>
   </si>
@@ -341,7 +341,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q114"/>
+  <dimension ref="A1:Q126"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F31" activeCellId="0" sqref="F31"/>
@@ -785,7 +785,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="7" t="n">
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="D22" s="0"/>
       <c r="E22" s="8" t="s">
@@ -862,36 +862,36 @@
         <v>300</v>
       </c>
       <c r="D24" s="1" t="n">
-        <v>13915</v>
+        <v>14681</v>
       </c>
       <c r="E24" s="12" t="n">
         <f aca="false">D24/60.48</f>
-        <v>230.076058201058</v>
+        <v>242.741402116402</v>
       </c>
       <c r="F24" s="12" t="n">
-        <v>760</v>
+        <v>766</v>
       </c>
       <c r="G24" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H24" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,G24)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I24" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J24" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I24)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K24" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="L24" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K24,G24)</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M24" s="0"/>
       <c r="N24" s="0"/>
@@ -907,20 +907,20 @@
         <v>230</v>
       </c>
       <c r="D25" s="1" t="n">
-        <v>10348</v>
+        <v>11198</v>
       </c>
       <c r="E25" s="12" t="n">
         <f aca="false">D25/46.75</f>
-        <v>221.347593582888</v>
+        <v>239.529411764706</v>
       </c>
       <c r="F25" s="12" t="n">
-        <v>961</v>
+        <v>850</v>
       </c>
       <c r="G25" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H25" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$22,G25)</f>
+        <f aca="false">_xlfn.DAYS($B$34,G25)</f>
         <v>16</v>
       </c>
       <c r="I25" s="13" t="n">
@@ -928,15 +928,15 @@
       </c>
       <c r="J25" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I25)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K25" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="L25" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K25,G25)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M25" s="0"/>
       <c r="N25" s="0"/>
@@ -952,20 +952,20 @@
         <v>330</v>
       </c>
       <c r="D26" s="1" t="n">
-        <v>5387</v>
+        <v>6507</v>
       </c>
       <c r="E26" s="12" t="n">
         <f aca="false">D26/65.27</f>
-        <v>82.5340891680711</v>
+        <v>99.6935805117206</v>
       </c>
       <c r="F26" s="12" t="n">
-        <v>1355</v>
+        <v>1120</v>
       </c>
       <c r="G26" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H26" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$22,G26)</f>
+        <f aca="false">_xlfn.DAYS($B$34,G26)</f>
         <v>11</v>
       </c>
       <c r="I26" s="13" t="n">
@@ -973,15 +973,15 @@
       </c>
       <c r="J26" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I26)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K26" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="L26" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K26,G26)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M26" s="0"/>
       <c r="N26" s="0"/>
@@ -997,25 +997,25 @@
         <v>50</v>
       </c>
       <c r="D27" s="12" t="n">
-        <v>308</v>
+        <v>358</v>
       </c>
       <c r="E27" s="12" t="n">
         <f aca="false">D27/10.36</f>
-        <v>29.7297297297297</v>
+        <v>34.5559845559846</v>
       </c>
       <c r="F27" s="12" t="n">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="G27" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H27" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$22,G27)</f>
+        <f aca="false">_xlfn.DAYS($B$34,G27)</f>
         <v>8</v>
       </c>
       <c r="I27" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="J27" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I27)</f>
@@ -1023,11 +1023,11 @@
       </c>
       <c r="K27" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="L27" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K27,G27)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M27" s="0"/>
       <c r="N27" s="0"/>
@@ -1043,25 +1043,25 @@
         <v>330</v>
       </c>
       <c r="D28" s="1" t="n">
-        <v>2921</v>
+        <v>3605</v>
       </c>
       <c r="E28" s="12" t="n">
         <f aca="false">D28/67.79</f>
-        <v>43.0889511727393</v>
+        <v>53.1789349461573</v>
       </c>
       <c r="F28" s="12" t="n">
-        <v>569</v>
+        <v>684</v>
       </c>
       <c r="G28" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H28" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$22,G28)</f>
+        <f aca="false">_xlfn.DAYS($B$34,G28)</f>
         <v>7</v>
       </c>
       <c r="I28" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="J28" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I28)</f>
@@ -1069,11 +1069,11 @@
       </c>
       <c r="K28" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="L28" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K28,G28)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M28" s="0"/>
       <c r="N28" s="0"/>
@@ -1089,25 +1089,25 @@
         <v>1660</v>
       </c>
       <c r="D29" s="1" t="n">
-        <v>6070</v>
+        <v>7392</v>
       </c>
       <c r="E29" s="12" t="n">
         <f aca="false">D29/331</f>
-        <v>18.3383685800604</v>
+        <v>22.3323262839879</v>
       </c>
       <c r="F29" s="12" t="n">
-        <v>968</v>
+        <v>1321</v>
       </c>
       <c r="G29" s="13" t="n">
         <v>43917</v>
       </c>
       <c r="H29" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$22,G29)</f>
+        <f aca="false">_xlfn.DAYS($B$34,G29)</f>
         <v>6</v>
       </c>
       <c r="I29" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="J29" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I29)</f>
@@ -1115,11 +1115,11 @@
       </c>
       <c r="K29" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="L29" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K29,G29)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M29" s="0"/>
       <c r="N29" s="0"/>
@@ -1135,25 +1135,25 @@
         <v>414</v>
       </c>
       <c r="D30" s="1" t="n">
-        <v>1107</v>
+        <v>1275</v>
       </c>
       <c r="E30" s="12" t="n">
         <f aca="false">D30/83.784</f>
-        <v>13.212546548267</v>
+        <v>15.2177026639931</v>
       </c>
       <c r="F30" s="12" t="n">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="G30" s="13" t="n">
         <v>43918</v>
       </c>
       <c r="H30" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$22,G30)</f>
+        <f aca="false">_xlfn.DAYS($B$34,G30)</f>
         <v>5</v>
       </c>
       <c r="I30" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="J30" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I30)</f>
@@ -1161,11 +1161,11 @@
       </c>
       <c r="K30" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="L30" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K30,G30)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M30" s="0"/>
       <c r="N30" s="0"/>
@@ -1230,7 +1230,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="7" t="n">
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="D34" s="0"/>
       <c r="E34" s="8" t="s">
@@ -1307,36 +1307,36 @@
         <v>300</v>
       </c>
       <c r="D36" s="1" t="n">
-        <v>13155</v>
+        <v>13915</v>
       </c>
       <c r="E36" s="12" t="n">
         <f aca="false">D36/60.48</f>
-        <v>217.509920634921</v>
+        <v>230.076058201058</v>
       </c>
       <c r="F36" s="12" t="n">
-        <v>727</v>
+        <v>760</v>
       </c>
       <c r="G36" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H36" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,G36)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I36" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J36" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I36)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K36" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="L36" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K36,G36)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M36" s="0"/>
       <c r="N36" s="0"/>
@@ -1352,36 +1352,36 @@
         <v>230</v>
       </c>
       <c r="D37" s="1" t="n">
-        <v>9387</v>
+        <v>10348</v>
       </c>
       <c r="E37" s="12" t="n">
         <f aca="false">D37/46.75</f>
-        <v>200.791443850267</v>
+        <v>221.347593582888</v>
       </c>
       <c r="F37" s="12" t="n">
-        <v>923</v>
+        <v>961</v>
       </c>
       <c r="G37" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H37" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,G37)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I37" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J37" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I37)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K37" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="L37" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K37,G37)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M37" s="0"/>
       <c r="N37" s="0"/>
@@ -1397,36 +1397,36 @@
         <v>330</v>
       </c>
       <c r="D38" s="1" t="n">
-        <v>4032</v>
+        <v>5387</v>
       </c>
       <c r="E38" s="12" t="n">
         <f aca="false">D38/65.27</f>
-        <v>61.7741688371381</v>
+        <v>82.5340891680711</v>
       </c>
       <c r="F38" s="12" t="n">
-        <v>509</v>
+        <v>1355</v>
       </c>
       <c r="G38" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H38" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,G38)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I38" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J38" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I38)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K38" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="L38" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K38,G38)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M38" s="0"/>
       <c r="N38" s="0"/>
@@ -1442,25 +1442,25 @@
         <v>50</v>
       </c>
       <c r="D39" s="12" t="n">
-        <v>239</v>
+        <v>308</v>
       </c>
       <c r="E39" s="12" t="n">
         <f aca="false">D39/10.36</f>
-        <v>23.0694980694981</v>
+        <v>29.7297297297297</v>
       </c>
       <c r="F39" s="12" t="n">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="G39" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H39" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,G39)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I39" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="J39" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I39)</f>
@@ -1468,11 +1468,11 @@
       </c>
       <c r="K39" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="L39" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K39,G39)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M39" s="0"/>
       <c r="N39" s="0"/>
@@ -1488,25 +1488,25 @@
         <v>330</v>
       </c>
       <c r="D40" s="1" t="n">
-        <v>2352</v>
+        <v>2921</v>
       </c>
       <c r="E40" s="12" t="n">
         <f aca="false">D40/67.79</f>
-        <v>34.695382799823</v>
+        <v>43.0889511727393</v>
       </c>
       <c r="F40" s="12" t="n">
-        <v>563</v>
+        <v>569</v>
       </c>
       <c r="G40" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H40" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,G40)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I40" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="J40" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I40)</f>
@@ -1514,11 +1514,11 @@
       </c>
       <c r="K40" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="L40" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K40,G40)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M40" s="0"/>
       <c r="N40" s="0"/>
@@ -1534,25 +1534,25 @@
         <v>1660</v>
       </c>
       <c r="D41" s="1" t="n">
-        <v>5102</v>
+        <v>6071</v>
       </c>
       <c r="E41" s="12" t="n">
         <f aca="false">D41/331</f>
-        <v>15.4138972809668</v>
+        <v>18.3413897280967</v>
       </c>
       <c r="F41" s="12" t="n">
-        <v>1049</v>
+        <v>969</v>
       </c>
       <c r="G41" s="13" t="n">
         <v>43917</v>
       </c>
       <c r="H41" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,G41)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I41" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="J41" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I41)</f>
@@ -1560,11 +1560,11 @@
       </c>
       <c r="K41" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="L41" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K41,G41)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M41" s="0"/>
       <c r="N41" s="0"/>
@@ -1580,25 +1580,25 @@
         <v>414</v>
       </c>
       <c r="D42" s="1" t="n">
-        <v>931</v>
+        <v>1107</v>
       </c>
       <c r="E42" s="12" t="n">
         <f aca="false">D42/83.784</f>
-        <v>11.1119068079824</v>
+        <v>13.212546548267</v>
       </c>
       <c r="F42" s="12" t="n">
-        <v>156</v>
+        <v>176</v>
       </c>
       <c r="G42" s="13" t="n">
         <v>43918</v>
       </c>
       <c r="H42" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,G42)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I42" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="J42" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I42)</f>
@@ -1606,11 +1606,11 @@
       </c>
       <c r="K42" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="L42" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K42,G42)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M42" s="0"/>
       <c r="N42" s="0"/>
@@ -1675,7 +1675,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="7" t="n">
-        <v>43921</v>
+        <v>43922</v>
       </c>
       <c r="D46" s="0"/>
       <c r="E46" s="8" t="s">
@@ -1752,36 +1752,36 @@
         <v>300</v>
       </c>
       <c r="D48" s="1" t="n">
-        <v>12428</v>
+        <v>13155</v>
       </c>
       <c r="E48" s="12" t="n">
         <f aca="false">D48/60.48</f>
-        <v>205.489417989418</v>
+        <v>217.509920634921</v>
       </c>
       <c r="F48" s="12" t="n">
-        <v>837</v>
+        <v>727</v>
       </c>
       <c r="G48" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H48" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,G48)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I48" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J48" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I48)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K48" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L48" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K48,G48)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M48" s="0"/>
       <c r="N48" s="0"/>
@@ -1797,36 +1797,36 @@
         <v>230</v>
       </c>
       <c r="D49" s="1" t="n">
-        <v>8464</v>
+        <v>9387</v>
       </c>
       <c r="E49" s="12" t="n">
         <f aca="false">D49/46.75</f>
-        <v>181.048128342246</v>
+        <v>200.791443850267</v>
       </c>
       <c r="F49" s="12" t="n">
-        <v>748</v>
+        <v>923</v>
       </c>
       <c r="G49" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H49" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,G49)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I49" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J49" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I49)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K49" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L49" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K49,G49)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M49" s="0"/>
       <c r="N49" s="0"/>
@@ -1842,36 +1842,36 @@
         <v>330</v>
       </c>
       <c r="D50" s="1" t="n">
-        <v>3523</v>
+        <v>4032</v>
       </c>
       <c r="E50" s="12" t="n">
         <f aca="false">D50/65.27</f>
-        <v>53.9757928604259</v>
+        <v>61.7741688371381</v>
       </c>
       <c r="F50" s="12" t="n">
-        <v>499</v>
+        <v>509</v>
       </c>
       <c r="G50" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H50" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,G50)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I50" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J50" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I50)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K50" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L50" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K50,G50)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M50" s="0"/>
       <c r="N50" s="0"/>
@@ -1887,25 +1887,25 @@
         <v>50</v>
       </c>
       <c r="D51" s="12" t="n">
-        <v>180</v>
+        <v>239</v>
       </c>
       <c r="E51" s="12" t="n">
         <f aca="false">D51/10.36</f>
-        <v>17.3745173745174</v>
+        <v>23.0694980694981</v>
       </c>
       <c r="F51" s="12" t="n">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="G51" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H51" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,G51)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I51" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="J51" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I51)</f>
@@ -1913,11 +1913,11 @@
       </c>
       <c r="K51" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L51" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K51,G51)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M51" s="0"/>
       <c r="N51" s="0"/>
@@ -1933,25 +1933,25 @@
         <v>330</v>
       </c>
       <c r="D52" s="1" t="n">
-        <v>1789</v>
+        <v>2352</v>
       </c>
       <c r="E52" s="12" t="n">
         <f aca="false">D52/67.79</f>
-        <v>26.390323056498</v>
+        <v>34.695382799823</v>
       </c>
       <c r="F52" s="12" t="n">
-        <v>381</v>
+        <v>563</v>
       </c>
       <c r="G52" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H52" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,G52)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I52" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="J52" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I52)</f>
@@ -1959,11 +1959,11 @@
       </c>
       <c r="K52" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L52" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K52,G52)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M52" s="0"/>
       <c r="N52" s="0"/>
@@ -1979,25 +1979,25 @@
         <v>1660</v>
       </c>
       <c r="D53" s="1" t="n">
-        <v>4053</v>
+        <v>5102</v>
       </c>
       <c r="E53" s="12" t="n">
         <f aca="false">D53/331</f>
-        <v>12.2447129909366</v>
+        <v>15.4138972809668</v>
       </c>
       <c r="F53" s="12" t="n">
-        <v>912</v>
+        <v>1049</v>
       </c>
       <c r="G53" s="13" t="n">
         <v>43917</v>
       </c>
       <c r="H53" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,G53)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I53" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="J53" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I53)</f>
@@ -2005,11 +2005,11 @@
       </c>
       <c r="K53" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L53" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K53,G53)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M53" s="0"/>
       <c r="N53" s="0"/>
@@ -2025,25 +2025,25 @@
         <v>414</v>
       </c>
       <c r="D54" s="1" t="n">
-        <v>775</v>
+        <v>931</v>
       </c>
       <c r="E54" s="12" t="n">
         <f aca="false">D54/83.784</f>
-        <v>9.24997612909386</v>
+        <v>11.1119068079824</v>
       </c>
       <c r="F54" s="12" t="n">
-        <v>130</v>
+        <v>156</v>
       </c>
       <c r="G54" s="13" t="n">
         <v>43918</v>
       </c>
       <c r="H54" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,G54)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I54" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="J54" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I54)</f>
@@ -2051,11 +2051,11 @@
       </c>
       <c r="K54" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L54" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K54,G54)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M54" s="0"/>
       <c r="N54" s="0"/>
@@ -2064,15 +2064,16 @@
       <c r="Q54" s="0"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C55" s="12"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="5"/>
       <c r="D55" s="0"/>
-      <c r="E55" s="12"/>
-      <c r="F55" s="12"/>
-      <c r="G55" s="13"/>
+      <c r="E55" s="0"/>
+      <c r="F55" s="0"/>
+      <c r="G55" s="0"/>
       <c r="H55" s="0"/>
-      <c r="I55" s="13"/>
+      <c r="I55" s="0"/>
       <c r="J55" s="0"/>
-      <c r="K55" s="13"/>
+      <c r="K55" s="0"/>
       <c r="L55" s="0"/>
       <c r="M55" s="0"/>
       <c r="N55" s="0"/>
@@ -2081,15 +2082,16 @@
       <c r="Q55" s="0"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C56" s="12"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="5"/>
       <c r="D56" s="0"/>
-      <c r="E56" s="12"/>
-      <c r="F56" s="12"/>
-      <c r="G56" s="13"/>
+      <c r="E56" s="0"/>
+      <c r="F56" s="0"/>
+      <c r="G56" s="0"/>
       <c r="H56" s="0"/>
-      <c r="I56" s="13"/>
+      <c r="I56" s="0"/>
       <c r="J56" s="0"/>
-      <c r="K56" s="13"/>
+      <c r="K56" s="0"/>
       <c r="L56" s="0"/>
       <c r="M56" s="0"/>
       <c r="N56" s="0"/>
@@ -2118,7 +2120,7 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="7" t="n">
-        <v>43920</v>
+        <v>43921</v>
       </c>
       <c r="D58" s="0"/>
       <c r="E58" s="8" t="s">
@@ -2140,7 +2142,9 @@
       <c r="K58" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="L58" s="0"/>
+      <c r="L58" s="8" t="s">
+        <v>33</v>
+      </c>
       <c r="M58" s="0"/>
       <c r="N58" s="0"/>
       <c r="O58" s="0"/>
@@ -2176,7 +2180,9 @@
       <c r="K59" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L59" s="0"/>
+      <c r="L59" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="M59" s="0"/>
       <c r="N59" s="0"/>
       <c r="O59" s="0"/>
@@ -2191,34 +2197,37 @@
         <v>300</v>
       </c>
       <c r="D60" s="1" t="n">
-        <v>11591</v>
+        <v>12428</v>
       </c>
       <c r="E60" s="12" t="n">
         <f aca="false">D60/60.48</f>
-        <v>191.650132275132</v>
+        <v>205.489417989418</v>
       </c>
       <c r="F60" s="12" t="n">
-        <v>812</v>
+        <v>837</v>
       </c>
       <c r="G60" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H60" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,G60)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I60" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J60" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I60)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K60" s="13" t="n">
-        <f aca="false">$B$70+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L60" s="0"/>
+        <f aca="false">$B$58+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L60" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K60,G60)</f>
+        <v>22</v>
+      </c>
       <c r="M60" s="0"/>
       <c r="N60" s="0"/>
       <c r="O60" s="0"/>
@@ -2233,34 +2242,37 @@
         <v>230</v>
       </c>
       <c r="D61" s="1" t="n">
-        <v>7716</v>
+        <v>8464</v>
       </c>
       <c r="E61" s="12" t="n">
         <f aca="false">D61/46.75</f>
-        <v>165.048128342246</v>
+        <v>181.048128342246</v>
       </c>
       <c r="F61" s="12" t="n">
-        <v>913</v>
+        <v>748</v>
       </c>
       <c r="G61" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H61" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,G61)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I61" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J61" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I61)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K61" s="13" t="n">
-        <f aca="false">$B$70+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L61" s="0"/>
+        <f aca="false">$B$58+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L61" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K61,G61)</f>
+        <v>15</v>
+      </c>
       <c r="M61" s="0"/>
       <c r="N61" s="0"/>
       <c r="O61" s="0"/>
@@ -2275,34 +2287,37 @@
         <v>330</v>
       </c>
       <c r="D62" s="1" t="n">
-        <v>3024</v>
+        <v>3523</v>
       </c>
       <c r="E62" s="12" t="n">
         <f aca="false">D62/65.27</f>
-        <v>46.3306266278535</v>
+        <v>53.9757928604259</v>
       </c>
       <c r="F62" s="12" t="n">
-        <v>418</v>
+        <v>499</v>
       </c>
       <c r="G62" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H62" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,G62)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I62" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J62" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I62)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K62" s="13" t="n">
-        <f aca="false">$B$70+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L62" s="0"/>
+        <f aca="false">$B$58+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L62" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K62,G62)</f>
+        <v>10</v>
+      </c>
       <c r="M62" s="0"/>
       <c r="N62" s="0"/>
       <c r="O62" s="0"/>
@@ -2317,35 +2332,38 @@
         <v>50</v>
       </c>
       <c r="D63" s="12" t="n">
-        <v>146</v>
+        <v>180</v>
       </c>
       <c r="E63" s="12" t="n">
         <f aca="false">D63/10.36</f>
-        <v>14.0926640926641</v>
+        <v>17.3745173745174</v>
       </c>
       <c r="F63" s="12" t="n">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G63" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H63" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,G63)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I63" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43921</v>
+        <v>43922</v>
       </c>
       <c r="J63" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I63)</f>
         <v>-1</v>
       </c>
       <c r="K63" s="13" t="n">
-        <f aca="false">$B$70+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L63" s="0"/>
+        <f aca="false">$B$58+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L63" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K63,G63)</f>
+        <v>7</v>
+      </c>
       <c r="M63" s="0"/>
       <c r="N63" s="0"/>
       <c r="O63" s="0"/>
@@ -2360,35 +2378,38 @@
         <v>330</v>
       </c>
       <c r="D64" s="1" t="n">
-        <v>1408</v>
+        <v>1789</v>
       </c>
       <c r="E64" s="12" t="n">
         <f aca="false">D64/67.79</f>
-        <v>20.770025077445</v>
+        <v>26.390323056498</v>
       </c>
       <c r="F64" s="12" t="n">
-        <v>180</v>
+        <v>381</v>
       </c>
       <c r="G64" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H64" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,G64)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I64" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43921</v>
+        <v>43922</v>
       </c>
       <c r="J64" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I64)</f>
         <v>-1</v>
       </c>
       <c r="K64" s="13" t="n">
-        <f aca="false">$B$70+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L64" s="0"/>
+        <f aca="false">$B$58+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L64" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K64,G64)</f>
+        <v>6</v>
+      </c>
       <c r="M64" s="0"/>
       <c r="N64" s="0"/>
       <c r="O64" s="0"/>
@@ -2403,34 +2424,38 @@
         <v>1660</v>
       </c>
       <c r="D65" s="1" t="n">
-        <v>3141</v>
+        <v>4053</v>
       </c>
       <c r="E65" s="12" t="n">
         <f aca="false">D65/331</f>
-        <v>9.48942598187311</v>
+        <v>12.2447129909366</v>
       </c>
       <c r="F65" s="12" t="n">
-        <v>573</v>
+        <v>912</v>
       </c>
       <c r="G65" s="13" t="n">
         <v>43917</v>
       </c>
       <c r="H65" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,G65)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I65" s="13" t="n">
-        <v>43920</v>
+        <f aca="false">$B$58+1</f>
+        <v>43922</v>
       </c>
       <c r="J65" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I65)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="K65" s="13" t="n">
-        <f aca="false">$B$70+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L65" s="0"/>
+        <f aca="false">$B$58+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L65" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K65,G65)</f>
+        <v>5</v>
+      </c>
       <c r="M65" s="0"/>
       <c r="N65" s="0"/>
       <c r="O65" s="0"/>
@@ -2445,35 +2470,38 @@
         <v>414</v>
       </c>
       <c r="D66" s="1" t="n">
-        <v>645</v>
+        <v>775</v>
       </c>
       <c r="E66" s="12" t="n">
         <f aca="false">D66/83.784</f>
-        <v>7.69836723002005</v>
+        <v>9.24997612909386</v>
       </c>
       <c r="F66" s="12" t="n">
-        <v>104</v>
+        <v>130</v>
       </c>
       <c r="G66" s="13" t="n">
         <v>43918</v>
       </c>
       <c r="H66" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,G66)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I66" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43921</v>
+        <v>43922</v>
       </c>
       <c r="J66" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I66)</f>
         <v>-1</v>
       </c>
       <c r="K66" s="13" t="n">
-        <f aca="false">$B$70+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L66" s="0"/>
+        <f aca="false">$B$58+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L66" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K66,G66)</f>
+        <v>4</v>
+      </c>
       <c r="M66" s="0"/>
       <c r="N66" s="0"/>
       <c r="O66" s="0"/>
@@ -2481,16 +2509,15 @@
       <c r="Q66" s="0"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B67" s="4"/>
-      <c r="C67" s="5"/>
+      <c r="C67" s="12"/>
       <c r="D67" s="0"/>
-      <c r="E67" s="0"/>
-      <c r="F67" s="0"/>
-      <c r="G67" s="0"/>
+      <c r="E67" s="12"/>
+      <c r="F67" s="12"/>
+      <c r="G67" s="13"/>
       <c r="H67" s="0"/>
-      <c r="I67" s="0"/>
+      <c r="I67" s="13"/>
       <c r="J67" s="0"/>
-      <c r="K67" s="0"/>
+      <c r="K67" s="13"/>
       <c r="L67" s="0"/>
       <c r="M67" s="0"/>
       <c r="N67" s="0"/>
@@ -2499,16 +2526,15 @@
       <c r="Q67" s="0"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="4"/>
-      <c r="C68" s="5"/>
+      <c r="C68" s="12"/>
       <c r="D68" s="0"/>
-      <c r="E68" s="0"/>
-      <c r="F68" s="0"/>
-      <c r="G68" s="0"/>
+      <c r="E68" s="12"/>
+      <c r="F68" s="12"/>
+      <c r="G68" s="13"/>
       <c r="H68" s="0"/>
-      <c r="I68" s="0"/>
+      <c r="I68" s="13"/>
       <c r="J68" s="0"/>
-      <c r="K68" s="0"/>
+      <c r="K68" s="13"/>
       <c r="L68" s="0"/>
       <c r="M68" s="0"/>
       <c r="N68" s="0"/>
@@ -2537,7 +2563,7 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="7" t="n">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="D70" s="0"/>
       <c r="E70" s="8" t="s">
@@ -2610,31 +2636,31 @@
         <v>300</v>
       </c>
       <c r="D72" s="1" t="n">
-        <v>10779</v>
+        <v>11591</v>
       </c>
       <c r="E72" s="12" t="n">
         <f aca="false">D72/60.48</f>
-        <v>178.224206349206</v>
+        <v>191.650132275132</v>
       </c>
       <c r="F72" s="12" t="n">
-        <v>756</v>
+        <v>812</v>
       </c>
       <c r="G72" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H72" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,G72)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I72" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J72" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,I72)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K72" s="13" t="n">
-        <f aca="false">$B$70+1</f>
+        <f aca="false">$B$82+1</f>
         <v>43920</v>
       </c>
       <c r="L72" s="0"/>
@@ -2652,31 +2678,31 @@
         <v>230</v>
       </c>
       <c r="D73" s="1" t="n">
-        <v>6803</v>
+        <v>7716</v>
       </c>
       <c r="E73" s="12" t="n">
         <f aca="false">D73/46.75</f>
-        <v>145.51871657754</v>
+        <v>165.048128342246</v>
       </c>
       <c r="F73" s="12" t="n">
-        <v>821</v>
+        <v>913</v>
       </c>
       <c r="G73" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H73" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,G73)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I73" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J73" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,I73)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K73" s="13" t="n">
-        <f aca="false">$B$70+1</f>
+        <f aca="false">$B$82+1</f>
         <v>43920</v>
       </c>
       <c r="L73" s="0"/>
@@ -2694,31 +2720,31 @@
         <v>330</v>
       </c>
       <c r="D74" s="1" t="n">
-        <v>2606</v>
+        <v>3024</v>
       </c>
       <c r="E74" s="12" t="n">
         <f aca="false">D74/65.27</f>
-        <v>39.9264593228129</v>
+        <v>46.3306266278535</v>
       </c>
       <c r="F74" s="12" t="n">
-        <v>292</v>
+        <v>418</v>
       </c>
       <c r="G74" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H74" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,G74)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I74" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J74" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,I74)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K74" s="13" t="n">
-        <f aca="false">$B$70+1</f>
+        <f aca="false">$B$82+1</f>
         <v>43920</v>
       </c>
       <c r="L74" s="0"/>
@@ -2730,38 +2756,38 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="0" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C75" s="12" t="n">
-        <v>1660</v>
-      </c>
-      <c r="D75" s="1" t="n">
-        <v>2583</v>
+        <v>50</v>
+      </c>
+      <c r="D75" s="12" t="n">
+        <v>146</v>
       </c>
       <c r="E75" s="12" t="n">
-        <f aca="false">D75/331</f>
-        <v>7.8036253776435</v>
+        <f aca="false">D75/10.36</f>
+        <v>14.0926640926641</v>
       </c>
       <c r="F75" s="12" t="n">
-        <v>363</v>
+        <v>36</v>
       </c>
       <c r="G75" s="13" t="n">
-        <v>43917</v>
+        <v>43915</v>
       </c>
       <c r="H75" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,G75)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I75" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43920</v>
+        <v>43921</v>
       </c>
       <c r="J75" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,I75)</f>
         <v>-1</v>
       </c>
       <c r="K75" s="13" t="n">
-        <f aca="false">$B$70+1</f>
+        <f aca="false">$B$82+1</f>
         <v>43920</v>
       </c>
       <c r="L75" s="0"/>
@@ -2779,32 +2805,32 @@
         <v>330</v>
       </c>
       <c r="D76" s="1" t="n">
-        <v>1228</v>
+        <v>1408</v>
       </c>
       <c r="E76" s="12" t="n">
         <f aca="false">D76/67.79</f>
-        <v>18.1147661897035</v>
+        <v>20.770025077445</v>
       </c>
       <c r="F76" s="12" t="n">
-        <v>209</v>
+        <v>180</v>
       </c>
       <c r="G76" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H76" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,G76)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I76" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43920</v>
+        <v>43921</v>
       </c>
       <c r="J76" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,I76)</f>
         <v>-1</v>
       </c>
       <c r="K76" s="13" t="n">
-        <f aca="false">$B$70+1</f>
+        <f aca="false">$B$82+1</f>
         <v>43920</v>
       </c>
       <c r="L76" s="0"/>
@@ -2816,38 +2842,37 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C77" s="12" t="n">
-        <v>414</v>
+        <v>1660</v>
       </c>
       <c r="D77" s="1" t="n">
-        <v>541</v>
+        <v>3141</v>
       </c>
       <c r="E77" s="12" t="n">
-        <f aca="false">D77/83.784</f>
-        <v>6.457080110761</v>
+        <f aca="false">D77/331</f>
+        <v>9.48942598187311</v>
       </c>
       <c r="F77" s="12" t="n">
-        <v>108</v>
+        <v>573</v>
       </c>
       <c r="G77" s="13" t="n">
-        <v>43918</v>
+        <v>43917</v>
       </c>
       <c r="H77" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,G77)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I77" s="13" t="n">
-        <f aca="false">$B$70+1</f>
         <v>43920</v>
       </c>
       <c r="J77" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,I77)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="K77" s="13" t="n">
-        <f aca="false">$B$70+1</f>
+        <f aca="false">$B$82+1</f>
         <v>43920</v>
       </c>
       <c r="L77" s="0"/>
@@ -2859,38 +2884,38 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C78" s="12" t="n">
-        <v>50</v>
-      </c>
-      <c r="D78" s="12" t="n">
-        <v>110</v>
+        <v>414</v>
+      </c>
+      <c r="D78" s="1" t="n">
+        <v>645</v>
       </c>
       <c r="E78" s="12" t="n">
-        <f aca="false">D78/10.36</f>
-        <v>10.6177606177606</v>
+        <f aca="false">D78/83.784</f>
+        <v>7.69836723002005</v>
       </c>
       <c r="F78" s="12" t="n">
-        <v>5</v>
+        <v>104</v>
       </c>
       <c r="G78" s="13" t="n">
-        <v>43915</v>
+        <v>43918</v>
       </c>
       <c r="H78" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,G78)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I78" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43920</v>
+        <v>43921</v>
       </c>
       <c r="J78" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,I78)</f>
         <v>-1</v>
       </c>
       <c r="K78" s="13" t="n">
-        <f aca="false">$B$70+1</f>
+        <f aca="false">$B$82+1</f>
         <v>43920</v>
       </c>
       <c r="L78" s="0"/>
@@ -2957,15 +2982,13 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="7" t="n">
-        <v>43918</v>
-      </c>
-      <c r="D82" s="8" t="s">
-        <v>6</v>
-      </c>
+        <v>43919</v>
+      </c>
+      <c r="D82" s="0"/>
       <c r="E82" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F82" s="8"/>
+      <c r="F82" s="0"/>
       <c r="G82" s="8" t="s">
         <v>29</v>
       </c>
@@ -2993,8 +3016,8 @@
       <c r="C83" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D83" s="10" t="s">
-        <v>2</v>
+      <c r="D83" s="8" t="s">
+        <v>6</v>
       </c>
       <c r="E83" s="10" t="s">
         <v>35</v>
@@ -3032,32 +3055,32 @@
         <v>300</v>
       </c>
       <c r="D84" s="1" t="n">
-        <v>10023</v>
+        <v>10779</v>
       </c>
       <c r="E84" s="12" t="n">
         <f aca="false">D84/60.48</f>
-        <v>165.724206349206</v>
+        <v>178.224206349206</v>
       </c>
       <c r="F84" s="12" t="n">
-        <v>889</v>
+        <v>756</v>
       </c>
       <c r="G84" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H84" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,G84)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I84" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J84" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$94,I84)</f>
-        <v>15</v>
+        <f aca="false">_xlfn.DAYS($B$82,I84)</f>
+        <v>17</v>
       </c>
       <c r="K84" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L84" s="0"/>
       <c r="M84" s="0"/>
@@ -3074,32 +3097,32 @@
         <v>230</v>
       </c>
       <c r="D85" s="1" t="n">
-        <v>5982</v>
+        <v>6803</v>
       </c>
       <c r="E85" s="12" t="n">
         <f aca="false">D85/46.75</f>
-        <v>127.957219251337</v>
+        <v>145.51871657754</v>
       </c>
       <c r="F85" s="12" t="n">
-        <v>844</v>
+        <v>821</v>
       </c>
       <c r="G85" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H85" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,G85)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I85" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J85" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$94,I85)</f>
-        <v>4</v>
+        <f aca="false">_xlfn.DAYS($B$82,I85)</f>
+        <v>6</v>
       </c>
       <c r="K85" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L85" s="0"/>
       <c r="M85" s="0"/>
@@ -3116,32 +3139,32 @@
         <v>330</v>
       </c>
       <c r="D86" s="1" t="n">
-        <v>2314</v>
+        <v>2606</v>
       </c>
       <c r="E86" s="12" t="n">
         <f aca="false">D86/65.27</f>
-        <v>35.4527347939329</v>
+        <v>39.9264593228129</v>
       </c>
       <c r="F86" s="12" t="n">
-        <v>319</v>
+        <v>292</v>
       </c>
       <c r="G86" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H86" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,G86)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I86" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J86" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$94,I86)</f>
-        <v>3</v>
+        <f aca="false">_xlfn.DAYS($B$82,I86)</f>
+        <v>5</v>
       </c>
       <c r="K86" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L86" s="0"/>
       <c r="M86" s="0"/>
@@ -3158,25 +3181,25 @@
         <v>1660</v>
       </c>
       <c r="D87" s="1" t="n">
-        <v>2221</v>
+        <v>2583</v>
       </c>
       <c r="E87" s="12" t="n">
         <f aca="false">D87/331</f>
-        <v>6.70996978851964</v>
+        <v>7.8036253776435</v>
       </c>
       <c r="F87" s="12" t="n">
-        <v>525</v>
+        <v>363</v>
       </c>
       <c r="G87" s="13" t="n">
         <v>43917</v>
       </c>
       <c r="H87" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,G87)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I87" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="J87" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,I87)</f>
@@ -3184,7 +3207,7 @@
       </c>
       <c r="K87" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L87" s="0"/>
       <c r="M87" s="0"/>
@@ -3201,25 +3224,25 @@
         <v>330</v>
       </c>
       <c r="D88" s="1" t="n">
-        <v>1019</v>
+        <v>1228</v>
       </c>
       <c r="E88" s="12" t="n">
         <f aca="false">D88/67.79</f>
-        <v>15.0317155922702</v>
+        <v>18.1147661897035</v>
       </c>
       <c r="F88" s="12" t="n">
-        <v>260</v>
+        <v>209</v>
       </c>
       <c r="G88" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H88" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,G88)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I88" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="J88" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,I88)</f>
@@ -3227,7 +3250,7 @@
       </c>
       <c r="K88" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L88" s="0"/>
       <c r="M88" s="0"/>
@@ -3244,25 +3267,25 @@
         <v>414</v>
       </c>
       <c r="D89" s="1" t="n">
-        <v>433</v>
+        <v>541</v>
       </c>
       <c r="E89" s="12" t="n">
         <f aca="false">D89/83.784</f>
-        <v>5.16805117922276</v>
+        <v>6.457080110761</v>
       </c>
       <c r="F89" s="12" t="n">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="G89" s="13" t="n">
         <v>43918</v>
       </c>
       <c r="H89" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,G89)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I89" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="J89" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,I89)</f>
@@ -3270,7 +3293,7 @@
       </c>
       <c r="K89" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L89" s="0"/>
       <c r="M89" s="0"/>
@@ -3287,25 +3310,25 @@
         <v>50</v>
       </c>
       <c r="D90" s="12" t="n">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="E90" s="12" t="n">
         <f aca="false">D90/10.36</f>
-        <v>10.1351351351351</v>
+        <v>10.6177606177606</v>
       </c>
       <c r="F90" s="12" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G90" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H90" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,G90)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I90" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="J90" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,I90)</f>
@@ -3313,7 +3336,7 @@
       </c>
       <c r="K90" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L90" s="0"/>
       <c r="M90" s="0"/>
@@ -3323,15 +3346,16 @@
       <c r="Q90" s="0"/>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C91" s="12"/>
-      <c r="D91" s="12"/>
-      <c r="E91" s="12"/>
-      <c r="F91" s="12"/>
-      <c r="G91" s="13"/>
+      <c r="B91" s="4"/>
+      <c r="C91" s="5"/>
+      <c r="D91" s="0"/>
+      <c r="E91" s="0"/>
+      <c r="F91" s="0"/>
+      <c r="G91" s="0"/>
       <c r="H91" s="0"/>
-      <c r="I91" s="13"/>
+      <c r="I91" s="0"/>
       <c r="J91" s="0"/>
-      <c r="K91" s="13"/>
+      <c r="K91" s="0"/>
       <c r="L91" s="0"/>
       <c r="M91" s="0"/>
       <c r="N91" s="0"/>
@@ -3376,11 +3400,10 @@
       <c r="P93" s="0"/>
       <c r="Q93" s="0"/>
     </row>
-    <row r="94" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="7" t="n">
-        <v>43917</v>
-      </c>
-      <c r="C94" s="0"/>
+        <v>43918</v>
+      </c>
       <c r="D94" s="8" t="s">
         <v>6</v>
       </c>
@@ -3403,10 +3426,14 @@
       <c r="K94" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="L94" s="8"/>
+      <c r="L94" s="0"/>
+      <c r="M94" s="0"/>
+      <c r="N94" s="0"/>
+      <c r="O94" s="0"/>
+      <c r="P94" s="0"/>
+      <c r="Q94" s="0"/>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="3"/>
       <c r="B95" s="9"/>
       <c r="C95" s="10" t="s">
         <v>34</v>
@@ -3435,7 +3462,7 @@
       <c r="K95" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L95" s="8"/>
+      <c r="L95" s="0"/>
       <c r="M95" s="0"/>
       <c r="N95" s="0"/>
       <c r="O95" s="0"/>
@@ -3450,32 +3477,32 @@
         <v>300</v>
       </c>
       <c r="D96" s="1" t="n">
-        <v>9134</v>
+        <v>10023</v>
       </c>
       <c r="E96" s="12" t="n">
         <f aca="false">D96/60.48</f>
-        <v>151.025132275132</v>
+        <v>165.724206349206</v>
       </c>
       <c r="F96" s="12" t="n">
-        <v>919</v>
+        <v>889</v>
       </c>
       <c r="G96" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H96" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,G96)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I96" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J96" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$94,I96)</f>
+        <f aca="false">_xlfn.DAYS(B$106,I96)</f>
         <v>15</v>
       </c>
       <c r="K96" s="13" t="n">
         <f aca="false">$B$94+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L96" s="0"/>
       <c r="M96" s="0"/>
@@ -3492,32 +3519,32 @@
         <v>230</v>
       </c>
       <c r="D97" s="1" t="n">
-        <v>5138</v>
+        <v>5982</v>
       </c>
       <c r="E97" s="12" t="n">
         <f aca="false">D97/46.75</f>
-        <v>109.903743315508</v>
+        <v>127.957219251337</v>
       </c>
       <c r="F97" s="12" t="n">
-        <v>773</v>
+        <v>844</v>
       </c>
       <c r="G97" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H97" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,G97)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I97" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J97" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$94,I97)</f>
+        <f aca="false">_xlfn.DAYS(B$106,I97)</f>
         <v>4</v>
       </c>
       <c r="K97" s="13" t="n">
         <f aca="false">$B$94+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L97" s="0"/>
       <c r="M97" s="0"/>
@@ -3534,32 +3561,32 @@
         <v>330</v>
       </c>
       <c r="D98" s="1" t="n">
-        <v>1995</v>
+        <v>2314</v>
       </c>
       <c r="E98" s="12" t="n">
         <f aca="false">D98/65.27</f>
-        <v>30.5653439558756</v>
+        <v>35.4527347939329</v>
       </c>
       <c r="F98" s="12" t="n">
-        <v>299</v>
+        <v>319</v>
       </c>
       <c r="G98" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H98" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,G98)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I98" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J98" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$94,I98)</f>
+        <f aca="false">_xlfn.DAYS(B$106,I98)</f>
         <v>3</v>
       </c>
       <c r="K98" s="13" t="n">
         <f aca="false">$B$94+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L98" s="0"/>
       <c r="M98" s="0"/>
@@ -3576,34 +3603,33 @@
         <v>1660</v>
       </c>
       <c r="D99" s="1" t="n">
-        <v>1696</v>
+        <v>2221</v>
       </c>
       <c r="E99" s="12" t="n">
         <f aca="false">D99/331</f>
-        <v>5.12386706948641</v>
+        <v>6.70996978851964</v>
       </c>
       <c r="F99" s="12" t="n">
-        <v>400</v>
+        <v>525</v>
       </c>
       <c r="G99" s="13" t="n">
-        <f aca="false">$B$94</f>
         <v>43917</v>
       </c>
       <c r="H99" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,G99)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I99" s="13" t="n">
         <f aca="false">$B$94+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="J99" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$94,I99)</f>
+        <f aca="false">_xlfn.DAYS($B$94,I99)</f>
         <v>-1</v>
       </c>
       <c r="K99" s="13" t="n">
         <f aca="false">$B$94+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L99" s="0"/>
       <c r="M99" s="0"/>
@@ -3620,33 +3646,33 @@
         <v>330</v>
       </c>
       <c r="D100" s="1" t="n">
-        <v>759</v>
+        <v>1019</v>
       </c>
       <c r="E100" s="12" t="n">
         <f aca="false">D100/67.79</f>
-        <v>11.1963416433102</v>
+        <v>15.0317155922702</v>
       </c>
       <c r="F100" s="12" t="n">
-        <v>181</v>
+        <v>260</v>
       </c>
       <c r="G100" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H100" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,G100)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I100" s="13" t="n">
         <f aca="false">$B$94+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="J100" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$94,I100)</f>
+        <f aca="false">_xlfn.DAYS($B$94,I100)</f>
         <v>-1</v>
       </c>
       <c r="K100" s="13" t="n">
         <f aca="false">$B$94+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L100" s="0"/>
       <c r="M100" s="0"/>
@@ -3663,34 +3689,33 @@
         <v>414</v>
       </c>
       <c r="D101" s="1" t="n">
-        <v>351</v>
+        <v>433</v>
       </c>
       <c r="E101" s="12" t="n">
         <f aca="false">D101/83.784</f>
-        <v>4.18934402749928</v>
+        <v>5.16805117922276</v>
       </c>
       <c r="F101" s="12" t="n">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G101" s="13" t="n">
-        <f aca="false">$B$94+1</f>
         <v>43918</v>
       </c>
       <c r="H101" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,G101)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="I101" s="13" t="n">
         <f aca="false">$B$94+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="J101" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$94,I101)</f>
+        <f aca="false">_xlfn.DAYS($B$94,I101)</f>
         <v>-1</v>
       </c>
       <c r="K101" s="13" t="n">
         <f aca="false">$B$94+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L101" s="0"/>
       <c r="M101" s="0"/>
@@ -3714,26 +3739,26 @@
         <v>10.1351351351351</v>
       </c>
       <c r="F102" s="12" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="G102" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H102" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,G102)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I102" s="13" t="n">
         <f aca="false">$B$94+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="J102" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$94,I102)</f>
+        <f aca="false">_xlfn.DAYS($B$94,I102)</f>
         <v>-1</v>
       </c>
       <c r="K102" s="13" t="n">
         <f aca="false">$B$94+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L102" s="0"/>
       <c r="M102" s="0"/>
@@ -3743,14 +3768,15 @@
       <c r="Q102" s="0"/>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D103" s="0"/>
-      <c r="E103" s="0"/>
-      <c r="F103" s="0"/>
-      <c r="G103" s="0"/>
+      <c r="C103" s="12"/>
+      <c r="D103" s="12"/>
+      <c r="E103" s="12"/>
+      <c r="F103" s="12"/>
+      <c r="G103" s="13"/>
       <c r="H103" s="0"/>
-      <c r="I103" s="0"/>
+      <c r="I103" s="13"/>
       <c r="J103" s="0"/>
-      <c r="K103" s="0"/>
+      <c r="K103" s="13"/>
       <c r="L103" s="0"/>
       <c r="M103" s="0"/>
       <c r="N103" s="0"/>
@@ -3759,6 +3785,8 @@
       <c r="Q103" s="0"/>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B104" s="4"/>
+      <c r="C104" s="5"/>
       <c r="D104" s="0"/>
       <c r="E104" s="0"/>
       <c r="F104" s="0"/>
@@ -3793,10 +3821,11 @@
       <c r="P105" s="0"/>
       <c r="Q105" s="0"/>
     </row>
-    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="7" t="n">
-        <v>43916</v>
-      </c>
+        <v>43917</v>
+      </c>
+      <c r="C106" s="0"/>
       <c r="D106" s="8" t="s">
         <v>6</v>
       </c>
@@ -3819,17 +3848,13 @@
       <c r="K106" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="L106" s="0"/>
-      <c r="M106" s="0"/>
-      <c r="N106" s="0"/>
-      <c r="O106" s="0"/>
-      <c r="P106" s="0"/>
-      <c r="Q106" s="0"/>
+      <c r="L106" s="8"/>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="3"/>
       <c r="B107" s="9"/>
       <c r="C107" s="10" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="D107" s="10" t="s">
         <v>2</v>
@@ -3855,7 +3880,7 @@
       <c r="K107" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L107" s="0"/>
+      <c r="L107" s="8"/>
       <c r="M107" s="0"/>
       <c r="N107" s="0"/>
       <c r="O107" s="0"/>
@@ -3870,32 +3895,32 @@
         <v>300</v>
       </c>
       <c r="D108" s="1" t="n">
-        <v>8215</v>
+        <v>9134</v>
       </c>
       <c r="E108" s="12" t="n">
         <f aca="false">D108/60.48</f>
-        <v>135.830026455026</v>
+        <v>151.025132275132</v>
       </c>
       <c r="F108" s="12" t="n">
-        <v>712</v>
+        <v>919</v>
       </c>
       <c r="G108" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H108" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$106,G108)</f>
-        <v>16</v>
+        <f aca="false">_xlfn.DAYS($B$106,G108)</f>
+        <v>17</v>
       </c>
       <c r="I108" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J108" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$106,I108)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K108" s="13" t="n">
-        <f aca="false">B$106+1</f>
-        <v>43917</v>
+        <f aca="false">$B$106+1</f>
+        <v>43918</v>
       </c>
       <c r="L108" s="0"/>
       <c r="M108" s="0"/>
@@ -3912,32 +3937,32 @@
         <v>230</v>
       </c>
       <c r="D109" s="1" t="n">
-        <v>4365</v>
+        <v>5138</v>
       </c>
       <c r="E109" s="12" t="n">
         <f aca="false">D109/46.75</f>
-        <v>93.3689839572193</v>
+        <v>109.903743315508</v>
       </c>
       <c r="F109" s="12" t="n">
-        <v>718</v>
+        <v>773</v>
       </c>
       <c r="G109" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H109" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$106,G109)</f>
-        <v>9</v>
+        <f aca="false">_xlfn.DAYS($B$106,G109)</f>
+        <v>10</v>
       </c>
       <c r="I109" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J109" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$106,I109)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K109" s="13" t="n">
-        <f aca="false">B$106+1</f>
-        <v>43917</v>
+        <f aca="false">$B$106+1</f>
+        <v>43918</v>
       </c>
       <c r="L109" s="0"/>
       <c r="M109" s="0"/>
@@ -3954,32 +3979,32 @@
         <v>330</v>
       </c>
       <c r="D110" s="1" t="n">
-        <v>1696</v>
+        <v>1995</v>
       </c>
       <c r="E110" s="12" t="n">
         <f aca="false">D110/65.27</f>
-        <v>25.9843726060978</v>
+        <v>30.5653439558756</v>
       </c>
       <c r="F110" s="12" t="n">
-        <v>365</v>
+        <v>299</v>
       </c>
       <c r="G110" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H110" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$106,G110)</f>
-        <v>4</v>
+        <f aca="false">_xlfn.DAYS($B$106,G110)</f>
+        <v>5</v>
       </c>
       <c r="I110" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J110" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$106,I110)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K110" s="13" t="n">
-        <f aca="false">B$106+1</f>
-        <v>43917</v>
+        <f aca="false">$B$106+1</f>
+        <v>43918</v>
       </c>
       <c r="L110" s="0"/>
       <c r="M110" s="0"/>
@@ -3996,33 +4021,34 @@
         <v>1660</v>
       </c>
       <c r="D111" s="1" t="n">
-        <v>1295</v>
+        <v>1696</v>
       </c>
       <c r="E111" s="12" t="n">
         <f aca="false">D111/331</f>
-        <v>3.91238670694864</v>
+        <v>5.12386706948641</v>
       </c>
       <c r="F111" s="12" t="n">
-        <v>268</v>
+        <v>400</v>
       </c>
       <c r="G111" s="13" t="n">
+        <f aca="false">$B$106</f>
         <v>43917</v>
       </c>
       <c r="H111" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$106,G111)</f>
+        <f aca="false">_xlfn.DAYS($B$106,G111)</f>
+        <v>0</v>
+      </c>
+      <c r="I111" s="13" t="n">
+        <f aca="false">$B$106+1</f>
+        <v>43918</v>
+      </c>
+      <c r="J111" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$106,I111)</f>
         <v>-1</v>
       </c>
-      <c r="I111" s="13" t="n">
-        <f aca="false">B$106+1</f>
-        <v>43917</v>
-      </c>
-      <c r="J111" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$106,I111)</f>
-        <v>-1</v>
-      </c>
       <c r="K111" s="13" t="n">
-        <f aca="false">B$106+1</f>
-        <v>43917</v>
+        <f aca="false">$B$106+1</f>
+        <v>43918</v>
       </c>
       <c r="L111" s="0"/>
       <c r="M111" s="0"/>
@@ -4039,33 +4065,33 @@
         <v>330</v>
       </c>
       <c r="D112" s="1" t="n">
-        <v>578</v>
+        <v>759</v>
       </c>
       <c r="E112" s="12" t="n">
         <f aca="false">D112/67.79</f>
-        <v>8.52633131730344</v>
+        <v>11.1963416433102</v>
       </c>
       <c r="F112" s="12" t="n">
-        <v>115</v>
+        <v>181</v>
       </c>
       <c r="G112" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H112" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$106,G112)</f>
-        <v>0</v>
+        <f aca="false">_xlfn.DAYS($B$106,G112)</f>
+        <v>1</v>
       </c>
       <c r="I112" s="13" t="n">
-        <f aca="false">B$106+1</f>
-        <v>43917</v>
+        <f aca="false">$B$106+1</f>
+        <v>43918</v>
       </c>
       <c r="J112" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$106,I112)</f>
         <v>-1</v>
       </c>
       <c r="K112" s="13" t="n">
-        <f aca="false">B$106+1</f>
-        <v>43917</v>
+        <f aca="false">$B$106+1</f>
+        <v>43918</v>
       </c>
       <c r="L112" s="0"/>
       <c r="M112" s="0"/>
@@ -4082,33 +4108,34 @@
         <v>414</v>
       </c>
       <c r="D113" s="1" t="n">
-        <v>267</v>
+        <v>351</v>
       </c>
       <c r="E113" s="12" t="n">
         <f aca="false">D113/83.784</f>
-        <v>3.18676596963621</v>
+        <v>4.18934402749928</v>
       </c>
       <c r="F113" s="12" t="n">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="G113" s="13" t="n">
-        <v>43917</v>
+        <f aca="false">$B$106+1</f>
+        <v>43918</v>
       </c>
       <c r="H113" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$106,G113)</f>
+        <f aca="false">_xlfn.DAYS($B$106,G113)</f>
         <v>-1</v>
       </c>
       <c r="I113" s="13" t="n">
-        <f aca="false">B$106+1</f>
-        <v>43917</v>
+        <f aca="false">$B$106+1</f>
+        <v>43918</v>
       </c>
       <c r="J113" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$106,I113)</f>
         <v>-1</v>
       </c>
       <c r="K113" s="13" t="n">
-        <f aca="false">B$106+1</f>
-        <v>43917</v>
+        <f aca="false">$B$106+1</f>
+        <v>43918</v>
       </c>
       <c r="L113" s="0"/>
       <c r="M113" s="0"/>
@@ -4125,33 +4152,33 @@
         <v>50</v>
       </c>
       <c r="D114" s="12" t="n">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="E114" s="12" t="n">
         <f aca="false">D114/10.36</f>
-        <v>7.43243243243243</v>
+        <v>10.1351351351351</v>
       </c>
       <c r="F114" s="12" t="n">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="G114" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H114" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$106,G114)</f>
-        <v>1</v>
+        <f aca="false">_xlfn.DAYS($B$106,G114)</f>
+        <v>2</v>
       </c>
       <c r="I114" s="13" t="n">
-        <f aca="false">B$106+1</f>
-        <v>43917</v>
+        <f aca="false">$B$106+1</f>
+        <v>43918</v>
       </c>
       <c r="J114" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$106,I114)</f>
         <v>-1</v>
       </c>
       <c r="K114" s="13" t="n">
-        <f aca="false">B$106+1</f>
-        <v>43917</v>
+        <f aca="false">$B$106+1</f>
+        <v>43918</v>
       </c>
       <c r="L114" s="0"/>
       <c r="M114" s="0"/>
@@ -4159,6 +4186,424 @@
       <c r="O114" s="0"/>
       <c r="P114" s="0"/>
       <c r="Q114" s="0"/>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D115" s="0"/>
+      <c r="E115" s="0"/>
+      <c r="F115" s="0"/>
+      <c r="G115" s="0"/>
+      <c r="H115" s="0"/>
+      <c r="I115" s="0"/>
+      <c r="J115" s="0"/>
+      <c r="K115" s="0"/>
+      <c r="L115" s="0"/>
+      <c r="M115" s="0"/>
+      <c r="N115" s="0"/>
+      <c r="O115" s="0"/>
+      <c r="P115" s="0"/>
+      <c r="Q115" s="0"/>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D116" s="0"/>
+      <c r="E116" s="0"/>
+      <c r="F116" s="0"/>
+      <c r="G116" s="0"/>
+      <c r="H116" s="0"/>
+      <c r="I116" s="0"/>
+      <c r="J116" s="0"/>
+      <c r="K116" s="0"/>
+      <c r="L116" s="0"/>
+      <c r="M116" s="0"/>
+      <c r="N116" s="0"/>
+      <c r="O116" s="0"/>
+      <c r="P116" s="0"/>
+      <c r="Q116" s="0"/>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B117" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D117" s="0"/>
+      <c r="E117" s="0"/>
+      <c r="F117" s="0"/>
+      <c r="G117" s="0"/>
+      <c r="H117" s="0"/>
+      <c r="I117" s="0"/>
+      <c r="J117" s="0"/>
+      <c r="K117" s="0"/>
+      <c r="L117" s="0"/>
+      <c r="M117" s="0"/>
+      <c r="N117" s="0"/>
+      <c r="O117" s="0"/>
+      <c r="P117" s="0"/>
+      <c r="Q117" s="0"/>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B118" s="7" t="n">
+        <v>43916</v>
+      </c>
+      <c r="D118" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E118" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F118" s="8"/>
+      <c r="G118" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H118" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I118" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="J118" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K118" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="L118" s="0"/>
+      <c r="M118" s="0"/>
+      <c r="N118" s="0"/>
+      <c r="O118" s="0"/>
+      <c r="P118" s="0"/>
+      <c r="Q118" s="0"/>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B119" s="9"/>
+      <c r="C119" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D119" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E119" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F119" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G119" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H119" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I119" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="J119" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K119" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L119" s="0"/>
+      <c r="M119" s="0"/>
+      <c r="N119" s="0"/>
+      <c r="O119" s="0"/>
+      <c r="P119" s="0"/>
+      <c r="Q119" s="0"/>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B120" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C120" s="12" t="n">
+        <v>300</v>
+      </c>
+      <c r="D120" s="1" t="n">
+        <v>8215</v>
+      </c>
+      <c r="E120" s="12" t="n">
+        <f aca="false">D120/60.48</f>
+        <v>135.830026455026</v>
+      </c>
+      <c r="F120" s="12" t="n">
+        <v>712</v>
+      </c>
+      <c r="G120" s="13" t="n">
+        <v>43900</v>
+      </c>
+      <c r="H120" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$118,G120)</f>
+        <v>16</v>
+      </c>
+      <c r="I120" s="13" t="n">
+        <v>43902</v>
+      </c>
+      <c r="J120" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$118,I120)</f>
+        <v>14</v>
+      </c>
+      <c r="K120" s="13" t="n">
+        <f aca="false">B$118+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L120" s="0"/>
+      <c r="M120" s="0"/>
+      <c r="N120" s="0"/>
+      <c r="O120" s="0"/>
+      <c r="P120" s="0"/>
+      <c r="Q120" s="0"/>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B121" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C121" s="12" t="n">
+        <v>230</v>
+      </c>
+      <c r="D121" s="1" t="n">
+        <v>4365</v>
+      </c>
+      <c r="E121" s="12" t="n">
+        <f aca="false">D121/46.75</f>
+        <v>93.3689839572193</v>
+      </c>
+      <c r="F121" s="12" t="n">
+        <v>718</v>
+      </c>
+      <c r="G121" s="13" t="n">
+        <v>43907</v>
+      </c>
+      <c r="H121" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$118,G121)</f>
+        <v>9</v>
+      </c>
+      <c r="I121" s="13" t="n">
+        <v>43913</v>
+      </c>
+      <c r="J121" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$118,I121)</f>
+        <v>3</v>
+      </c>
+      <c r="K121" s="13" t="n">
+        <f aca="false">B$118+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L121" s="0"/>
+      <c r="M121" s="0"/>
+      <c r="N121" s="0"/>
+      <c r="O121" s="0"/>
+      <c r="P121" s="0"/>
+      <c r="Q121" s="0"/>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B122" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C122" s="12" t="n">
+        <v>330</v>
+      </c>
+      <c r="D122" s="1" t="n">
+        <v>1696</v>
+      </c>
+      <c r="E122" s="12" t="n">
+        <f aca="false">D122/65.27</f>
+        <v>25.9843726060978</v>
+      </c>
+      <c r="F122" s="12" t="n">
+        <v>365</v>
+      </c>
+      <c r="G122" s="13" t="n">
+        <v>43912</v>
+      </c>
+      <c r="H122" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$118,G122)</f>
+        <v>4</v>
+      </c>
+      <c r="I122" s="13" t="n">
+        <v>43914</v>
+      </c>
+      <c r="J122" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$118,I122)</f>
+        <v>2</v>
+      </c>
+      <c r="K122" s="13" t="n">
+        <f aca="false">B$118+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L122" s="0"/>
+      <c r="M122" s="0"/>
+      <c r="N122" s="0"/>
+      <c r="O122" s="0"/>
+      <c r="P122" s="0"/>
+      <c r="Q122" s="0"/>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B123" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C123" s="12" t="n">
+        <v>1660</v>
+      </c>
+      <c r="D123" s="1" t="n">
+        <v>1295</v>
+      </c>
+      <c r="E123" s="12" t="n">
+        <f aca="false">D123/331</f>
+        <v>3.91238670694864</v>
+      </c>
+      <c r="F123" s="12" t="n">
+        <v>268</v>
+      </c>
+      <c r="G123" s="13" t="n">
+        <v>43917</v>
+      </c>
+      <c r="H123" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$118,G123)</f>
+        <v>-1</v>
+      </c>
+      <c r="I123" s="13" t="n">
+        <f aca="false">B$118+1</f>
+        <v>43917</v>
+      </c>
+      <c r="J123" s="1" t="n">
+        <f aca="false">_xlfn.DAYS($B$118,I123)</f>
+        <v>-1</v>
+      </c>
+      <c r="K123" s="13" t="n">
+        <f aca="false">B$118+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L123" s="0"/>
+      <c r="M123" s="0"/>
+      <c r="N123" s="0"/>
+      <c r="O123" s="0"/>
+      <c r="P123" s="0"/>
+      <c r="Q123" s="0"/>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B124" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C124" s="12" t="n">
+        <v>330</v>
+      </c>
+      <c r="D124" s="1" t="n">
+        <v>578</v>
+      </c>
+      <c r="E124" s="12" t="n">
+        <f aca="false">D124/67.79</f>
+        <v>8.52633131730344</v>
+      </c>
+      <c r="F124" s="12" t="n">
+        <v>115</v>
+      </c>
+      <c r="G124" s="13" t="n">
+        <v>43916</v>
+      </c>
+      <c r="H124" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$118,G124)</f>
+        <v>0</v>
+      </c>
+      <c r="I124" s="13" t="n">
+        <f aca="false">B$118+1</f>
+        <v>43917</v>
+      </c>
+      <c r="J124" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$118,I124)</f>
+        <v>-1</v>
+      </c>
+      <c r="K124" s="13" t="n">
+        <f aca="false">B$118+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L124" s="0"/>
+      <c r="M124" s="0"/>
+      <c r="N124" s="0"/>
+      <c r="O124" s="0"/>
+      <c r="P124" s="0"/>
+      <c r="Q124" s="0"/>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B125" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C125" s="12" t="n">
+        <v>414</v>
+      </c>
+      <c r="D125" s="1" t="n">
+        <v>267</v>
+      </c>
+      <c r="E125" s="12" t="n">
+        <f aca="false">D125/83.784</f>
+        <v>3.18676596963621</v>
+      </c>
+      <c r="F125" s="12" t="n">
+        <v>61</v>
+      </c>
+      <c r="G125" s="13" t="n">
+        <v>43917</v>
+      </c>
+      <c r="H125" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$118,G125)</f>
+        <v>-1</v>
+      </c>
+      <c r="I125" s="13" t="n">
+        <f aca="false">B$118+1</f>
+        <v>43917</v>
+      </c>
+      <c r="J125" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$118,I125)</f>
+        <v>-1</v>
+      </c>
+      <c r="K125" s="13" t="n">
+        <f aca="false">B$118+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L125" s="0"/>
+      <c r="M125" s="0"/>
+      <c r="N125" s="0"/>
+      <c r="O125" s="0"/>
+      <c r="P125" s="0"/>
+      <c r="Q125" s="0"/>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B126" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C126" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="D126" s="12" t="n">
+        <v>77</v>
+      </c>
+      <c r="E126" s="12" t="n">
+        <f aca="false">D126/10.36</f>
+        <v>7.43243243243243</v>
+      </c>
+      <c r="F126" s="12" t="n">
+        <v>15</v>
+      </c>
+      <c r="G126" s="13" t="n">
+        <v>43915</v>
+      </c>
+      <c r="H126" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$118,G126)</f>
+        <v>1</v>
+      </c>
+      <c r="I126" s="13" t="n">
+        <f aca="false">B$118+1</f>
+        <v>43917</v>
+      </c>
+      <c r="J126" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$118,I126)</f>
+        <v>-1</v>
+      </c>
+      <c r="K126" s="13" t="n">
+        <f aca="false">B$118+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L126" s="0"/>
+      <c r="M126" s="0"/>
+      <c r="N126" s="0"/>
+      <c r="O126" s="0"/>
+      <c r="P126" s="0"/>
+      <c r="Q126" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
updated with 2020-04-04 available data
</commit_message>
<xml_diff>
--- a/covid19 lockdown evaluation .xlsx
+++ b/covid19 lockdown evaluation .xlsx
@@ -15,12 +15,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="53">
   <si>
     <t>Effects of the lockdown issued by governments</t>
   </si>
   <si>
+    <t>notes:</t>
+  </si>
+  <si>
+    <t>0n Apr, 5th, data for USA changed: malues for 2, 3 was:  6071, 7232 – they becomes:  6076, 7121</t>
+  </si>
+  <si>
+    <t>6071, </t>
+  </si>
+  <si>
     <t>LEGENDA</t>
+  </si>
+  <si>
+    <t>- - - -&gt;  death todays was 969, 1321 - now: 974, 1045</t>
   </si>
   <si>
     <t>today</t>
@@ -267,7 +279,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -324,6 +336,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -341,9 +357,9 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q126"/>
+  <dimension ref="A1:Q138"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F31" activeCellId="0" sqref="F31"/>
     </sheetView>
   </sheetViews>
@@ -398,19 +414,25 @@
       <c r="F3" s="0"/>
       <c r="G3" s="0"/>
       <c r="H3" s="0"/>
-      <c r="I3" s="0"/>
-      <c r="J3" s="0"/>
+      <c r="I3" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>2</v>
+      </c>
       <c r="K3" s="0"/>
       <c r="L3" s="0"/>
       <c r="M3" s="0"/>
-      <c r="N3" s="0"/>
+      <c r="N3" s="0" t="s">
+        <v>3</v>
+      </c>
       <c r="O3" s="0"/>
       <c r="P3" s="0"/>
       <c r="Q3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D4" s="0"/>
       <c r="E4" s="0"/>
@@ -418,7 +440,9 @@
       <c r="G4" s="0"/>
       <c r="H4" s="0"/>
       <c r="I4" s="0"/>
-      <c r="J4" s="0"/>
+      <c r="J4" s="0" t="s">
+        <v>5</v>
+      </c>
       <c r="K4" s="0"/>
       <c r="L4" s="0"/>
       <c r="M4" s="0"/>
@@ -429,10 +453,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="4" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D5" s="0"/>
       <c r="E5" s="0"/>
@@ -451,10 +475,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="4" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D6" s="0"/>
       <c r="E6" s="0"/>
@@ -473,10 +497,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D7" s="0"/>
       <c r="E7" s="0"/>
@@ -495,10 +519,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D8" s="0"/>
       <c r="E8" s="0"/>
@@ -517,10 +541,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D9" s="0"/>
       <c r="E9" s="0"/>
@@ -539,10 +563,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D10" s="0"/>
       <c r="E10" s="0"/>
@@ -561,10 +585,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D11" s="0"/>
       <c r="E11" s="0"/>
@@ -583,10 +607,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D12" s="0"/>
       <c r="E12" s="0"/>
@@ -605,10 +629,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D13" s="0"/>
       <c r="E13" s="0"/>
@@ -627,10 +651,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D14" s="0"/>
       <c r="E14" s="0"/>
@@ -649,10 +673,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D15" s="0"/>
       <c r="E15" s="0"/>
@@ -688,10 +712,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D17" s="0"/>
       <c r="E17" s="0"/>
@@ -711,7 +735,7 @@
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="4"/>
       <c r="C18" s="5" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D18" s="0"/>
       <c r="E18" s="0"/>
@@ -766,7 +790,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="6" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D21" s="0"/>
       <c r="E21" s="0"/>
@@ -785,30 +809,30 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="7" t="n">
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="D22" s="0"/>
       <c r="E22" s="8" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F22" s="0"/>
       <c r="G22" s="8" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="K22" s="8" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="M22" s="0"/>
       <c r="N22" s="0"/>
@@ -819,34 +843,34 @@
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="9"/>
       <c r="C23" s="10" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="I23" s="11" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="J23" s="8" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="K23" s="8" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="M23" s="0"/>
       <c r="N23" s="0"/>
@@ -856,42 +880,42 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C24" s="12" t="n">
         <v>300</v>
       </c>
       <c r="D24" s="1" t="n">
-        <v>14681</v>
+        <v>15362</v>
       </c>
       <c r="E24" s="12" t="n">
         <f aca="false">D24/60.48</f>
-        <v>242.741402116402</v>
+        <v>254.001322751323</v>
       </c>
       <c r="F24" s="12" t="n">
-        <v>766</v>
+        <v>681</v>
       </c>
       <c r="G24" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H24" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,G24)</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I24" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J24" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I24)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K24" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="L24" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K24,G24)</f>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M24" s="0"/>
       <c r="N24" s="0"/>
@@ -901,42 +925,42 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C25" s="12" t="n">
         <v>230</v>
       </c>
       <c r="D25" s="1" t="n">
-        <v>11198</v>
+        <v>11947</v>
       </c>
       <c r="E25" s="12" t="n">
         <f aca="false">D25/46.75</f>
-        <v>239.529411764706</v>
+        <v>255.550802139037</v>
       </c>
       <c r="F25" s="12" t="n">
-        <v>850</v>
+        <v>749</v>
       </c>
       <c r="G25" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H25" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$34,G25)</f>
-        <v>16</v>
+        <f aca="false">_xlfn.DAYS($B$22,G25)</f>
+        <v>18</v>
       </c>
       <c r="I25" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J25" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I25)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K25" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="L25" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K25,G25)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M25" s="0"/>
       <c r="N25" s="0"/>
@@ -946,42 +970,42 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C26" s="12" t="n">
         <v>330</v>
       </c>
       <c r="D26" s="1" t="n">
-        <v>6507</v>
+        <v>7560</v>
       </c>
       <c r="E26" s="12" t="n">
         <f aca="false">D26/65.27</f>
-        <v>99.6935805117206</v>
+        <v>115.826566569634</v>
       </c>
       <c r="F26" s="12" t="n">
-        <v>1120</v>
+        <v>1053</v>
       </c>
       <c r="G26" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H26" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$34,G26)</f>
-        <v>11</v>
+        <f aca="false">_xlfn.DAYS($B$22,G26)</f>
+        <v>13</v>
       </c>
       <c r="I26" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J26" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I26)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K26" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="L26" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K26,G26)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="M26" s="0"/>
       <c r="N26" s="0"/>
@@ -991,43 +1015,43 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C27" s="12" t="n">
         <v>50</v>
       </c>
       <c r="D27" s="12" t="n">
-        <v>358</v>
+        <v>373</v>
       </c>
       <c r="E27" s="12" t="n">
         <f aca="false">D27/10.36</f>
-        <v>34.5559845559846</v>
+        <v>36.003861003861</v>
       </c>
       <c r="F27" s="12" t="n">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="G27" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H27" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$34,G27)</f>
-        <v>8</v>
+        <f aca="false">_xlfn.DAYS($B$22,G27)</f>
+        <v>10</v>
       </c>
       <c r="I27" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43925</v>
-      </c>
-      <c r="J27" s="1" t="n">
+        <v>43926</v>
+      </c>
+      <c r="J27" s="14" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I27)</f>
         <v>-1</v>
       </c>
       <c r="K27" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="L27" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K27,G27)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M27" s="0"/>
       <c r="N27" s="0"/>
@@ -1037,43 +1061,43 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C28" s="12" t="n">
         <v>330</v>
       </c>
       <c r="D28" s="1" t="n">
-        <v>3605</v>
+        <v>4313</v>
       </c>
       <c r="E28" s="12" t="n">
         <f aca="false">D28/67.79</f>
-        <v>53.1789349461573</v>
+        <v>63.6229532379407</v>
       </c>
       <c r="F28" s="12" t="n">
-        <v>684</v>
+        <v>708</v>
       </c>
       <c r="G28" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H28" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$34,G28)</f>
-        <v>7</v>
+        <f aca="false">_xlfn.DAYS($B$22,G28)</f>
+        <v>9</v>
       </c>
       <c r="I28" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43925</v>
-      </c>
-      <c r="J28" s="1" t="n">
+        <v>43926</v>
+      </c>
+      <c r="J28" s="14" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I28)</f>
         <v>-1</v>
       </c>
       <c r="K28" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="L28" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K28,G28)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M28" s="0"/>
       <c r="N28" s="0"/>
@@ -1083,43 +1107,43 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C29" s="12" t="n">
         <v>1660</v>
       </c>
       <c r="D29" s="1" t="n">
-        <v>7392</v>
+        <v>8452</v>
       </c>
       <c r="E29" s="12" t="n">
         <f aca="false">D29/331</f>
-        <v>22.3323262839879</v>
+        <v>25.5347432024169</v>
       </c>
       <c r="F29" s="12" t="n">
-        <v>1321</v>
+        <v>1331</v>
       </c>
       <c r="G29" s="13" t="n">
         <v>43917</v>
       </c>
       <c r="H29" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$34,G29)</f>
-        <v>6</v>
+        <f aca="false">_xlfn.DAYS($B$22,G29)</f>
+        <v>8</v>
       </c>
       <c r="I29" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43925</v>
-      </c>
-      <c r="J29" s="1" t="n">
+        <v>43926</v>
+      </c>
+      <c r="J29" s="14" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I29)</f>
         <v>-1</v>
       </c>
       <c r="K29" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="L29" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K29,G29)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M29" s="0"/>
       <c r="N29" s="0"/>
@@ -1129,43 +1153,43 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C30" s="12" t="n">
         <v>414</v>
       </c>
       <c r="D30" s="1" t="n">
-        <v>1275</v>
+        <v>1444</v>
       </c>
       <c r="E30" s="12" t="n">
         <f aca="false">D30/83.784</f>
-        <v>15.2177026639931</v>
+        <v>17.2347942327891</v>
       </c>
       <c r="F30" s="12" t="n">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G30" s="13" t="n">
         <v>43918</v>
       </c>
       <c r="H30" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$34,G30)</f>
-        <v>5</v>
+        <f aca="false">_xlfn.DAYS($B$22,G30)</f>
+        <v>7</v>
       </c>
       <c r="I30" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43925</v>
-      </c>
-      <c r="J30" s="1" t="n">
+        <v>43926</v>
+      </c>
+      <c r="J30" s="14" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I30)</f>
         <v>-1</v>
       </c>
       <c r="K30" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="L30" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K30,G30)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M30" s="0"/>
       <c r="N30" s="0"/>
@@ -1211,7 +1235,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="6" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D33" s="0"/>
       <c r="E33" s="0"/>
@@ -1230,30 +1254,30 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="7" t="n">
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="D34" s="0"/>
       <c r="E34" s="8" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F34" s="0"/>
       <c r="G34" s="8" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="J34" s="8" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="K34" s="8" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="L34" s="8" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="M34" s="0"/>
       <c r="N34" s="0"/>
@@ -1264,34 +1288,34 @@
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="9"/>
       <c r="C35" s="10" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="G35" s="11" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="I35" s="11" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="J35" s="8" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="K35" s="8" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="L35" s="8" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="M35" s="0"/>
       <c r="N35" s="0"/>
@@ -1301,42 +1325,42 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C36" s="12" t="n">
         <v>300</v>
       </c>
       <c r="D36" s="1" t="n">
-        <v>13915</v>
+        <v>14681</v>
       </c>
       <c r="E36" s="12" t="n">
         <f aca="false">D36/60.48</f>
-        <v>230.076058201058</v>
+        <v>242.741402116402</v>
       </c>
       <c r="F36" s="12" t="n">
-        <v>760</v>
+        <v>766</v>
       </c>
       <c r="G36" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H36" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,G36)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I36" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J36" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I36)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K36" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="L36" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K36,G36)</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M36" s="0"/>
       <c r="N36" s="0"/>
@@ -1346,26 +1370,26 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C37" s="12" t="n">
         <v>230</v>
       </c>
       <c r="D37" s="1" t="n">
-        <v>10348</v>
+        <v>11198</v>
       </c>
       <c r="E37" s="12" t="n">
         <f aca="false">D37/46.75</f>
-        <v>221.347593582888</v>
+        <v>239.529411764706</v>
       </c>
       <c r="F37" s="12" t="n">
-        <v>961</v>
+        <v>850</v>
       </c>
       <c r="G37" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H37" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$34,G37)</f>
+        <f aca="false">_xlfn.DAYS($B$46,G37)</f>
         <v>16</v>
       </c>
       <c r="I37" s="13" t="n">
@@ -1373,15 +1397,15 @@
       </c>
       <c r="J37" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I37)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K37" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="L37" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K37,G37)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M37" s="0"/>
       <c r="N37" s="0"/>
@@ -1391,26 +1415,26 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C38" s="12" t="n">
         <v>330</v>
       </c>
       <c r="D38" s="1" t="n">
-        <v>5387</v>
+        <v>6507</v>
       </c>
       <c r="E38" s="12" t="n">
         <f aca="false">D38/65.27</f>
-        <v>82.5340891680711</v>
+        <v>99.6935805117206</v>
       </c>
       <c r="F38" s="12" t="n">
-        <v>1355</v>
+        <v>1120</v>
       </c>
       <c r="G38" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H38" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$34,G38)</f>
+        <f aca="false">_xlfn.DAYS($B$46,G38)</f>
         <v>11</v>
       </c>
       <c r="I38" s="13" t="n">
@@ -1418,15 +1442,15 @@
       </c>
       <c r="J38" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I38)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K38" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="L38" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K38,G38)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M38" s="0"/>
       <c r="N38" s="0"/>
@@ -1436,31 +1460,31 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C39" s="12" t="n">
         <v>50</v>
       </c>
       <c r="D39" s="12" t="n">
-        <v>308</v>
+        <v>358</v>
       </c>
       <c r="E39" s="12" t="n">
         <f aca="false">D39/10.36</f>
-        <v>29.7297297297297</v>
+        <v>34.5559845559846</v>
       </c>
       <c r="F39" s="12" t="n">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="G39" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H39" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$34,G39)</f>
+        <f aca="false">_xlfn.DAYS($B$46,G39)</f>
         <v>8</v>
       </c>
       <c r="I39" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="J39" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I39)</f>
@@ -1468,11 +1492,11 @@
       </c>
       <c r="K39" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="L39" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K39,G39)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M39" s="0"/>
       <c r="N39" s="0"/>
@@ -1482,31 +1506,31 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C40" s="12" t="n">
         <v>330</v>
       </c>
       <c r="D40" s="1" t="n">
-        <v>2921</v>
+        <v>3605</v>
       </c>
       <c r="E40" s="12" t="n">
         <f aca="false">D40/67.79</f>
-        <v>43.0889511727393</v>
+        <v>53.1789349461573</v>
       </c>
       <c r="F40" s="12" t="n">
-        <v>569</v>
+        <v>684</v>
       </c>
       <c r="G40" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H40" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$34,G40)</f>
+        <f aca="false">_xlfn.DAYS($B$46,G40)</f>
         <v>7</v>
       </c>
       <c r="I40" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="J40" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I40)</f>
@@ -1514,11 +1538,11 @@
       </c>
       <c r="K40" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="L40" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K40,G40)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M40" s="0"/>
       <c r="N40" s="0"/>
@@ -1528,31 +1552,31 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C41" s="12" t="n">
         <v>1660</v>
       </c>
       <c r="D41" s="1" t="n">
-        <v>6071</v>
+        <v>7121</v>
       </c>
       <c r="E41" s="12" t="n">
         <f aca="false">D41/331</f>
-        <v>18.3413897280967</v>
+        <v>21.5135951661631</v>
       </c>
       <c r="F41" s="12" t="n">
-        <v>969</v>
+        <v>1045</v>
       </c>
       <c r="G41" s="13" t="n">
         <v>43917</v>
       </c>
       <c r="H41" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$34,G41)</f>
+        <f aca="false">_xlfn.DAYS($B$46,G41)</f>
         <v>6</v>
       </c>
       <c r="I41" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="J41" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I41)</f>
@@ -1560,11 +1584,11 @@
       </c>
       <c r="K41" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="L41" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K41,G41)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M41" s="0"/>
       <c r="N41" s="0"/>
@@ -1574,31 +1598,31 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C42" s="12" t="n">
         <v>414</v>
       </c>
       <c r="D42" s="1" t="n">
-        <v>1107</v>
+        <v>1275</v>
       </c>
       <c r="E42" s="12" t="n">
         <f aca="false">D42/83.784</f>
-        <v>13.212546548267</v>
+        <v>15.2177026639931</v>
       </c>
       <c r="F42" s="12" t="n">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="G42" s="13" t="n">
         <v>43918</v>
       </c>
       <c r="H42" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$34,G42)</f>
+        <f aca="false">_xlfn.DAYS($B$46,G42)</f>
         <v>5</v>
       </c>
       <c r="I42" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="J42" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I42)</f>
@@ -1606,11 +1630,11 @@
       </c>
       <c r="K42" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="L42" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K42,G42)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M42" s="0"/>
       <c r="N42" s="0"/>
@@ -1656,7 +1680,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="6" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D45" s="0"/>
       <c r="E45" s="0"/>
@@ -1675,30 +1699,30 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="7" t="n">
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="D46" s="0"/>
       <c r="E46" s="8" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F46" s="0"/>
       <c r="G46" s="8" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H46" s="8" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="I46" s="8" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="J46" s="8" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="K46" s="8" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="L46" s="8" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="M46" s="0"/>
       <c r="N46" s="0"/>
@@ -1709,34 +1733,34 @@
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="9"/>
       <c r="C47" s="10" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="G47" s="11" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H47" s="8" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="I47" s="11" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="J47" s="8" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="K47" s="8" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="L47" s="8" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="M47" s="0"/>
       <c r="N47" s="0"/>
@@ -1746,42 +1770,42 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C48" s="12" t="n">
         <v>300</v>
       </c>
       <c r="D48" s="1" t="n">
-        <v>13155</v>
+        <v>13915</v>
       </c>
       <c r="E48" s="12" t="n">
         <f aca="false">D48/60.48</f>
-        <v>217.509920634921</v>
+        <v>230.076058201058</v>
       </c>
       <c r="F48" s="12" t="n">
-        <v>727</v>
+        <v>760</v>
       </c>
       <c r="G48" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H48" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,G48)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I48" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J48" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I48)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K48" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="L48" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K48,G48)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M48" s="0"/>
       <c r="N48" s="0"/>
@@ -1791,42 +1815,42 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C49" s="12" t="n">
         <v>230</v>
       </c>
       <c r="D49" s="1" t="n">
-        <v>9387</v>
+        <v>10348</v>
       </c>
       <c r="E49" s="12" t="n">
         <f aca="false">D49/46.75</f>
-        <v>200.791443850267</v>
+        <v>221.347593582888</v>
       </c>
       <c r="F49" s="12" t="n">
-        <v>923</v>
+        <v>961</v>
       </c>
       <c r="G49" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H49" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,G49)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I49" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J49" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I49)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K49" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="L49" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K49,G49)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M49" s="0"/>
       <c r="N49" s="0"/>
@@ -1836,42 +1860,42 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C50" s="12" t="n">
         <v>330</v>
       </c>
       <c r="D50" s="1" t="n">
-        <v>4032</v>
+        <v>5387</v>
       </c>
       <c r="E50" s="12" t="n">
         <f aca="false">D50/65.27</f>
-        <v>61.7741688371381</v>
+        <v>82.5340891680711</v>
       </c>
       <c r="F50" s="12" t="n">
-        <v>509</v>
+        <v>1355</v>
       </c>
       <c r="G50" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H50" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,G50)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I50" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J50" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I50)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K50" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="L50" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K50,G50)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M50" s="0"/>
       <c r="N50" s="0"/>
@@ -1881,31 +1905,31 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C51" s="12" t="n">
         <v>50</v>
       </c>
       <c r="D51" s="12" t="n">
-        <v>239</v>
+        <v>308</v>
       </c>
       <c r="E51" s="12" t="n">
         <f aca="false">D51/10.36</f>
-        <v>23.0694980694981</v>
+        <v>29.7297297297297</v>
       </c>
       <c r="F51" s="12" t="n">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="G51" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H51" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,G51)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I51" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="J51" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I51)</f>
@@ -1913,11 +1937,11 @@
       </c>
       <c r="K51" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="L51" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K51,G51)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M51" s="0"/>
       <c r="N51" s="0"/>
@@ -1927,31 +1951,31 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C52" s="12" t="n">
         <v>330</v>
       </c>
       <c r="D52" s="1" t="n">
-        <v>2352</v>
+        <v>2921</v>
       </c>
       <c r="E52" s="12" t="n">
         <f aca="false">D52/67.79</f>
-        <v>34.695382799823</v>
+        <v>43.0889511727393</v>
       </c>
       <c r="F52" s="12" t="n">
-        <v>563</v>
+        <v>569</v>
       </c>
       <c r="G52" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H52" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,G52)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I52" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="J52" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I52)</f>
@@ -1959,11 +1983,11 @@
       </c>
       <c r="K52" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="L52" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K52,G52)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M52" s="0"/>
       <c r="N52" s="0"/>
@@ -1973,31 +1997,31 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C53" s="12" t="n">
         <v>1660</v>
       </c>
       <c r="D53" s="1" t="n">
-        <v>5102</v>
+        <v>6076</v>
       </c>
       <c r="E53" s="12" t="n">
         <f aca="false">D53/331</f>
-        <v>15.4138972809668</v>
+        <v>18.3564954682779</v>
       </c>
       <c r="F53" s="12" t="n">
-        <v>1049</v>
+        <v>969</v>
       </c>
       <c r="G53" s="13" t="n">
         <v>43917</v>
       </c>
       <c r="H53" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,G53)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I53" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="J53" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I53)</f>
@@ -2005,11 +2029,11 @@
       </c>
       <c r="K53" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="L53" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K53,G53)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M53" s="0"/>
       <c r="N53" s="0"/>
@@ -2019,31 +2043,31 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C54" s="12" t="n">
         <v>414</v>
       </c>
       <c r="D54" s="1" t="n">
-        <v>931</v>
+        <v>1107</v>
       </c>
       <c r="E54" s="12" t="n">
         <f aca="false">D54/83.784</f>
-        <v>11.1119068079824</v>
+        <v>13.212546548267</v>
       </c>
       <c r="F54" s="12" t="n">
-        <v>156</v>
+        <v>176</v>
       </c>
       <c r="G54" s="13" t="n">
         <v>43918</v>
       </c>
       <c r="H54" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,G54)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I54" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="J54" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I54)</f>
@@ -2051,11 +2075,11 @@
       </c>
       <c r="K54" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="L54" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K54,G54)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M54" s="0"/>
       <c r="N54" s="0"/>
@@ -2101,7 +2125,7 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="6" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D57" s="0"/>
       <c r="E57" s="0"/>
@@ -2120,30 +2144,30 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="7" t="n">
-        <v>43921</v>
+        <v>43922</v>
       </c>
       <c r="D58" s="0"/>
       <c r="E58" s="8" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F58" s="0"/>
       <c r="G58" s="8" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H58" s="8" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="I58" s="8" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="J58" s="8" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="K58" s="8" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="L58" s="8" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="M58" s="0"/>
       <c r="N58" s="0"/>
@@ -2154,34 +2178,34 @@
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="9"/>
       <c r="C59" s="10" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E59" s="10" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F59" s="10" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="G59" s="11" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H59" s="8" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="I59" s="11" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="J59" s="8" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="K59" s="8" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="L59" s="8" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="M59" s="0"/>
       <c r="N59" s="0"/>
@@ -2191,42 +2215,42 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C60" s="12" t="n">
         <v>300</v>
       </c>
       <c r="D60" s="1" t="n">
-        <v>12428</v>
+        <v>13155</v>
       </c>
       <c r="E60" s="12" t="n">
         <f aca="false">D60/60.48</f>
-        <v>205.489417989418</v>
+        <v>217.509920634921</v>
       </c>
       <c r="F60" s="12" t="n">
-        <v>837</v>
+        <v>727</v>
       </c>
       <c r="G60" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H60" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,G60)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I60" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J60" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I60)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K60" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L60" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K60,G60)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M60" s="0"/>
       <c r="N60" s="0"/>
@@ -2236,42 +2260,42 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C61" s="12" t="n">
         <v>230</v>
       </c>
       <c r="D61" s="1" t="n">
-        <v>8464</v>
+        <v>9387</v>
       </c>
       <c r="E61" s="12" t="n">
         <f aca="false">D61/46.75</f>
-        <v>181.048128342246</v>
+        <v>200.791443850267</v>
       </c>
       <c r="F61" s="12" t="n">
-        <v>748</v>
+        <v>923</v>
       </c>
       <c r="G61" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H61" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,G61)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I61" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J61" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I61)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K61" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L61" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K61,G61)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M61" s="0"/>
       <c r="N61" s="0"/>
@@ -2281,42 +2305,42 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C62" s="12" t="n">
         <v>330</v>
       </c>
       <c r="D62" s="1" t="n">
-        <v>3523</v>
+        <v>4032</v>
       </c>
       <c r="E62" s="12" t="n">
         <f aca="false">D62/65.27</f>
-        <v>53.9757928604259</v>
+        <v>61.7741688371381</v>
       </c>
       <c r="F62" s="12" t="n">
-        <v>499</v>
+        <v>509</v>
       </c>
       <c r="G62" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H62" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,G62)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I62" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J62" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I62)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K62" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L62" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K62,G62)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M62" s="0"/>
       <c r="N62" s="0"/>
@@ -2326,31 +2350,31 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C63" s="12" t="n">
         <v>50</v>
       </c>
       <c r="D63" s="12" t="n">
-        <v>180</v>
+        <v>239</v>
       </c>
       <c r="E63" s="12" t="n">
         <f aca="false">D63/10.36</f>
-        <v>17.3745173745174</v>
+        <v>23.0694980694981</v>
       </c>
       <c r="F63" s="12" t="n">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="G63" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H63" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,G63)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I63" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="J63" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I63)</f>
@@ -2358,11 +2382,11 @@
       </c>
       <c r="K63" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L63" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K63,G63)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M63" s="0"/>
       <c r="N63" s="0"/>
@@ -2372,31 +2396,31 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C64" s="12" t="n">
         <v>330</v>
       </c>
       <c r="D64" s="1" t="n">
-        <v>1789</v>
+        <v>2352</v>
       </c>
       <c r="E64" s="12" t="n">
         <f aca="false">D64/67.79</f>
-        <v>26.390323056498</v>
+        <v>34.695382799823</v>
       </c>
       <c r="F64" s="12" t="n">
-        <v>381</v>
+        <v>563</v>
       </c>
       <c r="G64" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H64" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,G64)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I64" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="J64" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I64)</f>
@@ -2404,11 +2428,11 @@
       </c>
       <c r="K64" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L64" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K64,G64)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M64" s="0"/>
       <c r="N64" s="0"/>
@@ -2418,31 +2442,31 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C65" s="12" t="n">
         <v>1660</v>
       </c>
       <c r="D65" s="1" t="n">
-        <v>4053</v>
+        <v>5102</v>
       </c>
       <c r="E65" s="12" t="n">
         <f aca="false">D65/331</f>
-        <v>12.2447129909366</v>
+        <v>15.4138972809668</v>
       </c>
       <c r="F65" s="12" t="n">
-        <v>912</v>
+        <v>1049</v>
       </c>
       <c r="G65" s="13" t="n">
         <v>43917</v>
       </c>
       <c r="H65" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,G65)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I65" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="J65" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I65)</f>
@@ -2450,11 +2474,11 @@
       </c>
       <c r="K65" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L65" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K65,G65)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M65" s="0"/>
       <c r="N65" s="0"/>
@@ -2464,31 +2488,31 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C66" s="12" t="n">
         <v>414</v>
       </c>
       <c r="D66" s="1" t="n">
-        <v>775</v>
+        <v>931</v>
       </c>
       <c r="E66" s="12" t="n">
         <f aca="false">D66/83.784</f>
-        <v>9.24997612909386</v>
+        <v>11.1119068079824</v>
       </c>
       <c r="F66" s="12" t="n">
-        <v>130</v>
+        <v>156</v>
       </c>
       <c r="G66" s="13" t="n">
         <v>43918</v>
       </c>
       <c r="H66" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,G66)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I66" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="J66" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I66)</f>
@@ -2496,11 +2520,11 @@
       </c>
       <c r="K66" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L66" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K66,G66)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M66" s="0"/>
       <c r="N66" s="0"/>
@@ -2509,15 +2533,16 @@
       <c r="Q66" s="0"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C67" s="12"/>
+      <c r="B67" s="4"/>
+      <c r="C67" s="5"/>
       <c r="D67" s="0"/>
-      <c r="E67" s="12"/>
-      <c r="F67" s="12"/>
-      <c r="G67" s="13"/>
+      <c r="E67" s="0"/>
+      <c r="F67" s="0"/>
+      <c r="G67" s="0"/>
       <c r="H67" s="0"/>
-      <c r="I67" s="13"/>
+      <c r="I67" s="0"/>
       <c r="J67" s="0"/>
-      <c r="K67" s="13"/>
+      <c r="K67" s="0"/>
       <c r="L67" s="0"/>
       <c r="M67" s="0"/>
       <c r="N67" s="0"/>
@@ -2526,15 +2551,16 @@
       <c r="Q67" s="0"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C68" s="12"/>
+      <c r="B68" s="4"/>
+      <c r="C68" s="5"/>
       <c r="D68" s="0"/>
-      <c r="E68" s="12"/>
-      <c r="F68" s="12"/>
-      <c r="G68" s="13"/>
+      <c r="E68" s="0"/>
+      <c r="F68" s="0"/>
+      <c r="G68" s="0"/>
       <c r="H68" s="0"/>
-      <c r="I68" s="13"/>
+      <c r="I68" s="0"/>
       <c r="J68" s="0"/>
-      <c r="K68" s="13"/>
+      <c r="K68" s="0"/>
       <c r="L68" s="0"/>
       <c r="M68" s="0"/>
       <c r="N68" s="0"/>
@@ -2544,7 +2570,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="6" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D69" s="0"/>
       <c r="E69" s="0"/>
@@ -2563,29 +2589,31 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="7" t="n">
-        <v>43920</v>
+        <v>43921</v>
       </c>
       <c r="D70" s="0"/>
       <c r="E70" s="8" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F70" s="0"/>
       <c r="G70" s="8" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H70" s="8" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="I70" s="8" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="J70" s="8" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="K70" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="L70" s="0"/>
+        <v>36</v>
+      </c>
+      <c r="L70" s="8" t="s">
+        <v>37</v>
+      </c>
       <c r="M70" s="0"/>
       <c r="N70" s="0"/>
       <c r="O70" s="0"/>
@@ -2595,33 +2623,35 @@
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="9"/>
       <c r="C71" s="10" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E71" s="10" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F71" s="10" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="G71" s="11" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H71" s="8" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="I71" s="11" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="J71" s="8" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="K71" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="L71" s="0"/>
+        <v>41</v>
+      </c>
+      <c r="L71" s="8" t="s">
+        <v>45</v>
+      </c>
       <c r="M71" s="0"/>
       <c r="N71" s="0"/>
       <c r="O71" s="0"/>
@@ -2630,40 +2660,43 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C72" s="12" t="n">
         <v>300</v>
       </c>
       <c r="D72" s="1" t="n">
-        <v>11591</v>
+        <v>12428</v>
       </c>
       <c r="E72" s="12" t="n">
         <f aca="false">D72/60.48</f>
-        <v>191.650132275132</v>
+        <v>205.489417989418</v>
       </c>
       <c r="F72" s="12" t="n">
-        <v>812</v>
+        <v>837</v>
       </c>
       <c r="G72" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H72" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,G72)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I72" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J72" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,I72)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K72" s="13" t="n">
-        <f aca="false">$B$82+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L72" s="0"/>
+        <f aca="false">$B$70+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L72" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K72,G72)</f>
+        <v>22</v>
+      </c>
       <c r="M72" s="0"/>
       <c r="N72" s="0"/>
       <c r="O72" s="0"/>
@@ -2672,40 +2705,43 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C73" s="12" t="n">
         <v>230</v>
       </c>
       <c r="D73" s="1" t="n">
-        <v>7716</v>
+        <v>8464</v>
       </c>
       <c r="E73" s="12" t="n">
         <f aca="false">D73/46.75</f>
-        <v>165.048128342246</v>
+        <v>181.048128342246</v>
       </c>
       <c r="F73" s="12" t="n">
-        <v>913</v>
+        <v>748</v>
       </c>
       <c r="G73" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H73" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,G73)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I73" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J73" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,I73)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K73" s="13" t="n">
-        <f aca="false">$B$82+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L73" s="0"/>
+        <f aca="false">$B$70+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L73" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K73,G73)</f>
+        <v>15</v>
+      </c>
       <c r="M73" s="0"/>
       <c r="N73" s="0"/>
       <c r="O73" s="0"/>
@@ -2714,40 +2750,43 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C74" s="12" t="n">
         <v>330</v>
       </c>
       <c r="D74" s="1" t="n">
-        <v>3024</v>
+        <v>3523</v>
       </c>
       <c r="E74" s="12" t="n">
         <f aca="false">D74/65.27</f>
-        <v>46.3306266278535</v>
+        <v>53.9757928604259</v>
       </c>
       <c r="F74" s="12" t="n">
-        <v>418</v>
+        <v>499</v>
       </c>
       <c r="G74" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H74" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,G74)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I74" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J74" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,I74)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K74" s="13" t="n">
-        <f aca="false">$B$82+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L74" s="0"/>
+        <f aca="false">$B$70+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L74" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K74,G74)</f>
+        <v>10</v>
+      </c>
       <c r="M74" s="0"/>
       <c r="N74" s="0"/>
       <c r="O74" s="0"/>
@@ -2756,41 +2795,44 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C75" s="12" t="n">
         <v>50</v>
       </c>
       <c r="D75" s="12" t="n">
-        <v>146</v>
+        <v>180</v>
       </c>
       <c r="E75" s="12" t="n">
         <f aca="false">D75/10.36</f>
-        <v>14.0926640926641</v>
+        <v>17.3745173745174</v>
       </c>
       <c r="F75" s="12" t="n">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G75" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H75" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,G75)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I75" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43921</v>
+        <v>43922</v>
       </c>
       <c r="J75" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,I75)</f>
         <v>-1</v>
       </c>
       <c r="K75" s="13" t="n">
-        <f aca="false">$B$82+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L75" s="0"/>
+        <f aca="false">$B$70+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L75" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K75,G75)</f>
+        <v>7</v>
+      </c>
       <c r="M75" s="0"/>
       <c r="N75" s="0"/>
       <c r="O75" s="0"/>
@@ -2799,41 +2841,44 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C76" s="12" t="n">
         <v>330</v>
       </c>
       <c r="D76" s="1" t="n">
-        <v>1408</v>
+        <v>1789</v>
       </c>
       <c r="E76" s="12" t="n">
         <f aca="false">D76/67.79</f>
-        <v>20.770025077445</v>
+        <v>26.390323056498</v>
       </c>
       <c r="F76" s="12" t="n">
-        <v>180</v>
+        <v>381</v>
       </c>
       <c r="G76" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H76" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,G76)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I76" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43921</v>
+        <v>43922</v>
       </c>
       <c r="J76" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,I76)</f>
         <v>-1</v>
       </c>
       <c r="K76" s="13" t="n">
-        <f aca="false">$B$82+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L76" s="0"/>
+        <f aca="false">$B$70+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L76" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K76,G76)</f>
+        <v>6</v>
+      </c>
       <c r="M76" s="0"/>
       <c r="N76" s="0"/>
       <c r="O76" s="0"/>
@@ -2842,40 +2887,44 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C77" s="12" t="n">
         <v>1660</v>
       </c>
       <c r="D77" s="1" t="n">
-        <v>3141</v>
+        <v>4053</v>
       </c>
       <c r="E77" s="12" t="n">
         <f aca="false">D77/331</f>
-        <v>9.48942598187311</v>
+        <v>12.2447129909366</v>
       </c>
       <c r="F77" s="12" t="n">
-        <v>573</v>
+        <v>912</v>
       </c>
       <c r="G77" s="13" t="n">
         <v>43917</v>
       </c>
       <c r="H77" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,G77)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I77" s="13" t="n">
-        <v>43920</v>
+        <f aca="false">$B$70+1</f>
+        <v>43922</v>
       </c>
       <c r="J77" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,I77)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="K77" s="13" t="n">
-        <f aca="false">$B$82+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L77" s="0"/>
+        <f aca="false">$B$70+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L77" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K77,G77)</f>
+        <v>5</v>
+      </c>
       <c r="M77" s="0"/>
       <c r="N77" s="0"/>
       <c r="O77" s="0"/>
@@ -2884,41 +2933,44 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C78" s="12" t="n">
         <v>414</v>
       </c>
       <c r="D78" s="1" t="n">
-        <v>645</v>
+        <v>775</v>
       </c>
       <c r="E78" s="12" t="n">
         <f aca="false">D78/83.784</f>
-        <v>7.69836723002005</v>
+        <v>9.24997612909386</v>
       </c>
       <c r="F78" s="12" t="n">
-        <v>104</v>
+        <v>130</v>
       </c>
       <c r="G78" s="13" t="n">
         <v>43918</v>
       </c>
       <c r="H78" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,G78)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I78" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43921</v>
+        <v>43922</v>
       </c>
       <c r="J78" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,I78)</f>
         <v>-1</v>
       </c>
       <c r="K78" s="13" t="n">
-        <f aca="false">$B$82+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L78" s="0"/>
+        <f aca="false">$B$70+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L78" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K78,G78)</f>
+        <v>4</v>
+      </c>
       <c r="M78" s="0"/>
       <c r="N78" s="0"/>
       <c r="O78" s="0"/>
@@ -2926,16 +2978,15 @@
       <c r="Q78" s="0"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B79" s="4"/>
-      <c r="C79" s="5"/>
+      <c r="C79" s="12"/>
       <c r="D79" s="0"/>
-      <c r="E79" s="0"/>
-      <c r="F79" s="0"/>
-      <c r="G79" s="0"/>
+      <c r="E79" s="12"/>
+      <c r="F79" s="12"/>
+      <c r="G79" s="13"/>
       <c r="H79" s="0"/>
-      <c r="I79" s="0"/>
+      <c r="I79" s="13"/>
       <c r="J79" s="0"/>
-      <c r="K79" s="0"/>
+      <c r="K79" s="13"/>
       <c r="L79" s="0"/>
       <c r="M79" s="0"/>
       <c r="N79" s="0"/>
@@ -2944,16 +2995,15 @@
       <c r="Q79" s="0"/>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="4"/>
-      <c r="C80" s="5"/>
+      <c r="C80" s="12"/>
       <c r="D80" s="0"/>
-      <c r="E80" s="0"/>
-      <c r="F80" s="0"/>
-      <c r="G80" s="0"/>
+      <c r="E80" s="12"/>
+      <c r="F80" s="12"/>
+      <c r="G80" s="13"/>
       <c r="H80" s="0"/>
-      <c r="I80" s="0"/>
+      <c r="I80" s="13"/>
       <c r="J80" s="0"/>
-      <c r="K80" s="0"/>
+      <c r="K80" s="13"/>
       <c r="L80" s="0"/>
       <c r="M80" s="0"/>
       <c r="N80" s="0"/>
@@ -2963,7 +3013,7 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="6" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D81" s="0"/>
       <c r="E81" s="0"/>
@@ -2982,27 +3032,27 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="7" t="n">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="D82" s="0"/>
       <c r="E82" s="8" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F82" s="0"/>
       <c r="G82" s="8" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H82" s="8" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="I82" s="8" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="J82" s="8" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="K82" s="8" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="L82" s="0"/>
       <c r="M82" s="0"/>
@@ -3014,31 +3064,31 @@
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="9"/>
       <c r="C83" s="10" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E83" s="10" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F83" s="10" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="G83" s="11" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H83" s="8" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="I83" s="11" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="J83" s="8" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="K83" s="8" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="L83" s="0"/>
       <c r="M83" s="0"/>
@@ -3049,37 +3099,37 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C84" s="12" t="n">
         <v>300</v>
       </c>
       <c r="D84" s="1" t="n">
-        <v>10779</v>
+        <v>11591</v>
       </c>
       <c r="E84" s="12" t="n">
         <f aca="false">D84/60.48</f>
-        <v>178.224206349206</v>
+        <v>191.650132275132</v>
       </c>
       <c r="F84" s="12" t="n">
-        <v>756</v>
+        <v>812</v>
       </c>
       <c r="G84" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H84" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,G84)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I84" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J84" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,I84)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K84" s="13" t="n">
-        <f aca="false">$B$82+1</f>
+        <f aca="false">$B$94+1</f>
         <v>43920</v>
       </c>
       <c r="L84" s="0"/>
@@ -3091,37 +3141,37 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C85" s="12" t="n">
         <v>230</v>
       </c>
       <c r="D85" s="1" t="n">
-        <v>6803</v>
+        <v>7716</v>
       </c>
       <c r="E85" s="12" t="n">
         <f aca="false">D85/46.75</f>
-        <v>145.51871657754</v>
+        <v>165.048128342246</v>
       </c>
       <c r="F85" s="12" t="n">
-        <v>821</v>
+        <v>913</v>
       </c>
       <c r="G85" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H85" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,G85)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I85" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J85" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,I85)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K85" s="13" t="n">
-        <f aca="false">$B$82+1</f>
+        <f aca="false">$B$94+1</f>
         <v>43920</v>
       </c>
       <c r="L85" s="0"/>
@@ -3133,37 +3183,37 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C86" s="12" t="n">
         <v>330</v>
       </c>
       <c r="D86" s="1" t="n">
-        <v>2606</v>
+        <v>3024</v>
       </c>
       <c r="E86" s="12" t="n">
         <f aca="false">D86/65.27</f>
-        <v>39.9264593228129</v>
+        <v>46.3306266278535</v>
       </c>
       <c r="F86" s="12" t="n">
-        <v>292</v>
+        <v>418</v>
       </c>
       <c r="G86" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H86" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,G86)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I86" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J86" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,I86)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K86" s="13" t="n">
-        <f aca="false">$B$82+1</f>
+        <f aca="false">$B$94+1</f>
         <v>43920</v>
       </c>
       <c r="L86" s="0"/>
@@ -3175,38 +3225,38 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C87" s="12" t="n">
-        <v>1660</v>
-      </c>
-      <c r="D87" s="1" t="n">
-        <v>2583</v>
+        <v>50</v>
+      </c>
+      <c r="D87" s="12" t="n">
+        <v>146</v>
       </c>
       <c r="E87" s="12" t="n">
-        <f aca="false">D87/331</f>
-        <v>7.8036253776435</v>
+        <f aca="false">D87/10.36</f>
+        <v>14.0926640926641</v>
       </c>
       <c r="F87" s="12" t="n">
-        <v>363</v>
+        <v>36</v>
       </c>
       <c r="G87" s="13" t="n">
-        <v>43917</v>
+        <v>43915</v>
       </c>
       <c r="H87" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,G87)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I87" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43920</v>
+        <v>43921</v>
       </c>
       <c r="J87" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,I87)</f>
         <v>-1</v>
       </c>
       <c r="K87" s="13" t="n">
-        <f aca="false">$B$82+1</f>
+        <f aca="false">$B$94+1</f>
         <v>43920</v>
       </c>
       <c r="L87" s="0"/>
@@ -3218,38 +3268,38 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C88" s="12" t="n">
         <v>330</v>
       </c>
       <c r="D88" s="1" t="n">
-        <v>1228</v>
+        <v>1408</v>
       </c>
       <c r="E88" s="12" t="n">
         <f aca="false">D88/67.79</f>
-        <v>18.1147661897035</v>
+        <v>20.770025077445</v>
       </c>
       <c r="F88" s="12" t="n">
-        <v>209</v>
+        <v>180</v>
       </c>
       <c r="G88" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H88" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,G88)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I88" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43920</v>
+        <v>43921</v>
       </c>
       <c r="J88" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,I88)</f>
         <v>-1</v>
       </c>
       <c r="K88" s="13" t="n">
-        <f aca="false">$B$82+1</f>
+        <f aca="false">$B$94+1</f>
         <v>43920</v>
       </c>
       <c r="L88" s="0"/>
@@ -3261,38 +3311,37 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C89" s="12" t="n">
-        <v>414</v>
+        <v>1660</v>
       </c>
       <c r="D89" s="1" t="n">
-        <v>541</v>
+        <v>3141</v>
       </c>
       <c r="E89" s="12" t="n">
-        <f aca="false">D89/83.784</f>
-        <v>6.457080110761</v>
+        <f aca="false">D89/331</f>
+        <v>9.48942598187311</v>
       </c>
       <c r="F89" s="12" t="n">
-        <v>108</v>
+        <v>573</v>
       </c>
       <c r="G89" s="13" t="n">
-        <v>43918</v>
+        <v>43917</v>
       </c>
       <c r="H89" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,G89)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I89" s="13" t="n">
-        <f aca="false">$B$82+1</f>
         <v>43920</v>
       </c>
       <c r="J89" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,I89)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="K89" s="13" t="n">
-        <f aca="false">$B$82+1</f>
+        <f aca="false">$B$94+1</f>
         <v>43920</v>
       </c>
       <c r="L89" s="0"/>
@@ -3304,38 +3353,38 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="0" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C90" s="12" t="n">
-        <v>50</v>
-      </c>
-      <c r="D90" s="12" t="n">
-        <v>110</v>
+        <v>414</v>
+      </c>
+      <c r="D90" s="1" t="n">
+        <v>645</v>
       </c>
       <c r="E90" s="12" t="n">
-        <f aca="false">D90/10.36</f>
-        <v>10.6177606177606</v>
+        <f aca="false">D90/83.784</f>
+        <v>7.69836723002005</v>
       </c>
       <c r="F90" s="12" t="n">
-        <v>5</v>
+        <v>104</v>
       </c>
       <c r="G90" s="13" t="n">
-        <v>43915</v>
+        <v>43918</v>
       </c>
       <c r="H90" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,G90)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I90" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43920</v>
+        <v>43921</v>
       </c>
       <c r="J90" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,I90)</f>
         <v>-1</v>
       </c>
       <c r="K90" s="13" t="n">
-        <f aca="false">$B$82+1</f>
+        <f aca="false">$B$94+1</f>
         <v>43920</v>
       </c>
       <c r="L90" s="0"/>
@@ -3383,7 +3432,7 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B93" s="6" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D93" s="0"/>
       <c r="E93" s="0"/>
@@ -3402,29 +3451,27 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="7" t="n">
-        <v>43918</v>
-      </c>
-      <c r="D94" s="8" t="s">
-        <v>6</v>
-      </c>
+        <v>43919</v>
+      </c>
+      <c r="D94" s="0"/>
       <c r="E94" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F94" s="8"/>
+        <v>32</v>
+      </c>
+      <c r="F94" s="0"/>
       <c r="G94" s="8" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H94" s="8" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="I94" s="8" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="J94" s="8" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="K94" s="8" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="L94" s="0"/>
       <c r="M94" s="0"/>
@@ -3436,31 +3483,31 @@
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="9"/>
       <c r="C95" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D95" s="10" t="s">
-        <v>2</v>
+        <v>38</v>
+      </c>
+      <c r="D95" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="E95" s="10" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F95" s="10" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="G95" s="11" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H95" s="8" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="I95" s="11" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="J95" s="8" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="K95" s="8" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="L95" s="0"/>
       <c r="M95" s="0"/>
@@ -3471,38 +3518,38 @@
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C96" s="12" t="n">
         <v>300</v>
       </c>
       <c r="D96" s="1" t="n">
-        <v>10023</v>
+        <v>10779</v>
       </c>
       <c r="E96" s="12" t="n">
         <f aca="false">D96/60.48</f>
-        <v>165.724206349206</v>
+        <v>178.224206349206</v>
       </c>
       <c r="F96" s="12" t="n">
-        <v>889</v>
+        <v>756</v>
       </c>
       <c r="G96" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H96" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,G96)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I96" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J96" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$106,I96)</f>
-        <v>15</v>
+        <f aca="false">_xlfn.DAYS($B$94,I96)</f>
+        <v>17</v>
       </c>
       <c r="K96" s="13" t="n">
         <f aca="false">$B$94+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L96" s="0"/>
       <c r="M96" s="0"/>
@@ -3513,38 +3560,38 @@
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C97" s="12" t="n">
         <v>230</v>
       </c>
       <c r="D97" s="1" t="n">
-        <v>5982</v>
+        <v>6803</v>
       </c>
       <c r="E97" s="12" t="n">
         <f aca="false">D97/46.75</f>
-        <v>127.957219251337</v>
+        <v>145.51871657754</v>
       </c>
       <c r="F97" s="12" t="n">
-        <v>844</v>
+        <v>821</v>
       </c>
       <c r="G97" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H97" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,G97)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I97" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J97" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$106,I97)</f>
-        <v>4</v>
+        <f aca="false">_xlfn.DAYS($B$94,I97)</f>
+        <v>6</v>
       </c>
       <c r="K97" s="13" t="n">
         <f aca="false">$B$94+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L97" s="0"/>
       <c r="M97" s="0"/>
@@ -3555,38 +3602,38 @@
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C98" s="12" t="n">
         <v>330</v>
       </c>
       <c r="D98" s="1" t="n">
-        <v>2314</v>
+        <v>2606</v>
       </c>
       <c r="E98" s="12" t="n">
         <f aca="false">D98/65.27</f>
-        <v>35.4527347939329</v>
+        <v>39.9264593228129</v>
       </c>
       <c r="F98" s="12" t="n">
-        <v>319</v>
+        <v>292</v>
       </c>
       <c r="G98" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H98" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,G98)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I98" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J98" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$106,I98)</f>
-        <v>3</v>
+        <f aca="false">_xlfn.DAYS($B$94,I98)</f>
+        <v>5</v>
       </c>
       <c r="K98" s="13" t="n">
         <f aca="false">$B$94+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L98" s="0"/>
       <c r="M98" s="0"/>
@@ -3597,31 +3644,31 @@
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C99" s="12" t="n">
         <v>1660</v>
       </c>
       <c r="D99" s="1" t="n">
-        <v>2221</v>
+        <v>2583</v>
       </c>
       <c r="E99" s="12" t="n">
         <f aca="false">D99/331</f>
-        <v>6.70996978851964</v>
+        <v>7.8036253776435</v>
       </c>
       <c r="F99" s="12" t="n">
-        <v>525</v>
+        <v>363</v>
       </c>
       <c r="G99" s="13" t="n">
         <v>43917</v>
       </c>
       <c r="H99" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,G99)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I99" s="13" t="n">
         <f aca="false">$B$94+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="J99" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,I99)</f>
@@ -3629,7 +3676,7 @@
       </c>
       <c r="K99" s="13" t="n">
         <f aca="false">$B$94+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L99" s="0"/>
       <c r="M99" s="0"/>
@@ -3640,31 +3687,31 @@
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C100" s="12" t="n">
         <v>330</v>
       </c>
       <c r="D100" s="1" t="n">
-        <v>1019</v>
+        <v>1228</v>
       </c>
       <c r="E100" s="12" t="n">
         <f aca="false">D100/67.79</f>
-        <v>15.0317155922702</v>
+        <v>18.1147661897035</v>
       </c>
       <c r="F100" s="12" t="n">
-        <v>260</v>
+        <v>209</v>
       </c>
       <c r="G100" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H100" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,G100)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I100" s="13" t="n">
         <f aca="false">$B$94+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="J100" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,I100)</f>
@@ -3672,7 +3719,7 @@
       </c>
       <c r="K100" s="13" t="n">
         <f aca="false">$B$94+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L100" s="0"/>
       <c r="M100" s="0"/>
@@ -3683,31 +3730,31 @@
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C101" s="12" t="n">
         <v>414</v>
       </c>
       <c r="D101" s="1" t="n">
-        <v>433</v>
+        <v>541</v>
       </c>
       <c r="E101" s="12" t="n">
         <f aca="false">D101/83.784</f>
-        <v>5.16805117922276</v>
+        <v>6.457080110761</v>
       </c>
       <c r="F101" s="12" t="n">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="G101" s="13" t="n">
         <v>43918</v>
       </c>
       <c r="H101" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,G101)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I101" s="13" t="n">
         <f aca="false">$B$94+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="J101" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,I101)</f>
@@ -3715,7 +3762,7 @@
       </c>
       <c r="K101" s="13" t="n">
         <f aca="false">$B$94+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L101" s="0"/>
       <c r="M101" s="0"/>
@@ -3726,31 +3773,31 @@
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C102" s="12" t="n">
         <v>50</v>
       </c>
       <c r="D102" s="12" t="n">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="E102" s="12" t="n">
         <f aca="false">D102/10.36</f>
-        <v>10.1351351351351</v>
+        <v>10.6177606177606</v>
       </c>
       <c r="F102" s="12" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G102" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H102" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,G102)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I102" s="13" t="n">
         <f aca="false">$B$94+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="J102" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,I102)</f>
@@ -3758,7 +3805,7 @@
       </c>
       <c r="K102" s="13" t="n">
         <f aca="false">$B$94+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L102" s="0"/>
       <c r="M102" s="0"/>
@@ -3768,15 +3815,16 @@
       <c r="Q102" s="0"/>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C103" s="12"/>
-      <c r="D103" s="12"/>
-      <c r="E103" s="12"/>
-      <c r="F103" s="12"/>
-      <c r="G103" s="13"/>
+      <c r="B103" s="4"/>
+      <c r="C103" s="5"/>
+      <c r="D103" s="0"/>
+      <c r="E103" s="0"/>
+      <c r="F103" s="0"/>
+      <c r="G103" s="0"/>
       <c r="H103" s="0"/>
-      <c r="I103" s="13"/>
+      <c r="I103" s="0"/>
       <c r="J103" s="0"/>
-      <c r="K103" s="13"/>
+      <c r="K103" s="0"/>
       <c r="L103" s="0"/>
       <c r="M103" s="0"/>
       <c r="N103" s="0"/>
@@ -3804,7 +3852,7 @@
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="6" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D105" s="0"/>
       <c r="E105" s="0"/>
@@ -3821,66 +3869,69 @@
       <c r="P105" s="0"/>
       <c r="Q105" s="0"/>
     </row>
-    <row r="106" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="7" t="n">
-        <v>43917</v>
-      </c>
-      <c r="C106" s="0"/>
+        <v>43918</v>
+      </c>
       <c r="D106" s="8" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E106" s="8" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F106" s="8"/>
       <c r="G106" s="8" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H106" s="8" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="I106" s="8" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="J106" s="8" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="K106" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="L106" s="8"/>
+        <v>36</v>
+      </c>
+      <c r="L106" s="0"/>
+      <c r="M106" s="0"/>
+      <c r="N106" s="0"/>
+      <c r="O106" s="0"/>
+      <c r="P106" s="0"/>
+      <c r="Q106" s="0"/>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="3"/>
       <c r="B107" s="9"/>
       <c r="C107" s="10" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D107" s="10" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E107" s="10" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F107" s="10" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="G107" s="11" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H107" s="8" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="I107" s="11" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="J107" s="8" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="K107" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="L107" s="8"/>
+        <v>41</v>
+      </c>
+      <c r="L107" s="0"/>
       <c r="M107" s="0"/>
       <c r="N107" s="0"/>
       <c r="O107" s="0"/>
@@ -3889,38 +3940,38 @@
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C108" s="12" t="n">
         <v>300</v>
       </c>
       <c r="D108" s="1" t="n">
-        <v>9134</v>
+        <v>10023</v>
       </c>
       <c r="E108" s="12" t="n">
         <f aca="false">D108/60.48</f>
-        <v>151.025132275132</v>
+        <v>165.724206349206</v>
       </c>
       <c r="F108" s="12" t="n">
-        <v>919</v>
+        <v>889</v>
       </c>
       <c r="G108" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H108" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,G108)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I108" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J108" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$106,I108)</f>
+        <f aca="false">_xlfn.DAYS(B$118,I108)</f>
         <v>15</v>
       </c>
       <c r="K108" s="13" t="n">
         <f aca="false">$B$106+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L108" s="0"/>
       <c r="M108" s="0"/>
@@ -3931,38 +3982,38 @@
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C109" s="12" t="n">
         <v>230</v>
       </c>
       <c r="D109" s="1" t="n">
-        <v>5138</v>
+        <v>5982</v>
       </c>
       <c r="E109" s="12" t="n">
         <f aca="false">D109/46.75</f>
-        <v>109.903743315508</v>
+        <v>127.957219251337</v>
       </c>
       <c r="F109" s="12" t="n">
-        <v>773</v>
+        <v>844</v>
       </c>
       <c r="G109" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H109" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,G109)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I109" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J109" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$106,I109)</f>
+        <f aca="false">_xlfn.DAYS(B$118,I109)</f>
         <v>4</v>
       </c>
       <c r="K109" s="13" t="n">
         <f aca="false">$B$106+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L109" s="0"/>
       <c r="M109" s="0"/>
@@ -3973,38 +4024,38 @@
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C110" s="12" t="n">
         <v>330</v>
       </c>
       <c r="D110" s="1" t="n">
-        <v>1995</v>
+        <v>2314</v>
       </c>
       <c r="E110" s="12" t="n">
         <f aca="false">D110/65.27</f>
-        <v>30.5653439558756</v>
+        <v>35.4527347939329</v>
       </c>
       <c r="F110" s="12" t="n">
-        <v>299</v>
+        <v>319</v>
       </c>
       <c r="G110" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H110" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,G110)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I110" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J110" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$106,I110)</f>
+        <f aca="false">_xlfn.DAYS(B$118,I110)</f>
         <v>3</v>
       </c>
       <c r="K110" s="13" t="n">
         <f aca="false">$B$106+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L110" s="0"/>
       <c r="M110" s="0"/>
@@ -4015,40 +4066,39 @@
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B111" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C111" s="12" t="n">
         <v>1660</v>
       </c>
       <c r="D111" s="1" t="n">
-        <v>1696</v>
+        <v>2221</v>
       </c>
       <c r="E111" s="12" t="n">
         <f aca="false">D111/331</f>
-        <v>5.12386706948641</v>
+        <v>6.70996978851964</v>
       </c>
       <c r="F111" s="12" t="n">
-        <v>400</v>
+        <v>525</v>
       </c>
       <c r="G111" s="13" t="n">
-        <f aca="false">$B$106</f>
         <v>43917</v>
       </c>
       <c r="H111" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,G111)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I111" s="13" t="n">
         <f aca="false">$B$106+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="J111" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$106,I111)</f>
+        <f aca="false">_xlfn.DAYS($B$106,I111)</f>
         <v>-1</v>
       </c>
       <c r="K111" s="13" t="n">
         <f aca="false">$B$106+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L111" s="0"/>
       <c r="M111" s="0"/>
@@ -4059,39 +4109,39 @@
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C112" s="12" t="n">
         <v>330</v>
       </c>
       <c r="D112" s="1" t="n">
-        <v>759</v>
+        <v>1019</v>
       </c>
       <c r="E112" s="12" t="n">
         <f aca="false">D112/67.79</f>
-        <v>11.1963416433102</v>
+        <v>15.0317155922702</v>
       </c>
       <c r="F112" s="12" t="n">
-        <v>181</v>
+        <v>260</v>
       </c>
       <c r="G112" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H112" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,G112)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I112" s="13" t="n">
         <f aca="false">$B$106+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="J112" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$106,I112)</f>
+        <f aca="false">_xlfn.DAYS($B$106,I112)</f>
         <v>-1</v>
       </c>
       <c r="K112" s="13" t="n">
         <f aca="false">$B$106+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L112" s="0"/>
       <c r="M112" s="0"/>
@@ -4102,40 +4152,39 @@
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C113" s="12" t="n">
         <v>414</v>
       </c>
       <c r="D113" s="1" t="n">
-        <v>351</v>
+        <v>433</v>
       </c>
       <c r="E113" s="12" t="n">
         <f aca="false">D113/83.784</f>
-        <v>4.18934402749928</v>
+        <v>5.16805117922276</v>
       </c>
       <c r="F113" s="12" t="n">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G113" s="13" t="n">
-        <f aca="false">$B$106+1</f>
         <v>43918</v>
       </c>
       <c r="H113" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,G113)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="I113" s="13" t="n">
         <f aca="false">$B$106+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="J113" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$106,I113)</f>
+        <f aca="false">_xlfn.DAYS($B$106,I113)</f>
         <v>-1</v>
       </c>
       <c r="K113" s="13" t="n">
         <f aca="false">$B$106+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L113" s="0"/>
       <c r="M113" s="0"/>
@@ -4146,7 +4195,7 @@
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C114" s="12" t="n">
         <v>50</v>
@@ -4159,26 +4208,26 @@
         <v>10.1351351351351</v>
       </c>
       <c r="F114" s="12" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="G114" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H114" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,G114)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I114" s="13" t="n">
         <f aca="false">$B$106+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="J114" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$106,I114)</f>
+        <f aca="false">_xlfn.DAYS($B$106,I114)</f>
         <v>-1</v>
       </c>
       <c r="K114" s="13" t="n">
         <f aca="false">$B$106+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L114" s="0"/>
       <c r="M114" s="0"/>
@@ -4188,14 +4237,15 @@
       <c r="Q114" s="0"/>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D115" s="0"/>
-      <c r="E115" s="0"/>
-      <c r="F115" s="0"/>
-      <c r="G115" s="0"/>
+      <c r="C115" s="12"/>
+      <c r="D115" s="12"/>
+      <c r="E115" s="12"/>
+      <c r="F115" s="12"/>
+      <c r="G115" s="13"/>
       <c r="H115" s="0"/>
-      <c r="I115" s="0"/>
+      <c r="I115" s="13"/>
       <c r="J115" s="0"/>
-      <c r="K115" s="0"/>
+      <c r="K115" s="13"/>
       <c r="L115" s="0"/>
       <c r="M115" s="0"/>
       <c r="N115" s="0"/>
@@ -4204,6 +4254,8 @@
       <c r="Q115" s="0"/>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B116" s="4"/>
+      <c r="C116" s="5"/>
       <c r="D116" s="0"/>
       <c r="E116" s="0"/>
       <c r="F116" s="0"/>
@@ -4221,7 +4273,7 @@
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B117" s="6" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D117" s="0"/>
       <c r="E117" s="0"/>
@@ -4238,69 +4290,66 @@
       <c r="P117" s="0"/>
       <c r="Q117" s="0"/>
     </row>
-    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="7" t="n">
-        <v>43916</v>
-      </c>
+        <v>43917</v>
+      </c>
+      <c r="C118" s="0"/>
       <c r="D118" s="8" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E118" s="8" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F118" s="8"/>
       <c r="G118" s="8" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H118" s="8" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="I118" s="8" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="J118" s="8" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="K118" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="L118" s="0"/>
-      <c r="M118" s="0"/>
-      <c r="N118" s="0"/>
-      <c r="O118" s="0"/>
-      <c r="P118" s="0"/>
-      <c r="Q118" s="0"/>
+        <v>36</v>
+      </c>
+      <c r="L118" s="8"/>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="3"/>
       <c r="B119" s="9"/>
       <c r="C119" s="10" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="D119" s="10" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E119" s="10" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F119" s="10" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="G119" s="11" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H119" s="8" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="I119" s="11" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="J119" s="8" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="K119" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="L119" s="0"/>
+        <v>41</v>
+      </c>
+      <c r="L119" s="8"/>
       <c r="M119" s="0"/>
       <c r="N119" s="0"/>
       <c r="O119" s="0"/>
@@ -4309,38 +4358,38 @@
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C120" s="12" t="n">
         <v>300</v>
       </c>
       <c r="D120" s="1" t="n">
-        <v>8215</v>
+        <v>9134</v>
       </c>
       <c r="E120" s="12" t="n">
         <f aca="false">D120/60.48</f>
-        <v>135.830026455026</v>
+        <v>151.025132275132</v>
       </c>
       <c r="F120" s="12" t="n">
-        <v>712</v>
+        <v>919</v>
       </c>
       <c r="G120" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H120" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$118,G120)</f>
-        <v>16</v>
+        <f aca="false">_xlfn.DAYS($B$118,G120)</f>
+        <v>17</v>
       </c>
       <c r="I120" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J120" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$118,I120)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K120" s="13" t="n">
-        <f aca="false">B$118+1</f>
-        <v>43917</v>
+        <f aca="false">$B$118+1</f>
+        <v>43918</v>
       </c>
       <c r="L120" s="0"/>
       <c r="M120" s="0"/>
@@ -4351,38 +4400,38 @@
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C121" s="12" t="n">
         <v>230</v>
       </c>
       <c r="D121" s="1" t="n">
-        <v>4365</v>
+        <v>5138</v>
       </c>
       <c r="E121" s="12" t="n">
         <f aca="false">D121/46.75</f>
-        <v>93.3689839572193</v>
+        <v>109.903743315508</v>
       </c>
       <c r="F121" s="12" t="n">
-        <v>718</v>
+        <v>773</v>
       </c>
       <c r="G121" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H121" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$118,G121)</f>
-        <v>9</v>
+        <f aca="false">_xlfn.DAYS($B$118,G121)</f>
+        <v>10</v>
       </c>
       <c r="I121" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J121" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$118,I121)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K121" s="13" t="n">
-        <f aca="false">B$118+1</f>
-        <v>43917</v>
+        <f aca="false">$B$118+1</f>
+        <v>43918</v>
       </c>
       <c r="L121" s="0"/>
       <c r="M121" s="0"/>
@@ -4393,38 +4442,38 @@
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C122" s="12" t="n">
         <v>330</v>
       </c>
       <c r="D122" s="1" t="n">
-        <v>1696</v>
+        <v>1995</v>
       </c>
       <c r="E122" s="12" t="n">
         <f aca="false">D122/65.27</f>
-        <v>25.9843726060978</v>
+        <v>30.5653439558756</v>
       </c>
       <c r="F122" s="12" t="n">
-        <v>365</v>
+        <v>299</v>
       </c>
       <c r="G122" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H122" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$118,G122)</f>
-        <v>4</v>
+        <f aca="false">_xlfn.DAYS($B$118,G122)</f>
+        <v>5</v>
       </c>
       <c r="I122" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J122" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$118,I122)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K122" s="13" t="n">
-        <f aca="false">B$118+1</f>
-        <v>43917</v>
+        <f aca="false">$B$118+1</f>
+        <v>43918</v>
       </c>
       <c r="L122" s="0"/>
       <c r="M122" s="0"/>
@@ -4435,39 +4484,40 @@
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C123" s="12" t="n">
         <v>1660</v>
       </c>
       <c r="D123" s="1" t="n">
-        <v>1295</v>
+        <v>1696</v>
       </c>
       <c r="E123" s="12" t="n">
         <f aca="false">D123/331</f>
-        <v>3.91238670694864</v>
+        <v>5.12386706948641</v>
       </c>
       <c r="F123" s="12" t="n">
-        <v>268</v>
+        <v>400</v>
       </c>
       <c r="G123" s="13" t="n">
+        <f aca="false">$B$118</f>
         <v>43917</v>
       </c>
       <c r="H123" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$118,G123)</f>
+        <f aca="false">_xlfn.DAYS($B$118,G123)</f>
+        <v>0</v>
+      </c>
+      <c r="I123" s="13" t="n">
+        <f aca="false">$B$118+1</f>
+        <v>43918</v>
+      </c>
+      <c r="J123" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$118,I123)</f>
         <v>-1</v>
       </c>
-      <c r="I123" s="13" t="n">
-        <f aca="false">B$118+1</f>
-        <v>43917</v>
-      </c>
-      <c r="J123" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$118,I123)</f>
-        <v>-1</v>
-      </c>
       <c r="K123" s="13" t="n">
-        <f aca="false">B$118+1</f>
-        <v>43917</v>
+        <f aca="false">$B$118+1</f>
+        <v>43918</v>
       </c>
       <c r="L123" s="0"/>
       <c r="M123" s="0"/>
@@ -4478,39 +4528,39 @@
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C124" s="12" t="n">
         <v>330</v>
       </c>
       <c r="D124" s="1" t="n">
-        <v>578</v>
+        <v>759</v>
       </c>
       <c r="E124" s="12" t="n">
         <f aca="false">D124/67.79</f>
-        <v>8.52633131730344</v>
+        <v>11.1963416433102</v>
       </c>
       <c r="F124" s="12" t="n">
-        <v>115</v>
+        <v>181</v>
       </c>
       <c r="G124" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H124" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$118,G124)</f>
-        <v>0</v>
+        <f aca="false">_xlfn.DAYS($B$118,G124)</f>
+        <v>1</v>
       </c>
       <c r="I124" s="13" t="n">
-        <f aca="false">B$118+1</f>
-        <v>43917</v>
+        <f aca="false">$B$118+1</f>
+        <v>43918</v>
       </c>
       <c r="J124" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$118,I124)</f>
         <v>-1</v>
       </c>
       <c r="K124" s="13" t="n">
-        <f aca="false">B$118+1</f>
-        <v>43917</v>
+        <f aca="false">$B$118+1</f>
+        <v>43918</v>
       </c>
       <c r="L124" s="0"/>
       <c r="M124" s="0"/>
@@ -4521,39 +4571,40 @@
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C125" s="12" t="n">
         <v>414</v>
       </c>
       <c r="D125" s="1" t="n">
-        <v>267</v>
+        <v>351</v>
       </c>
       <c r="E125" s="12" t="n">
         <f aca="false">D125/83.784</f>
-        <v>3.18676596963621</v>
+        <v>4.18934402749928</v>
       </c>
       <c r="F125" s="12" t="n">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="G125" s="13" t="n">
-        <v>43917</v>
+        <f aca="false">$B$118+1</f>
+        <v>43918</v>
       </c>
       <c r="H125" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$118,G125)</f>
+        <f aca="false">_xlfn.DAYS($B$118,G125)</f>
         <v>-1</v>
       </c>
       <c r="I125" s="13" t="n">
-        <f aca="false">B$118+1</f>
-        <v>43917</v>
+        <f aca="false">$B$118+1</f>
+        <v>43918</v>
       </c>
       <c r="J125" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$118,I125)</f>
         <v>-1</v>
       </c>
       <c r="K125" s="13" t="n">
-        <f aca="false">B$118+1</f>
-        <v>43917</v>
+        <f aca="false">$B$118+1</f>
+        <v>43918</v>
       </c>
       <c r="L125" s="0"/>
       <c r="M125" s="0"/>
@@ -4564,39 +4615,39 @@
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C126" s="12" t="n">
         <v>50</v>
       </c>
       <c r="D126" s="12" t="n">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="E126" s="12" t="n">
         <f aca="false">D126/10.36</f>
-        <v>7.43243243243243</v>
+        <v>10.1351351351351</v>
       </c>
       <c r="F126" s="12" t="n">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="G126" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H126" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$118,G126)</f>
-        <v>1</v>
+        <f aca="false">_xlfn.DAYS($B$118,G126)</f>
+        <v>2</v>
       </c>
       <c r="I126" s="13" t="n">
-        <f aca="false">B$118+1</f>
-        <v>43917</v>
+        <f aca="false">$B$118+1</f>
+        <v>43918</v>
       </c>
       <c r="J126" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$118,I126)</f>
         <v>-1</v>
       </c>
       <c r="K126" s="13" t="n">
-        <f aca="false">B$118+1</f>
-        <v>43917</v>
+        <f aca="false">$B$118+1</f>
+        <v>43918</v>
       </c>
       <c r="L126" s="0"/>
       <c r="M126" s="0"/>
@@ -4604,6 +4655,424 @@
       <c r="O126" s="0"/>
       <c r="P126" s="0"/>
       <c r="Q126" s="0"/>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D127" s="0"/>
+      <c r="E127" s="0"/>
+      <c r="F127" s="0"/>
+      <c r="G127" s="0"/>
+      <c r="H127" s="0"/>
+      <c r="I127" s="0"/>
+      <c r="J127" s="0"/>
+      <c r="K127" s="0"/>
+      <c r="L127" s="0"/>
+      <c r="M127" s="0"/>
+      <c r="N127" s="0"/>
+      <c r="O127" s="0"/>
+      <c r="P127" s="0"/>
+      <c r="Q127" s="0"/>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D128" s="0"/>
+      <c r="E128" s="0"/>
+      <c r="F128" s="0"/>
+      <c r="G128" s="0"/>
+      <c r="H128" s="0"/>
+      <c r="I128" s="0"/>
+      <c r="J128" s="0"/>
+      <c r="K128" s="0"/>
+      <c r="L128" s="0"/>
+      <c r="M128" s="0"/>
+      <c r="N128" s="0"/>
+      <c r="O128" s="0"/>
+      <c r="P128" s="0"/>
+      <c r="Q128" s="0"/>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B129" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D129" s="0"/>
+      <c r="E129" s="0"/>
+      <c r="F129" s="0"/>
+      <c r="G129" s="0"/>
+      <c r="H129" s="0"/>
+      <c r="I129" s="0"/>
+      <c r="J129" s="0"/>
+      <c r="K129" s="0"/>
+      <c r="L129" s="0"/>
+      <c r="M129" s="0"/>
+      <c r="N129" s="0"/>
+      <c r="O129" s="0"/>
+      <c r="P129" s="0"/>
+      <c r="Q129" s="0"/>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B130" s="7" t="n">
+        <v>43916</v>
+      </c>
+      <c r="D130" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E130" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F130" s="8"/>
+      <c r="G130" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H130" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I130" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J130" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="K130" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="L130" s="0"/>
+      <c r="M130" s="0"/>
+      <c r="N130" s="0"/>
+      <c r="O130" s="0"/>
+      <c r="P130" s="0"/>
+      <c r="Q130" s="0"/>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B131" s="9"/>
+      <c r="C131" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D131" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E131" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F131" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G131" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H131" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I131" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="J131" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="K131" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="L131" s="0"/>
+      <c r="M131" s="0"/>
+      <c r="N131" s="0"/>
+      <c r="O131" s="0"/>
+      <c r="P131" s="0"/>
+      <c r="Q131" s="0"/>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B132" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C132" s="12" t="n">
+        <v>300</v>
+      </c>
+      <c r="D132" s="1" t="n">
+        <v>8215</v>
+      </c>
+      <c r="E132" s="12" t="n">
+        <f aca="false">D132/60.48</f>
+        <v>135.830026455026</v>
+      </c>
+      <c r="F132" s="12" t="n">
+        <v>712</v>
+      </c>
+      <c r="G132" s="13" t="n">
+        <v>43900</v>
+      </c>
+      <c r="H132" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$130,G132)</f>
+        <v>16</v>
+      </c>
+      <c r="I132" s="13" t="n">
+        <v>43902</v>
+      </c>
+      <c r="J132" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$130,I132)</f>
+        <v>14</v>
+      </c>
+      <c r="K132" s="13" t="n">
+        <f aca="false">B$130+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L132" s="0"/>
+      <c r="M132" s="0"/>
+      <c r="N132" s="0"/>
+      <c r="O132" s="0"/>
+      <c r="P132" s="0"/>
+      <c r="Q132" s="0"/>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B133" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C133" s="12" t="n">
+        <v>230</v>
+      </c>
+      <c r="D133" s="1" t="n">
+        <v>4365</v>
+      </c>
+      <c r="E133" s="12" t="n">
+        <f aca="false">D133/46.75</f>
+        <v>93.3689839572193</v>
+      </c>
+      <c r="F133" s="12" t="n">
+        <v>718</v>
+      </c>
+      <c r="G133" s="13" t="n">
+        <v>43907</v>
+      </c>
+      <c r="H133" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$130,G133)</f>
+        <v>9</v>
+      </c>
+      <c r="I133" s="13" t="n">
+        <v>43913</v>
+      </c>
+      <c r="J133" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$130,I133)</f>
+        <v>3</v>
+      </c>
+      <c r="K133" s="13" t="n">
+        <f aca="false">B$130+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L133" s="0"/>
+      <c r="M133" s="0"/>
+      <c r="N133" s="0"/>
+      <c r="O133" s="0"/>
+      <c r="P133" s="0"/>
+      <c r="Q133" s="0"/>
+    </row>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B134" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C134" s="12" t="n">
+        <v>330</v>
+      </c>
+      <c r="D134" s="1" t="n">
+        <v>1696</v>
+      </c>
+      <c r="E134" s="12" t="n">
+        <f aca="false">D134/65.27</f>
+        <v>25.9843726060978</v>
+      </c>
+      <c r="F134" s="12" t="n">
+        <v>365</v>
+      </c>
+      <c r="G134" s="13" t="n">
+        <v>43912</v>
+      </c>
+      <c r="H134" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$130,G134)</f>
+        <v>4</v>
+      </c>
+      <c r="I134" s="13" t="n">
+        <v>43914</v>
+      </c>
+      <c r="J134" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$130,I134)</f>
+        <v>2</v>
+      </c>
+      <c r="K134" s="13" t="n">
+        <f aca="false">B$130+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L134" s="0"/>
+      <c r="M134" s="0"/>
+      <c r="N134" s="0"/>
+      <c r="O134" s="0"/>
+      <c r="P134" s="0"/>
+      <c r="Q134" s="0"/>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B135" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C135" s="12" t="n">
+        <v>1660</v>
+      </c>
+      <c r="D135" s="1" t="n">
+        <v>1295</v>
+      </c>
+      <c r="E135" s="12" t="n">
+        <f aca="false">D135/331</f>
+        <v>3.91238670694864</v>
+      </c>
+      <c r="F135" s="12" t="n">
+        <v>268</v>
+      </c>
+      <c r="G135" s="13" t="n">
+        <v>43917</v>
+      </c>
+      <c r="H135" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$130,G135)</f>
+        <v>-1</v>
+      </c>
+      <c r="I135" s="13" t="n">
+        <f aca="false">B$130+1</f>
+        <v>43917</v>
+      </c>
+      <c r="J135" s="1" t="n">
+        <f aca="false">_xlfn.DAYS($B$130,I135)</f>
+        <v>-1</v>
+      </c>
+      <c r="K135" s="13" t="n">
+        <f aca="false">B$130+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L135" s="0"/>
+      <c r="M135" s="0"/>
+      <c r="N135" s="0"/>
+      <c r="O135" s="0"/>
+      <c r="P135" s="0"/>
+      <c r="Q135" s="0"/>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B136" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C136" s="12" t="n">
+        <v>330</v>
+      </c>
+      <c r="D136" s="1" t="n">
+        <v>578</v>
+      </c>
+      <c r="E136" s="12" t="n">
+        <f aca="false">D136/67.79</f>
+        <v>8.52633131730344</v>
+      </c>
+      <c r="F136" s="12" t="n">
+        <v>115</v>
+      </c>
+      <c r="G136" s="13" t="n">
+        <v>43916</v>
+      </c>
+      <c r="H136" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$130,G136)</f>
+        <v>0</v>
+      </c>
+      <c r="I136" s="13" t="n">
+        <f aca="false">B$130+1</f>
+        <v>43917</v>
+      </c>
+      <c r="J136" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$130,I136)</f>
+        <v>-1</v>
+      </c>
+      <c r="K136" s="13" t="n">
+        <f aca="false">B$130+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L136" s="0"/>
+      <c r="M136" s="0"/>
+      <c r="N136" s="0"/>
+      <c r="O136" s="0"/>
+      <c r="P136" s="0"/>
+      <c r="Q136" s="0"/>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B137" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C137" s="12" t="n">
+        <v>414</v>
+      </c>
+      <c r="D137" s="1" t="n">
+        <v>267</v>
+      </c>
+      <c r="E137" s="12" t="n">
+        <f aca="false">D137/83.784</f>
+        <v>3.18676596963621</v>
+      </c>
+      <c r="F137" s="12" t="n">
+        <v>61</v>
+      </c>
+      <c r="G137" s="13" t="n">
+        <v>43917</v>
+      </c>
+      <c r="H137" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$130,G137)</f>
+        <v>-1</v>
+      </c>
+      <c r="I137" s="13" t="n">
+        <f aca="false">B$130+1</f>
+        <v>43917</v>
+      </c>
+      <c r="J137" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$130,I137)</f>
+        <v>-1</v>
+      </c>
+      <c r="K137" s="13" t="n">
+        <f aca="false">B$130+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L137" s="0"/>
+      <c r="M137" s="0"/>
+      <c r="N137" s="0"/>
+      <c r="O137" s="0"/>
+      <c r="P137" s="0"/>
+      <c r="Q137" s="0"/>
+    </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B138" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C138" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="D138" s="12" t="n">
+        <v>77</v>
+      </c>
+      <c r="E138" s="12" t="n">
+        <f aca="false">D138/10.36</f>
+        <v>7.43243243243243</v>
+      </c>
+      <c r="F138" s="12" t="n">
+        <v>15</v>
+      </c>
+      <c r="G138" s="13" t="n">
+        <v>43915</v>
+      </c>
+      <c r="H138" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$130,G138)</f>
+        <v>1</v>
+      </c>
+      <c r="I138" s="13" t="n">
+        <f aca="false">B$130+1</f>
+        <v>43917</v>
+      </c>
+      <c r="J138" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$130,I138)</f>
+        <v>-1</v>
+      </c>
+      <c r="K138" s="13" t="n">
+        <f aca="false">B$130+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L138" s="0"/>
+      <c r="M138" s="0"/>
+      <c r="N138" s="0"/>
+      <c r="O138" s="0"/>
+      <c r="P138" s="0"/>
+      <c r="Q138" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
updated with 2020-04-05 available data
</commit_message>
<xml_diff>
--- a/covid19 lockdown evaluation .xlsx
+++ b/covid19 lockdown evaluation .xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="53">
   <si>
     <t>Effects of the lockdown issued by governments</t>
   </si>
@@ -26,7 +26,7 @@
     <t>0n Apr, 5th, data for USA changed: malues for 2, 3 was:  6071, 7232 – they becomes:  6076, 7121</t>
   </si>
   <si>
-    <t>6071, </t>
+    <t>6071,</t>
   </si>
   <si>
     <t>LEGENDA</t>
@@ -279,7 +279,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -336,10 +336,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -357,9 +353,9 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q138"/>
+  <dimension ref="A1:Q150"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F31" activeCellId="0" sqref="F31"/>
     </sheetView>
   </sheetViews>
@@ -809,7 +805,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="7" t="n">
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="D22" s="0"/>
       <c r="E22" s="8" t="s">
@@ -886,31 +882,31 @@
         <v>300</v>
       </c>
       <c r="D24" s="1" t="n">
-        <v>15362</v>
+        <v>15887</v>
       </c>
       <c r="E24" s="12" t="n">
         <f aca="false">D24/60.48</f>
-        <v>254.001322751323</v>
+        <v>262.681878306878</v>
       </c>
       <c r="F24" s="12" t="n">
-        <v>681</v>
+        <v>525</v>
       </c>
       <c r="G24" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H24" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,G24)</f>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I24" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J24" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I24)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K24" s="13" t="n">
-        <f aca="false">$B$22+1</f>
+        <f aca="false">$B$34+1</f>
         <v>43926</v>
       </c>
       <c r="L24" s="0" t="n">
@@ -931,31 +927,31 @@
         <v>230</v>
       </c>
       <c r="D25" s="1" t="n">
-        <v>11947</v>
+        <v>12641</v>
       </c>
       <c r="E25" s="12" t="n">
         <f aca="false">D25/46.75</f>
-        <v>255.550802139037</v>
+        <v>270.395721925134</v>
       </c>
       <c r="F25" s="12" t="n">
-        <v>749</v>
+        <v>694</v>
       </c>
       <c r="G25" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H25" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,G25)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I25" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J25" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I25)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K25" s="13" t="n">
-        <f aca="false">$B$22+1</f>
+        <f aca="false">$B$34+1</f>
         <v>43926</v>
       </c>
       <c r="L25" s="0" t="n">
@@ -976,31 +972,31 @@
         <v>330</v>
       </c>
       <c r="D26" s="1" t="n">
-        <v>7560</v>
+        <v>8078</v>
       </c>
       <c r="E26" s="12" t="n">
         <f aca="false">D26/65.27</f>
-        <v>115.826566569634</v>
+        <v>123.762831316072</v>
       </c>
       <c r="F26" s="12" t="n">
-        <v>1053</v>
+        <v>518</v>
       </c>
       <c r="G26" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H26" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,G26)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I26" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J26" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I26)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K26" s="13" t="n">
-        <f aca="false">$B$22+1</f>
+        <f aca="false">$B$34+1</f>
         <v>43926</v>
       </c>
       <c r="L26" s="0" t="n">
@@ -1021,32 +1017,32 @@
         <v>50</v>
       </c>
       <c r="D27" s="12" t="n">
-        <v>373</v>
+        <v>401</v>
       </c>
       <c r="E27" s="12" t="n">
         <f aca="false">D27/10.36</f>
-        <v>36.003861003861</v>
+        <v>38.7065637065637</v>
       </c>
       <c r="F27" s="12" t="n">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="G27" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H27" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,G27)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I27" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43926</v>
-      </c>
-      <c r="J27" s="14" t="n">
+        <v>43927</v>
+      </c>
+      <c r="J27" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I27)</f>
         <v>-1</v>
       </c>
       <c r="K27" s="13" t="n">
-        <f aca="false">$B$22+1</f>
+        <f aca="false">$B$34+1</f>
         <v>43926</v>
       </c>
       <c r="L27" s="0" t="n">
@@ -1067,32 +1063,32 @@
         <v>330</v>
       </c>
       <c r="D28" s="1" t="n">
-        <v>4313</v>
+        <v>4934</v>
       </c>
       <c r="E28" s="12" t="n">
         <f aca="false">D28/67.79</f>
-        <v>63.6229532379407</v>
+        <v>72.7835964006491</v>
       </c>
       <c r="F28" s="12" t="n">
-        <v>708</v>
+        <v>621</v>
       </c>
       <c r="G28" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H28" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,G28)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I28" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43926</v>
-      </c>
-      <c r="J28" s="14" t="n">
+        <v>43927</v>
+      </c>
+      <c r="J28" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I28)</f>
         <v>-1</v>
       </c>
       <c r="K28" s="13" t="n">
-        <f aca="false">$B$22+1</f>
+        <f aca="false">$B$34+1</f>
         <v>43926</v>
       </c>
       <c r="L28" s="0" t="n">
@@ -1113,32 +1109,32 @@
         <v>1660</v>
       </c>
       <c r="D29" s="1" t="n">
-        <v>8452</v>
+        <v>9616</v>
       </c>
       <c r="E29" s="12" t="n">
         <f aca="false">D29/331</f>
-        <v>25.5347432024169</v>
+        <v>29.0513595166163</v>
       </c>
       <c r="F29" s="12" t="n">
-        <v>1331</v>
+        <v>1165</v>
       </c>
       <c r="G29" s="13" t="n">
         <v>43917</v>
       </c>
       <c r="H29" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,G29)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I29" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43926</v>
-      </c>
-      <c r="J29" s="14" t="n">
+        <v>43927</v>
+      </c>
+      <c r="J29" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I29)</f>
         <v>-1</v>
       </c>
       <c r="K29" s="13" t="n">
-        <f aca="false">$B$22+1</f>
+        <f aca="false">$B$34+1</f>
         <v>43926</v>
       </c>
       <c r="L29" s="0" t="n">
@@ -1159,32 +1155,32 @@
         <v>414</v>
       </c>
       <c r="D30" s="1" t="n">
-        <v>1444</v>
+        <v>1584</v>
       </c>
       <c r="E30" s="12" t="n">
         <f aca="false">D30/83.784</f>
-        <v>17.2347942327891</v>
+        <v>18.9057576625609</v>
       </c>
       <c r="F30" s="12" t="n">
-        <v>169</v>
+        <v>140</v>
       </c>
       <c r="G30" s="13" t="n">
         <v>43918</v>
       </c>
       <c r="H30" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,G30)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I30" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43926</v>
-      </c>
-      <c r="J30" s="14" t="n">
+        <v>43927</v>
+      </c>
+      <c r="J30" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I30)</f>
         <v>-1</v>
       </c>
       <c r="K30" s="13" t="n">
-        <f aca="false">$B$22+1</f>
+        <f aca="false">$B$34+1</f>
         <v>43926</v>
       </c>
       <c r="L30" s="0" t="n">
@@ -1254,7 +1250,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="7" t="n">
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="D34" s="0"/>
       <c r="E34" s="8" t="s">
@@ -1331,36 +1327,36 @@
         <v>300</v>
       </c>
       <c r="D36" s="1" t="n">
-        <v>14681</v>
+        <v>15362</v>
       </c>
       <c r="E36" s="12" t="n">
         <f aca="false">D36/60.48</f>
-        <v>242.741402116402</v>
+        <v>254.001322751323</v>
       </c>
       <c r="F36" s="12" t="n">
-        <v>766</v>
+        <v>681</v>
       </c>
       <c r="G36" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H36" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,G36)</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I36" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J36" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I36)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K36" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="L36" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K36,G36)</f>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M36" s="0"/>
       <c r="N36" s="0"/>
@@ -1376,36 +1372,36 @@
         <v>230</v>
       </c>
       <c r="D37" s="1" t="n">
-        <v>11198</v>
+        <v>11947</v>
       </c>
       <c r="E37" s="12" t="n">
         <f aca="false">D37/46.75</f>
-        <v>239.529411764706</v>
+        <v>255.550802139037</v>
       </c>
       <c r="F37" s="12" t="n">
-        <v>850</v>
+        <v>749</v>
       </c>
       <c r="G37" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H37" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$46,G37)</f>
-        <v>16</v>
+        <f aca="false">_xlfn.DAYS($B$34,G37)</f>
+        <v>18</v>
       </c>
       <c r="I37" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J37" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I37)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K37" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="L37" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K37,G37)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M37" s="0"/>
       <c r="N37" s="0"/>
@@ -1421,36 +1417,36 @@
         <v>330</v>
       </c>
       <c r="D38" s="1" t="n">
-        <v>6507</v>
+        <v>7560</v>
       </c>
       <c r="E38" s="12" t="n">
         <f aca="false">D38/65.27</f>
-        <v>99.6935805117206</v>
+        <v>115.826566569634</v>
       </c>
       <c r="F38" s="12" t="n">
-        <v>1120</v>
+        <v>1053</v>
       </c>
       <c r="G38" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H38" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$46,G38)</f>
-        <v>11</v>
+        <f aca="false">_xlfn.DAYS($B$34,G38)</f>
+        <v>13</v>
       </c>
       <c r="I38" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J38" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I38)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K38" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="L38" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K38,G38)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="M38" s="0"/>
       <c r="N38" s="0"/>
@@ -1466,25 +1462,25 @@
         <v>50</v>
       </c>
       <c r="D39" s="12" t="n">
-        <v>358</v>
+        <v>373</v>
       </c>
       <c r="E39" s="12" t="n">
         <f aca="false">D39/10.36</f>
-        <v>34.5559845559846</v>
+        <v>36.003861003861</v>
       </c>
       <c r="F39" s="12" t="n">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="G39" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H39" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$46,G39)</f>
-        <v>8</v>
+        <f aca="false">_xlfn.DAYS($B$34,G39)</f>
+        <v>10</v>
       </c>
       <c r="I39" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="J39" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I39)</f>
@@ -1492,11 +1488,11 @@
       </c>
       <c r="K39" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="L39" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K39,G39)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M39" s="0"/>
       <c r="N39" s="0"/>
@@ -1512,25 +1508,25 @@
         <v>330</v>
       </c>
       <c r="D40" s="1" t="n">
-        <v>3605</v>
+        <v>4313</v>
       </c>
       <c r="E40" s="12" t="n">
         <f aca="false">D40/67.79</f>
-        <v>53.1789349461573</v>
+        <v>63.6229532379407</v>
       </c>
       <c r="F40" s="12" t="n">
-        <v>684</v>
+        <v>708</v>
       </c>
       <c r="G40" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H40" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$46,G40)</f>
-        <v>7</v>
+        <f aca="false">_xlfn.DAYS($B$34,G40)</f>
+        <v>9</v>
       </c>
       <c r="I40" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="J40" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I40)</f>
@@ -1538,11 +1534,11 @@
       </c>
       <c r="K40" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="L40" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K40,G40)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M40" s="0"/>
       <c r="N40" s="0"/>
@@ -1558,25 +1554,25 @@
         <v>1660</v>
       </c>
       <c r="D41" s="1" t="n">
-        <v>7121</v>
+        <v>8451</v>
       </c>
       <c r="E41" s="12" t="n">
         <f aca="false">D41/331</f>
-        <v>21.5135951661631</v>
+        <v>25.5317220543807</v>
       </c>
       <c r="F41" s="12" t="n">
-        <v>1045</v>
+        <v>1330</v>
       </c>
       <c r="G41" s="13" t="n">
         <v>43917</v>
       </c>
       <c r="H41" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$46,G41)</f>
-        <v>6</v>
+        <f aca="false">_xlfn.DAYS($B$34,G41)</f>
+        <v>8</v>
       </c>
       <c r="I41" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="J41" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I41)</f>
@@ -1584,11 +1580,11 @@
       </c>
       <c r="K41" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="L41" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K41,G41)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M41" s="0"/>
       <c r="N41" s="0"/>
@@ -1604,25 +1600,25 @@
         <v>414</v>
       </c>
       <c r="D42" s="1" t="n">
-        <v>1275</v>
+        <v>1444</v>
       </c>
       <c r="E42" s="12" t="n">
         <f aca="false">D42/83.784</f>
-        <v>15.2177026639931</v>
+        <v>17.2347942327891</v>
       </c>
       <c r="F42" s="12" t="n">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G42" s="13" t="n">
         <v>43918</v>
       </c>
       <c r="H42" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$46,G42)</f>
-        <v>5</v>
+        <f aca="false">_xlfn.DAYS($B$34,G42)</f>
+        <v>7</v>
       </c>
       <c r="I42" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="J42" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I42)</f>
@@ -1630,11 +1626,11 @@
       </c>
       <c r="K42" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="L42" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K42,G42)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M42" s="0"/>
       <c r="N42" s="0"/>
@@ -1699,7 +1695,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="7" t="n">
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="D46" s="0"/>
       <c r="E46" s="8" t="s">
@@ -1776,36 +1772,36 @@
         <v>300</v>
       </c>
       <c r="D48" s="1" t="n">
-        <v>13915</v>
+        <v>14681</v>
       </c>
       <c r="E48" s="12" t="n">
         <f aca="false">D48/60.48</f>
-        <v>230.076058201058</v>
+        <v>242.741402116402</v>
       </c>
       <c r="F48" s="12" t="n">
-        <v>760</v>
+        <v>766</v>
       </c>
       <c r="G48" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H48" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,G48)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I48" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J48" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I48)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K48" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="L48" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K48,G48)</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M48" s="0"/>
       <c r="N48" s="0"/>
@@ -1821,20 +1817,20 @@
         <v>230</v>
       </c>
       <c r="D49" s="1" t="n">
-        <v>10348</v>
+        <v>11198</v>
       </c>
       <c r="E49" s="12" t="n">
         <f aca="false">D49/46.75</f>
-        <v>221.347593582888</v>
+        <v>239.529411764706</v>
       </c>
       <c r="F49" s="12" t="n">
-        <v>961</v>
+        <v>850</v>
       </c>
       <c r="G49" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H49" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$46,G49)</f>
+        <f aca="false">_xlfn.DAYS($B$58,G49)</f>
         <v>16</v>
       </c>
       <c r="I49" s="13" t="n">
@@ -1842,15 +1838,15 @@
       </c>
       <c r="J49" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I49)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K49" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="L49" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K49,G49)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M49" s="0"/>
       <c r="N49" s="0"/>
@@ -1866,20 +1862,20 @@
         <v>330</v>
       </c>
       <c r="D50" s="1" t="n">
-        <v>5387</v>
+        <v>6507</v>
       </c>
       <c r="E50" s="12" t="n">
         <f aca="false">D50/65.27</f>
-        <v>82.5340891680711</v>
+        <v>99.6935805117206</v>
       </c>
       <c r="F50" s="12" t="n">
-        <v>1355</v>
+        <v>1120</v>
       </c>
       <c r="G50" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H50" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$46,G50)</f>
+        <f aca="false">_xlfn.DAYS($B$58,G50)</f>
         <v>11</v>
       </c>
       <c r="I50" s="13" t="n">
@@ -1887,15 +1883,15 @@
       </c>
       <c r="J50" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I50)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K50" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="L50" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K50,G50)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M50" s="0"/>
       <c r="N50" s="0"/>
@@ -1911,25 +1907,25 @@
         <v>50</v>
       </c>
       <c r="D51" s="12" t="n">
-        <v>308</v>
+        <v>358</v>
       </c>
       <c r="E51" s="12" t="n">
         <f aca="false">D51/10.36</f>
-        <v>29.7297297297297</v>
+        <v>34.5559845559846</v>
       </c>
       <c r="F51" s="12" t="n">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="G51" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H51" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$46,G51)</f>
+        <f aca="false">_xlfn.DAYS($B$58,G51)</f>
         <v>8</v>
       </c>
       <c r="I51" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="J51" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I51)</f>
@@ -1937,11 +1933,11 @@
       </c>
       <c r="K51" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="L51" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K51,G51)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M51" s="0"/>
       <c r="N51" s="0"/>
@@ -1957,25 +1953,25 @@
         <v>330</v>
       </c>
       <c r="D52" s="1" t="n">
-        <v>2921</v>
+        <v>3605</v>
       </c>
       <c r="E52" s="12" t="n">
         <f aca="false">D52/67.79</f>
-        <v>43.0889511727393</v>
+        <v>53.1789349461573</v>
       </c>
       <c r="F52" s="12" t="n">
-        <v>569</v>
+        <v>684</v>
       </c>
       <c r="G52" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H52" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$46,G52)</f>
+        <f aca="false">_xlfn.DAYS($B$58,G52)</f>
         <v>7</v>
       </c>
       <c r="I52" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="J52" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I52)</f>
@@ -1983,11 +1979,11 @@
       </c>
       <c r="K52" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="L52" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K52,G52)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M52" s="0"/>
       <c r="N52" s="0"/>
@@ -2003,25 +1999,25 @@
         <v>1660</v>
       </c>
       <c r="D53" s="1" t="n">
-        <v>6076</v>
+        <v>7121</v>
       </c>
       <c r="E53" s="12" t="n">
         <f aca="false">D53/331</f>
-        <v>18.3564954682779</v>
+        <v>21.5135951661631</v>
       </c>
       <c r="F53" s="12" t="n">
-        <v>969</v>
+        <v>1045</v>
       </c>
       <c r="G53" s="13" t="n">
         <v>43917</v>
       </c>
       <c r="H53" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$46,G53)</f>
+        <f aca="false">_xlfn.DAYS($B$58,G53)</f>
         <v>6</v>
       </c>
       <c r="I53" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="J53" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I53)</f>
@@ -2029,11 +2025,11 @@
       </c>
       <c r="K53" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="L53" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K53,G53)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M53" s="0"/>
       <c r="N53" s="0"/>
@@ -2049,25 +2045,25 @@
         <v>414</v>
       </c>
       <c r="D54" s="1" t="n">
-        <v>1107</v>
+        <v>1275</v>
       </c>
       <c r="E54" s="12" t="n">
         <f aca="false">D54/83.784</f>
-        <v>13.212546548267</v>
+        <v>15.2177026639931</v>
       </c>
       <c r="F54" s="12" t="n">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="G54" s="13" t="n">
         <v>43918</v>
       </c>
       <c r="H54" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$46,G54)</f>
+        <f aca="false">_xlfn.DAYS($B$58,G54)</f>
         <v>5</v>
       </c>
       <c r="I54" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="J54" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I54)</f>
@@ -2075,11 +2071,11 @@
       </c>
       <c r="K54" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="L54" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K54,G54)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M54" s="0"/>
       <c r="N54" s="0"/>
@@ -2144,7 +2140,7 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="7" t="n">
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="D58" s="0"/>
       <c r="E58" s="8" t="s">
@@ -2221,36 +2217,36 @@
         <v>300</v>
       </c>
       <c r="D60" s="1" t="n">
-        <v>13155</v>
+        <v>13915</v>
       </c>
       <c r="E60" s="12" t="n">
         <f aca="false">D60/60.48</f>
-        <v>217.509920634921</v>
+        <v>230.076058201058</v>
       </c>
       <c r="F60" s="12" t="n">
-        <v>727</v>
+        <v>760</v>
       </c>
       <c r="G60" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H60" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,G60)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I60" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J60" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I60)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K60" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="L60" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K60,G60)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M60" s="0"/>
       <c r="N60" s="0"/>
@@ -2266,36 +2262,36 @@
         <v>230</v>
       </c>
       <c r="D61" s="1" t="n">
-        <v>9387</v>
+        <v>10348</v>
       </c>
       <c r="E61" s="12" t="n">
         <f aca="false">D61/46.75</f>
-        <v>200.791443850267</v>
+        <v>221.347593582888</v>
       </c>
       <c r="F61" s="12" t="n">
-        <v>923</v>
+        <v>961</v>
       </c>
       <c r="G61" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H61" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,G61)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I61" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J61" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I61)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K61" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="L61" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K61,G61)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M61" s="0"/>
       <c r="N61" s="0"/>
@@ -2311,36 +2307,36 @@
         <v>330</v>
       </c>
       <c r="D62" s="1" t="n">
-        <v>4032</v>
+        <v>5387</v>
       </c>
       <c r="E62" s="12" t="n">
         <f aca="false">D62/65.27</f>
-        <v>61.7741688371381</v>
+        <v>82.5340891680711</v>
       </c>
       <c r="F62" s="12" t="n">
-        <v>509</v>
+        <v>1355</v>
       </c>
       <c r="G62" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H62" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,G62)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I62" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J62" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I62)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K62" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="L62" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K62,G62)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M62" s="0"/>
       <c r="N62" s="0"/>
@@ -2356,25 +2352,25 @@
         <v>50</v>
       </c>
       <c r="D63" s="12" t="n">
-        <v>239</v>
+        <v>308</v>
       </c>
       <c r="E63" s="12" t="n">
         <f aca="false">D63/10.36</f>
-        <v>23.0694980694981</v>
+        <v>29.7297297297297</v>
       </c>
       <c r="F63" s="12" t="n">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="G63" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H63" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,G63)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I63" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="J63" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I63)</f>
@@ -2382,11 +2378,11 @@
       </c>
       <c r="K63" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="L63" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K63,G63)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M63" s="0"/>
       <c r="N63" s="0"/>
@@ -2402,25 +2398,25 @@
         <v>330</v>
       </c>
       <c r="D64" s="1" t="n">
-        <v>2352</v>
+        <v>2921</v>
       </c>
       <c r="E64" s="12" t="n">
         <f aca="false">D64/67.79</f>
-        <v>34.695382799823</v>
+        <v>43.0889511727393</v>
       </c>
       <c r="F64" s="12" t="n">
-        <v>563</v>
+        <v>569</v>
       </c>
       <c r="G64" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H64" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,G64)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I64" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="J64" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I64)</f>
@@ -2428,11 +2424,11 @@
       </c>
       <c r="K64" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="L64" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K64,G64)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M64" s="0"/>
       <c r="N64" s="0"/>
@@ -2448,25 +2444,25 @@
         <v>1660</v>
       </c>
       <c r="D65" s="1" t="n">
-        <v>5102</v>
+        <v>6076</v>
       </c>
       <c r="E65" s="12" t="n">
         <f aca="false">D65/331</f>
-        <v>15.4138972809668</v>
+        <v>18.3564954682779</v>
       </c>
       <c r="F65" s="12" t="n">
-        <v>1049</v>
+        <v>969</v>
       </c>
       <c r="G65" s="13" t="n">
         <v>43917</v>
       </c>
       <c r="H65" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,G65)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I65" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="J65" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I65)</f>
@@ -2474,11 +2470,11 @@
       </c>
       <c r="K65" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="L65" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K65,G65)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M65" s="0"/>
       <c r="N65" s="0"/>
@@ -2494,25 +2490,25 @@
         <v>414</v>
       </c>
       <c r="D66" s="1" t="n">
-        <v>931</v>
+        <v>1107</v>
       </c>
       <c r="E66" s="12" t="n">
         <f aca="false">D66/83.784</f>
-        <v>11.1119068079824</v>
+        <v>13.212546548267</v>
       </c>
       <c r="F66" s="12" t="n">
-        <v>156</v>
+        <v>176</v>
       </c>
       <c r="G66" s="13" t="n">
         <v>43918</v>
       </c>
       <c r="H66" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,G66)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I66" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="J66" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I66)</f>
@@ -2520,11 +2516,11 @@
       </c>
       <c r="K66" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="L66" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K66,G66)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M66" s="0"/>
       <c r="N66" s="0"/>
@@ -2589,7 +2585,7 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="7" t="n">
-        <v>43921</v>
+        <v>43922</v>
       </c>
       <c r="D70" s="0"/>
       <c r="E70" s="8" t="s">
@@ -2666,36 +2662,36 @@
         <v>300</v>
       </c>
       <c r="D72" s="1" t="n">
-        <v>12428</v>
+        <v>13155</v>
       </c>
       <c r="E72" s="12" t="n">
         <f aca="false">D72/60.48</f>
-        <v>205.489417989418</v>
+        <v>217.509920634921</v>
       </c>
       <c r="F72" s="12" t="n">
-        <v>837</v>
+        <v>727</v>
       </c>
       <c r="G72" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H72" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,G72)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I72" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J72" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,I72)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K72" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L72" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K72,G72)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M72" s="0"/>
       <c r="N72" s="0"/>
@@ -2711,36 +2707,36 @@
         <v>230</v>
       </c>
       <c r="D73" s="1" t="n">
-        <v>8464</v>
+        <v>9387</v>
       </c>
       <c r="E73" s="12" t="n">
         <f aca="false">D73/46.75</f>
-        <v>181.048128342246</v>
+        <v>200.791443850267</v>
       </c>
       <c r="F73" s="12" t="n">
-        <v>748</v>
+        <v>923</v>
       </c>
       <c r="G73" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H73" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,G73)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I73" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J73" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,I73)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K73" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L73" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K73,G73)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M73" s="0"/>
       <c r="N73" s="0"/>
@@ -2756,36 +2752,36 @@
         <v>330</v>
       </c>
       <c r="D74" s="1" t="n">
-        <v>3523</v>
+        <v>4032</v>
       </c>
       <c r="E74" s="12" t="n">
         <f aca="false">D74/65.27</f>
-        <v>53.9757928604259</v>
+        <v>61.7741688371381</v>
       </c>
       <c r="F74" s="12" t="n">
-        <v>499</v>
+        <v>509</v>
       </c>
       <c r="G74" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H74" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,G74)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I74" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J74" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,I74)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K74" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L74" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K74,G74)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M74" s="0"/>
       <c r="N74" s="0"/>
@@ -2801,25 +2797,25 @@
         <v>50</v>
       </c>
       <c r="D75" s="12" t="n">
-        <v>180</v>
+        <v>239</v>
       </c>
       <c r="E75" s="12" t="n">
         <f aca="false">D75/10.36</f>
-        <v>17.3745173745174</v>
+        <v>23.0694980694981</v>
       </c>
       <c r="F75" s="12" t="n">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="G75" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H75" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,G75)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I75" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="J75" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,I75)</f>
@@ -2827,11 +2823,11 @@
       </c>
       <c r="K75" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L75" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K75,G75)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M75" s="0"/>
       <c r="N75" s="0"/>
@@ -2847,25 +2843,25 @@
         <v>330</v>
       </c>
       <c r="D76" s="1" t="n">
-        <v>1789</v>
+        <v>2352</v>
       </c>
       <c r="E76" s="12" t="n">
         <f aca="false">D76/67.79</f>
-        <v>26.390323056498</v>
+        <v>34.695382799823</v>
       </c>
       <c r="F76" s="12" t="n">
-        <v>381</v>
+        <v>563</v>
       </c>
       <c r="G76" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H76" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,G76)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I76" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="J76" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,I76)</f>
@@ -2873,11 +2869,11 @@
       </c>
       <c r="K76" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L76" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K76,G76)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M76" s="0"/>
       <c r="N76" s="0"/>
@@ -2893,25 +2889,25 @@
         <v>1660</v>
       </c>
       <c r="D77" s="1" t="n">
-        <v>4053</v>
+        <v>5102</v>
       </c>
       <c r="E77" s="12" t="n">
         <f aca="false">D77/331</f>
-        <v>12.2447129909366</v>
+        <v>15.4138972809668</v>
       </c>
       <c r="F77" s="12" t="n">
-        <v>912</v>
+        <v>1049</v>
       </c>
       <c r="G77" s="13" t="n">
         <v>43917</v>
       </c>
       <c r="H77" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,G77)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I77" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="J77" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,I77)</f>
@@ -2919,11 +2915,11 @@
       </c>
       <c r="K77" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L77" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K77,G77)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M77" s="0"/>
       <c r="N77" s="0"/>
@@ -2939,25 +2935,25 @@
         <v>414</v>
       </c>
       <c r="D78" s="1" t="n">
-        <v>775</v>
+        <v>931</v>
       </c>
       <c r="E78" s="12" t="n">
         <f aca="false">D78/83.784</f>
-        <v>9.24997612909386</v>
+        <v>11.1119068079824</v>
       </c>
       <c r="F78" s="12" t="n">
-        <v>130</v>
+        <v>156</v>
       </c>
       <c r="G78" s="13" t="n">
         <v>43918</v>
       </c>
       <c r="H78" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,G78)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I78" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="J78" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,I78)</f>
@@ -2965,11 +2961,11 @@
       </c>
       <c r="K78" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L78" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K78,G78)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M78" s="0"/>
       <c r="N78" s="0"/>
@@ -2978,15 +2974,16 @@
       <c r="Q78" s="0"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C79" s="12"/>
+      <c r="B79" s="4"/>
+      <c r="C79" s="5"/>
       <c r="D79" s="0"/>
-      <c r="E79" s="12"/>
-      <c r="F79" s="12"/>
-      <c r="G79" s="13"/>
+      <c r="E79" s="0"/>
+      <c r="F79" s="0"/>
+      <c r="G79" s="0"/>
       <c r="H79" s="0"/>
-      <c r="I79" s="13"/>
+      <c r="I79" s="0"/>
       <c r="J79" s="0"/>
-      <c r="K79" s="13"/>
+      <c r="K79" s="0"/>
       <c r="L79" s="0"/>
       <c r="M79" s="0"/>
       <c r="N79" s="0"/>
@@ -2995,15 +2992,16 @@
       <c r="Q79" s="0"/>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C80" s="12"/>
+      <c r="B80" s="4"/>
+      <c r="C80" s="5"/>
       <c r="D80" s="0"/>
-      <c r="E80" s="12"/>
-      <c r="F80" s="12"/>
-      <c r="G80" s="13"/>
+      <c r="E80" s="0"/>
+      <c r="F80" s="0"/>
+      <c r="G80" s="0"/>
       <c r="H80" s="0"/>
-      <c r="I80" s="13"/>
+      <c r="I80" s="0"/>
       <c r="J80" s="0"/>
-      <c r="K80" s="13"/>
+      <c r="K80" s="0"/>
       <c r="L80" s="0"/>
       <c r="M80" s="0"/>
       <c r="N80" s="0"/>
@@ -3032,7 +3030,7 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="7" t="n">
-        <v>43920</v>
+        <v>43921</v>
       </c>
       <c r="D82" s="0"/>
       <c r="E82" s="8" t="s">
@@ -3054,7 +3052,9 @@
       <c r="K82" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="L82" s="0"/>
+      <c r="L82" s="8" t="s">
+        <v>37</v>
+      </c>
       <c r="M82" s="0"/>
       <c r="N82" s="0"/>
       <c r="O82" s="0"/>
@@ -3090,7 +3090,9 @@
       <c r="K83" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="L83" s="0"/>
+      <c r="L83" s="8" t="s">
+        <v>45</v>
+      </c>
       <c r="M83" s="0"/>
       <c r="N83" s="0"/>
       <c r="O83" s="0"/>
@@ -3105,34 +3107,37 @@
         <v>300</v>
       </c>
       <c r="D84" s="1" t="n">
-        <v>11591</v>
+        <v>12428</v>
       </c>
       <c r="E84" s="12" t="n">
         <f aca="false">D84/60.48</f>
-        <v>191.650132275132</v>
+        <v>205.489417989418</v>
       </c>
       <c r="F84" s="12" t="n">
-        <v>812</v>
+        <v>837</v>
       </c>
       <c r="G84" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H84" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,G84)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I84" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J84" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,I84)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K84" s="13" t="n">
-        <f aca="false">$B$94+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L84" s="0"/>
+        <f aca="false">$B$82+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L84" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K84,G84)</f>
+        <v>22</v>
+      </c>
       <c r="M84" s="0"/>
       <c r="N84" s="0"/>
       <c r="O84" s="0"/>
@@ -3147,34 +3152,37 @@
         <v>230</v>
       </c>
       <c r="D85" s="1" t="n">
-        <v>7716</v>
+        <v>8464</v>
       </c>
       <c r="E85" s="12" t="n">
         <f aca="false">D85/46.75</f>
-        <v>165.048128342246</v>
+        <v>181.048128342246</v>
       </c>
       <c r="F85" s="12" t="n">
-        <v>913</v>
+        <v>748</v>
       </c>
       <c r="G85" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H85" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,G85)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I85" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J85" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,I85)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K85" s="13" t="n">
-        <f aca="false">$B$94+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L85" s="0"/>
+        <f aca="false">$B$82+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L85" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K85,G85)</f>
+        <v>15</v>
+      </c>
       <c r="M85" s="0"/>
       <c r="N85" s="0"/>
       <c r="O85" s="0"/>
@@ -3189,34 +3197,37 @@
         <v>330</v>
       </c>
       <c r="D86" s="1" t="n">
-        <v>3024</v>
+        <v>3523</v>
       </c>
       <c r="E86" s="12" t="n">
         <f aca="false">D86/65.27</f>
-        <v>46.3306266278535</v>
+        <v>53.9757928604259</v>
       </c>
       <c r="F86" s="12" t="n">
-        <v>418</v>
+        <v>499</v>
       </c>
       <c r="G86" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H86" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,G86)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I86" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J86" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,I86)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K86" s="13" t="n">
-        <f aca="false">$B$94+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L86" s="0"/>
+        <f aca="false">$B$82+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L86" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K86,G86)</f>
+        <v>10</v>
+      </c>
       <c r="M86" s="0"/>
       <c r="N86" s="0"/>
       <c r="O86" s="0"/>
@@ -3231,35 +3242,38 @@
         <v>50</v>
       </c>
       <c r="D87" s="12" t="n">
-        <v>146</v>
+        <v>180</v>
       </c>
       <c r="E87" s="12" t="n">
         <f aca="false">D87/10.36</f>
-        <v>14.0926640926641</v>
+        <v>17.3745173745174</v>
       </c>
       <c r="F87" s="12" t="n">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G87" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H87" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,G87)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I87" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43921</v>
+        <v>43922</v>
       </c>
       <c r="J87" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,I87)</f>
         <v>-1</v>
       </c>
       <c r="K87" s="13" t="n">
-        <f aca="false">$B$94+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L87" s="0"/>
+        <f aca="false">$B$82+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L87" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K87,G87)</f>
+        <v>7</v>
+      </c>
       <c r="M87" s="0"/>
       <c r="N87" s="0"/>
       <c r="O87" s="0"/>
@@ -3274,35 +3288,38 @@
         <v>330</v>
       </c>
       <c r="D88" s="1" t="n">
-        <v>1408</v>
+        <v>1789</v>
       </c>
       <c r="E88" s="12" t="n">
         <f aca="false">D88/67.79</f>
-        <v>20.770025077445</v>
+        <v>26.390323056498</v>
       </c>
       <c r="F88" s="12" t="n">
-        <v>180</v>
+        <v>381</v>
       </c>
       <c r="G88" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H88" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,G88)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I88" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43921</v>
+        <v>43922</v>
       </c>
       <c r="J88" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,I88)</f>
         <v>-1</v>
       </c>
       <c r="K88" s="13" t="n">
-        <f aca="false">$B$94+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L88" s="0"/>
+        <f aca="false">$B$82+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L88" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K88,G88)</f>
+        <v>6</v>
+      </c>
       <c r="M88" s="0"/>
       <c r="N88" s="0"/>
       <c r="O88" s="0"/>
@@ -3317,34 +3334,38 @@
         <v>1660</v>
       </c>
       <c r="D89" s="1" t="n">
-        <v>3141</v>
+        <v>4053</v>
       </c>
       <c r="E89" s="12" t="n">
         <f aca="false">D89/331</f>
-        <v>9.48942598187311</v>
+        <v>12.2447129909366</v>
       </c>
       <c r="F89" s="12" t="n">
-        <v>573</v>
+        <v>912</v>
       </c>
       <c r="G89" s="13" t="n">
         <v>43917</v>
       </c>
       <c r="H89" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,G89)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I89" s="13" t="n">
-        <v>43920</v>
+        <f aca="false">$B$82+1</f>
+        <v>43922</v>
       </c>
       <c r="J89" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,I89)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="K89" s="13" t="n">
-        <f aca="false">$B$94+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L89" s="0"/>
+        <f aca="false">$B$82+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L89" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K89,G89)</f>
+        <v>5</v>
+      </c>
       <c r="M89" s="0"/>
       <c r="N89" s="0"/>
       <c r="O89" s="0"/>
@@ -3359,35 +3380,38 @@
         <v>414</v>
       </c>
       <c r="D90" s="1" t="n">
-        <v>645</v>
+        <v>775</v>
       </c>
       <c r="E90" s="12" t="n">
         <f aca="false">D90/83.784</f>
-        <v>7.69836723002005</v>
+        <v>9.24997612909386</v>
       </c>
       <c r="F90" s="12" t="n">
-        <v>104</v>
+        <v>130</v>
       </c>
       <c r="G90" s="13" t="n">
         <v>43918</v>
       </c>
       <c r="H90" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,G90)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I90" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43921</v>
+        <v>43922</v>
       </c>
       <c r="J90" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,I90)</f>
         <v>-1</v>
       </c>
       <c r="K90" s="13" t="n">
-        <f aca="false">$B$94+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L90" s="0"/>
+        <f aca="false">$B$82+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L90" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K90,G90)</f>
+        <v>4</v>
+      </c>
       <c r="M90" s="0"/>
       <c r="N90" s="0"/>
       <c r="O90" s="0"/>
@@ -3395,16 +3419,15 @@
       <c r="Q90" s="0"/>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B91" s="4"/>
-      <c r="C91" s="5"/>
+      <c r="C91" s="12"/>
       <c r="D91" s="0"/>
-      <c r="E91" s="0"/>
-      <c r="F91" s="0"/>
-      <c r="G91" s="0"/>
+      <c r="E91" s="12"/>
+      <c r="F91" s="12"/>
+      <c r="G91" s="13"/>
       <c r="H91" s="0"/>
-      <c r="I91" s="0"/>
+      <c r="I91" s="13"/>
       <c r="J91" s="0"/>
-      <c r="K91" s="0"/>
+      <c r="K91" s="13"/>
       <c r="L91" s="0"/>
       <c r="M91" s="0"/>
       <c r="N91" s="0"/>
@@ -3413,16 +3436,15 @@
       <c r="Q91" s="0"/>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B92" s="4"/>
-      <c r="C92" s="5"/>
+      <c r="C92" s="12"/>
       <c r="D92" s="0"/>
-      <c r="E92" s="0"/>
-      <c r="F92" s="0"/>
-      <c r="G92" s="0"/>
+      <c r="E92" s="12"/>
+      <c r="F92" s="12"/>
+      <c r="G92" s="13"/>
       <c r="H92" s="0"/>
-      <c r="I92" s="0"/>
+      <c r="I92" s="13"/>
       <c r="J92" s="0"/>
-      <c r="K92" s="0"/>
+      <c r="K92" s="13"/>
       <c r="L92" s="0"/>
       <c r="M92" s="0"/>
       <c r="N92" s="0"/>
@@ -3451,7 +3473,7 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="7" t="n">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="D94" s="0"/>
       <c r="E94" s="8" t="s">
@@ -3524,31 +3546,31 @@
         <v>300</v>
       </c>
       <c r="D96" s="1" t="n">
-        <v>10779</v>
+        <v>11591</v>
       </c>
       <c r="E96" s="12" t="n">
         <f aca="false">D96/60.48</f>
-        <v>178.224206349206</v>
+        <v>191.650132275132</v>
       </c>
       <c r="F96" s="12" t="n">
-        <v>756</v>
+        <v>812</v>
       </c>
       <c r="G96" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H96" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,G96)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I96" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J96" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,I96)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K96" s="13" t="n">
-        <f aca="false">$B$94+1</f>
+        <f aca="false">$B$106+1</f>
         <v>43920</v>
       </c>
       <c r="L96" s="0"/>
@@ -3566,31 +3588,31 @@
         <v>230</v>
       </c>
       <c r="D97" s="1" t="n">
-        <v>6803</v>
+        <v>7716</v>
       </c>
       <c r="E97" s="12" t="n">
         <f aca="false">D97/46.75</f>
-        <v>145.51871657754</v>
+        <v>165.048128342246</v>
       </c>
       <c r="F97" s="12" t="n">
-        <v>821</v>
+        <v>913</v>
       </c>
       <c r="G97" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H97" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,G97)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I97" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J97" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,I97)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K97" s="13" t="n">
-        <f aca="false">$B$94+1</f>
+        <f aca="false">$B$106+1</f>
         <v>43920</v>
       </c>
       <c r="L97" s="0"/>
@@ -3608,31 +3630,31 @@
         <v>330</v>
       </c>
       <c r="D98" s="1" t="n">
-        <v>2606</v>
+        <v>3024</v>
       </c>
       <c r="E98" s="12" t="n">
         <f aca="false">D98/65.27</f>
-        <v>39.9264593228129</v>
+        <v>46.3306266278535</v>
       </c>
       <c r="F98" s="12" t="n">
-        <v>292</v>
+        <v>418</v>
       </c>
       <c r="G98" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H98" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,G98)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I98" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J98" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,I98)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K98" s="13" t="n">
-        <f aca="false">$B$94+1</f>
+        <f aca="false">$B$106+1</f>
         <v>43920</v>
       </c>
       <c r="L98" s="0"/>
@@ -3644,38 +3666,38 @@
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="0" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C99" s="12" t="n">
-        <v>1660</v>
-      </c>
-      <c r="D99" s="1" t="n">
-        <v>2583</v>
+        <v>50</v>
+      </c>
+      <c r="D99" s="12" t="n">
+        <v>146</v>
       </c>
       <c r="E99" s="12" t="n">
-        <f aca="false">D99/331</f>
-        <v>7.8036253776435</v>
+        <f aca="false">D99/10.36</f>
+        <v>14.0926640926641</v>
       </c>
       <c r="F99" s="12" t="n">
-        <v>363</v>
+        <v>36</v>
       </c>
       <c r="G99" s="13" t="n">
-        <v>43917</v>
+        <v>43915</v>
       </c>
       <c r="H99" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,G99)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I99" s="13" t="n">
         <f aca="false">$B$94+1</f>
-        <v>43920</v>
+        <v>43921</v>
       </c>
       <c r="J99" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,I99)</f>
         <v>-1</v>
       </c>
       <c r="K99" s="13" t="n">
-        <f aca="false">$B$94+1</f>
+        <f aca="false">$B$106+1</f>
         <v>43920</v>
       </c>
       <c r="L99" s="0"/>
@@ -3693,32 +3715,32 @@
         <v>330</v>
       </c>
       <c r="D100" s="1" t="n">
-        <v>1228</v>
+        <v>1408</v>
       </c>
       <c r="E100" s="12" t="n">
         <f aca="false">D100/67.79</f>
-        <v>18.1147661897035</v>
+        <v>20.770025077445</v>
       </c>
       <c r="F100" s="12" t="n">
-        <v>209</v>
+        <v>180</v>
       </c>
       <c r="G100" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H100" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,G100)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I100" s="13" t="n">
         <f aca="false">$B$94+1</f>
-        <v>43920</v>
+        <v>43921</v>
       </c>
       <c r="J100" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,I100)</f>
         <v>-1</v>
       </c>
       <c r="K100" s="13" t="n">
-        <f aca="false">$B$94+1</f>
+        <f aca="false">$B$106+1</f>
         <v>43920</v>
       </c>
       <c r="L100" s="0"/>
@@ -3730,38 +3752,37 @@
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C101" s="12" t="n">
-        <v>414</v>
+        <v>1660</v>
       </c>
       <c r="D101" s="1" t="n">
-        <v>541</v>
+        <v>3141</v>
       </c>
       <c r="E101" s="12" t="n">
-        <f aca="false">D101/83.784</f>
-        <v>6.457080110761</v>
+        <f aca="false">D101/331</f>
+        <v>9.48942598187311</v>
       </c>
       <c r="F101" s="12" t="n">
-        <v>108</v>
+        <v>573</v>
       </c>
       <c r="G101" s="13" t="n">
-        <v>43918</v>
+        <v>43917</v>
       </c>
       <c r="H101" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,G101)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I101" s="13" t="n">
-        <f aca="false">$B$94+1</f>
         <v>43920</v>
       </c>
       <c r="J101" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,I101)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="K101" s="13" t="n">
-        <f aca="false">$B$94+1</f>
+        <f aca="false">$B$106+1</f>
         <v>43920</v>
       </c>
       <c r="L101" s="0"/>
@@ -3773,38 +3794,38 @@
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C102" s="12" t="n">
-        <v>50</v>
-      </c>
-      <c r="D102" s="12" t="n">
-        <v>110</v>
+        <v>414</v>
+      </c>
+      <c r="D102" s="1" t="n">
+        <v>645</v>
       </c>
       <c r="E102" s="12" t="n">
-        <f aca="false">D102/10.36</f>
-        <v>10.6177606177606</v>
+        <f aca="false">D102/83.784</f>
+        <v>7.69836723002005</v>
       </c>
       <c r="F102" s="12" t="n">
-        <v>5</v>
+        <v>104</v>
       </c>
       <c r="G102" s="13" t="n">
-        <v>43915</v>
+        <v>43918</v>
       </c>
       <c r="H102" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,G102)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I102" s="13" t="n">
         <f aca="false">$B$94+1</f>
-        <v>43920</v>
+        <v>43921</v>
       </c>
       <c r="J102" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,I102)</f>
         <v>-1</v>
       </c>
       <c r="K102" s="13" t="n">
-        <f aca="false">$B$94+1</f>
+        <f aca="false">$B$106+1</f>
         <v>43920</v>
       </c>
       <c r="L102" s="0"/>
@@ -3871,15 +3892,13 @@
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="7" t="n">
-        <v>43918</v>
-      </c>
-      <c r="D106" s="8" t="s">
-        <v>10</v>
-      </c>
+        <v>43919</v>
+      </c>
+      <c r="D106" s="0"/>
       <c r="E106" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F106" s="8"/>
+      <c r="F106" s="0"/>
       <c r="G106" s="8" t="s">
         <v>33</v>
       </c>
@@ -3907,8 +3926,8 @@
       <c r="C107" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D107" s="10" t="s">
-        <v>6</v>
+      <c r="D107" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="E107" s="10" t="s">
         <v>39</v>
@@ -3946,32 +3965,32 @@
         <v>300</v>
       </c>
       <c r="D108" s="1" t="n">
-        <v>10023</v>
+        <v>10779</v>
       </c>
       <c r="E108" s="12" t="n">
         <f aca="false">D108/60.48</f>
-        <v>165.724206349206</v>
+        <v>178.224206349206</v>
       </c>
       <c r="F108" s="12" t="n">
-        <v>889</v>
+        <v>756</v>
       </c>
       <c r="G108" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H108" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,G108)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I108" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J108" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$118,I108)</f>
-        <v>15</v>
+        <f aca="false">_xlfn.DAYS($B$106,I108)</f>
+        <v>17</v>
       </c>
       <c r="K108" s="13" t="n">
         <f aca="false">$B$106+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L108" s="0"/>
       <c r="M108" s="0"/>
@@ -3988,32 +4007,32 @@
         <v>230</v>
       </c>
       <c r="D109" s="1" t="n">
-        <v>5982</v>
+        <v>6803</v>
       </c>
       <c r="E109" s="12" t="n">
         <f aca="false">D109/46.75</f>
-        <v>127.957219251337</v>
+        <v>145.51871657754</v>
       </c>
       <c r="F109" s="12" t="n">
-        <v>844</v>
+        <v>821</v>
       </c>
       <c r="G109" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H109" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,G109)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I109" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J109" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$118,I109)</f>
-        <v>4</v>
+        <f aca="false">_xlfn.DAYS($B$106,I109)</f>
+        <v>6</v>
       </c>
       <c r="K109" s="13" t="n">
         <f aca="false">$B$106+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L109" s="0"/>
       <c r="M109" s="0"/>
@@ -4030,32 +4049,32 @@
         <v>330</v>
       </c>
       <c r="D110" s="1" t="n">
-        <v>2314</v>
+        <v>2606</v>
       </c>
       <c r="E110" s="12" t="n">
         <f aca="false">D110/65.27</f>
-        <v>35.4527347939329</v>
+        <v>39.9264593228129</v>
       </c>
       <c r="F110" s="12" t="n">
-        <v>319</v>
+        <v>292</v>
       </c>
       <c r="G110" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H110" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,G110)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I110" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J110" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$118,I110)</f>
-        <v>3</v>
+        <f aca="false">_xlfn.DAYS($B$106,I110)</f>
+        <v>5</v>
       </c>
       <c r="K110" s="13" t="n">
         <f aca="false">$B$106+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L110" s="0"/>
       <c r="M110" s="0"/>
@@ -4072,25 +4091,25 @@
         <v>1660</v>
       </c>
       <c r="D111" s="1" t="n">
-        <v>2221</v>
+        <v>2583</v>
       </c>
       <c r="E111" s="12" t="n">
         <f aca="false">D111/331</f>
-        <v>6.70996978851964</v>
+        <v>7.8036253776435</v>
       </c>
       <c r="F111" s="12" t="n">
-        <v>525</v>
+        <v>363</v>
       </c>
       <c r="G111" s="13" t="n">
         <v>43917</v>
       </c>
       <c r="H111" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,G111)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I111" s="13" t="n">
         <f aca="false">$B$106+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="J111" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,I111)</f>
@@ -4098,7 +4117,7 @@
       </c>
       <c r="K111" s="13" t="n">
         <f aca="false">$B$106+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L111" s="0"/>
       <c r="M111" s="0"/>
@@ -4115,25 +4134,25 @@
         <v>330</v>
       </c>
       <c r="D112" s="1" t="n">
-        <v>1019</v>
+        <v>1228</v>
       </c>
       <c r="E112" s="12" t="n">
         <f aca="false">D112/67.79</f>
-        <v>15.0317155922702</v>
+        <v>18.1147661897035</v>
       </c>
       <c r="F112" s="12" t="n">
-        <v>260</v>
+        <v>209</v>
       </c>
       <c r="G112" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H112" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,G112)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I112" s="13" t="n">
         <f aca="false">$B$106+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="J112" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,I112)</f>
@@ -4141,7 +4160,7 @@
       </c>
       <c r="K112" s="13" t="n">
         <f aca="false">$B$106+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L112" s="0"/>
       <c r="M112" s="0"/>
@@ -4158,25 +4177,25 @@
         <v>414</v>
       </c>
       <c r="D113" s="1" t="n">
-        <v>433</v>
+        <v>541</v>
       </c>
       <c r="E113" s="12" t="n">
         <f aca="false">D113/83.784</f>
-        <v>5.16805117922276</v>
+        <v>6.457080110761</v>
       </c>
       <c r="F113" s="12" t="n">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="G113" s="13" t="n">
         <v>43918</v>
       </c>
       <c r="H113" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,G113)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I113" s="13" t="n">
         <f aca="false">$B$106+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="J113" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,I113)</f>
@@ -4184,7 +4203,7 @@
       </c>
       <c r="K113" s="13" t="n">
         <f aca="false">$B$106+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L113" s="0"/>
       <c r="M113" s="0"/>
@@ -4201,25 +4220,25 @@
         <v>50</v>
       </c>
       <c r="D114" s="12" t="n">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="E114" s="12" t="n">
         <f aca="false">D114/10.36</f>
-        <v>10.1351351351351</v>
+        <v>10.6177606177606</v>
       </c>
       <c r="F114" s="12" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G114" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H114" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,G114)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I114" s="13" t="n">
         <f aca="false">$B$106+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="J114" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,I114)</f>
@@ -4227,7 +4246,7 @@
       </c>
       <c r="K114" s="13" t="n">
         <f aca="false">$B$106+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L114" s="0"/>
       <c r="M114" s="0"/>
@@ -4237,15 +4256,16 @@
       <c r="Q114" s="0"/>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C115" s="12"/>
-      <c r="D115" s="12"/>
-      <c r="E115" s="12"/>
-      <c r="F115" s="12"/>
-      <c r="G115" s="13"/>
+      <c r="B115" s="4"/>
+      <c r="C115" s="5"/>
+      <c r="D115" s="0"/>
+      <c r="E115" s="0"/>
+      <c r="F115" s="0"/>
+      <c r="G115" s="0"/>
       <c r="H115" s="0"/>
-      <c r="I115" s="13"/>
+      <c r="I115" s="0"/>
       <c r="J115" s="0"/>
-      <c r="K115" s="13"/>
+      <c r="K115" s="0"/>
       <c r="L115" s="0"/>
       <c r="M115" s="0"/>
       <c r="N115" s="0"/>
@@ -4290,11 +4310,10 @@
       <c r="P117" s="0"/>
       <c r="Q117" s="0"/>
     </row>
-    <row r="118" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="7" t="n">
-        <v>43917</v>
-      </c>
-      <c r="C118" s="0"/>
+        <v>43918</v>
+      </c>
       <c r="D118" s="8" t="s">
         <v>10</v>
       </c>
@@ -4317,10 +4336,14 @@
       <c r="K118" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="L118" s="8"/>
+      <c r="L118" s="0"/>
+      <c r="M118" s="0"/>
+      <c r="N118" s="0"/>
+      <c r="O118" s="0"/>
+      <c r="P118" s="0"/>
+      <c r="Q118" s="0"/>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="3"/>
       <c r="B119" s="9"/>
       <c r="C119" s="10" t="s">
         <v>38</v>
@@ -4349,7 +4372,7 @@
       <c r="K119" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="L119" s="8"/>
+      <c r="L119" s="0"/>
       <c r="M119" s="0"/>
       <c r="N119" s="0"/>
       <c r="O119" s="0"/>
@@ -4364,32 +4387,32 @@
         <v>300</v>
       </c>
       <c r="D120" s="1" t="n">
-        <v>9134</v>
+        <v>10023</v>
       </c>
       <c r="E120" s="12" t="n">
         <f aca="false">D120/60.48</f>
-        <v>151.025132275132</v>
+        <v>165.724206349206</v>
       </c>
       <c r="F120" s="12" t="n">
-        <v>919</v>
+        <v>889</v>
       </c>
       <c r="G120" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H120" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$118,G120)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I120" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J120" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$118,I120)</f>
+        <f aca="false">_xlfn.DAYS(B$130,I120)</f>
         <v>15</v>
       </c>
       <c r="K120" s="13" t="n">
         <f aca="false">$B$118+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L120" s="0"/>
       <c r="M120" s="0"/>
@@ -4406,32 +4429,32 @@
         <v>230</v>
       </c>
       <c r="D121" s="1" t="n">
-        <v>5138</v>
+        <v>5982</v>
       </c>
       <c r="E121" s="12" t="n">
         <f aca="false">D121/46.75</f>
-        <v>109.903743315508</v>
+        <v>127.957219251337</v>
       </c>
       <c r="F121" s="12" t="n">
-        <v>773</v>
+        <v>844</v>
       </c>
       <c r="G121" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H121" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$118,G121)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I121" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J121" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$118,I121)</f>
+        <f aca="false">_xlfn.DAYS(B$130,I121)</f>
         <v>4</v>
       </c>
       <c r="K121" s="13" t="n">
         <f aca="false">$B$118+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L121" s="0"/>
       <c r="M121" s="0"/>
@@ -4448,32 +4471,32 @@
         <v>330</v>
       </c>
       <c r="D122" s="1" t="n">
-        <v>1995</v>
+        <v>2314</v>
       </c>
       <c r="E122" s="12" t="n">
         <f aca="false">D122/65.27</f>
-        <v>30.5653439558756</v>
+        <v>35.4527347939329</v>
       </c>
       <c r="F122" s="12" t="n">
-        <v>299</v>
+        <v>319</v>
       </c>
       <c r="G122" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H122" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$118,G122)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I122" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J122" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$118,I122)</f>
+        <f aca="false">_xlfn.DAYS(B$130,I122)</f>
         <v>3</v>
       </c>
       <c r="K122" s="13" t="n">
         <f aca="false">$B$118+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L122" s="0"/>
       <c r="M122" s="0"/>
@@ -4490,34 +4513,33 @@
         <v>1660</v>
       </c>
       <c r="D123" s="1" t="n">
-        <v>1696</v>
+        <v>2221</v>
       </c>
       <c r="E123" s="12" t="n">
         <f aca="false">D123/331</f>
-        <v>5.12386706948641</v>
+        <v>6.70996978851964</v>
       </c>
       <c r="F123" s="12" t="n">
-        <v>400</v>
+        <v>525</v>
       </c>
       <c r="G123" s="13" t="n">
-        <f aca="false">$B$118</f>
         <v>43917</v>
       </c>
       <c r="H123" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$118,G123)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I123" s="13" t="n">
         <f aca="false">$B$118+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="J123" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$118,I123)</f>
+        <f aca="false">_xlfn.DAYS($B$118,I123)</f>
         <v>-1</v>
       </c>
       <c r="K123" s="13" t="n">
         <f aca="false">$B$118+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L123" s="0"/>
       <c r="M123" s="0"/>
@@ -4534,33 +4556,33 @@
         <v>330</v>
       </c>
       <c r="D124" s="1" t="n">
-        <v>759</v>
+        <v>1019</v>
       </c>
       <c r="E124" s="12" t="n">
         <f aca="false">D124/67.79</f>
-        <v>11.1963416433102</v>
+        <v>15.0317155922702</v>
       </c>
       <c r="F124" s="12" t="n">
-        <v>181</v>
+        <v>260</v>
       </c>
       <c r="G124" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H124" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$118,G124)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I124" s="13" t="n">
         <f aca="false">$B$118+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="J124" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$118,I124)</f>
+        <f aca="false">_xlfn.DAYS($B$118,I124)</f>
         <v>-1</v>
       </c>
       <c r="K124" s="13" t="n">
         <f aca="false">$B$118+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L124" s="0"/>
       <c r="M124" s="0"/>
@@ -4577,34 +4599,33 @@
         <v>414</v>
       </c>
       <c r="D125" s="1" t="n">
-        <v>351</v>
+        <v>433</v>
       </c>
       <c r="E125" s="12" t="n">
         <f aca="false">D125/83.784</f>
-        <v>4.18934402749928</v>
+        <v>5.16805117922276</v>
       </c>
       <c r="F125" s="12" t="n">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G125" s="13" t="n">
-        <f aca="false">$B$118+1</f>
         <v>43918</v>
       </c>
       <c r="H125" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$118,G125)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="I125" s="13" t="n">
         <f aca="false">$B$118+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="J125" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$118,I125)</f>
+        <f aca="false">_xlfn.DAYS($B$118,I125)</f>
         <v>-1</v>
       </c>
       <c r="K125" s="13" t="n">
         <f aca="false">$B$118+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L125" s="0"/>
       <c r="M125" s="0"/>
@@ -4628,26 +4649,26 @@
         <v>10.1351351351351</v>
       </c>
       <c r="F126" s="12" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="G126" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H126" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$118,G126)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I126" s="13" t="n">
         <f aca="false">$B$118+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="J126" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$118,I126)</f>
+        <f aca="false">_xlfn.DAYS($B$118,I126)</f>
         <v>-1</v>
       </c>
       <c r="K126" s="13" t="n">
         <f aca="false">$B$118+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L126" s="0"/>
       <c r="M126" s="0"/>
@@ -4657,14 +4678,15 @@
       <c r="Q126" s="0"/>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D127" s="0"/>
-      <c r="E127" s="0"/>
-      <c r="F127" s="0"/>
-      <c r="G127" s="0"/>
+      <c r="C127" s="12"/>
+      <c r="D127" s="12"/>
+      <c r="E127" s="12"/>
+      <c r="F127" s="12"/>
+      <c r="G127" s="13"/>
       <c r="H127" s="0"/>
-      <c r="I127" s="0"/>
+      <c r="I127" s="13"/>
       <c r="J127" s="0"/>
-      <c r="K127" s="0"/>
+      <c r="K127" s="13"/>
       <c r="L127" s="0"/>
       <c r="M127" s="0"/>
       <c r="N127" s="0"/>
@@ -4673,6 +4695,8 @@
       <c r="Q127" s="0"/>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B128" s="4"/>
+      <c r="C128" s="5"/>
       <c r="D128" s="0"/>
       <c r="E128" s="0"/>
       <c r="F128" s="0"/>
@@ -4707,10 +4731,11 @@
       <c r="P129" s="0"/>
       <c r="Q129" s="0"/>
     </row>
-    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B130" s="7" t="n">
-        <v>43916</v>
-      </c>
+        <v>43917</v>
+      </c>
+      <c r="C130" s="0"/>
       <c r="D130" s="8" t="s">
         <v>10</v>
       </c>
@@ -4733,17 +4758,13 @@
       <c r="K130" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="L130" s="0"/>
-      <c r="M130" s="0"/>
-      <c r="N130" s="0"/>
-      <c r="O130" s="0"/>
-      <c r="P130" s="0"/>
-      <c r="Q130" s="0"/>
+      <c r="L130" s="8"/>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="3"/>
       <c r="B131" s="9"/>
       <c r="C131" s="10" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D131" s="10" t="s">
         <v>6</v>
@@ -4769,7 +4790,7 @@
       <c r="K131" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="L131" s="0"/>
+      <c r="L131" s="8"/>
       <c r="M131" s="0"/>
       <c r="N131" s="0"/>
       <c r="O131" s="0"/>
@@ -4784,32 +4805,32 @@
         <v>300</v>
       </c>
       <c r="D132" s="1" t="n">
-        <v>8215</v>
+        <v>9134</v>
       </c>
       <c r="E132" s="12" t="n">
         <f aca="false">D132/60.48</f>
-        <v>135.830026455026</v>
+        <v>151.025132275132</v>
       </c>
       <c r="F132" s="12" t="n">
-        <v>712</v>
+        <v>919</v>
       </c>
       <c r="G132" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H132" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$130,G132)</f>
-        <v>16</v>
+        <f aca="false">_xlfn.DAYS($B$130,G132)</f>
+        <v>17</v>
       </c>
       <c r="I132" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J132" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$130,I132)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K132" s="13" t="n">
-        <f aca="false">B$130+1</f>
-        <v>43917</v>
+        <f aca="false">$B$130+1</f>
+        <v>43918</v>
       </c>
       <c r="L132" s="0"/>
       <c r="M132" s="0"/>
@@ -4826,32 +4847,32 @@
         <v>230</v>
       </c>
       <c r="D133" s="1" t="n">
-        <v>4365</v>
+        <v>5138</v>
       </c>
       <c r="E133" s="12" t="n">
         <f aca="false">D133/46.75</f>
-        <v>93.3689839572193</v>
+        <v>109.903743315508</v>
       </c>
       <c r="F133" s="12" t="n">
-        <v>718</v>
+        <v>773</v>
       </c>
       <c r="G133" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H133" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$130,G133)</f>
-        <v>9</v>
+        <f aca="false">_xlfn.DAYS($B$130,G133)</f>
+        <v>10</v>
       </c>
       <c r="I133" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J133" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$130,I133)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K133" s="13" t="n">
-        <f aca="false">B$130+1</f>
-        <v>43917</v>
+        <f aca="false">$B$130+1</f>
+        <v>43918</v>
       </c>
       <c r="L133" s="0"/>
       <c r="M133" s="0"/>
@@ -4868,32 +4889,32 @@
         <v>330</v>
       </c>
       <c r="D134" s="1" t="n">
-        <v>1696</v>
+        <v>1995</v>
       </c>
       <c r="E134" s="12" t="n">
         <f aca="false">D134/65.27</f>
-        <v>25.9843726060978</v>
+        <v>30.5653439558756</v>
       </c>
       <c r="F134" s="12" t="n">
-        <v>365</v>
+        <v>299</v>
       </c>
       <c r="G134" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H134" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$130,G134)</f>
-        <v>4</v>
+        <f aca="false">_xlfn.DAYS($B$130,G134)</f>
+        <v>5</v>
       </c>
       <c r="I134" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J134" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$130,I134)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K134" s="13" t="n">
-        <f aca="false">B$130+1</f>
-        <v>43917</v>
+        <f aca="false">$B$130+1</f>
+        <v>43918</v>
       </c>
       <c r="L134" s="0"/>
       <c r="M134" s="0"/>
@@ -4910,33 +4931,34 @@
         <v>1660</v>
       </c>
       <c r="D135" s="1" t="n">
-        <v>1295</v>
+        <v>1696</v>
       </c>
       <c r="E135" s="12" t="n">
         <f aca="false">D135/331</f>
-        <v>3.91238670694864</v>
+        <v>5.12386706948641</v>
       </c>
       <c r="F135" s="12" t="n">
-        <v>268</v>
+        <v>400</v>
       </c>
       <c r="G135" s="13" t="n">
+        <f aca="false">$B$130</f>
         <v>43917</v>
       </c>
       <c r="H135" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$130,G135)</f>
+        <f aca="false">_xlfn.DAYS($B$130,G135)</f>
+        <v>0</v>
+      </c>
+      <c r="I135" s="13" t="n">
+        <f aca="false">$B$130+1</f>
+        <v>43918</v>
+      </c>
+      <c r="J135" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$130,I135)</f>
         <v>-1</v>
       </c>
-      <c r="I135" s="13" t="n">
-        <f aca="false">B$130+1</f>
-        <v>43917</v>
-      </c>
-      <c r="J135" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$130,I135)</f>
-        <v>-1</v>
-      </c>
       <c r="K135" s="13" t="n">
-        <f aca="false">B$130+1</f>
-        <v>43917</v>
+        <f aca="false">$B$130+1</f>
+        <v>43918</v>
       </c>
       <c r="L135" s="0"/>
       <c r="M135" s="0"/>
@@ -4953,33 +4975,33 @@
         <v>330</v>
       </c>
       <c r="D136" s="1" t="n">
-        <v>578</v>
+        <v>759</v>
       </c>
       <c r="E136" s="12" t="n">
         <f aca="false">D136/67.79</f>
-        <v>8.52633131730344</v>
+        <v>11.1963416433102</v>
       </c>
       <c r="F136" s="12" t="n">
-        <v>115</v>
+        <v>181</v>
       </c>
       <c r="G136" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H136" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$130,G136)</f>
-        <v>0</v>
+        <f aca="false">_xlfn.DAYS($B$130,G136)</f>
+        <v>1</v>
       </c>
       <c r="I136" s="13" t="n">
-        <f aca="false">B$130+1</f>
-        <v>43917</v>
+        <f aca="false">$B$130+1</f>
+        <v>43918</v>
       </c>
       <c r="J136" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$130,I136)</f>
         <v>-1</v>
       </c>
       <c r="K136" s="13" t="n">
-        <f aca="false">B$130+1</f>
-        <v>43917</v>
+        <f aca="false">$B$130+1</f>
+        <v>43918</v>
       </c>
       <c r="L136" s="0"/>
       <c r="M136" s="0"/>
@@ -4996,33 +5018,34 @@
         <v>414</v>
       </c>
       <c r="D137" s="1" t="n">
-        <v>267</v>
+        <v>351</v>
       </c>
       <c r="E137" s="12" t="n">
         <f aca="false">D137/83.784</f>
-        <v>3.18676596963621</v>
+        <v>4.18934402749928</v>
       </c>
       <c r="F137" s="12" t="n">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="G137" s="13" t="n">
-        <v>43917</v>
+        <f aca="false">$B$130+1</f>
+        <v>43918</v>
       </c>
       <c r="H137" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$130,G137)</f>
+        <f aca="false">_xlfn.DAYS($B$130,G137)</f>
         <v>-1</v>
       </c>
       <c r="I137" s="13" t="n">
-        <f aca="false">B$130+1</f>
-        <v>43917</v>
+        <f aca="false">$B$130+1</f>
+        <v>43918</v>
       </c>
       <c r="J137" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$130,I137)</f>
         <v>-1</v>
       </c>
       <c r="K137" s="13" t="n">
-        <f aca="false">B$130+1</f>
-        <v>43917</v>
+        <f aca="false">$B$130+1</f>
+        <v>43918</v>
       </c>
       <c r="L137" s="0"/>
       <c r="M137" s="0"/>
@@ -5039,33 +5062,33 @@
         <v>50</v>
       </c>
       <c r="D138" s="12" t="n">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="E138" s="12" t="n">
         <f aca="false">D138/10.36</f>
-        <v>7.43243243243243</v>
+        <v>10.1351351351351</v>
       </c>
       <c r="F138" s="12" t="n">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="G138" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H138" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$130,G138)</f>
-        <v>1</v>
+        <f aca="false">_xlfn.DAYS($B$130,G138)</f>
+        <v>2</v>
       </c>
       <c r="I138" s="13" t="n">
-        <f aca="false">B$130+1</f>
-        <v>43917</v>
+        <f aca="false">$B$130+1</f>
+        <v>43918</v>
       </c>
       <c r="J138" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$130,I138)</f>
         <v>-1</v>
       </c>
       <c r="K138" s="13" t="n">
-        <f aca="false">B$130+1</f>
-        <v>43917</v>
+        <f aca="false">$B$130+1</f>
+        <v>43918</v>
       </c>
       <c r="L138" s="0"/>
       <c r="M138" s="0"/>
@@ -5073,6 +5096,424 @@
       <c r="O138" s="0"/>
       <c r="P138" s="0"/>
       <c r="Q138" s="0"/>
+    </row>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D139" s="0"/>
+      <c r="E139" s="0"/>
+      <c r="F139" s="0"/>
+      <c r="G139" s="0"/>
+      <c r="H139" s="0"/>
+      <c r="I139" s="0"/>
+      <c r="J139" s="0"/>
+      <c r="K139" s="0"/>
+      <c r="L139" s="0"/>
+      <c r="M139" s="0"/>
+      <c r="N139" s="0"/>
+      <c r="O139" s="0"/>
+      <c r="P139" s="0"/>
+      <c r="Q139" s="0"/>
+    </row>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D140" s="0"/>
+      <c r="E140" s="0"/>
+      <c r="F140" s="0"/>
+      <c r="G140" s="0"/>
+      <c r="H140" s="0"/>
+      <c r="I140" s="0"/>
+      <c r="J140" s="0"/>
+      <c r="K140" s="0"/>
+      <c r="L140" s="0"/>
+      <c r="M140" s="0"/>
+      <c r="N140" s="0"/>
+      <c r="O140" s="0"/>
+      <c r="P140" s="0"/>
+      <c r="Q140" s="0"/>
+    </row>
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B141" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D141" s="0"/>
+      <c r="E141" s="0"/>
+      <c r="F141" s="0"/>
+      <c r="G141" s="0"/>
+      <c r="H141" s="0"/>
+      <c r="I141" s="0"/>
+      <c r="J141" s="0"/>
+      <c r="K141" s="0"/>
+      <c r="L141" s="0"/>
+      <c r="M141" s="0"/>
+      <c r="N141" s="0"/>
+      <c r="O141" s="0"/>
+      <c r="P141" s="0"/>
+      <c r="Q141" s="0"/>
+    </row>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B142" s="7" t="n">
+        <v>43916</v>
+      </c>
+      <c r="D142" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E142" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F142" s="8"/>
+      <c r="G142" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H142" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I142" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J142" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="K142" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="L142" s="0"/>
+      <c r="M142" s="0"/>
+      <c r="N142" s="0"/>
+      <c r="O142" s="0"/>
+      <c r="P142" s="0"/>
+      <c r="Q142" s="0"/>
+    </row>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B143" s="9"/>
+      <c r="C143" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D143" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E143" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F143" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G143" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H143" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I143" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="J143" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="K143" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="L143" s="0"/>
+      <c r="M143" s="0"/>
+      <c r="N143" s="0"/>
+      <c r="O143" s="0"/>
+      <c r="P143" s="0"/>
+      <c r="Q143" s="0"/>
+    </row>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B144" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C144" s="12" t="n">
+        <v>300</v>
+      </c>
+      <c r="D144" s="1" t="n">
+        <v>8215</v>
+      </c>
+      <c r="E144" s="12" t="n">
+        <f aca="false">D144/60.48</f>
+        <v>135.830026455026</v>
+      </c>
+      <c r="F144" s="12" t="n">
+        <v>712</v>
+      </c>
+      <c r="G144" s="13" t="n">
+        <v>43900</v>
+      </c>
+      <c r="H144" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$142,G144)</f>
+        <v>16</v>
+      </c>
+      <c r="I144" s="13" t="n">
+        <v>43902</v>
+      </c>
+      <c r="J144" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$142,I144)</f>
+        <v>14</v>
+      </c>
+      <c r="K144" s="13" t="n">
+        <f aca="false">B$142+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L144" s="0"/>
+      <c r="M144" s="0"/>
+      <c r="N144" s="0"/>
+      <c r="O144" s="0"/>
+      <c r="P144" s="0"/>
+      <c r="Q144" s="0"/>
+    </row>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B145" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C145" s="12" t="n">
+        <v>230</v>
+      </c>
+      <c r="D145" s="1" t="n">
+        <v>4365</v>
+      </c>
+      <c r="E145" s="12" t="n">
+        <f aca="false">D145/46.75</f>
+        <v>93.3689839572193</v>
+      </c>
+      <c r="F145" s="12" t="n">
+        <v>718</v>
+      </c>
+      <c r="G145" s="13" t="n">
+        <v>43907</v>
+      </c>
+      <c r="H145" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$142,G145)</f>
+        <v>9</v>
+      </c>
+      <c r="I145" s="13" t="n">
+        <v>43913</v>
+      </c>
+      <c r="J145" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$142,I145)</f>
+        <v>3</v>
+      </c>
+      <c r="K145" s="13" t="n">
+        <f aca="false">B$142+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L145" s="0"/>
+      <c r="M145" s="0"/>
+      <c r="N145" s="0"/>
+      <c r="O145" s="0"/>
+      <c r="P145" s="0"/>
+      <c r="Q145" s="0"/>
+    </row>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B146" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C146" s="12" t="n">
+        <v>330</v>
+      </c>
+      <c r="D146" s="1" t="n">
+        <v>1696</v>
+      </c>
+      <c r="E146" s="12" t="n">
+        <f aca="false">D146/65.27</f>
+        <v>25.9843726060978</v>
+      </c>
+      <c r="F146" s="12" t="n">
+        <v>365</v>
+      </c>
+      <c r="G146" s="13" t="n">
+        <v>43912</v>
+      </c>
+      <c r="H146" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$142,G146)</f>
+        <v>4</v>
+      </c>
+      <c r="I146" s="13" t="n">
+        <v>43914</v>
+      </c>
+      <c r="J146" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$142,I146)</f>
+        <v>2</v>
+      </c>
+      <c r="K146" s="13" t="n">
+        <f aca="false">B$142+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L146" s="0"/>
+      <c r="M146" s="0"/>
+      <c r="N146" s="0"/>
+      <c r="O146" s="0"/>
+      <c r="P146" s="0"/>
+      <c r="Q146" s="0"/>
+    </row>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B147" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C147" s="12" t="n">
+        <v>1660</v>
+      </c>
+      <c r="D147" s="1" t="n">
+        <v>1295</v>
+      </c>
+      <c r="E147" s="12" t="n">
+        <f aca="false">D147/331</f>
+        <v>3.91238670694864</v>
+      </c>
+      <c r="F147" s="12" t="n">
+        <v>268</v>
+      </c>
+      <c r="G147" s="13" t="n">
+        <v>43917</v>
+      </c>
+      <c r="H147" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$142,G147)</f>
+        <v>-1</v>
+      </c>
+      <c r="I147" s="13" t="n">
+        <f aca="false">B$142+1</f>
+        <v>43917</v>
+      </c>
+      <c r="J147" s="1" t="n">
+        <f aca="false">_xlfn.DAYS($B$142,I147)</f>
+        <v>-1</v>
+      </c>
+      <c r="K147" s="13" t="n">
+        <f aca="false">B$142+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L147" s="0"/>
+      <c r="M147" s="0"/>
+      <c r="N147" s="0"/>
+      <c r="O147" s="0"/>
+      <c r="P147" s="0"/>
+      <c r="Q147" s="0"/>
+    </row>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B148" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C148" s="12" t="n">
+        <v>330</v>
+      </c>
+      <c r="D148" s="1" t="n">
+        <v>578</v>
+      </c>
+      <c r="E148" s="12" t="n">
+        <f aca="false">D148/67.79</f>
+        <v>8.52633131730344</v>
+      </c>
+      <c r="F148" s="12" t="n">
+        <v>115</v>
+      </c>
+      <c r="G148" s="13" t="n">
+        <v>43916</v>
+      </c>
+      <c r="H148" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$142,G148)</f>
+        <v>0</v>
+      </c>
+      <c r="I148" s="13" t="n">
+        <f aca="false">B$142+1</f>
+        <v>43917</v>
+      </c>
+      <c r="J148" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$142,I148)</f>
+        <v>-1</v>
+      </c>
+      <c r="K148" s="13" t="n">
+        <f aca="false">B$142+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L148" s="0"/>
+      <c r="M148" s="0"/>
+      <c r="N148" s="0"/>
+      <c r="O148" s="0"/>
+      <c r="P148" s="0"/>
+      <c r="Q148" s="0"/>
+    </row>
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B149" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C149" s="12" t="n">
+        <v>414</v>
+      </c>
+      <c r="D149" s="1" t="n">
+        <v>267</v>
+      </c>
+      <c r="E149" s="12" t="n">
+        <f aca="false">D149/83.784</f>
+        <v>3.18676596963621</v>
+      </c>
+      <c r="F149" s="12" t="n">
+        <v>61</v>
+      </c>
+      <c r="G149" s="13" t="n">
+        <v>43917</v>
+      </c>
+      <c r="H149" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$142,G149)</f>
+        <v>-1</v>
+      </c>
+      <c r="I149" s="13" t="n">
+        <f aca="false">B$142+1</f>
+        <v>43917</v>
+      </c>
+      <c r="J149" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$142,I149)</f>
+        <v>-1</v>
+      </c>
+      <c r="K149" s="13" t="n">
+        <f aca="false">B$142+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L149" s="0"/>
+      <c r="M149" s="0"/>
+      <c r="N149" s="0"/>
+      <c r="O149" s="0"/>
+      <c r="P149" s="0"/>
+      <c r="Q149" s="0"/>
+    </row>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B150" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C150" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="D150" s="12" t="n">
+        <v>77</v>
+      </c>
+      <c r="E150" s="12" t="n">
+        <f aca="false">D150/10.36</f>
+        <v>7.43243243243243</v>
+      </c>
+      <c r="F150" s="12" t="n">
+        <v>15</v>
+      </c>
+      <c r="G150" s="13" t="n">
+        <v>43915</v>
+      </c>
+      <c r="H150" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$142,G150)</f>
+        <v>1</v>
+      </c>
+      <c r="I150" s="13" t="n">
+        <f aca="false">B$142+1</f>
+        <v>43917</v>
+      </c>
+      <c r="J150" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$142,I150)</f>
+        <v>-1</v>
+      </c>
+      <c r="K150" s="13" t="n">
+        <f aca="false">B$142+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L150" s="0"/>
+      <c r="M150" s="0"/>
+      <c r="N150" s="0"/>
+      <c r="O150" s="0"/>
+      <c r="P150" s="0"/>
+      <c r="Q150" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
updated with 2020-04-06 available data
</commit_message>
<xml_diff>
--- a/covid19 lockdown evaluation .xlsx
+++ b/covid19 lockdown evaluation .xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="53">
   <si>
     <t>Effects of the lockdown issued by governments</t>
   </si>
@@ -353,7 +353,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q150"/>
+  <dimension ref="A1:Q162"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F31" activeCellId="0" sqref="F31"/>
@@ -805,7 +805,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="7" t="n">
-        <v>43926</v>
+        <v>43927</v>
       </c>
       <c r="D22" s="0"/>
       <c r="E22" s="8" t="s">
@@ -882,36 +882,36 @@
         <v>300</v>
       </c>
       <c r="D24" s="1" t="n">
-        <v>15887</v>
+        <v>16523</v>
       </c>
       <c r="E24" s="12" t="n">
         <f aca="false">D24/60.48</f>
-        <v>262.681878306878</v>
+        <v>273.197751322751</v>
       </c>
       <c r="F24" s="12" t="n">
-        <v>525</v>
+        <v>636</v>
       </c>
       <c r="G24" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H24" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,G24)</f>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I24" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J24" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I24)</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K24" s="13" t="n">
-        <f aca="false">$B$34+1</f>
-        <v>43926</v>
+        <f aca="false">$B$22+1</f>
+        <v>43928</v>
       </c>
       <c r="L24" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K24,G24)</f>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="M24" s="0"/>
       <c r="N24" s="0"/>
@@ -927,36 +927,36 @@
         <v>230</v>
       </c>
       <c r="D25" s="1" t="n">
-        <v>12641</v>
+        <v>13341</v>
       </c>
       <c r="E25" s="12" t="n">
         <f aca="false">D25/46.75</f>
-        <v>270.395721925134</v>
+        <v>285.368983957219</v>
       </c>
       <c r="F25" s="12" t="n">
-        <v>694</v>
+        <v>700</v>
       </c>
       <c r="G25" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H25" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,G25)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I25" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J25" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I25)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K25" s="13" t="n">
-        <f aca="false">$B$34+1</f>
-        <v>43926</v>
+        <f aca="false">$B$22+1</f>
+        <v>43928</v>
       </c>
       <c r="L25" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K25,G25)</f>
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="M25" s="0"/>
       <c r="N25" s="0"/>
@@ -972,36 +972,36 @@
         <v>330</v>
       </c>
       <c r="D26" s="1" t="n">
-        <v>8078</v>
+        <v>8911</v>
       </c>
       <c r="E26" s="12" t="n">
         <f aca="false">D26/65.27</f>
-        <v>123.762831316072</v>
+        <v>136.525203002911</v>
       </c>
       <c r="F26" s="12" t="n">
-        <v>518</v>
+        <v>833</v>
       </c>
       <c r="G26" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H26" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,G26)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I26" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J26" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I26)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K26" s="13" t="n">
-        <f aca="false">$B$34+1</f>
-        <v>43926</v>
+        <f aca="false">$B$22+1</f>
+        <v>43928</v>
       </c>
       <c r="L26" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K26,G26)</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M26" s="0"/>
       <c r="N26" s="0"/>
@@ -1017,37 +1017,37 @@
         <v>50</v>
       </c>
       <c r="D27" s="12" t="n">
-        <v>401</v>
+        <v>477</v>
       </c>
       <c r="E27" s="12" t="n">
         <f aca="false">D27/10.36</f>
-        <v>38.7065637065637</v>
+        <v>46.042471042471</v>
       </c>
       <c r="F27" s="12" t="n">
-        <v>28</v>
+        <v>76</v>
       </c>
       <c r="G27" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H27" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,G27)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I27" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43927</v>
+        <v>43928</v>
       </c>
       <c r="J27" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I27)</f>
         <v>-1</v>
       </c>
       <c r="K27" s="13" t="n">
-        <f aca="false">$B$34+1</f>
-        <v>43926</v>
+        <f aca="false">$B$22+1</f>
+        <v>43928</v>
       </c>
       <c r="L27" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K27,G27)</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="M27" s="0"/>
       <c r="N27" s="0"/>
@@ -1063,37 +1063,37 @@
         <v>330</v>
       </c>
       <c r="D28" s="1" t="n">
-        <v>4934</v>
+        <v>5373</v>
       </c>
       <c r="E28" s="12" t="n">
         <f aca="false">D28/67.79</f>
-        <v>72.7835964006491</v>
+        <v>79.2594777990854</v>
       </c>
       <c r="F28" s="12" t="n">
-        <v>621</v>
+        <v>439</v>
       </c>
       <c r="G28" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H28" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,G28)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I28" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43927</v>
+        <v>43928</v>
       </c>
       <c r="J28" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I28)</f>
         <v>-1</v>
       </c>
       <c r="K28" s="13" t="n">
-        <f aca="false">$B$34+1</f>
-        <v>43926</v>
+        <f aca="false">$B$22+1</f>
+        <v>43928</v>
       </c>
       <c r="L28" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K28,G28)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="M28" s="0"/>
       <c r="N28" s="0"/>
@@ -1109,37 +1109,37 @@
         <v>1660</v>
       </c>
       <c r="D29" s="1" t="n">
-        <v>9616</v>
+        <v>10871</v>
       </c>
       <c r="E29" s="12" t="n">
         <f aca="false">D29/331</f>
-        <v>29.0513595166163</v>
+        <v>32.8429003021148</v>
       </c>
       <c r="F29" s="12" t="n">
-        <v>1165</v>
+        <v>1255</v>
       </c>
       <c r="G29" s="13" t="n">
         <v>43917</v>
       </c>
       <c r="H29" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,G29)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I29" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43927</v>
+        <v>43928</v>
       </c>
       <c r="J29" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I29)</f>
         <v>-1</v>
       </c>
       <c r="K29" s="13" t="n">
-        <f aca="false">$B$34+1</f>
-        <v>43926</v>
+        <f aca="false">$B$22+1</f>
+        <v>43928</v>
       </c>
       <c r="L29" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K29,G29)</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="M29" s="0"/>
       <c r="N29" s="0"/>
@@ -1155,37 +1155,37 @@
         <v>414</v>
       </c>
       <c r="D30" s="1" t="n">
-        <v>1584</v>
+        <v>1810</v>
       </c>
       <c r="E30" s="12" t="n">
         <f aca="false">D30/83.784</f>
-        <v>18.9057576625609</v>
+        <v>21.6031700563353</v>
       </c>
       <c r="F30" s="12" t="n">
-        <v>140</v>
+        <v>226</v>
       </c>
       <c r="G30" s="13" t="n">
         <v>43918</v>
       </c>
       <c r="H30" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,G30)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I30" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43927</v>
+        <v>43928</v>
       </c>
       <c r="J30" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I30)</f>
         <v>-1</v>
       </c>
       <c r="K30" s="13" t="n">
-        <f aca="false">$B$34+1</f>
-        <v>43926</v>
+        <f aca="false">$B$22+1</f>
+        <v>43928</v>
       </c>
       <c r="L30" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K30,G30)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="M30" s="0"/>
       <c r="N30" s="0"/>
@@ -1250,7 +1250,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="7" t="n">
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="D34" s="0"/>
       <c r="E34" s="8" t="s">
@@ -1327,36 +1327,36 @@
         <v>300</v>
       </c>
       <c r="D36" s="1" t="n">
-        <v>15362</v>
+        <v>15887</v>
       </c>
       <c r="E36" s="12" t="n">
         <f aca="false">D36/60.48</f>
-        <v>254.001322751323</v>
+        <v>262.681878306878</v>
       </c>
       <c r="F36" s="12" t="n">
-        <v>681</v>
+        <v>525</v>
       </c>
       <c r="G36" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H36" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,G36)</f>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I36" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J36" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I36)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K36" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43926</v>
+        <v>43927</v>
       </c>
       <c r="L36" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K36,G36)</f>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M36" s="0"/>
       <c r="N36" s="0"/>
@@ -1372,36 +1372,36 @@
         <v>230</v>
       </c>
       <c r="D37" s="1" t="n">
-        <v>11947</v>
+        <v>12641</v>
       </c>
       <c r="E37" s="12" t="n">
         <f aca="false">D37/46.75</f>
-        <v>255.550802139037</v>
+        <v>270.395721925134</v>
       </c>
       <c r="F37" s="12" t="n">
-        <v>749</v>
+        <v>694</v>
       </c>
       <c r="G37" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H37" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,G37)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I37" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J37" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I37)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K37" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43926</v>
+        <v>43927</v>
       </c>
       <c r="L37" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K37,G37)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M37" s="0"/>
       <c r="N37" s="0"/>
@@ -1417,36 +1417,36 @@
         <v>330</v>
       </c>
       <c r="D38" s="1" t="n">
-        <v>7560</v>
+        <v>8078</v>
       </c>
       <c r="E38" s="12" t="n">
         <f aca="false">D38/65.27</f>
-        <v>115.826566569634</v>
+        <v>123.762831316072</v>
       </c>
       <c r="F38" s="12" t="n">
-        <v>1053</v>
+        <v>518</v>
       </c>
       <c r="G38" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H38" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,G38)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I38" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J38" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I38)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K38" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43926</v>
+        <v>43927</v>
       </c>
       <c r="L38" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K38,G38)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M38" s="0"/>
       <c r="N38" s="0"/>
@@ -1462,25 +1462,25 @@
         <v>50</v>
       </c>
       <c r="D39" s="12" t="n">
-        <v>373</v>
+        <v>401</v>
       </c>
       <c r="E39" s="12" t="n">
         <f aca="false">D39/10.36</f>
-        <v>36.003861003861</v>
+        <v>38.7065637065637</v>
       </c>
       <c r="F39" s="12" t="n">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="G39" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H39" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,G39)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I39" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43926</v>
+        <v>43927</v>
       </c>
       <c r="J39" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I39)</f>
@@ -1488,11 +1488,11 @@
       </c>
       <c r="K39" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43926</v>
+        <v>43927</v>
       </c>
       <c r="L39" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K39,G39)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M39" s="0"/>
       <c r="N39" s="0"/>
@@ -1508,25 +1508,25 @@
         <v>330</v>
       </c>
       <c r="D40" s="1" t="n">
-        <v>4313</v>
+        <v>4934</v>
       </c>
       <c r="E40" s="12" t="n">
         <f aca="false">D40/67.79</f>
-        <v>63.6229532379407</v>
+        <v>72.7835964006491</v>
       </c>
       <c r="F40" s="12" t="n">
-        <v>708</v>
+        <v>621</v>
       </c>
       <c r="G40" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H40" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,G40)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I40" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43926</v>
+        <v>43927</v>
       </c>
       <c r="J40" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I40)</f>
@@ -1534,11 +1534,11 @@
       </c>
       <c r="K40" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43926</v>
+        <v>43927</v>
       </c>
       <c r="L40" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K40,G40)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M40" s="0"/>
       <c r="N40" s="0"/>
@@ -1554,25 +1554,25 @@
         <v>1660</v>
       </c>
       <c r="D41" s="1" t="n">
-        <v>8451</v>
+        <v>9616</v>
       </c>
       <c r="E41" s="12" t="n">
         <f aca="false">D41/331</f>
-        <v>25.5317220543807</v>
+        <v>29.0513595166163</v>
       </c>
       <c r="F41" s="12" t="n">
-        <v>1330</v>
+        <v>1165</v>
       </c>
       <c r="G41" s="13" t="n">
         <v>43917</v>
       </c>
       <c r="H41" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,G41)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I41" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43926</v>
+        <v>43927</v>
       </c>
       <c r="J41" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I41)</f>
@@ -1580,11 +1580,11 @@
       </c>
       <c r="K41" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43926</v>
+        <v>43927</v>
       </c>
       <c r="L41" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K41,G41)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M41" s="0"/>
       <c r="N41" s="0"/>
@@ -1600,25 +1600,25 @@
         <v>414</v>
       </c>
       <c r="D42" s="1" t="n">
-        <v>1444</v>
+        <v>1584</v>
       </c>
       <c r="E42" s="12" t="n">
         <f aca="false">D42/83.784</f>
-        <v>17.2347942327891</v>
+        <v>18.9057576625609</v>
       </c>
       <c r="F42" s="12" t="n">
-        <v>169</v>
+        <v>140</v>
       </c>
       <c r="G42" s="13" t="n">
         <v>43918</v>
       </c>
       <c r="H42" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,G42)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I42" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43926</v>
+        <v>43927</v>
       </c>
       <c r="J42" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I42)</f>
@@ -1626,11 +1626,11 @@
       </c>
       <c r="K42" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43926</v>
+        <v>43927</v>
       </c>
       <c r="L42" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K42,G42)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M42" s="0"/>
       <c r="N42" s="0"/>
@@ -1695,7 +1695,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="7" t="n">
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="D46" s="0"/>
       <c r="E46" s="8" t="s">
@@ -1772,36 +1772,36 @@
         <v>300</v>
       </c>
       <c r="D48" s="1" t="n">
-        <v>14681</v>
+        <v>15362</v>
       </c>
       <c r="E48" s="12" t="n">
         <f aca="false">D48/60.48</f>
-        <v>242.741402116402</v>
+        <v>254.001322751323</v>
       </c>
       <c r="F48" s="12" t="n">
-        <v>766</v>
+        <v>681</v>
       </c>
       <c r="G48" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H48" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,G48)</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I48" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J48" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I48)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K48" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="L48" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K48,G48)</f>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M48" s="0"/>
       <c r="N48" s="0"/>
@@ -1817,36 +1817,36 @@
         <v>230</v>
       </c>
       <c r="D49" s="1" t="n">
-        <v>11198</v>
+        <v>11947</v>
       </c>
       <c r="E49" s="12" t="n">
         <f aca="false">D49/46.75</f>
-        <v>239.529411764706</v>
+        <v>255.550802139037</v>
       </c>
       <c r="F49" s="12" t="n">
-        <v>850</v>
+        <v>749</v>
       </c>
       <c r="G49" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H49" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$58,G49)</f>
-        <v>16</v>
+        <f aca="false">_xlfn.DAYS($B$46,G49)</f>
+        <v>18</v>
       </c>
       <c r="I49" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J49" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I49)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K49" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="L49" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K49,G49)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M49" s="0"/>
       <c r="N49" s="0"/>
@@ -1862,36 +1862,36 @@
         <v>330</v>
       </c>
       <c r="D50" s="1" t="n">
-        <v>6507</v>
+        <v>7560</v>
       </c>
       <c r="E50" s="12" t="n">
         <f aca="false">D50/65.27</f>
-        <v>99.6935805117206</v>
+        <v>115.826566569634</v>
       </c>
       <c r="F50" s="12" t="n">
-        <v>1120</v>
+        <v>1053</v>
       </c>
       <c r="G50" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H50" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$58,G50)</f>
-        <v>11</v>
+        <f aca="false">_xlfn.DAYS($B$46,G50)</f>
+        <v>13</v>
       </c>
       <c r="I50" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J50" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I50)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K50" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="L50" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K50,G50)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="M50" s="0"/>
       <c r="N50" s="0"/>
@@ -1907,25 +1907,25 @@
         <v>50</v>
       </c>
       <c r="D51" s="12" t="n">
-        <v>358</v>
+        <v>373</v>
       </c>
       <c r="E51" s="12" t="n">
         <f aca="false">D51/10.36</f>
-        <v>34.5559845559846</v>
+        <v>36.003861003861</v>
       </c>
       <c r="F51" s="12" t="n">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="G51" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H51" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$58,G51)</f>
-        <v>8</v>
+        <f aca="false">_xlfn.DAYS($B$46,G51)</f>
+        <v>10</v>
       </c>
       <c r="I51" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="J51" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I51)</f>
@@ -1933,11 +1933,11 @@
       </c>
       <c r="K51" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="L51" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K51,G51)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M51" s="0"/>
       <c r="N51" s="0"/>
@@ -1953,25 +1953,25 @@
         <v>330</v>
       </c>
       <c r="D52" s="1" t="n">
-        <v>3605</v>
+        <v>4313</v>
       </c>
       <c r="E52" s="12" t="n">
         <f aca="false">D52/67.79</f>
-        <v>53.1789349461573</v>
+        <v>63.6229532379407</v>
       </c>
       <c r="F52" s="12" t="n">
-        <v>684</v>
+        <v>708</v>
       </c>
       <c r="G52" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H52" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$58,G52)</f>
-        <v>7</v>
+        <f aca="false">_xlfn.DAYS($B$46,G52)</f>
+        <v>9</v>
       </c>
       <c r="I52" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="J52" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I52)</f>
@@ -1979,11 +1979,11 @@
       </c>
       <c r="K52" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="L52" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K52,G52)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M52" s="0"/>
       <c r="N52" s="0"/>
@@ -1999,25 +1999,25 @@
         <v>1660</v>
       </c>
       <c r="D53" s="1" t="n">
-        <v>7121</v>
+        <v>8451</v>
       </c>
       <c r="E53" s="12" t="n">
         <f aca="false">D53/331</f>
-        <v>21.5135951661631</v>
+        <v>25.5317220543807</v>
       </c>
       <c r="F53" s="12" t="n">
-        <v>1045</v>
+        <v>1330</v>
       </c>
       <c r="G53" s="13" t="n">
         <v>43917</v>
       </c>
       <c r="H53" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$58,G53)</f>
-        <v>6</v>
+        <f aca="false">_xlfn.DAYS($B$46,G53)</f>
+        <v>8</v>
       </c>
       <c r="I53" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="J53" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I53)</f>
@@ -2025,11 +2025,11 @@
       </c>
       <c r="K53" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="L53" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K53,G53)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M53" s="0"/>
       <c r="N53" s="0"/>
@@ -2045,25 +2045,25 @@
         <v>414</v>
       </c>
       <c r="D54" s="1" t="n">
-        <v>1275</v>
+        <v>1444</v>
       </c>
       <c r="E54" s="12" t="n">
         <f aca="false">D54/83.784</f>
-        <v>15.2177026639931</v>
+        <v>17.2347942327891</v>
       </c>
       <c r="F54" s="12" t="n">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G54" s="13" t="n">
         <v>43918</v>
       </c>
       <c r="H54" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$58,G54)</f>
-        <v>5</v>
+        <f aca="false">_xlfn.DAYS($B$46,G54)</f>
+        <v>7</v>
       </c>
       <c r="I54" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="J54" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I54)</f>
@@ -2071,11 +2071,11 @@
       </c>
       <c r="K54" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="L54" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K54,G54)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M54" s="0"/>
       <c r="N54" s="0"/>
@@ -2140,7 +2140,7 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="7" t="n">
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="D58" s="0"/>
       <c r="E58" s="8" t="s">
@@ -2217,36 +2217,36 @@
         <v>300</v>
       </c>
       <c r="D60" s="1" t="n">
-        <v>13915</v>
+        <v>14681</v>
       </c>
       <c r="E60" s="12" t="n">
         <f aca="false">D60/60.48</f>
-        <v>230.076058201058</v>
+        <v>242.741402116402</v>
       </c>
       <c r="F60" s="12" t="n">
-        <v>760</v>
+        <v>766</v>
       </c>
       <c r="G60" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H60" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,G60)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I60" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J60" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I60)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K60" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="L60" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K60,G60)</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M60" s="0"/>
       <c r="N60" s="0"/>
@@ -2262,20 +2262,20 @@
         <v>230</v>
       </c>
       <c r="D61" s="1" t="n">
-        <v>10348</v>
+        <v>11198</v>
       </c>
       <c r="E61" s="12" t="n">
         <f aca="false">D61/46.75</f>
-        <v>221.347593582888</v>
+        <v>239.529411764706</v>
       </c>
       <c r="F61" s="12" t="n">
-        <v>961</v>
+        <v>850</v>
       </c>
       <c r="G61" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H61" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$58,G61)</f>
+        <f aca="false">_xlfn.DAYS($B$70,G61)</f>
         <v>16</v>
       </c>
       <c r="I61" s="13" t="n">
@@ -2283,15 +2283,15 @@
       </c>
       <c r="J61" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I61)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K61" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="L61" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K61,G61)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M61" s="0"/>
       <c r="N61" s="0"/>
@@ -2307,20 +2307,20 @@
         <v>330</v>
       </c>
       <c r="D62" s="1" t="n">
-        <v>5387</v>
+        <v>6507</v>
       </c>
       <c r="E62" s="12" t="n">
         <f aca="false">D62/65.27</f>
-        <v>82.5340891680711</v>
+        <v>99.6935805117206</v>
       </c>
       <c r="F62" s="12" t="n">
-        <v>1355</v>
+        <v>1120</v>
       </c>
       <c r="G62" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H62" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$58,G62)</f>
+        <f aca="false">_xlfn.DAYS($B$70,G62)</f>
         <v>11</v>
       </c>
       <c r="I62" s="13" t="n">
@@ -2328,15 +2328,15 @@
       </c>
       <c r="J62" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I62)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K62" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="L62" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K62,G62)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M62" s="0"/>
       <c r="N62" s="0"/>
@@ -2352,25 +2352,25 @@
         <v>50</v>
       </c>
       <c r="D63" s="12" t="n">
-        <v>308</v>
+        <v>358</v>
       </c>
       <c r="E63" s="12" t="n">
         <f aca="false">D63/10.36</f>
-        <v>29.7297297297297</v>
+        <v>34.5559845559846</v>
       </c>
       <c r="F63" s="12" t="n">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="G63" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H63" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$58,G63)</f>
+        <f aca="false">_xlfn.DAYS($B$70,G63)</f>
         <v>8</v>
       </c>
       <c r="I63" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="J63" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I63)</f>
@@ -2378,11 +2378,11 @@
       </c>
       <c r="K63" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="L63" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K63,G63)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M63" s="0"/>
       <c r="N63" s="0"/>
@@ -2398,25 +2398,25 @@
         <v>330</v>
       </c>
       <c r="D64" s="1" t="n">
-        <v>2921</v>
+        <v>3605</v>
       </c>
       <c r="E64" s="12" t="n">
         <f aca="false">D64/67.79</f>
-        <v>43.0889511727393</v>
+        <v>53.1789349461573</v>
       </c>
       <c r="F64" s="12" t="n">
-        <v>569</v>
+        <v>684</v>
       </c>
       <c r="G64" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H64" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$58,G64)</f>
+        <f aca="false">_xlfn.DAYS($B$70,G64)</f>
         <v>7</v>
       </c>
       <c r="I64" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="J64" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I64)</f>
@@ -2424,11 +2424,11 @@
       </c>
       <c r="K64" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="L64" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K64,G64)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M64" s="0"/>
       <c r="N64" s="0"/>
@@ -2444,25 +2444,25 @@
         <v>1660</v>
       </c>
       <c r="D65" s="1" t="n">
-        <v>6076</v>
+        <v>7121</v>
       </c>
       <c r="E65" s="12" t="n">
         <f aca="false">D65/331</f>
-        <v>18.3564954682779</v>
+        <v>21.5135951661631</v>
       </c>
       <c r="F65" s="12" t="n">
-        <v>969</v>
+        <v>1045</v>
       </c>
       <c r="G65" s="13" t="n">
         <v>43917</v>
       </c>
       <c r="H65" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$58,G65)</f>
+        <f aca="false">_xlfn.DAYS($B$70,G65)</f>
         <v>6</v>
       </c>
       <c r="I65" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="J65" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I65)</f>
@@ -2470,11 +2470,11 @@
       </c>
       <c r="K65" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="L65" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K65,G65)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M65" s="0"/>
       <c r="N65" s="0"/>
@@ -2490,25 +2490,25 @@
         <v>414</v>
       </c>
       <c r="D66" s="1" t="n">
-        <v>1107</v>
+        <v>1275</v>
       </c>
       <c r="E66" s="12" t="n">
         <f aca="false">D66/83.784</f>
-        <v>13.212546548267</v>
+        <v>15.2177026639931</v>
       </c>
       <c r="F66" s="12" t="n">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="G66" s="13" t="n">
         <v>43918</v>
       </c>
       <c r="H66" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$58,G66)</f>
+        <f aca="false">_xlfn.DAYS($B$70,G66)</f>
         <v>5</v>
       </c>
       <c r="I66" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="J66" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I66)</f>
@@ -2516,11 +2516,11 @@
       </c>
       <c r="K66" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="L66" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K66,G66)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M66" s="0"/>
       <c r="N66" s="0"/>
@@ -2585,7 +2585,7 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="7" t="n">
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="D70" s="0"/>
       <c r="E70" s="8" t="s">
@@ -2662,36 +2662,36 @@
         <v>300</v>
       </c>
       <c r="D72" s="1" t="n">
-        <v>13155</v>
+        <v>13915</v>
       </c>
       <c r="E72" s="12" t="n">
         <f aca="false">D72/60.48</f>
-        <v>217.509920634921</v>
+        <v>230.076058201058</v>
       </c>
       <c r="F72" s="12" t="n">
-        <v>727</v>
+        <v>760</v>
       </c>
       <c r="G72" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H72" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,G72)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I72" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J72" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,I72)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K72" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="L72" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K72,G72)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M72" s="0"/>
       <c r="N72" s="0"/>
@@ -2707,36 +2707,36 @@
         <v>230</v>
       </c>
       <c r="D73" s="1" t="n">
-        <v>9387</v>
+        <v>10348</v>
       </c>
       <c r="E73" s="12" t="n">
         <f aca="false">D73/46.75</f>
-        <v>200.791443850267</v>
+        <v>221.347593582888</v>
       </c>
       <c r="F73" s="12" t="n">
-        <v>923</v>
+        <v>961</v>
       </c>
       <c r="G73" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H73" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,G73)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I73" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J73" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,I73)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K73" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="L73" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K73,G73)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M73" s="0"/>
       <c r="N73" s="0"/>
@@ -2752,36 +2752,36 @@
         <v>330</v>
       </c>
       <c r="D74" s="1" t="n">
-        <v>4032</v>
+        <v>5387</v>
       </c>
       <c r="E74" s="12" t="n">
         <f aca="false">D74/65.27</f>
-        <v>61.7741688371381</v>
+        <v>82.5340891680711</v>
       </c>
       <c r="F74" s="12" t="n">
-        <v>509</v>
+        <v>1355</v>
       </c>
       <c r="G74" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H74" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,G74)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I74" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J74" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,I74)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K74" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="L74" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K74,G74)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M74" s="0"/>
       <c r="N74" s="0"/>
@@ -2797,25 +2797,25 @@
         <v>50</v>
       </c>
       <c r="D75" s="12" t="n">
-        <v>239</v>
+        <v>308</v>
       </c>
       <c r="E75" s="12" t="n">
         <f aca="false">D75/10.36</f>
-        <v>23.0694980694981</v>
+        <v>29.7297297297297</v>
       </c>
       <c r="F75" s="12" t="n">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="G75" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H75" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,G75)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I75" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="J75" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,I75)</f>
@@ -2823,11 +2823,11 @@
       </c>
       <c r="K75" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="L75" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K75,G75)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M75" s="0"/>
       <c r="N75" s="0"/>
@@ -2843,25 +2843,25 @@
         <v>330</v>
       </c>
       <c r="D76" s="1" t="n">
-        <v>2352</v>
+        <v>2921</v>
       </c>
       <c r="E76" s="12" t="n">
         <f aca="false">D76/67.79</f>
-        <v>34.695382799823</v>
+        <v>43.0889511727393</v>
       </c>
       <c r="F76" s="12" t="n">
-        <v>563</v>
+        <v>569</v>
       </c>
       <c r="G76" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H76" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,G76)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I76" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="J76" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,I76)</f>
@@ -2869,11 +2869,11 @@
       </c>
       <c r="K76" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="L76" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K76,G76)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M76" s="0"/>
       <c r="N76" s="0"/>
@@ -2889,25 +2889,25 @@
         <v>1660</v>
       </c>
       <c r="D77" s="1" t="n">
-        <v>5102</v>
+        <v>6076</v>
       </c>
       <c r="E77" s="12" t="n">
         <f aca="false">D77/331</f>
-        <v>15.4138972809668</v>
+        <v>18.3564954682779</v>
       </c>
       <c r="F77" s="12" t="n">
-        <v>1049</v>
+        <v>969</v>
       </c>
       <c r="G77" s="13" t="n">
         <v>43917</v>
       </c>
       <c r="H77" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,G77)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I77" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="J77" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,I77)</f>
@@ -2915,11 +2915,11 @@
       </c>
       <c r="K77" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="L77" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K77,G77)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M77" s="0"/>
       <c r="N77" s="0"/>
@@ -2935,25 +2935,25 @@
         <v>414</v>
       </c>
       <c r="D78" s="1" t="n">
-        <v>931</v>
+        <v>1107</v>
       </c>
       <c r="E78" s="12" t="n">
         <f aca="false">D78/83.784</f>
-        <v>11.1119068079824</v>
+        <v>13.212546548267</v>
       </c>
       <c r="F78" s="12" t="n">
-        <v>156</v>
+        <v>176</v>
       </c>
       <c r="G78" s="13" t="n">
         <v>43918</v>
       </c>
       <c r="H78" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,G78)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I78" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="J78" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,I78)</f>
@@ -2961,11 +2961,11 @@
       </c>
       <c r="K78" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="L78" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K78,G78)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M78" s="0"/>
       <c r="N78" s="0"/>
@@ -3030,7 +3030,7 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="7" t="n">
-        <v>43921</v>
+        <v>43922</v>
       </c>
       <c r="D82" s="0"/>
       <c r="E82" s="8" t="s">
@@ -3107,36 +3107,36 @@
         <v>300</v>
       </c>
       <c r="D84" s="1" t="n">
-        <v>12428</v>
+        <v>13155</v>
       </c>
       <c r="E84" s="12" t="n">
         <f aca="false">D84/60.48</f>
-        <v>205.489417989418</v>
+        <v>217.509920634921</v>
       </c>
       <c r="F84" s="12" t="n">
-        <v>837</v>
+        <v>727</v>
       </c>
       <c r="G84" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H84" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,G84)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I84" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J84" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,I84)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K84" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L84" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K84,G84)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M84" s="0"/>
       <c r="N84" s="0"/>
@@ -3152,36 +3152,36 @@
         <v>230</v>
       </c>
       <c r="D85" s="1" t="n">
-        <v>8464</v>
+        <v>9387</v>
       </c>
       <c r="E85" s="12" t="n">
         <f aca="false">D85/46.75</f>
-        <v>181.048128342246</v>
+        <v>200.791443850267</v>
       </c>
       <c r="F85" s="12" t="n">
-        <v>748</v>
+        <v>923</v>
       </c>
       <c r="G85" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H85" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,G85)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I85" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J85" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,I85)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K85" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L85" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K85,G85)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M85" s="0"/>
       <c r="N85" s="0"/>
@@ -3197,36 +3197,36 @@
         <v>330</v>
       </c>
       <c r="D86" s="1" t="n">
-        <v>3523</v>
+        <v>4032</v>
       </c>
       <c r="E86" s="12" t="n">
         <f aca="false">D86/65.27</f>
-        <v>53.9757928604259</v>
+        <v>61.7741688371381</v>
       </c>
       <c r="F86" s="12" t="n">
-        <v>499</v>
+        <v>509</v>
       </c>
       <c r="G86" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H86" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,G86)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I86" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J86" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,I86)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K86" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L86" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K86,G86)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M86" s="0"/>
       <c r="N86" s="0"/>
@@ -3242,25 +3242,25 @@
         <v>50</v>
       </c>
       <c r="D87" s="12" t="n">
-        <v>180</v>
+        <v>239</v>
       </c>
       <c r="E87" s="12" t="n">
         <f aca="false">D87/10.36</f>
-        <v>17.3745173745174</v>
+        <v>23.0694980694981</v>
       </c>
       <c r="F87" s="12" t="n">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="G87" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H87" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,G87)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I87" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="J87" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,I87)</f>
@@ -3268,11 +3268,11 @@
       </c>
       <c r="K87" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L87" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K87,G87)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M87" s="0"/>
       <c r="N87" s="0"/>
@@ -3288,25 +3288,25 @@
         <v>330</v>
       </c>
       <c r="D88" s="1" t="n">
-        <v>1789</v>
+        <v>2352</v>
       </c>
       <c r="E88" s="12" t="n">
         <f aca="false">D88/67.79</f>
-        <v>26.390323056498</v>
+        <v>34.695382799823</v>
       </c>
       <c r="F88" s="12" t="n">
-        <v>381</v>
+        <v>563</v>
       </c>
       <c r="G88" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H88" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,G88)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I88" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="J88" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,I88)</f>
@@ -3314,11 +3314,11 @@
       </c>
       <c r="K88" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L88" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K88,G88)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M88" s="0"/>
       <c r="N88" s="0"/>
@@ -3334,25 +3334,25 @@
         <v>1660</v>
       </c>
       <c r="D89" s="1" t="n">
-        <v>4053</v>
+        <v>5102</v>
       </c>
       <c r="E89" s="12" t="n">
         <f aca="false">D89/331</f>
-        <v>12.2447129909366</v>
+        <v>15.4138972809668</v>
       </c>
       <c r="F89" s="12" t="n">
-        <v>912</v>
+        <v>1049</v>
       </c>
       <c r="G89" s="13" t="n">
         <v>43917</v>
       </c>
       <c r="H89" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,G89)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I89" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="J89" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,I89)</f>
@@ -3360,11 +3360,11 @@
       </c>
       <c r="K89" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L89" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K89,G89)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M89" s="0"/>
       <c r="N89" s="0"/>
@@ -3380,25 +3380,25 @@
         <v>414</v>
       </c>
       <c r="D90" s="1" t="n">
-        <v>775</v>
+        <v>931</v>
       </c>
       <c r="E90" s="12" t="n">
         <f aca="false">D90/83.784</f>
-        <v>9.24997612909386</v>
+        <v>11.1119068079824</v>
       </c>
       <c r="F90" s="12" t="n">
-        <v>130</v>
+        <v>156</v>
       </c>
       <c r="G90" s="13" t="n">
         <v>43918</v>
       </c>
       <c r="H90" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,G90)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I90" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="J90" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,I90)</f>
@@ -3406,11 +3406,11 @@
       </c>
       <c r="K90" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L90" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K90,G90)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M90" s="0"/>
       <c r="N90" s="0"/>
@@ -3419,15 +3419,16 @@
       <c r="Q90" s="0"/>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C91" s="12"/>
+      <c r="B91" s="4"/>
+      <c r="C91" s="5"/>
       <c r="D91" s="0"/>
-      <c r="E91" s="12"/>
-      <c r="F91" s="12"/>
-      <c r="G91" s="13"/>
+      <c r="E91" s="0"/>
+      <c r="F91" s="0"/>
+      <c r="G91" s="0"/>
       <c r="H91" s="0"/>
-      <c r="I91" s="13"/>
+      <c r="I91" s="0"/>
       <c r="J91" s="0"/>
-      <c r="K91" s="13"/>
+      <c r="K91" s="0"/>
       <c r="L91" s="0"/>
       <c r="M91" s="0"/>
       <c r="N91" s="0"/>
@@ -3436,15 +3437,16 @@
       <c r="Q91" s="0"/>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C92" s="12"/>
+      <c r="B92" s="4"/>
+      <c r="C92" s="5"/>
       <c r="D92" s="0"/>
-      <c r="E92" s="12"/>
-      <c r="F92" s="12"/>
-      <c r="G92" s="13"/>
+      <c r="E92" s="0"/>
+      <c r="F92" s="0"/>
+      <c r="G92" s="0"/>
       <c r="H92" s="0"/>
-      <c r="I92" s="13"/>
+      <c r="I92" s="0"/>
       <c r="J92" s="0"/>
-      <c r="K92" s="13"/>
+      <c r="K92" s="0"/>
       <c r="L92" s="0"/>
       <c r="M92" s="0"/>
       <c r="N92" s="0"/>
@@ -3473,7 +3475,7 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="7" t="n">
-        <v>43920</v>
+        <v>43921</v>
       </c>
       <c r="D94" s="0"/>
       <c r="E94" s="8" t="s">
@@ -3495,7 +3497,9 @@
       <c r="K94" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="L94" s="0"/>
+      <c r="L94" s="8" t="s">
+        <v>37</v>
+      </c>
       <c r="M94" s="0"/>
       <c r="N94" s="0"/>
       <c r="O94" s="0"/>
@@ -3531,7 +3535,9 @@
       <c r="K95" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="L95" s="0"/>
+      <c r="L95" s="8" t="s">
+        <v>45</v>
+      </c>
       <c r="M95" s="0"/>
       <c r="N95" s="0"/>
       <c r="O95" s="0"/>
@@ -3546,34 +3552,37 @@
         <v>300</v>
       </c>
       <c r="D96" s="1" t="n">
-        <v>11591</v>
+        <v>12428</v>
       </c>
       <c r="E96" s="12" t="n">
         <f aca="false">D96/60.48</f>
-        <v>191.650132275132</v>
+        <v>205.489417989418</v>
       </c>
       <c r="F96" s="12" t="n">
-        <v>812</v>
+        <v>837</v>
       </c>
       <c r="G96" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H96" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,G96)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I96" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J96" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,I96)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K96" s="13" t="n">
-        <f aca="false">$B$106+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L96" s="0"/>
+        <f aca="false">$B$94+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L96" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K96,G96)</f>
+        <v>22</v>
+      </c>
       <c r="M96" s="0"/>
       <c r="N96" s="0"/>
       <c r="O96" s="0"/>
@@ -3588,34 +3597,37 @@
         <v>230</v>
       </c>
       <c r="D97" s="1" t="n">
-        <v>7716</v>
+        <v>8464</v>
       </c>
       <c r="E97" s="12" t="n">
         <f aca="false">D97/46.75</f>
-        <v>165.048128342246</v>
+        <v>181.048128342246</v>
       </c>
       <c r="F97" s="12" t="n">
-        <v>913</v>
+        <v>748</v>
       </c>
       <c r="G97" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H97" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,G97)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I97" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J97" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,I97)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K97" s="13" t="n">
-        <f aca="false">$B$106+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L97" s="0"/>
+        <f aca="false">$B$94+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L97" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K97,G97)</f>
+        <v>15</v>
+      </c>
       <c r="M97" s="0"/>
       <c r="N97" s="0"/>
       <c r="O97" s="0"/>
@@ -3630,34 +3642,37 @@
         <v>330</v>
       </c>
       <c r="D98" s="1" t="n">
-        <v>3024</v>
+        <v>3523</v>
       </c>
       <c r="E98" s="12" t="n">
         <f aca="false">D98/65.27</f>
-        <v>46.3306266278535</v>
+        <v>53.9757928604259</v>
       </c>
       <c r="F98" s="12" t="n">
-        <v>418</v>
+        <v>499</v>
       </c>
       <c r="G98" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H98" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,G98)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I98" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J98" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,I98)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K98" s="13" t="n">
-        <f aca="false">$B$106+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L98" s="0"/>
+        <f aca="false">$B$94+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L98" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K98,G98)</f>
+        <v>10</v>
+      </c>
       <c r="M98" s="0"/>
       <c r="N98" s="0"/>
       <c r="O98" s="0"/>
@@ -3672,35 +3687,38 @@
         <v>50</v>
       </c>
       <c r="D99" s="12" t="n">
-        <v>146</v>
+        <v>180</v>
       </c>
       <c r="E99" s="12" t="n">
         <f aca="false">D99/10.36</f>
-        <v>14.0926640926641</v>
+        <v>17.3745173745174</v>
       </c>
       <c r="F99" s="12" t="n">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G99" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H99" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,G99)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I99" s="13" t="n">
         <f aca="false">$B$94+1</f>
-        <v>43921</v>
+        <v>43922</v>
       </c>
       <c r="J99" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,I99)</f>
         <v>-1</v>
       </c>
       <c r="K99" s="13" t="n">
-        <f aca="false">$B$106+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L99" s="0"/>
+        <f aca="false">$B$94+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L99" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K99,G99)</f>
+        <v>7</v>
+      </c>
       <c r="M99" s="0"/>
       <c r="N99" s="0"/>
       <c r="O99" s="0"/>
@@ -3715,35 +3733,38 @@
         <v>330</v>
       </c>
       <c r="D100" s="1" t="n">
-        <v>1408</v>
+        <v>1789</v>
       </c>
       <c r="E100" s="12" t="n">
         <f aca="false">D100/67.79</f>
-        <v>20.770025077445</v>
+        <v>26.390323056498</v>
       </c>
       <c r="F100" s="12" t="n">
-        <v>180</v>
+        <v>381</v>
       </c>
       <c r="G100" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H100" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,G100)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I100" s="13" t="n">
         <f aca="false">$B$94+1</f>
-        <v>43921</v>
+        <v>43922</v>
       </c>
       <c r="J100" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,I100)</f>
         <v>-1</v>
       </c>
       <c r="K100" s="13" t="n">
-        <f aca="false">$B$106+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L100" s="0"/>
+        <f aca="false">$B$94+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L100" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K100,G100)</f>
+        <v>6</v>
+      </c>
       <c r="M100" s="0"/>
       <c r="N100" s="0"/>
       <c r="O100" s="0"/>
@@ -3758,34 +3779,38 @@
         <v>1660</v>
       </c>
       <c r="D101" s="1" t="n">
-        <v>3141</v>
+        <v>4053</v>
       </c>
       <c r="E101" s="12" t="n">
         <f aca="false">D101/331</f>
-        <v>9.48942598187311</v>
+        <v>12.2447129909366</v>
       </c>
       <c r="F101" s="12" t="n">
-        <v>573</v>
+        <v>912</v>
       </c>
       <c r="G101" s="13" t="n">
         <v>43917</v>
       </c>
       <c r="H101" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,G101)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I101" s="13" t="n">
-        <v>43920</v>
+        <f aca="false">$B$94+1</f>
+        <v>43922</v>
       </c>
       <c r="J101" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,I101)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="K101" s="13" t="n">
-        <f aca="false">$B$106+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L101" s="0"/>
+        <f aca="false">$B$94+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L101" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K101,G101)</f>
+        <v>5</v>
+      </c>
       <c r="M101" s="0"/>
       <c r="N101" s="0"/>
       <c r="O101" s="0"/>
@@ -3800,35 +3825,38 @@
         <v>414</v>
       </c>
       <c r="D102" s="1" t="n">
-        <v>645</v>
+        <v>775</v>
       </c>
       <c r="E102" s="12" t="n">
         <f aca="false">D102/83.784</f>
-        <v>7.69836723002005</v>
+        <v>9.24997612909386</v>
       </c>
       <c r="F102" s="12" t="n">
-        <v>104</v>
+        <v>130</v>
       </c>
       <c r="G102" s="13" t="n">
         <v>43918</v>
       </c>
       <c r="H102" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,G102)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I102" s="13" t="n">
         <f aca="false">$B$94+1</f>
-        <v>43921</v>
+        <v>43922</v>
       </c>
       <c r="J102" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,I102)</f>
         <v>-1</v>
       </c>
       <c r="K102" s="13" t="n">
-        <f aca="false">$B$106+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L102" s="0"/>
+        <f aca="false">$B$94+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L102" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K102,G102)</f>
+        <v>4</v>
+      </c>
       <c r="M102" s="0"/>
       <c r="N102" s="0"/>
       <c r="O102" s="0"/>
@@ -3836,16 +3864,15 @@
       <c r="Q102" s="0"/>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B103" s="4"/>
-      <c r="C103" s="5"/>
+      <c r="C103" s="12"/>
       <c r="D103" s="0"/>
-      <c r="E103" s="0"/>
-      <c r="F103" s="0"/>
-      <c r="G103" s="0"/>
+      <c r="E103" s="12"/>
+      <c r="F103" s="12"/>
+      <c r="G103" s="13"/>
       <c r="H103" s="0"/>
-      <c r="I103" s="0"/>
+      <c r="I103" s="13"/>
       <c r="J103" s="0"/>
-      <c r="K103" s="0"/>
+      <c r="K103" s="13"/>
       <c r="L103" s="0"/>
       <c r="M103" s="0"/>
       <c r="N103" s="0"/>
@@ -3854,16 +3881,15 @@
       <c r="Q103" s="0"/>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B104" s="4"/>
-      <c r="C104" s="5"/>
+      <c r="C104" s="12"/>
       <c r="D104" s="0"/>
-      <c r="E104" s="0"/>
-      <c r="F104" s="0"/>
-      <c r="G104" s="0"/>
+      <c r="E104" s="12"/>
+      <c r="F104" s="12"/>
+      <c r="G104" s="13"/>
       <c r="H104" s="0"/>
-      <c r="I104" s="0"/>
+      <c r="I104" s="13"/>
       <c r="J104" s="0"/>
-      <c r="K104" s="0"/>
+      <c r="K104" s="13"/>
       <c r="L104" s="0"/>
       <c r="M104" s="0"/>
       <c r="N104" s="0"/>
@@ -3892,7 +3918,7 @@
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="7" t="n">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="D106" s="0"/>
       <c r="E106" s="8" t="s">
@@ -3965,31 +3991,31 @@
         <v>300</v>
       </c>
       <c r="D108" s="1" t="n">
-        <v>10779</v>
+        <v>11591</v>
       </c>
       <c r="E108" s="12" t="n">
         <f aca="false">D108/60.48</f>
-        <v>178.224206349206</v>
+        <v>191.650132275132</v>
       </c>
       <c r="F108" s="12" t="n">
-        <v>756</v>
+        <v>812</v>
       </c>
       <c r="G108" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H108" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,G108)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I108" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J108" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,I108)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K108" s="13" t="n">
-        <f aca="false">$B$106+1</f>
+        <f aca="false">$B$118+1</f>
         <v>43920</v>
       </c>
       <c r="L108" s="0"/>
@@ -4007,31 +4033,31 @@
         <v>230</v>
       </c>
       <c r="D109" s="1" t="n">
-        <v>6803</v>
+        <v>7716</v>
       </c>
       <c r="E109" s="12" t="n">
         <f aca="false">D109/46.75</f>
-        <v>145.51871657754</v>
+        <v>165.048128342246</v>
       </c>
       <c r="F109" s="12" t="n">
-        <v>821</v>
+        <v>913</v>
       </c>
       <c r="G109" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H109" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,G109)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I109" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J109" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,I109)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K109" s="13" t="n">
-        <f aca="false">$B$106+1</f>
+        <f aca="false">$B$118+1</f>
         <v>43920</v>
       </c>
       <c r="L109" s="0"/>
@@ -4049,31 +4075,31 @@
         <v>330</v>
       </c>
       <c r="D110" s="1" t="n">
-        <v>2606</v>
+        <v>3024</v>
       </c>
       <c r="E110" s="12" t="n">
         <f aca="false">D110/65.27</f>
-        <v>39.9264593228129</v>
+        <v>46.3306266278535</v>
       </c>
       <c r="F110" s="12" t="n">
-        <v>292</v>
+        <v>418</v>
       </c>
       <c r="G110" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H110" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,G110)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I110" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J110" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,I110)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K110" s="13" t="n">
-        <f aca="false">$B$106+1</f>
+        <f aca="false">$B$118+1</f>
         <v>43920</v>
       </c>
       <c r="L110" s="0"/>
@@ -4085,38 +4111,38 @@
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B111" s="0" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C111" s="12" t="n">
-        <v>1660</v>
-      </c>
-      <c r="D111" s="1" t="n">
-        <v>2583</v>
+        <v>50</v>
+      </c>
+      <c r="D111" s="12" t="n">
+        <v>146</v>
       </c>
       <c r="E111" s="12" t="n">
-        <f aca="false">D111/331</f>
-        <v>7.8036253776435</v>
+        <f aca="false">D111/10.36</f>
+        <v>14.0926640926641</v>
       </c>
       <c r="F111" s="12" t="n">
-        <v>363</v>
+        <v>36</v>
       </c>
       <c r="G111" s="13" t="n">
-        <v>43917</v>
+        <v>43915</v>
       </c>
       <c r="H111" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,G111)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I111" s="13" t="n">
         <f aca="false">$B$106+1</f>
-        <v>43920</v>
+        <v>43921</v>
       </c>
       <c r="J111" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,I111)</f>
         <v>-1</v>
       </c>
       <c r="K111" s="13" t="n">
-        <f aca="false">$B$106+1</f>
+        <f aca="false">$B$118+1</f>
         <v>43920</v>
       </c>
       <c r="L111" s="0"/>
@@ -4134,32 +4160,32 @@
         <v>330</v>
       </c>
       <c r="D112" s="1" t="n">
-        <v>1228</v>
+        <v>1408</v>
       </c>
       <c r="E112" s="12" t="n">
         <f aca="false">D112/67.79</f>
-        <v>18.1147661897035</v>
+        <v>20.770025077445</v>
       </c>
       <c r="F112" s="12" t="n">
-        <v>209</v>
+        <v>180</v>
       </c>
       <c r="G112" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H112" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,G112)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I112" s="13" t="n">
         <f aca="false">$B$106+1</f>
-        <v>43920</v>
+        <v>43921</v>
       </c>
       <c r="J112" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,I112)</f>
         <v>-1</v>
       </c>
       <c r="K112" s="13" t="n">
-        <f aca="false">$B$106+1</f>
+        <f aca="false">$B$118+1</f>
         <v>43920</v>
       </c>
       <c r="L112" s="0"/>
@@ -4171,38 +4197,37 @@
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C113" s="12" t="n">
-        <v>414</v>
+        <v>1660</v>
       </c>
       <c r="D113" s="1" t="n">
-        <v>541</v>
+        <v>3141</v>
       </c>
       <c r="E113" s="12" t="n">
-        <f aca="false">D113/83.784</f>
-        <v>6.457080110761</v>
+        <f aca="false">D113/331</f>
+        <v>9.48942598187311</v>
       </c>
       <c r="F113" s="12" t="n">
-        <v>108</v>
+        <v>573</v>
       </c>
       <c r="G113" s="13" t="n">
-        <v>43918</v>
+        <v>43917</v>
       </c>
       <c r="H113" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,G113)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I113" s="13" t="n">
-        <f aca="false">$B$106+1</f>
         <v>43920</v>
       </c>
       <c r="J113" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,I113)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="K113" s="13" t="n">
-        <f aca="false">$B$106+1</f>
+        <f aca="false">$B$118+1</f>
         <v>43920</v>
       </c>
       <c r="L113" s="0"/>
@@ -4214,38 +4239,38 @@
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C114" s="12" t="n">
-        <v>50</v>
-      </c>
-      <c r="D114" s="12" t="n">
-        <v>110</v>
+        <v>414</v>
+      </c>
+      <c r="D114" s="1" t="n">
+        <v>645</v>
       </c>
       <c r="E114" s="12" t="n">
-        <f aca="false">D114/10.36</f>
-        <v>10.6177606177606</v>
+        <f aca="false">D114/83.784</f>
+        <v>7.69836723002005</v>
       </c>
       <c r="F114" s="12" t="n">
-        <v>5</v>
+        <v>104</v>
       </c>
       <c r="G114" s="13" t="n">
-        <v>43915</v>
+        <v>43918</v>
       </c>
       <c r="H114" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,G114)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I114" s="13" t="n">
         <f aca="false">$B$106+1</f>
-        <v>43920</v>
+        <v>43921</v>
       </c>
       <c r="J114" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,I114)</f>
         <v>-1</v>
       </c>
       <c r="K114" s="13" t="n">
-        <f aca="false">$B$106+1</f>
+        <f aca="false">$B$118+1</f>
         <v>43920</v>
       </c>
       <c r="L114" s="0"/>
@@ -4312,15 +4337,13 @@
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="7" t="n">
-        <v>43918</v>
-      </c>
-      <c r="D118" s="8" t="s">
-        <v>10</v>
-      </c>
+        <v>43919</v>
+      </c>
+      <c r="D118" s="0"/>
       <c r="E118" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F118" s="8"/>
+      <c r="F118" s="0"/>
       <c r="G118" s="8" t="s">
         <v>33</v>
       </c>
@@ -4348,8 +4371,8 @@
       <c r="C119" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D119" s="10" t="s">
-        <v>6</v>
+      <c r="D119" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="E119" s="10" t="s">
         <v>39</v>
@@ -4387,32 +4410,32 @@
         <v>300</v>
       </c>
       <c r="D120" s="1" t="n">
-        <v>10023</v>
+        <v>10779</v>
       </c>
       <c r="E120" s="12" t="n">
         <f aca="false">D120/60.48</f>
-        <v>165.724206349206</v>
+        <v>178.224206349206</v>
       </c>
       <c r="F120" s="12" t="n">
-        <v>889</v>
+        <v>756</v>
       </c>
       <c r="G120" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H120" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$118,G120)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I120" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J120" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$130,I120)</f>
-        <v>15</v>
+        <f aca="false">_xlfn.DAYS($B$118,I120)</f>
+        <v>17</v>
       </c>
       <c r="K120" s="13" t="n">
         <f aca="false">$B$118+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L120" s="0"/>
       <c r="M120" s="0"/>
@@ -4429,32 +4452,32 @@
         <v>230</v>
       </c>
       <c r="D121" s="1" t="n">
-        <v>5982</v>
+        <v>6803</v>
       </c>
       <c r="E121" s="12" t="n">
         <f aca="false">D121/46.75</f>
-        <v>127.957219251337</v>
+        <v>145.51871657754</v>
       </c>
       <c r="F121" s="12" t="n">
-        <v>844</v>
+        <v>821</v>
       </c>
       <c r="G121" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H121" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$118,G121)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I121" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J121" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$130,I121)</f>
-        <v>4</v>
+        <f aca="false">_xlfn.DAYS($B$118,I121)</f>
+        <v>6</v>
       </c>
       <c r="K121" s="13" t="n">
         <f aca="false">$B$118+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L121" s="0"/>
       <c r="M121" s="0"/>
@@ -4471,32 +4494,32 @@
         <v>330</v>
       </c>
       <c r="D122" s="1" t="n">
-        <v>2314</v>
+        <v>2606</v>
       </c>
       <c r="E122" s="12" t="n">
         <f aca="false">D122/65.27</f>
-        <v>35.4527347939329</v>
+        <v>39.9264593228129</v>
       </c>
       <c r="F122" s="12" t="n">
-        <v>319</v>
+        <v>292</v>
       </c>
       <c r="G122" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H122" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$118,G122)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I122" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J122" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$130,I122)</f>
-        <v>3</v>
+        <f aca="false">_xlfn.DAYS($B$118,I122)</f>
+        <v>5</v>
       </c>
       <c r="K122" s="13" t="n">
         <f aca="false">$B$118+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L122" s="0"/>
       <c r="M122" s="0"/>
@@ -4513,25 +4536,25 @@
         <v>1660</v>
       </c>
       <c r="D123" s="1" t="n">
-        <v>2221</v>
+        <v>2583</v>
       </c>
       <c r="E123" s="12" t="n">
         <f aca="false">D123/331</f>
-        <v>6.70996978851964</v>
+        <v>7.8036253776435</v>
       </c>
       <c r="F123" s="12" t="n">
-        <v>525</v>
+        <v>363</v>
       </c>
       <c r="G123" s="13" t="n">
         <v>43917</v>
       </c>
       <c r="H123" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$118,G123)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I123" s="13" t="n">
         <f aca="false">$B$118+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="J123" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$118,I123)</f>
@@ -4539,7 +4562,7 @@
       </c>
       <c r="K123" s="13" t="n">
         <f aca="false">$B$118+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L123" s="0"/>
       <c r="M123" s="0"/>
@@ -4556,25 +4579,25 @@
         <v>330</v>
       </c>
       <c r="D124" s="1" t="n">
-        <v>1019</v>
+        <v>1228</v>
       </c>
       <c r="E124" s="12" t="n">
         <f aca="false">D124/67.79</f>
-        <v>15.0317155922702</v>
+        <v>18.1147661897035</v>
       </c>
       <c r="F124" s="12" t="n">
-        <v>260</v>
+        <v>209</v>
       </c>
       <c r="G124" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H124" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$118,G124)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I124" s="13" t="n">
         <f aca="false">$B$118+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="J124" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$118,I124)</f>
@@ -4582,7 +4605,7 @@
       </c>
       <c r="K124" s="13" t="n">
         <f aca="false">$B$118+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L124" s="0"/>
       <c r="M124" s="0"/>
@@ -4599,25 +4622,25 @@
         <v>414</v>
       </c>
       <c r="D125" s="1" t="n">
-        <v>433</v>
+        <v>541</v>
       </c>
       <c r="E125" s="12" t="n">
         <f aca="false">D125/83.784</f>
-        <v>5.16805117922276</v>
+        <v>6.457080110761</v>
       </c>
       <c r="F125" s="12" t="n">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="G125" s="13" t="n">
         <v>43918</v>
       </c>
       <c r="H125" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$118,G125)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I125" s="13" t="n">
         <f aca="false">$B$118+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="J125" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$118,I125)</f>
@@ -4625,7 +4648,7 @@
       </c>
       <c r="K125" s="13" t="n">
         <f aca="false">$B$118+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L125" s="0"/>
       <c r="M125" s="0"/>
@@ -4642,25 +4665,25 @@
         <v>50</v>
       </c>
       <c r="D126" s="12" t="n">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="E126" s="12" t="n">
         <f aca="false">D126/10.36</f>
-        <v>10.1351351351351</v>
+        <v>10.6177606177606</v>
       </c>
       <c r="F126" s="12" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G126" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H126" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$118,G126)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I126" s="13" t="n">
         <f aca="false">$B$118+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="J126" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$118,I126)</f>
@@ -4668,7 +4691,7 @@
       </c>
       <c r="K126" s="13" t="n">
         <f aca="false">$B$118+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L126" s="0"/>
       <c r="M126" s="0"/>
@@ -4678,15 +4701,16 @@
       <c r="Q126" s="0"/>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C127" s="12"/>
-      <c r="D127" s="12"/>
-      <c r="E127" s="12"/>
-      <c r="F127" s="12"/>
-      <c r="G127" s="13"/>
+      <c r="B127" s="4"/>
+      <c r="C127" s="5"/>
+      <c r="D127" s="0"/>
+      <c r="E127" s="0"/>
+      <c r="F127" s="0"/>
+      <c r="G127" s="0"/>
       <c r="H127" s="0"/>
-      <c r="I127" s="13"/>
+      <c r="I127" s="0"/>
       <c r="J127" s="0"/>
-      <c r="K127" s="13"/>
+      <c r="K127" s="0"/>
       <c r="L127" s="0"/>
       <c r="M127" s="0"/>
       <c r="N127" s="0"/>
@@ -4731,11 +4755,10 @@
       <c r="P129" s="0"/>
       <c r="Q129" s="0"/>
     </row>
-    <row r="130" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B130" s="7" t="n">
-        <v>43917</v>
-      </c>
-      <c r="C130" s="0"/>
+        <v>43918</v>
+      </c>
       <c r="D130" s="8" t="s">
         <v>10</v>
       </c>
@@ -4758,10 +4781,14 @@
       <c r="K130" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="L130" s="8"/>
+      <c r="L130" s="0"/>
+      <c r="M130" s="0"/>
+      <c r="N130" s="0"/>
+      <c r="O130" s="0"/>
+      <c r="P130" s="0"/>
+      <c r="Q130" s="0"/>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="3"/>
       <c r="B131" s="9"/>
       <c r="C131" s="10" t="s">
         <v>38</v>
@@ -4790,7 +4817,7 @@
       <c r="K131" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="L131" s="8"/>
+      <c r="L131" s="0"/>
       <c r="M131" s="0"/>
       <c r="N131" s="0"/>
       <c r="O131" s="0"/>
@@ -4805,32 +4832,32 @@
         <v>300</v>
       </c>
       <c r="D132" s="1" t="n">
-        <v>9134</v>
+        <v>10023</v>
       </c>
       <c r="E132" s="12" t="n">
         <f aca="false">D132/60.48</f>
-        <v>151.025132275132</v>
+        <v>165.724206349206</v>
       </c>
       <c r="F132" s="12" t="n">
-        <v>919</v>
+        <v>889</v>
       </c>
       <c r="G132" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H132" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$130,G132)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I132" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J132" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$130,I132)</f>
+        <f aca="false">_xlfn.DAYS(B$142,I132)</f>
         <v>15</v>
       </c>
       <c r="K132" s="13" t="n">
         <f aca="false">$B$130+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L132" s="0"/>
       <c r="M132" s="0"/>
@@ -4847,32 +4874,32 @@
         <v>230</v>
       </c>
       <c r="D133" s="1" t="n">
-        <v>5138</v>
+        <v>5982</v>
       </c>
       <c r="E133" s="12" t="n">
         <f aca="false">D133/46.75</f>
-        <v>109.903743315508</v>
+        <v>127.957219251337</v>
       </c>
       <c r="F133" s="12" t="n">
-        <v>773</v>
+        <v>844</v>
       </c>
       <c r="G133" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H133" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$130,G133)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I133" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J133" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$130,I133)</f>
+        <f aca="false">_xlfn.DAYS(B$142,I133)</f>
         <v>4</v>
       </c>
       <c r="K133" s="13" t="n">
         <f aca="false">$B$130+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L133" s="0"/>
       <c r="M133" s="0"/>
@@ -4889,32 +4916,32 @@
         <v>330</v>
       </c>
       <c r="D134" s="1" t="n">
-        <v>1995</v>
+        <v>2314</v>
       </c>
       <c r="E134" s="12" t="n">
         <f aca="false">D134/65.27</f>
-        <v>30.5653439558756</v>
+        <v>35.4527347939329</v>
       </c>
       <c r="F134" s="12" t="n">
-        <v>299</v>
+        <v>319</v>
       </c>
       <c r="G134" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H134" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$130,G134)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I134" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J134" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$130,I134)</f>
+        <f aca="false">_xlfn.DAYS(B$142,I134)</f>
         <v>3</v>
       </c>
       <c r="K134" s="13" t="n">
         <f aca="false">$B$130+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L134" s="0"/>
       <c r="M134" s="0"/>
@@ -4931,34 +4958,33 @@
         <v>1660</v>
       </c>
       <c r="D135" s="1" t="n">
-        <v>1696</v>
+        <v>2221</v>
       </c>
       <c r="E135" s="12" t="n">
         <f aca="false">D135/331</f>
-        <v>5.12386706948641</v>
+        <v>6.70996978851964</v>
       </c>
       <c r="F135" s="12" t="n">
-        <v>400</v>
+        <v>525</v>
       </c>
       <c r="G135" s="13" t="n">
-        <f aca="false">$B$130</f>
         <v>43917</v>
       </c>
       <c r="H135" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$130,G135)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I135" s="13" t="n">
         <f aca="false">$B$130+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="J135" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$130,I135)</f>
+        <f aca="false">_xlfn.DAYS($B$130,I135)</f>
         <v>-1</v>
       </c>
       <c r="K135" s="13" t="n">
         <f aca="false">$B$130+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L135" s="0"/>
       <c r="M135" s="0"/>
@@ -4975,33 +5001,33 @@
         <v>330</v>
       </c>
       <c r="D136" s="1" t="n">
-        <v>759</v>
+        <v>1019</v>
       </c>
       <c r="E136" s="12" t="n">
         <f aca="false">D136/67.79</f>
-        <v>11.1963416433102</v>
+        <v>15.0317155922702</v>
       </c>
       <c r="F136" s="12" t="n">
-        <v>181</v>
+        <v>260</v>
       </c>
       <c r="G136" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H136" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$130,G136)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I136" s="13" t="n">
         <f aca="false">$B$130+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="J136" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$130,I136)</f>
+        <f aca="false">_xlfn.DAYS($B$130,I136)</f>
         <v>-1</v>
       </c>
       <c r="K136" s="13" t="n">
         <f aca="false">$B$130+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L136" s="0"/>
       <c r="M136" s="0"/>
@@ -5018,34 +5044,33 @@
         <v>414</v>
       </c>
       <c r="D137" s="1" t="n">
-        <v>351</v>
+        <v>433</v>
       </c>
       <c r="E137" s="12" t="n">
         <f aca="false">D137/83.784</f>
-        <v>4.18934402749928</v>
+        <v>5.16805117922276</v>
       </c>
       <c r="F137" s="12" t="n">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G137" s="13" t="n">
-        <f aca="false">$B$130+1</f>
         <v>43918</v>
       </c>
       <c r="H137" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$130,G137)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="I137" s="13" t="n">
         <f aca="false">$B$130+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="J137" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$130,I137)</f>
+        <f aca="false">_xlfn.DAYS($B$130,I137)</f>
         <v>-1</v>
       </c>
       <c r="K137" s="13" t="n">
         <f aca="false">$B$130+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L137" s="0"/>
       <c r="M137" s="0"/>
@@ -5069,26 +5094,26 @@
         <v>10.1351351351351</v>
       </c>
       <c r="F138" s="12" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="G138" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H138" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$130,G138)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I138" s="13" t="n">
         <f aca="false">$B$130+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="J138" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$130,I138)</f>
+        <f aca="false">_xlfn.DAYS($B$130,I138)</f>
         <v>-1</v>
       </c>
       <c r="K138" s="13" t="n">
         <f aca="false">$B$130+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L138" s="0"/>
       <c r="M138" s="0"/>
@@ -5098,14 +5123,15 @@
       <c r="Q138" s="0"/>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D139" s="0"/>
-      <c r="E139" s="0"/>
-      <c r="F139" s="0"/>
-      <c r="G139" s="0"/>
+      <c r="C139" s="12"/>
+      <c r="D139" s="12"/>
+      <c r="E139" s="12"/>
+      <c r="F139" s="12"/>
+      <c r="G139" s="13"/>
       <c r="H139" s="0"/>
-      <c r="I139" s="0"/>
+      <c r="I139" s="13"/>
       <c r="J139" s="0"/>
-      <c r="K139" s="0"/>
+      <c r="K139" s="13"/>
       <c r="L139" s="0"/>
       <c r="M139" s="0"/>
       <c r="N139" s="0"/>
@@ -5114,6 +5140,8 @@
       <c r="Q139" s="0"/>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B140" s="4"/>
+      <c r="C140" s="5"/>
       <c r="D140" s="0"/>
       <c r="E140" s="0"/>
       <c r="F140" s="0"/>
@@ -5148,10 +5176,11 @@
       <c r="P141" s="0"/>
       <c r="Q141" s="0"/>
     </row>
-    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B142" s="7" t="n">
-        <v>43916</v>
-      </c>
+        <v>43917</v>
+      </c>
+      <c r="C142" s="0"/>
       <c r="D142" s="8" t="s">
         <v>10</v>
       </c>
@@ -5174,17 +5203,13 @@
       <c r="K142" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="L142" s="0"/>
-      <c r="M142" s="0"/>
-      <c r="N142" s="0"/>
-      <c r="O142" s="0"/>
-      <c r="P142" s="0"/>
-      <c r="Q142" s="0"/>
+      <c r="L142" s="8"/>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="3"/>
       <c r="B143" s="9"/>
       <c r="C143" s="10" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D143" s="10" t="s">
         <v>6</v>
@@ -5210,7 +5235,7 @@
       <c r="K143" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="L143" s="0"/>
+      <c r="L143" s="8"/>
       <c r="M143" s="0"/>
       <c r="N143" s="0"/>
       <c r="O143" s="0"/>
@@ -5225,32 +5250,32 @@
         <v>300</v>
       </c>
       <c r="D144" s="1" t="n">
-        <v>8215</v>
+        <v>9134</v>
       </c>
       <c r="E144" s="12" t="n">
         <f aca="false">D144/60.48</f>
-        <v>135.830026455026</v>
+        <v>151.025132275132</v>
       </c>
       <c r="F144" s="12" t="n">
-        <v>712</v>
+        <v>919</v>
       </c>
       <c r="G144" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H144" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$142,G144)</f>
-        <v>16</v>
+        <f aca="false">_xlfn.DAYS($B$142,G144)</f>
+        <v>17</v>
       </c>
       <c r="I144" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J144" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$142,I144)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K144" s="13" t="n">
-        <f aca="false">B$142+1</f>
-        <v>43917</v>
+        <f aca="false">$B$142+1</f>
+        <v>43918</v>
       </c>
       <c r="L144" s="0"/>
       <c r="M144" s="0"/>
@@ -5267,32 +5292,32 @@
         <v>230</v>
       </c>
       <c r="D145" s="1" t="n">
-        <v>4365</v>
+        <v>5138</v>
       </c>
       <c r="E145" s="12" t="n">
         <f aca="false">D145/46.75</f>
-        <v>93.3689839572193</v>
+        <v>109.903743315508</v>
       </c>
       <c r="F145" s="12" t="n">
-        <v>718</v>
+        <v>773</v>
       </c>
       <c r="G145" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H145" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$142,G145)</f>
-        <v>9</v>
+        <f aca="false">_xlfn.DAYS($B$142,G145)</f>
+        <v>10</v>
       </c>
       <c r="I145" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J145" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$142,I145)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K145" s="13" t="n">
-        <f aca="false">B$142+1</f>
-        <v>43917</v>
+        <f aca="false">$B$142+1</f>
+        <v>43918</v>
       </c>
       <c r="L145" s="0"/>
       <c r="M145" s="0"/>
@@ -5309,32 +5334,32 @@
         <v>330</v>
       </c>
       <c r="D146" s="1" t="n">
-        <v>1696</v>
+        <v>1995</v>
       </c>
       <c r="E146" s="12" t="n">
         <f aca="false">D146/65.27</f>
-        <v>25.9843726060978</v>
+        <v>30.5653439558756</v>
       </c>
       <c r="F146" s="12" t="n">
-        <v>365</v>
+        <v>299</v>
       </c>
       <c r="G146" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H146" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$142,G146)</f>
-        <v>4</v>
+        <f aca="false">_xlfn.DAYS($B$142,G146)</f>
+        <v>5</v>
       </c>
       <c r="I146" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J146" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$142,I146)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K146" s="13" t="n">
-        <f aca="false">B$142+1</f>
-        <v>43917</v>
+        <f aca="false">$B$142+1</f>
+        <v>43918</v>
       </c>
       <c r="L146" s="0"/>
       <c r="M146" s="0"/>
@@ -5351,33 +5376,34 @@
         <v>1660</v>
       </c>
       <c r="D147" s="1" t="n">
-        <v>1295</v>
+        <v>1696</v>
       </c>
       <c r="E147" s="12" t="n">
         <f aca="false">D147/331</f>
-        <v>3.91238670694864</v>
+        <v>5.12386706948641</v>
       </c>
       <c r="F147" s="12" t="n">
-        <v>268</v>
+        <v>400</v>
       </c>
       <c r="G147" s="13" t="n">
+        <f aca="false">$B$142</f>
         <v>43917</v>
       </c>
       <c r="H147" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$142,G147)</f>
+        <f aca="false">_xlfn.DAYS($B$142,G147)</f>
+        <v>0</v>
+      </c>
+      <c r="I147" s="13" t="n">
+        <f aca="false">$B$142+1</f>
+        <v>43918</v>
+      </c>
+      <c r="J147" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$142,I147)</f>
         <v>-1</v>
       </c>
-      <c r="I147" s="13" t="n">
-        <f aca="false">B$142+1</f>
-        <v>43917</v>
-      </c>
-      <c r="J147" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$142,I147)</f>
-        <v>-1</v>
-      </c>
       <c r="K147" s="13" t="n">
-        <f aca="false">B$142+1</f>
-        <v>43917</v>
+        <f aca="false">$B$142+1</f>
+        <v>43918</v>
       </c>
       <c r="L147" s="0"/>
       <c r="M147" s="0"/>
@@ -5394,33 +5420,33 @@
         <v>330</v>
       </c>
       <c r="D148" s="1" t="n">
-        <v>578</v>
+        <v>759</v>
       </c>
       <c r="E148" s="12" t="n">
         <f aca="false">D148/67.79</f>
-        <v>8.52633131730344</v>
+        <v>11.1963416433102</v>
       </c>
       <c r="F148" s="12" t="n">
-        <v>115</v>
+        <v>181</v>
       </c>
       <c r="G148" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H148" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$142,G148)</f>
-        <v>0</v>
+        <f aca="false">_xlfn.DAYS($B$142,G148)</f>
+        <v>1</v>
       </c>
       <c r="I148" s="13" t="n">
-        <f aca="false">B$142+1</f>
-        <v>43917</v>
+        <f aca="false">$B$142+1</f>
+        <v>43918</v>
       </c>
       <c r="J148" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$142,I148)</f>
         <v>-1</v>
       </c>
       <c r="K148" s="13" t="n">
-        <f aca="false">B$142+1</f>
-        <v>43917</v>
+        <f aca="false">$B$142+1</f>
+        <v>43918</v>
       </c>
       <c r="L148" s="0"/>
       <c r="M148" s="0"/>
@@ -5437,33 +5463,34 @@
         <v>414</v>
       </c>
       <c r="D149" s="1" t="n">
-        <v>267</v>
+        <v>351</v>
       </c>
       <c r="E149" s="12" t="n">
         <f aca="false">D149/83.784</f>
-        <v>3.18676596963621</v>
+        <v>4.18934402749928</v>
       </c>
       <c r="F149" s="12" t="n">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="G149" s="13" t="n">
-        <v>43917</v>
+        <f aca="false">$B$142+1</f>
+        <v>43918</v>
       </c>
       <c r="H149" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$142,G149)</f>
+        <f aca="false">_xlfn.DAYS($B$142,G149)</f>
         <v>-1</v>
       </c>
       <c r="I149" s="13" t="n">
-        <f aca="false">B$142+1</f>
-        <v>43917</v>
+        <f aca="false">$B$142+1</f>
+        <v>43918</v>
       </c>
       <c r="J149" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$142,I149)</f>
         <v>-1</v>
       </c>
       <c r="K149" s="13" t="n">
-        <f aca="false">B$142+1</f>
-        <v>43917</v>
+        <f aca="false">$B$142+1</f>
+        <v>43918</v>
       </c>
       <c r="L149" s="0"/>
       <c r="M149" s="0"/>
@@ -5480,33 +5507,33 @@
         <v>50</v>
       </c>
       <c r="D150" s="12" t="n">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="E150" s="12" t="n">
         <f aca="false">D150/10.36</f>
-        <v>7.43243243243243</v>
+        <v>10.1351351351351</v>
       </c>
       <c r="F150" s="12" t="n">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="G150" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H150" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$142,G150)</f>
-        <v>1</v>
+        <f aca="false">_xlfn.DAYS($B$142,G150)</f>
+        <v>2</v>
       </c>
       <c r="I150" s="13" t="n">
-        <f aca="false">B$142+1</f>
-        <v>43917</v>
+        <f aca="false">$B$142+1</f>
+        <v>43918</v>
       </c>
       <c r="J150" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$142,I150)</f>
         <v>-1</v>
       </c>
       <c r="K150" s="13" t="n">
-        <f aca="false">B$142+1</f>
-        <v>43917</v>
+        <f aca="false">$B$142+1</f>
+        <v>43918</v>
       </c>
       <c r="L150" s="0"/>
       <c r="M150" s="0"/>
@@ -5514,6 +5541,424 @@
       <c r="O150" s="0"/>
       <c r="P150" s="0"/>
       <c r="Q150" s="0"/>
+    </row>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D151" s="0"/>
+      <c r="E151" s="0"/>
+      <c r="F151" s="0"/>
+      <c r="G151" s="0"/>
+      <c r="H151" s="0"/>
+      <c r="I151" s="0"/>
+      <c r="J151" s="0"/>
+      <c r="K151" s="0"/>
+      <c r="L151" s="0"/>
+      <c r="M151" s="0"/>
+      <c r="N151" s="0"/>
+      <c r="O151" s="0"/>
+      <c r="P151" s="0"/>
+      <c r="Q151" s="0"/>
+    </row>
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D152" s="0"/>
+      <c r="E152" s="0"/>
+      <c r="F152" s="0"/>
+      <c r="G152" s="0"/>
+      <c r="H152" s="0"/>
+      <c r="I152" s="0"/>
+      <c r="J152" s="0"/>
+      <c r="K152" s="0"/>
+      <c r="L152" s="0"/>
+      <c r="M152" s="0"/>
+      <c r="N152" s="0"/>
+      <c r="O152" s="0"/>
+      <c r="P152" s="0"/>
+      <c r="Q152" s="0"/>
+    </row>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B153" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D153" s="0"/>
+      <c r="E153" s="0"/>
+      <c r="F153" s="0"/>
+      <c r="G153" s="0"/>
+      <c r="H153" s="0"/>
+      <c r="I153" s="0"/>
+      <c r="J153" s="0"/>
+      <c r="K153" s="0"/>
+      <c r="L153" s="0"/>
+      <c r="M153" s="0"/>
+      <c r="N153" s="0"/>
+      <c r="O153" s="0"/>
+      <c r="P153" s="0"/>
+      <c r="Q153" s="0"/>
+    </row>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B154" s="7" t="n">
+        <v>43916</v>
+      </c>
+      <c r="D154" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E154" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F154" s="8"/>
+      <c r="G154" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H154" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I154" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J154" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="K154" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="L154" s="0"/>
+      <c r="M154" s="0"/>
+      <c r="N154" s="0"/>
+      <c r="O154" s="0"/>
+      <c r="P154" s="0"/>
+      <c r="Q154" s="0"/>
+    </row>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B155" s="9"/>
+      <c r="C155" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D155" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E155" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F155" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G155" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H155" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I155" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="J155" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="K155" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="L155" s="0"/>
+      <c r="M155" s="0"/>
+      <c r="N155" s="0"/>
+      <c r="O155" s="0"/>
+      <c r="P155" s="0"/>
+      <c r="Q155" s="0"/>
+    </row>
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B156" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C156" s="12" t="n">
+        <v>300</v>
+      </c>
+      <c r="D156" s="1" t="n">
+        <v>8215</v>
+      </c>
+      <c r="E156" s="12" t="n">
+        <f aca="false">D156/60.48</f>
+        <v>135.830026455026</v>
+      </c>
+      <c r="F156" s="12" t="n">
+        <v>712</v>
+      </c>
+      <c r="G156" s="13" t="n">
+        <v>43900</v>
+      </c>
+      <c r="H156" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$154,G156)</f>
+        <v>16</v>
+      </c>
+      <c r="I156" s="13" t="n">
+        <v>43902</v>
+      </c>
+      <c r="J156" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$154,I156)</f>
+        <v>14</v>
+      </c>
+      <c r="K156" s="13" t="n">
+        <f aca="false">B$154+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L156" s="0"/>
+      <c r="M156" s="0"/>
+      <c r="N156" s="0"/>
+      <c r="O156" s="0"/>
+      <c r="P156" s="0"/>
+      <c r="Q156" s="0"/>
+    </row>
+    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B157" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C157" s="12" t="n">
+        <v>230</v>
+      </c>
+      <c r="D157" s="1" t="n">
+        <v>4365</v>
+      </c>
+      <c r="E157" s="12" t="n">
+        <f aca="false">D157/46.75</f>
+        <v>93.3689839572193</v>
+      </c>
+      <c r="F157" s="12" t="n">
+        <v>718</v>
+      </c>
+      <c r="G157" s="13" t="n">
+        <v>43907</v>
+      </c>
+      <c r="H157" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$154,G157)</f>
+        <v>9</v>
+      </c>
+      <c r="I157" s="13" t="n">
+        <v>43913</v>
+      </c>
+      <c r="J157" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$154,I157)</f>
+        <v>3</v>
+      </c>
+      <c r="K157" s="13" t="n">
+        <f aca="false">B$154+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L157" s="0"/>
+      <c r="M157" s="0"/>
+      <c r="N157" s="0"/>
+      <c r="O157" s="0"/>
+      <c r="P157" s="0"/>
+      <c r="Q157" s="0"/>
+    </row>
+    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B158" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C158" s="12" t="n">
+        <v>330</v>
+      </c>
+      <c r="D158" s="1" t="n">
+        <v>1696</v>
+      </c>
+      <c r="E158" s="12" t="n">
+        <f aca="false">D158/65.27</f>
+        <v>25.9843726060978</v>
+      </c>
+      <c r="F158" s="12" t="n">
+        <v>365</v>
+      </c>
+      <c r="G158" s="13" t="n">
+        <v>43912</v>
+      </c>
+      <c r="H158" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$154,G158)</f>
+        <v>4</v>
+      </c>
+      <c r="I158" s="13" t="n">
+        <v>43914</v>
+      </c>
+      <c r="J158" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$154,I158)</f>
+        <v>2</v>
+      </c>
+      <c r="K158" s="13" t="n">
+        <f aca="false">B$154+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L158" s="0"/>
+      <c r="M158" s="0"/>
+      <c r="N158" s="0"/>
+      <c r="O158" s="0"/>
+      <c r="P158" s="0"/>
+      <c r="Q158" s="0"/>
+    </row>
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B159" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C159" s="12" t="n">
+        <v>1660</v>
+      </c>
+      <c r="D159" s="1" t="n">
+        <v>1295</v>
+      </c>
+      <c r="E159" s="12" t="n">
+        <f aca="false">D159/331</f>
+        <v>3.91238670694864</v>
+      </c>
+      <c r="F159" s="12" t="n">
+        <v>268</v>
+      </c>
+      <c r="G159" s="13" t="n">
+        <v>43917</v>
+      </c>
+      <c r="H159" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$154,G159)</f>
+        <v>-1</v>
+      </c>
+      <c r="I159" s="13" t="n">
+        <f aca="false">B$154+1</f>
+        <v>43917</v>
+      </c>
+      <c r="J159" s="1" t="n">
+        <f aca="false">_xlfn.DAYS($B$154,I159)</f>
+        <v>-1</v>
+      </c>
+      <c r="K159" s="13" t="n">
+        <f aca="false">B$154+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L159" s="0"/>
+      <c r="M159" s="0"/>
+      <c r="N159" s="0"/>
+      <c r="O159" s="0"/>
+      <c r="P159" s="0"/>
+      <c r="Q159" s="0"/>
+    </row>
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B160" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C160" s="12" t="n">
+        <v>330</v>
+      </c>
+      <c r="D160" s="1" t="n">
+        <v>578</v>
+      </c>
+      <c r="E160" s="12" t="n">
+        <f aca="false">D160/67.79</f>
+        <v>8.52633131730344</v>
+      </c>
+      <c r="F160" s="12" t="n">
+        <v>115</v>
+      </c>
+      <c r="G160" s="13" t="n">
+        <v>43916</v>
+      </c>
+      <c r="H160" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$154,G160)</f>
+        <v>0</v>
+      </c>
+      <c r="I160" s="13" t="n">
+        <f aca="false">B$154+1</f>
+        <v>43917</v>
+      </c>
+      <c r="J160" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$154,I160)</f>
+        <v>-1</v>
+      </c>
+      <c r="K160" s="13" t="n">
+        <f aca="false">B$154+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L160" s="0"/>
+      <c r="M160" s="0"/>
+      <c r="N160" s="0"/>
+      <c r="O160" s="0"/>
+      <c r="P160" s="0"/>
+      <c r="Q160" s="0"/>
+    </row>
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B161" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C161" s="12" t="n">
+        <v>414</v>
+      </c>
+      <c r="D161" s="1" t="n">
+        <v>267</v>
+      </c>
+      <c r="E161" s="12" t="n">
+        <f aca="false">D161/83.784</f>
+        <v>3.18676596963621</v>
+      </c>
+      <c r="F161" s="12" t="n">
+        <v>61</v>
+      </c>
+      <c r="G161" s="13" t="n">
+        <v>43917</v>
+      </c>
+      <c r="H161" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$154,G161)</f>
+        <v>-1</v>
+      </c>
+      <c r="I161" s="13" t="n">
+        <f aca="false">B$154+1</f>
+        <v>43917</v>
+      </c>
+      <c r="J161" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$154,I161)</f>
+        <v>-1</v>
+      </c>
+      <c r="K161" s="13" t="n">
+        <f aca="false">B$154+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L161" s="0"/>
+      <c r="M161" s="0"/>
+      <c r="N161" s="0"/>
+      <c r="O161" s="0"/>
+      <c r="P161" s="0"/>
+      <c r="Q161" s="0"/>
+    </row>
+    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B162" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C162" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="D162" s="12" t="n">
+        <v>77</v>
+      </c>
+      <c r="E162" s="12" t="n">
+        <f aca="false">D162/10.36</f>
+        <v>7.43243243243243</v>
+      </c>
+      <c r="F162" s="12" t="n">
+        <v>15</v>
+      </c>
+      <c r="G162" s="13" t="n">
+        <v>43915</v>
+      </c>
+      <c r="H162" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$154,G162)</f>
+        <v>1</v>
+      </c>
+      <c r="I162" s="13" t="n">
+        <f aca="false">B$154+1</f>
+        <v>43917</v>
+      </c>
+      <c r="J162" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$154,I162)</f>
+        <v>-1</v>
+      </c>
+      <c r="K162" s="13" t="n">
+        <f aca="false">B$154+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L162" s="0"/>
+      <c r="M162" s="0"/>
+      <c r="N162" s="0"/>
+      <c r="O162" s="0"/>
+      <c r="P162" s="0"/>
+      <c r="Q162" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
updated with 2020-04-07 available data
</commit_message>
<xml_diff>
--- a/covid19 lockdown evaluation .xlsx
+++ b/covid19 lockdown evaluation .xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="53">
   <si>
     <t>Effects of the lockdown issued by governments</t>
   </si>
@@ -353,7 +353,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q162"/>
+  <dimension ref="A1:Q174"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F31" activeCellId="0" sqref="F31"/>
@@ -805,7 +805,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="7" t="n">
-        <v>43927</v>
+        <v>43928</v>
       </c>
       <c r="D22" s="0"/>
       <c r="E22" s="8" t="s">
@@ -882,36 +882,36 @@
         <v>300</v>
       </c>
       <c r="D24" s="1" t="n">
-        <v>16523</v>
+        <v>17127</v>
       </c>
       <c r="E24" s="12" t="n">
         <f aca="false">D24/60.48</f>
-        <v>273.197751322751</v>
+        <v>283.184523809524</v>
       </c>
       <c r="F24" s="12" t="n">
-        <v>636</v>
+        <v>604</v>
       </c>
       <c r="G24" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H24" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,G24)</f>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I24" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J24" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I24)</f>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K24" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43928</v>
+        <v>43929</v>
       </c>
       <c r="L24" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K24,G24)</f>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M24" s="0"/>
       <c r="N24" s="0"/>
@@ -927,36 +927,36 @@
         <v>230</v>
       </c>
       <c r="D25" s="1" t="n">
-        <v>13341</v>
+        <v>14045</v>
       </c>
       <c r="E25" s="12" t="n">
         <f aca="false">D25/46.75</f>
-        <v>285.368983957219</v>
+        <v>300.427807486631</v>
       </c>
       <c r="F25" s="12" t="n">
-        <v>700</v>
+        <v>704</v>
       </c>
       <c r="G25" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H25" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,G25)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I25" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J25" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I25)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K25" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43928</v>
+        <v>43929</v>
       </c>
       <c r="L25" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K25,G25)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M25" s="0"/>
       <c r="N25" s="0"/>
@@ -972,36 +972,36 @@
         <v>330</v>
       </c>
       <c r="D26" s="1" t="n">
-        <v>8911</v>
+        <v>10328</v>
       </c>
       <c r="E26" s="12" t="n">
         <f aca="false">D26/65.27</f>
-        <v>136.525203002911</v>
+        <v>158.23502374751</v>
       </c>
       <c r="F26" s="12" t="n">
-        <v>833</v>
+        <v>1417</v>
       </c>
       <c r="G26" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H26" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,G26)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I26" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J26" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I26)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K26" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43928</v>
+        <v>43929</v>
       </c>
       <c r="L26" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K26,G26)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M26" s="0"/>
       <c r="N26" s="0"/>
@@ -1017,37 +1017,36 @@
         <v>50</v>
       </c>
       <c r="D27" s="12" t="n">
-        <v>477</v>
+        <v>591</v>
       </c>
       <c r="E27" s="12" t="n">
         <f aca="false">D27/10.36</f>
-        <v>46.042471042471</v>
+        <v>57.0463320463321</v>
       </c>
       <c r="F27" s="12" t="n">
-        <v>76</v>
+        <v>114</v>
       </c>
       <c r="G27" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H27" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,G27)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I27" s="13" t="n">
-        <f aca="false">$B$22+1</f>
         <v>43928</v>
       </c>
       <c r="J27" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I27)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="K27" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43928</v>
+        <v>43929</v>
       </c>
       <c r="L27" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K27,G27)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="M27" s="0"/>
       <c r="N27" s="0"/>
@@ -1063,37 +1062,36 @@
         <v>330</v>
       </c>
       <c r="D28" s="1" t="n">
-        <v>5373</v>
+        <v>6159</v>
       </c>
       <c r="E28" s="12" t="n">
         <f aca="false">D28/67.79</f>
-        <v>79.2594777990854</v>
+        <v>90.8541082755569</v>
       </c>
       <c r="F28" s="12" t="n">
-        <v>439</v>
+        <v>786</v>
       </c>
       <c r="G28" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H28" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,G28)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I28" s="13" t="n">
-        <f aca="false">$B$22+1</f>
-        <v>43928</v>
+        <v>43919</v>
       </c>
       <c r="J28" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I28)</f>
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="K28" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43928</v>
+        <v>43929</v>
       </c>
       <c r="L28" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K28,G28)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M28" s="0"/>
       <c r="N28" s="0"/>
@@ -1109,37 +1107,36 @@
         <v>1660</v>
       </c>
       <c r="D29" s="1" t="n">
-        <v>10871</v>
+        <v>12481</v>
       </c>
       <c r="E29" s="12" t="n">
         <f aca="false">D29/331</f>
-        <v>32.8429003021148</v>
+        <v>37.7069486404834</v>
       </c>
       <c r="F29" s="12" t="n">
-        <v>1255</v>
+        <v>1970</v>
       </c>
       <c r="G29" s="13" t="n">
         <v>43917</v>
       </c>
       <c r="H29" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,G29)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I29" s="13" t="n">
-        <f aca="false">$B$22+1</f>
-        <v>43928</v>
+        <v>43921</v>
       </c>
       <c r="J29" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I29)</f>
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="K29" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43928</v>
+        <v>43929</v>
       </c>
       <c r="L29" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K29,G29)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M29" s="0"/>
       <c r="N29" s="0"/>
@@ -1155,37 +1152,36 @@
         <v>414</v>
       </c>
       <c r="D30" s="1" t="n">
-        <v>1810</v>
+        <v>2016</v>
       </c>
       <c r="E30" s="12" t="n">
         <f aca="false">D30/83.784</f>
-        <v>21.6031700563353</v>
+        <v>24.0618733887138</v>
       </c>
       <c r="F30" s="12" t="n">
-        <v>226</v>
+        <v>206</v>
       </c>
       <c r="G30" s="13" t="n">
         <v>43918</v>
       </c>
       <c r="H30" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,G30)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I30" s="13" t="n">
-        <f aca="false">$B$22+1</f>
-        <v>43928</v>
+        <v>43920</v>
       </c>
       <c r="J30" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$22,I30)</f>
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="K30" s="13" t="n">
         <f aca="false">$B$22+1</f>
-        <v>43928</v>
+        <v>43929</v>
       </c>
       <c r="L30" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K30,G30)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M30" s="0"/>
       <c r="N30" s="0"/>
@@ -1250,7 +1246,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="7" t="n">
-        <v>43926</v>
+        <v>43927</v>
       </c>
       <c r="D34" s="0"/>
       <c r="E34" s="8" t="s">
@@ -1327,36 +1323,36 @@
         <v>300</v>
       </c>
       <c r="D36" s="1" t="n">
-        <v>15887</v>
+        <v>16523</v>
       </c>
       <c r="E36" s="12" t="n">
         <f aca="false">D36/60.48</f>
-        <v>262.681878306878</v>
+        <v>273.197751322751</v>
       </c>
       <c r="F36" s="12" t="n">
-        <v>525</v>
+        <v>636</v>
       </c>
       <c r="G36" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H36" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,G36)</f>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I36" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J36" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I36)</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K36" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43927</v>
+        <v>43928</v>
       </c>
       <c r="L36" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K36,G36)</f>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M36" s="0"/>
       <c r="N36" s="0"/>
@@ -1372,36 +1368,36 @@
         <v>230</v>
       </c>
       <c r="D37" s="1" t="n">
-        <v>12641</v>
+        <v>13341</v>
       </c>
       <c r="E37" s="12" t="n">
         <f aca="false">D37/46.75</f>
-        <v>270.395721925134</v>
+        <v>285.368983957219</v>
       </c>
       <c r="F37" s="12" t="n">
-        <v>694</v>
+        <v>700</v>
       </c>
       <c r="G37" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H37" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,G37)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I37" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J37" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I37)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K37" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43927</v>
+        <v>43928</v>
       </c>
       <c r="L37" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K37,G37)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M37" s="0"/>
       <c r="N37" s="0"/>
@@ -1417,36 +1413,36 @@
         <v>330</v>
       </c>
       <c r="D38" s="1" t="n">
-        <v>8078</v>
+        <v>8911</v>
       </c>
       <c r="E38" s="12" t="n">
         <f aca="false">D38/65.27</f>
-        <v>123.762831316072</v>
+        <v>136.525203002911</v>
       </c>
       <c r="F38" s="12" t="n">
-        <v>518</v>
+        <v>833</v>
       </c>
       <c r="G38" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H38" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,G38)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I38" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J38" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I38)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K38" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43927</v>
+        <v>43928</v>
       </c>
       <c r="L38" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K38,G38)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M38" s="0"/>
       <c r="N38" s="0"/>
@@ -1462,25 +1458,25 @@
         <v>50</v>
       </c>
       <c r="D39" s="12" t="n">
-        <v>401</v>
+        <v>477</v>
       </c>
       <c r="E39" s="12" t="n">
         <f aca="false">D39/10.36</f>
-        <v>38.7065637065637</v>
+        <v>46.042471042471</v>
       </c>
       <c r="F39" s="12" t="n">
-        <v>28</v>
+        <v>76</v>
       </c>
       <c r="G39" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H39" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,G39)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I39" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43927</v>
+        <v>43928</v>
       </c>
       <c r="J39" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I39)</f>
@@ -1488,11 +1484,11 @@
       </c>
       <c r="K39" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43927</v>
+        <v>43928</v>
       </c>
       <c r="L39" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K39,G39)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M39" s="0"/>
       <c r="N39" s="0"/>
@@ -1508,25 +1504,25 @@
         <v>330</v>
       </c>
       <c r="D40" s="1" t="n">
-        <v>4934</v>
+        <v>5373</v>
       </c>
       <c r="E40" s="12" t="n">
         <f aca="false">D40/67.79</f>
-        <v>72.7835964006491</v>
+        <v>79.2594777990854</v>
       </c>
       <c r="F40" s="12" t="n">
-        <v>621</v>
+        <v>439</v>
       </c>
       <c r="G40" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H40" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,G40)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I40" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43927</v>
+        <v>43928</v>
       </c>
       <c r="J40" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I40)</f>
@@ -1534,11 +1530,11 @@
       </c>
       <c r="K40" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43927</v>
+        <v>43928</v>
       </c>
       <c r="L40" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K40,G40)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M40" s="0"/>
       <c r="N40" s="0"/>
@@ -1554,25 +1550,25 @@
         <v>1660</v>
       </c>
       <c r="D41" s="1" t="n">
-        <v>9616</v>
+        <v>10871</v>
       </c>
       <c r="E41" s="12" t="n">
         <f aca="false">D41/331</f>
-        <v>29.0513595166163</v>
+        <v>32.8429003021148</v>
       </c>
       <c r="F41" s="12" t="n">
-        <v>1165</v>
+        <v>1255</v>
       </c>
       <c r="G41" s="13" t="n">
         <v>43917</v>
       </c>
       <c r="H41" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,G41)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I41" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43927</v>
+        <v>43928</v>
       </c>
       <c r="J41" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I41)</f>
@@ -1580,11 +1576,11 @@
       </c>
       <c r="K41" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43927</v>
+        <v>43928</v>
       </c>
       <c r="L41" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K41,G41)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M41" s="0"/>
       <c r="N41" s="0"/>
@@ -1600,25 +1596,25 @@
         <v>414</v>
       </c>
       <c r="D42" s="1" t="n">
-        <v>1584</v>
+        <v>1810</v>
       </c>
       <c r="E42" s="12" t="n">
         <f aca="false">D42/83.784</f>
-        <v>18.9057576625609</v>
+        <v>21.6031700563353</v>
       </c>
       <c r="F42" s="12" t="n">
-        <v>140</v>
+        <v>226</v>
       </c>
       <c r="G42" s="13" t="n">
         <v>43918</v>
       </c>
       <c r="H42" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,G42)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I42" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43927</v>
+        <v>43928</v>
       </c>
       <c r="J42" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$34,I42)</f>
@@ -1626,11 +1622,11 @@
       </c>
       <c r="K42" s="13" t="n">
         <f aca="false">$B$34+1</f>
-        <v>43927</v>
+        <v>43928</v>
       </c>
       <c r="L42" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K42,G42)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M42" s="0"/>
       <c r="N42" s="0"/>
@@ -1695,7 +1691,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="7" t="n">
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="D46" s="0"/>
       <c r="E46" s="8" t="s">
@@ -1772,36 +1768,36 @@
         <v>300</v>
       </c>
       <c r="D48" s="1" t="n">
-        <v>15362</v>
+        <v>15887</v>
       </c>
       <c r="E48" s="12" t="n">
         <f aca="false">D48/60.48</f>
-        <v>254.001322751323</v>
+        <v>262.681878306878</v>
       </c>
       <c r="F48" s="12" t="n">
-        <v>681</v>
+        <v>525</v>
       </c>
       <c r="G48" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H48" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,G48)</f>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I48" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J48" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I48)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K48" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43926</v>
+        <v>43927</v>
       </c>
       <c r="L48" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K48,G48)</f>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M48" s="0"/>
       <c r="N48" s="0"/>
@@ -1817,36 +1813,36 @@
         <v>230</v>
       </c>
       <c r="D49" s="1" t="n">
-        <v>11947</v>
+        <v>12641</v>
       </c>
       <c r="E49" s="12" t="n">
         <f aca="false">D49/46.75</f>
-        <v>255.550802139037</v>
+        <v>270.395721925134</v>
       </c>
       <c r="F49" s="12" t="n">
-        <v>749</v>
+        <v>694</v>
       </c>
       <c r="G49" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H49" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,G49)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I49" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J49" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I49)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K49" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43926</v>
+        <v>43927</v>
       </c>
       <c r="L49" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K49,G49)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M49" s="0"/>
       <c r="N49" s="0"/>
@@ -1862,36 +1858,36 @@
         <v>330</v>
       </c>
       <c r="D50" s="1" t="n">
-        <v>7560</v>
+        <v>8078</v>
       </c>
       <c r="E50" s="12" t="n">
         <f aca="false">D50/65.27</f>
-        <v>115.826566569634</v>
+        <v>123.762831316072</v>
       </c>
       <c r="F50" s="12" t="n">
-        <v>1053</v>
+        <v>518</v>
       </c>
       <c r="G50" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H50" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,G50)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I50" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J50" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I50)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K50" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43926</v>
+        <v>43927</v>
       </c>
       <c r="L50" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K50,G50)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M50" s="0"/>
       <c r="N50" s="0"/>
@@ -1907,25 +1903,25 @@
         <v>50</v>
       </c>
       <c r="D51" s="12" t="n">
-        <v>373</v>
+        <v>401</v>
       </c>
       <c r="E51" s="12" t="n">
         <f aca="false">D51/10.36</f>
-        <v>36.003861003861</v>
+        <v>38.7065637065637</v>
       </c>
       <c r="F51" s="12" t="n">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="G51" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H51" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,G51)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I51" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43926</v>
+        <v>43927</v>
       </c>
       <c r="J51" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I51)</f>
@@ -1933,11 +1929,11 @@
       </c>
       <c r="K51" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43926</v>
+        <v>43927</v>
       </c>
       <c r="L51" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K51,G51)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M51" s="0"/>
       <c r="N51" s="0"/>
@@ -1953,25 +1949,25 @@
         <v>330</v>
       </c>
       <c r="D52" s="1" t="n">
-        <v>4313</v>
+        <v>4934</v>
       </c>
       <c r="E52" s="12" t="n">
         <f aca="false">D52/67.79</f>
-        <v>63.6229532379407</v>
+        <v>72.7835964006491</v>
       </c>
       <c r="F52" s="12" t="n">
-        <v>708</v>
+        <v>621</v>
       </c>
       <c r="G52" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H52" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,G52)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I52" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43926</v>
+        <v>43927</v>
       </c>
       <c r="J52" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I52)</f>
@@ -1979,11 +1975,11 @@
       </c>
       <c r="K52" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43926</v>
+        <v>43927</v>
       </c>
       <c r="L52" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K52,G52)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M52" s="0"/>
       <c r="N52" s="0"/>
@@ -1999,25 +1995,25 @@
         <v>1660</v>
       </c>
       <c r="D53" s="1" t="n">
-        <v>8451</v>
+        <v>9616</v>
       </c>
       <c r="E53" s="12" t="n">
         <f aca="false">D53/331</f>
-        <v>25.5317220543807</v>
+        <v>29.0513595166163</v>
       </c>
       <c r="F53" s="12" t="n">
-        <v>1330</v>
+        <v>1165</v>
       </c>
       <c r="G53" s="13" t="n">
         <v>43917</v>
       </c>
       <c r="H53" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,G53)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I53" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43926</v>
+        <v>43927</v>
       </c>
       <c r="J53" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I53)</f>
@@ -2025,11 +2021,11 @@
       </c>
       <c r="K53" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43926</v>
+        <v>43927</v>
       </c>
       <c r="L53" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K53,G53)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M53" s="0"/>
       <c r="N53" s="0"/>
@@ -2045,25 +2041,25 @@
         <v>414</v>
       </c>
       <c r="D54" s="1" t="n">
-        <v>1444</v>
+        <v>1584</v>
       </c>
       <c r="E54" s="12" t="n">
         <f aca="false">D54/83.784</f>
-        <v>17.2347942327891</v>
+        <v>18.9057576625609</v>
       </c>
       <c r="F54" s="12" t="n">
-        <v>169</v>
+        <v>140</v>
       </c>
       <c r="G54" s="13" t="n">
         <v>43918</v>
       </c>
       <c r="H54" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,G54)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I54" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43926</v>
+        <v>43927</v>
       </c>
       <c r="J54" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$46,I54)</f>
@@ -2071,11 +2067,11 @@
       </c>
       <c r="K54" s="13" t="n">
         <f aca="false">$B$46+1</f>
-        <v>43926</v>
+        <v>43927</v>
       </c>
       <c r="L54" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K54,G54)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M54" s="0"/>
       <c r="N54" s="0"/>
@@ -2140,7 +2136,7 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="7" t="n">
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="D58" s="0"/>
       <c r="E58" s="8" t="s">
@@ -2217,36 +2213,36 @@
         <v>300</v>
       </c>
       <c r="D60" s="1" t="n">
-        <v>14681</v>
+        <v>15362</v>
       </c>
       <c r="E60" s="12" t="n">
         <f aca="false">D60/60.48</f>
-        <v>242.741402116402</v>
+        <v>254.001322751323</v>
       </c>
       <c r="F60" s="12" t="n">
-        <v>766</v>
+        <v>681</v>
       </c>
       <c r="G60" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H60" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,G60)</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I60" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J60" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I60)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K60" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="L60" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K60,G60)</f>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M60" s="0"/>
       <c r="N60" s="0"/>
@@ -2262,36 +2258,36 @@
         <v>230</v>
       </c>
       <c r="D61" s="1" t="n">
-        <v>11198</v>
+        <v>11947</v>
       </c>
       <c r="E61" s="12" t="n">
         <f aca="false">D61/46.75</f>
-        <v>239.529411764706</v>
+        <v>255.550802139037</v>
       </c>
       <c r="F61" s="12" t="n">
-        <v>850</v>
+        <v>749</v>
       </c>
       <c r="G61" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H61" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$70,G61)</f>
-        <v>16</v>
+        <f aca="false">_xlfn.DAYS($B$58,G61)</f>
+        <v>18</v>
       </c>
       <c r="I61" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J61" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I61)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K61" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="L61" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K61,G61)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M61" s="0"/>
       <c r="N61" s="0"/>
@@ -2307,36 +2303,36 @@
         <v>330</v>
       </c>
       <c r="D62" s="1" t="n">
-        <v>6507</v>
+        <v>7560</v>
       </c>
       <c r="E62" s="12" t="n">
         <f aca="false">D62/65.27</f>
-        <v>99.6935805117206</v>
+        <v>115.826566569634</v>
       </c>
       <c r="F62" s="12" t="n">
-        <v>1120</v>
+        <v>1053</v>
       </c>
       <c r="G62" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H62" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$70,G62)</f>
-        <v>11</v>
+        <f aca="false">_xlfn.DAYS($B$58,G62)</f>
+        <v>13</v>
       </c>
       <c r="I62" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J62" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I62)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K62" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="L62" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K62,G62)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="M62" s="0"/>
       <c r="N62" s="0"/>
@@ -2352,25 +2348,25 @@
         <v>50</v>
       </c>
       <c r="D63" s="12" t="n">
-        <v>358</v>
+        <v>373</v>
       </c>
       <c r="E63" s="12" t="n">
         <f aca="false">D63/10.36</f>
-        <v>34.5559845559846</v>
+        <v>36.003861003861</v>
       </c>
       <c r="F63" s="12" t="n">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="G63" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H63" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$70,G63)</f>
-        <v>8</v>
+        <f aca="false">_xlfn.DAYS($B$58,G63)</f>
+        <v>10</v>
       </c>
       <c r="I63" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="J63" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I63)</f>
@@ -2378,11 +2374,11 @@
       </c>
       <c r="K63" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="L63" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K63,G63)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M63" s="0"/>
       <c r="N63" s="0"/>
@@ -2398,25 +2394,25 @@
         <v>330</v>
       </c>
       <c r="D64" s="1" t="n">
-        <v>3605</v>
+        <v>4313</v>
       </c>
       <c r="E64" s="12" t="n">
         <f aca="false">D64/67.79</f>
-        <v>53.1789349461573</v>
+        <v>63.6229532379407</v>
       </c>
       <c r="F64" s="12" t="n">
-        <v>684</v>
+        <v>708</v>
       </c>
       <c r="G64" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H64" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$70,G64)</f>
-        <v>7</v>
+        <f aca="false">_xlfn.DAYS($B$58,G64)</f>
+        <v>9</v>
       </c>
       <c r="I64" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="J64" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I64)</f>
@@ -2424,11 +2420,11 @@
       </c>
       <c r="K64" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="L64" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K64,G64)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M64" s="0"/>
       <c r="N64" s="0"/>
@@ -2444,25 +2440,25 @@
         <v>1660</v>
       </c>
       <c r="D65" s="1" t="n">
-        <v>7121</v>
+        <v>8451</v>
       </c>
       <c r="E65" s="12" t="n">
         <f aca="false">D65/331</f>
-        <v>21.5135951661631</v>
+        <v>25.5317220543807</v>
       </c>
       <c r="F65" s="12" t="n">
-        <v>1045</v>
+        <v>1330</v>
       </c>
       <c r="G65" s="13" t="n">
         <v>43917</v>
       </c>
       <c r="H65" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$70,G65)</f>
-        <v>6</v>
+        <f aca="false">_xlfn.DAYS($B$58,G65)</f>
+        <v>8</v>
       </c>
       <c r="I65" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="J65" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I65)</f>
@@ -2470,11 +2466,11 @@
       </c>
       <c r="K65" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="L65" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K65,G65)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M65" s="0"/>
       <c r="N65" s="0"/>
@@ -2490,25 +2486,25 @@
         <v>414</v>
       </c>
       <c r="D66" s="1" t="n">
-        <v>1275</v>
+        <v>1444</v>
       </c>
       <c r="E66" s="12" t="n">
         <f aca="false">D66/83.784</f>
-        <v>15.2177026639931</v>
+        <v>17.2347942327891</v>
       </c>
       <c r="F66" s="12" t="n">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G66" s="13" t="n">
         <v>43918</v>
       </c>
       <c r="H66" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$70,G66)</f>
-        <v>5</v>
+        <f aca="false">_xlfn.DAYS($B$58,G66)</f>
+        <v>7</v>
       </c>
       <c r="I66" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="J66" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$58,I66)</f>
@@ -2516,11 +2512,11 @@
       </c>
       <c r="K66" s="13" t="n">
         <f aca="false">$B$58+1</f>
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="L66" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K66,G66)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M66" s="0"/>
       <c r="N66" s="0"/>
@@ -2585,7 +2581,7 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="7" t="n">
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="D70" s="0"/>
       <c r="E70" s="8" t="s">
@@ -2662,36 +2658,36 @@
         <v>300</v>
       </c>
       <c r="D72" s="1" t="n">
-        <v>13915</v>
+        <v>14681</v>
       </c>
       <c r="E72" s="12" t="n">
         <f aca="false">D72/60.48</f>
-        <v>230.076058201058</v>
+        <v>242.741402116402</v>
       </c>
       <c r="F72" s="12" t="n">
-        <v>760</v>
+        <v>766</v>
       </c>
       <c r="G72" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H72" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,G72)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I72" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J72" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,I72)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K72" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="L72" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K72,G72)</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M72" s="0"/>
       <c r="N72" s="0"/>
@@ -2707,20 +2703,20 @@
         <v>230</v>
       </c>
       <c r="D73" s="1" t="n">
-        <v>10348</v>
+        <v>11198</v>
       </c>
       <c r="E73" s="12" t="n">
         <f aca="false">D73/46.75</f>
-        <v>221.347593582888</v>
+        <v>239.529411764706</v>
       </c>
       <c r="F73" s="12" t="n">
-        <v>961</v>
+        <v>850</v>
       </c>
       <c r="G73" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H73" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$70,G73)</f>
+        <f aca="false">_xlfn.DAYS($B$82,G73)</f>
         <v>16</v>
       </c>
       <c r="I73" s="13" t="n">
@@ -2728,15 +2724,15 @@
       </c>
       <c r="J73" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,I73)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K73" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="L73" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K73,G73)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M73" s="0"/>
       <c r="N73" s="0"/>
@@ -2752,20 +2748,20 @@
         <v>330</v>
       </c>
       <c r="D74" s="1" t="n">
-        <v>5387</v>
+        <v>6507</v>
       </c>
       <c r="E74" s="12" t="n">
         <f aca="false">D74/65.27</f>
-        <v>82.5340891680711</v>
+        <v>99.6935805117206</v>
       </c>
       <c r="F74" s="12" t="n">
-        <v>1355</v>
+        <v>1120</v>
       </c>
       <c r="G74" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H74" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$70,G74)</f>
+        <f aca="false">_xlfn.DAYS($B$82,G74)</f>
         <v>11</v>
       </c>
       <c r="I74" s="13" t="n">
@@ -2773,15 +2769,15 @@
       </c>
       <c r="J74" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,I74)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K74" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="L74" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K74,G74)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M74" s="0"/>
       <c r="N74" s="0"/>
@@ -2797,25 +2793,25 @@
         <v>50</v>
       </c>
       <c r="D75" s="12" t="n">
-        <v>308</v>
+        <v>358</v>
       </c>
       <c r="E75" s="12" t="n">
         <f aca="false">D75/10.36</f>
-        <v>29.7297297297297</v>
+        <v>34.5559845559846</v>
       </c>
       <c r="F75" s="12" t="n">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="G75" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H75" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$70,G75)</f>
+        <f aca="false">_xlfn.DAYS($B$82,G75)</f>
         <v>8</v>
       </c>
       <c r="I75" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="J75" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,I75)</f>
@@ -2823,11 +2819,11 @@
       </c>
       <c r="K75" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="L75" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K75,G75)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M75" s="0"/>
       <c r="N75" s="0"/>
@@ -2843,25 +2839,25 @@
         <v>330</v>
       </c>
       <c r="D76" s="1" t="n">
-        <v>2921</v>
+        <v>3605</v>
       </c>
       <c r="E76" s="12" t="n">
         <f aca="false">D76/67.79</f>
-        <v>43.0889511727393</v>
+        <v>53.1789349461573</v>
       </c>
       <c r="F76" s="12" t="n">
-        <v>569</v>
+        <v>684</v>
       </c>
       <c r="G76" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H76" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$70,G76)</f>
+        <f aca="false">_xlfn.DAYS($B$82,G76)</f>
         <v>7</v>
       </c>
       <c r="I76" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="J76" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,I76)</f>
@@ -2869,11 +2865,11 @@
       </c>
       <c r="K76" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="L76" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K76,G76)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M76" s="0"/>
       <c r="N76" s="0"/>
@@ -2889,25 +2885,25 @@
         <v>1660</v>
       </c>
       <c r="D77" s="1" t="n">
-        <v>6076</v>
+        <v>7121</v>
       </c>
       <c r="E77" s="12" t="n">
         <f aca="false">D77/331</f>
-        <v>18.3564954682779</v>
+        <v>21.5135951661631</v>
       </c>
       <c r="F77" s="12" t="n">
-        <v>969</v>
+        <v>1045</v>
       </c>
       <c r="G77" s="13" t="n">
         <v>43917</v>
       </c>
       <c r="H77" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$70,G77)</f>
+        <f aca="false">_xlfn.DAYS($B$82,G77)</f>
         <v>6</v>
       </c>
       <c r="I77" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="J77" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,I77)</f>
@@ -2915,11 +2911,11 @@
       </c>
       <c r="K77" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="L77" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K77,G77)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M77" s="0"/>
       <c r="N77" s="0"/>
@@ -2935,25 +2931,25 @@
         <v>414</v>
       </c>
       <c r="D78" s="1" t="n">
-        <v>1107</v>
+        <v>1275</v>
       </c>
       <c r="E78" s="12" t="n">
         <f aca="false">D78/83.784</f>
-        <v>13.212546548267</v>
+        <v>15.2177026639931</v>
       </c>
       <c r="F78" s="12" t="n">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="G78" s="13" t="n">
         <v>43918</v>
       </c>
       <c r="H78" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$70,G78)</f>
+        <f aca="false">_xlfn.DAYS($B$82,G78)</f>
         <v>5</v>
       </c>
       <c r="I78" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="J78" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$70,I78)</f>
@@ -2961,11 +2957,11 @@
       </c>
       <c r="K78" s="13" t="n">
         <f aca="false">$B$70+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="L78" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K78,G78)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M78" s="0"/>
       <c r="N78" s="0"/>
@@ -3030,7 +3026,7 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="7" t="n">
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="D82" s="0"/>
       <c r="E82" s="8" t="s">
@@ -3107,36 +3103,36 @@
         <v>300</v>
       </c>
       <c r="D84" s="1" t="n">
-        <v>13155</v>
+        <v>13915</v>
       </c>
       <c r="E84" s="12" t="n">
         <f aca="false">D84/60.48</f>
-        <v>217.509920634921</v>
+        <v>230.076058201058</v>
       </c>
       <c r="F84" s="12" t="n">
-        <v>727</v>
+        <v>760</v>
       </c>
       <c r="G84" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H84" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,G84)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I84" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J84" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,I84)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K84" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="L84" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K84,G84)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M84" s="0"/>
       <c r="N84" s="0"/>
@@ -3152,36 +3148,36 @@
         <v>230</v>
       </c>
       <c r="D85" s="1" t="n">
-        <v>9387</v>
+        <v>10348</v>
       </c>
       <c r="E85" s="12" t="n">
         <f aca="false">D85/46.75</f>
-        <v>200.791443850267</v>
+        <v>221.347593582888</v>
       </c>
       <c r="F85" s="12" t="n">
-        <v>923</v>
+        <v>961</v>
       </c>
       <c r="G85" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H85" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,G85)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I85" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J85" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,I85)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K85" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="L85" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K85,G85)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M85" s="0"/>
       <c r="N85" s="0"/>
@@ -3197,36 +3193,36 @@
         <v>330</v>
       </c>
       <c r="D86" s="1" t="n">
-        <v>4032</v>
+        <v>5387</v>
       </c>
       <c r="E86" s="12" t="n">
         <f aca="false">D86/65.27</f>
-        <v>61.7741688371381</v>
+        <v>82.5340891680711</v>
       </c>
       <c r="F86" s="12" t="n">
-        <v>509</v>
+        <v>1355</v>
       </c>
       <c r="G86" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H86" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,G86)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I86" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J86" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,I86)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K86" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="L86" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K86,G86)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M86" s="0"/>
       <c r="N86" s="0"/>
@@ -3242,25 +3238,25 @@
         <v>50</v>
       </c>
       <c r="D87" s="12" t="n">
-        <v>239</v>
+        <v>308</v>
       </c>
       <c r="E87" s="12" t="n">
         <f aca="false">D87/10.36</f>
-        <v>23.0694980694981</v>
+        <v>29.7297297297297</v>
       </c>
       <c r="F87" s="12" t="n">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="G87" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H87" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,G87)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I87" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="J87" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,I87)</f>
@@ -3268,11 +3264,11 @@
       </c>
       <c r="K87" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="L87" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K87,G87)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M87" s="0"/>
       <c r="N87" s="0"/>
@@ -3288,25 +3284,25 @@
         <v>330</v>
       </c>
       <c r="D88" s="1" t="n">
-        <v>2352</v>
+        <v>2921</v>
       </c>
       <c r="E88" s="12" t="n">
         <f aca="false">D88/67.79</f>
-        <v>34.695382799823</v>
+        <v>43.0889511727393</v>
       </c>
       <c r="F88" s="12" t="n">
-        <v>563</v>
+        <v>569</v>
       </c>
       <c r="G88" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H88" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,G88)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I88" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="J88" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,I88)</f>
@@ -3314,11 +3310,11 @@
       </c>
       <c r="K88" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="L88" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K88,G88)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M88" s="0"/>
       <c r="N88" s="0"/>
@@ -3334,25 +3330,25 @@
         <v>1660</v>
       </c>
       <c r="D89" s="1" t="n">
-        <v>5102</v>
+        <v>6076</v>
       </c>
       <c r="E89" s="12" t="n">
         <f aca="false">D89/331</f>
-        <v>15.4138972809668</v>
+        <v>18.3564954682779</v>
       </c>
       <c r="F89" s="12" t="n">
-        <v>1049</v>
+        <v>969</v>
       </c>
       <c r="G89" s="13" t="n">
         <v>43917</v>
       </c>
       <c r="H89" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,G89)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I89" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="J89" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,I89)</f>
@@ -3360,11 +3356,11 @@
       </c>
       <c r="K89" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="L89" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K89,G89)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M89" s="0"/>
       <c r="N89" s="0"/>
@@ -3380,25 +3376,25 @@
         <v>414</v>
       </c>
       <c r="D90" s="1" t="n">
-        <v>931</v>
+        <v>1107</v>
       </c>
       <c r="E90" s="12" t="n">
         <f aca="false">D90/83.784</f>
-        <v>11.1119068079824</v>
+        <v>13.212546548267</v>
       </c>
       <c r="F90" s="12" t="n">
-        <v>156</v>
+        <v>176</v>
       </c>
       <c r="G90" s="13" t="n">
         <v>43918</v>
       </c>
       <c r="H90" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,G90)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I90" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="J90" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$82,I90)</f>
@@ -3406,11 +3402,11 @@
       </c>
       <c r="K90" s="13" t="n">
         <f aca="false">$B$82+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="L90" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K90,G90)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M90" s="0"/>
       <c r="N90" s="0"/>
@@ -3475,7 +3471,7 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="7" t="n">
-        <v>43921</v>
+        <v>43922</v>
       </c>
       <c r="D94" s="0"/>
       <c r="E94" s="8" t="s">
@@ -3552,36 +3548,36 @@
         <v>300</v>
       </c>
       <c r="D96" s="1" t="n">
-        <v>12428</v>
+        <v>13155</v>
       </c>
       <c r="E96" s="12" t="n">
         <f aca="false">D96/60.48</f>
-        <v>205.489417989418</v>
+        <v>217.509920634921</v>
       </c>
       <c r="F96" s="12" t="n">
-        <v>837</v>
+        <v>727</v>
       </c>
       <c r="G96" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H96" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,G96)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I96" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J96" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,I96)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K96" s="13" t="n">
         <f aca="false">$B$94+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L96" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K96,G96)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M96" s="0"/>
       <c r="N96" s="0"/>
@@ -3597,36 +3593,36 @@
         <v>230</v>
       </c>
       <c r="D97" s="1" t="n">
-        <v>8464</v>
+        <v>9387</v>
       </c>
       <c r="E97" s="12" t="n">
         <f aca="false">D97/46.75</f>
-        <v>181.048128342246</v>
+        <v>200.791443850267</v>
       </c>
       <c r="F97" s="12" t="n">
-        <v>748</v>
+        <v>923</v>
       </c>
       <c r="G97" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H97" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,G97)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I97" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J97" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,I97)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K97" s="13" t="n">
         <f aca="false">$B$94+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L97" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K97,G97)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M97" s="0"/>
       <c r="N97" s="0"/>
@@ -3642,36 +3638,36 @@
         <v>330</v>
       </c>
       <c r="D98" s="1" t="n">
-        <v>3523</v>
+        <v>4032</v>
       </c>
       <c r="E98" s="12" t="n">
         <f aca="false">D98/65.27</f>
-        <v>53.9757928604259</v>
+        <v>61.7741688371381</v>
       </c>
       <c r="F98" s="12" t="n">
-        <v>499</v>
+        <v>509</v>
       </c>
       <c r="G98" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H98" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,G98)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I98" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J98" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,I98)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K98" s="13" t="n">
         <f aca="false">$B$94+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L98" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K98,G98)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M98" s="0"/>
       <c r="N98" s="0"/>
@@ -3687,25 +3683,25 @@
         <v>50</v>
       </c>
       <c r="D99" s="12" t="n">
-        <v>180</v>
+        <v>239</v>
       </c>
       <c r="E99" s="12" t="n">
         <f aca="false">D99/10.36</f>
-        <v>17.3745173745174</v>
+        <v>23.0694980694981</v>
       </c>
       <c r="F99" s="12" t="n">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="G99" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H99" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,G99)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I99" s="13" t="n">
         <f aca="false">$B$94+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="J99" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,I99)</f>
@@ -3713,11 +3709,11 @@
       </c>
       <c r="K99" s="13" t="n">
         <f aca="false">$B$94+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L99" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K99,G99)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M99" s="0"/>
       <c r="N99" s="0"/>
@@ -3733,25 +3729,25 @@
         <v>330</v>
       </c>
       <c r="D100" s="1" t="n">
-        <v>1789</v>
+        <v>2352</v>
       </c>
       <c r="E100" s="12" t="n">
         <f aca="false">D100/67.79</f>
-        <v>26.390323056498</v>
+        <v>34.695382799823</v>
       </c>
       <c r="F100" s="12" t="n">
-        <v>381</v>
+        <v>563</v>
       </c>
       <c r="G100" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H100" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,G100)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I100" s="13" t="n">
         <f aca="false">$B$94+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="J100" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,I100)</f>
@@ -3759,11 +3755,11 @@
       </c>
       <c r="K100" s="13" t="n">
         <f aca="false">$B$94+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L100" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K100,G100)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M100" s="0"/>
       <c r="N100" s="0"/>
@@ -3779,25 +3775,25 @@
         <v>1660</v>
       </c>
       <c r="D101" s="1" t="n">
-        <v>4053</v>
+        <v>5102</v>
       </c>
       <c r="E101" s="12" t="n">
         <f aca="false">D101/331</f>
-        <v>12.2447129909366</v>
+        <v>15.4138972809668</v>
       </c>
       <c r="F101" s="12" t="n">
-        <v>912</v>
+        <v>1049</v>
       </c>
       <c r="G101" s="13" t="n">
         <v>43917</v>
       </c>
       <c r="H101" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,G101)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I101" s="13" t="n">
         <f aca="false">$B$94+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="J101" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,I101)</f>
@@ -3805,11 +3801,11 @@
       </c>
       <c r="K101" s="13" t="n">
         <f aca="false">$B$94+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L101" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K101,G101)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M101" s="0"/>
       <c r="N101" s="0"/>
@@ -3825,25 +3821,25 @@
         <v>414</v>
       </c>
       <c r="D102" s="1" t="n">
-        <v>775</v>
+        <v>931</v>
       </c>
       <c r="E102" s="12" t="n">
         <f aca="false">D102/83.784</f>
-        <v>9.24997612909386</v>
+        <v>11.1119068079824</v>
       </c>
       <c r="F102" s="12" t="n">
-        <v>130</v>
+        <v>156</v>
       </c>
       <c r="G102" s="13" t="n">
         <v>43918</v>
       </c>
       <c r="H102" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,G102)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I102" s="13" t="n">
         <f aca="false">$B$94+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="J102" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$94,I102)</f>
@@ -3851,11 +3847,11 @@
       </c>
       <c r="K102" s="13" t="n">
         <f aca="false">$B$94+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="L102" s="0" t="n">
         <f aca="false">_xlfn.DAYS(K102,G102)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M102" s="0"/>
       <c r="N102" s="0"/>
@@ -3864,15 +3860,16 @@
       <c r="Q102" s="0"/>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C103" s="12"/>
+      <c r="B103" s="4"/>
+      <c r="C103" s="5"/>
       <c r="D103" s="0"/>
-      <c r="E103" s="12"/>
-      <c r="F103" s="12"/>
-      <c r="G103" s="13"/>
+      <c r="E103" s="0"/>
+      <c r="F103" s="0"/>
+      <c r="G103" s="0"/>
       <c r="H103" s="0"/>
-      <c r="I103" s="13"/>
+      <c r="I103" s="0"/>
       <c r="J103" s="0"/>
-      <c r="K103" s="13"/>
+      <c r="K103" s="0"/>
       <c r="L103" s="0"/>
       <c r="M103" s="0"/>
       <c r="N103" s="0"/>
@@ -3881,15 +3878,16 @@
       <c r="Q103" s="0"/>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C104" s="12"/>
+      <c r="B104" s="4"/>
+      <c r="C104" s="5"/>
       <c r="D104" s="0"/>
-      <c r="E104" s="12"/>
-      <c r="F104" s="12"/>
-      <c r="G104" s="13"/>
+      <c r="E104" s="0"/>
+      <c r="F104" s="0"/>
+      <c r="G104" s="0"/>
       <c r="H104" s="0"/>
-      <c r="I104" s="13"/>
+      <c r="I104" s="0"/>
       <c r="J104" s="0"/>
-      <c r="K104" s="13"/>
+      <c r="K104" s="0"/>
       <c r="L104" s="0"/>
       <c r="M104" s="0"/>
       <c r="N104" s="0"/>
@@ -3918,7 +3916,7 @@
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="7" t="n">
-        <v>43920</v>
+        <v>43921</v>
       </c>
       <c r="D106" s="0"/>
       <c r="E106" s="8" t="s">
@@ -3940,7 +3938,9 @@
       <c r="K106" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="L106" s="0"/>
+      <c r="L106" s="8" t="s">
+        <v>37</v>
+      </c>
       <c r="M106" s="0"/>
       <c r="N106" s="0"/>
       <c r="O106" s="0"/>
@@ -3976,7 +3976,9 @@
       <c r="K107" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="L107" s="0"/>
+      <c r="L107" s="8" t="s">
+        <v>45</v>
+      </c>
       <c r="M107" s="0"/>
       <c r="N107" s="0"/>
       <c r="O107" s="0"/>
@@ -3991,34 +3993,37 @@
         <v>300</v>
       </c>
       <c r="D108" s="1" t="n">
-        <v>11591</v>
+        <v>12428</v>
       </c>
       <c r="E108" s="12" t="n">
         <f aca="false">D108/60.48</f>
-        <v>191.650132275132</v>
+        <v>205.489417989418</v>
       </c>
       <c r="F108" s="12" t="n">
-        <v>812</v>
+        <v>837</v>
       </c>
       <c r="G108" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H108" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,G108)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I108" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J108" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,I108)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K108" s="13" t="n">
-        <f aca="false">$B$118+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L108" s="0"/>
+        <f aca="false">$B$106+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L108" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K108,G108)</f>
+        <v>22</v>
+      </c>
       <c r="M108" s="0"/>
       <c r="N108" s="0"/>
       <c r="O108" s="0"/>
@@ -4033,34 +4038,37 @@
         <v>230</v>
       </c>
       <c r="D109" s="1" t="n">
-        <v>7716</v>
+        <v>8464</v>
       </c>
       <c r="E109" s="12" t="n">
         <f aca="false">D109/46.75</f>
-        <v>165.048128342246</v>
+        <v>181.048128342246</v>
       </c>
       <c r="F109" s="12" t="n">
-        <v>913</v>
+        <v>748</v>
       </c>
       <c r="G109" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H109" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,G109)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I109" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J109" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,I109)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K109" s="13" t="n">
-        <f aca="false">$B$118+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L109" s="0"/>
+        <f aca="false">$B$106+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L109" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K109,G109)</f>
+        <v>15</v>
+      </c>
       <c r="M109" s="0"/>
       <c r="N109" s="0"/>
       <c r="O109" s="0"/>
@@ -4075,34 +4083,37 @@
         <v>330</v>
       </c>
       <c r="D110" s="1" t="n">
-        <v>3024</v>
+        <v>3523</v>
       </c>
       <c r="E110" s="12" t="n">
         <f aca="false">D110/65.27</f>
-        <v>46.3306266278535</v>
+        <v>53.9757928604259</v>
       </c>
       <c r="F110" s="12" t="n">
-        <v>418</v>
+        <v>499</v>
       </c>
       <c r="G110" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H110" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,G110)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I110" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J110" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,I110)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K110" s="13" t="n">
-        <f aca="false">$B$118+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L110" s="0"/>
+        <f aca="false">$B$106+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L110" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K110,G110)</f>
+        <v>10</v>
+      </c>
       <c r="M110" s="0"/>
       <c r="N110" s="0"/>
       <c r="O110" s="0"/>
@@ -4117,35 +4128,38 @@
         <v>50</v>
       </c>
       <c r="D111" s="12" t="n">
-        <v>146</v>
+        <v>180</v>
       </c>
       <c r="E111" s="12" t="n">
         <f aca="false">D111/10.36</f>
-        <v>14.0926640926641</v>
+        <v>17.3745173745174</v>
       </c>
       <c r="F111" s="12" t="n">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G111" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H111" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,G111)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I111" s="13" t="n">
         <f aca="false">$B$106+1</f>
-        <v>43921</v>
+        <v>43922</v>
       </c>
       <c r="J111" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,I111)</f>
         <v>-1</v>
       </c>
       <c r="K111" s="13" t="n">
-        <f aca="false">$B$118+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L111" s="0"/>
+        <f aca="false">$B$106+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L111" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K111,G111)</f>
+        <v>7</v>
+      </c>
       <c r="M111" s="0"/>
       <c r="N111" s="0"/>
       <c r="O111" s="0"/>
@@ -4160,35 +4174,38 @@
         <v>330</v>
       </c>
       <c r="D112" s="1" t="n">
-        <v>1408</v>
+        <v>1789</v>
       </c>
       <c r="E112" s="12" t="n">
         <f aca="false">D112/67.79</f>
-        <v>20.770025077445</v>
+        <v>26.390323056498</v>
       </c>
       <c r="F112" s="12" t="n">
-        <v>180</v>
+        <v>381</v>
       </c>
       <c r="G112" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H112" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,G112)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I112" s="13" t="n">
         <f aca="false">$B$106+1</f>
-        <v>43921</v>
+        <v>43922</v>
       </c>
       <c r="J112" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,I112)</f>
         <v>-1</v>
       </c>
       <c r="K112" s="13" t="n">
-        <f aca="false">$B$118+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L112" s="0"/>
+        <f aca="false">$B$106+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L112" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K112,G112)</f>
+        <v>6</v>
+      </c>
       <c r="M112" s="0"/>
       <c r="N112" s="0"/>
       <c r="O112" s="0"/>
@@ -4203,34 +4220,38 @@
         <v>1660</v>
       </c>
       <c r="D113" s="1" t="n">
-        <v>3141</v>
+        <v>4053</v>
       </c>
       <c r="E113" s="12" t="n">
         <f aca="false">D113/331</f>
-        <v>9.48942598187311</v>
+        <v>12.2447129909366</v>
       </c>
       <c r="F113" s="12" t="n">
-        <v>573</v>
+        <v>912</v>
       </c>
       <c r="G113" s="13" t="n">
         <v>43917</v>
       </c>
       <c r="H113" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,G113)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I113" s="13" t="n">
-        <v>43920</v>
+        <f aca="false">$B$106+1</f>
+        <v>43922</v>
       </c>
       <c r="J113" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,I113)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="K113" s="13" t="n">
-        <f aca="false">$B$118+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L113" s="0"/>
+        <f aca="false">$B$106+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L113" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K113,G113)</f>
+        <v>5</v>
+      </c>
       <c r="M113" s="0"/>
       <c r="N113" s="0"/>
       <c r="O113" s="0"/>
@@ -4245,35 +4266,38 @@
         <v>414</v>
       </c>
       <c r="D114" s="1" t="n">
-        <v>645</v>
+        <v>775</v>
       </c>
       <c r="E114" s="12" t="n">
         <f aca="false">D114/83.784</f>
-        <v>7.69836723002005</v>
+        <v>9.24997612909386</v>
       </c>
       <c r="F114" s="12" t="n">
-        <v>104</v>
+        <v>130</v>
       </c>
       <c r="G114" s="13" t="n">
         <v>43918</v>
       </c>
       <c r="H114" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,G114)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I114" s="13" t="n">
         <f aca="false">$B$106+1</f>
-        <v>43921</v>
+        <v>43922</v>
       </c>
       <c r="J114" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$106,I114)</f>
         <v>-1</v>
       </c>
       <c r="K114" s="13" t="n">
-        <f aca="false">$B$118+1</f>
-        <v>43920</v>
-      </c>
-      <c r="L114" s="0"/>
+        <f aca="false">$B$106+1</f>
+        <v>43922</v>
+      </c>
+      <c r="L114" s="0" t="n">
+        <f aca="false">_xlfn.DAYS(K114,G114)</f>
+        <v>4</v>
+      </c>
       <c r="M114" s="0"/>
       <c r="N114" s="0"/>
       <c r="O114" s="0"/>
@@ -4281,16 +4305,15 @@
       <c r="Q114" s="0"/>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B115" s="4"/>
-      <c r="C115" s="5"/>
+      <c r="C115" s="12"/>
       <c r="D115" s="0"/>
-      <c r="E115" s="0"/>
-      <c r="F115" s="0"/>
-      <c r="G115" s="0"/>
+      <c r="E115" s="12"/>
+      <c r="F115" s="12"/>
+      <c r="G115" s="13"/>
       <c r="H115" s="0"/>
-      <c r="I115" s="0"/>
+      <c r="I115" s="13"/>
       <c r="J115" s="0"/>
-      <c r="K115" s="0"/>
+      <c r="K115" s="13"/>
       <c r="L115" s="0"/>
       <c r="M115" s="0"/>
       <c r="N115" s="0"/>
@@ -4299,16 +4322,15 @@
       <c r="Q115" s="0"/>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B116" s="4"/>
-      <c r="C116" s="5"/>
+      <c r="C116" s="12"/>
       <c r="D116" s="0"/>
-      <c r="E116" s="0"/>
-      <c r="F116" s="0"/>
-      <c r="G116" s="0"/>
+      <c r="E116" s="12"/>
+      <c r="F116" s="12"/>
+      <c r="G116" s="13"/>
       <c r="H116" s="0"/>
-      <c r="I116" s="0"/>
+      <c r="I116" s="13"/>
       <c r="J116" s="0"/>
-      <c r="K116" s="0"/>
+      <c r="K116" s="13"/>
       <c r="L116" s="0"/>
       <c r="M116" s="0"/>
       <c r="N116" s="0"/>
@@ -4337,7 +4359,7 @@
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="7" t="n">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="D118" s="0"/>
       <c r="E118" s="8" t="s">
@@ -4410,31 +4432,31 @@
         <v>300</v>
       </c>
       <c r="D120" s="1" t="n">
-        <v>10779</v>
+        <v>11591</v>
       </c>
       <c r="E120" s="12" t="n">
         <f aca="false">D120/60.48</f>
-        <v>178.224206349206</v>
+        <v>191.650132275132</v>
       </c>
       <c r="F120" s="12" t="n">
-        <v>756</v>
+        <v>812</v>
       </c>
       <c r="G120" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H120" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$118,G120)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I120" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J120" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$118,I120)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K120" s="13" t="n">
-        <f aca="false">$B$118+1</f>
+        <f aca="false">$B$130+1</f>
         <v>43920</v>
       </c>
       <c r="L120" s="0"/>
@@ -4452,31 +4474,31 @@
         <v>230</v>
       </c>
       <c r="D121" s="1" t="n">
-        <v>6803</v>
+        <v>7716</v>
       </c>
       <c r="E121" s="12" t="n">
         <f aca="false">D121/46.75</f>
-        <v>145.51871657754</v>
+        <v>165.048128342246</v>
       </c>
       <c r="F121" s="12" t="n">
-        <v>821</v>
+        <v>913</v>
       </c>
       <c r="G121" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H121" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$118,G121)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I121" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J121" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$118,I121)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K121" s="13" t="n">
-        <f aca="false">$B$118+1</f>
+        <f aca="false">$B$130+1</f>
         <v>43920</v>
       </c>
       <c r="L121" s="0"/>
@@ -4494,31 +4516,31 @@
         <v>330</v>
       </c>
       <c r="D122" s="1" t="n">
-        <v>2606</v>
+        <v>3024</v>
       </c>
       <c r="E122" s="12" t="n">
         <f aca="false">D122/65.27</f>
-        <v>39.9264593228129</v>
+        <v>46.3306266278535</v>
       </c>
       <c r="F122" s="12" t="n">
-        <v>292</v>
+        <v>418</v>
       </c>
       <c r="G122" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H122" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$118,G122)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I122" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J122" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$118,I122)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K122" s="13" t="n">
-        <f aca="false">$B$118+1</f>
+        <f aca="false">$B$130+1</f>
         <v>43920</v>
       </c>
       <c r="L122" s="0"/>
@@ -4530,38 +4552,38 @@
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="0" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C123" s="12" t="n">
-        <v>1660</v>
-      </c>
-      <c r="D123" s="1" t="n">
-        <v>2583</v>
+        <v>50</v>
+      </c>
+      <c r="D123" s="12" t="n">
+        <v>146</v>
       </c>
       <c r="E123" s="12" t="n">
-        <f aca="false">D123/331</f>
-        <v>7.8036253776435</v>
+        <f aca="false">D123/10.36</f>
+        <v>14.0926640926641</v>
       </c>
       <c r="F123" s="12" t="n">
-        <v>363</v>
+        <v>36</v>
       </c>
       <c r="G123" s="13" t="n">
-        <v>43917</v>
+        <v>43915</v>
       </c>
       <c r="H123" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$118,G123)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I123" s="13" t="n">
         <f aca="false">$B$118+1</f>
-        <v>43920</v>
+        <v>43921</v>
       </c>
       <c r="J123" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$118,I123)</f>
         <v>-1</v>
       </c>
       <c r="K123" s="13" t="n">
-        <f aca="false">$B$118+1</f>
+        <f aca="false">$B$130+1</f>
         <v>43920</v>
       </c>
       <c r="L123" s="0"/>
@@ -4579,32 +4601,32 @@
         <v>330</v>
       </c>
       <c r="D124" s="1" t="n">
-        <v>1228</v>
+        <v>1408</v>
       </c>
       <c r="E124" s="12" t="n">
         <f aca="false">D124/67.79</f>
-        <v>18.1147661897035</v>
+        <v>20.770025077445</v>
       </c>
       <c r="F124" s="12" t="n">
-        <v>209</v>
+        <v>180</v>
       </c>
       <c r="G124" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H124" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$118,G124)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I124" s="13" t="n">
         <f aca="false">$B$118+1</f>
-        <v>43920</v>
+        <v>43921</v>
       </c>
       <c r="J124" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$118,I124)</f>
         <v>-1</v>
       </c>
       <c r="K124" s="13" t="n">
-        <f aca="false">$B$118+1</f>
+        <f aca="false">$B$130+1</f>
         <v>43920</v>
       </c>
       <c r="L124" s="0"/>
@@ -4616,38 +4638,37 @@
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C125" s="12" t="n">
-        <v>414</v>
+        <v>1660</v>
       </c>
       <c r="D125" s="1" t="n">
-        <v>541</v>
+        <v>3141</v>
       </c>
       <c r="E125" s="12" t="n">
-        <f aca="false">D125/83.784</f>
-        <v>6.457080110761</v>
+        <f aca="false">D125/331</f>
+        <v>9.48942598187311</v>
       </c>
       <c r="F125" s="12" t="n">
-        <v>108</v>
+        <v>573</v>
       </c>
       <c r="G125" s="13" t="n">
-        <v>43918</v>
+        <v>43917</v>
       </c>
       <c r="H125" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$118,G125)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I125" s="13" t="n">
-        <f aca="false">$B$118+1</f>
         <v>43920</v>
       </c>
       <c r="J125" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$118,I125)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="K125" s="13" t="n">
-        <f aca="false">$B$118+1</f>
+        <f aca="false">$B$130+1</f>
         <v>43920</v>
       </c>
       <c r="L125" s="0"/>
@@ -4659,38 +4680,38 @@
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C126" s="12" t="n">
-        <v>50</v>
-      </c>
-      <c r="D126" s="12" t="n">
-        <v>110</v>
+        <v>414</v>
+      </c>
+      <c r="D126" s="1" t="n">
+        <v>645</v>
       </c>
       <c r="E126" s="12" t="n">
-        <f aca="false">D126/10.36</f>
-        <v>10.6177606177606</v>
+        <f aca="false">D126/83.784</f>
+        <v>7.69836723002005</v>
       </c>
       <c r="F126" s="12" t="n">
-        <v>5</v>
+        <v>104</v>
       </c>
       <c r="G126" s="13" t="n">
-        <v>43915</v>
+        <v>43918</v>
       </c>
       <c r="H126" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$118,G126)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I126" s="13" t="n">
         <f aca="false">$B$118+1</f>
-        <v>43920</v>
+        <v>43921</v>
       </c>
       <c r="J126" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$118,I126)</f>
         <v>-1</v>
       </c>
       <c r="K126" s="13" t="n">
-        <f aca="false">$B$118+1</f>
+        <f aca="false">$B$130+1</f>
         <v>43920</v>
       </c>
       <c r="L126" s="0"/>
@@ -4757,15 +4778,13 @@
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B130" s="7" t="n">
-        <v>43918</v>
-      </c>
-      <c r="D130" s="8" t="s">
-        <v>10</v>
-      </c>
+        <v>43919</v>
+      </c>
+      <c r="D130" s="0"/>
       <c r="E130" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F130" s="8"/>
+      <c r="F130" s="0"/>
       <c r="G130" s="8" t="s">
         <v>33</v>
       </c>
@@ -4793,8 +4812,8 @@
       <c r="C131" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D131" s="10" t="s">
-        <v>6</v>
+      <c r="D131" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="E131" s="10" t="s">
         <v>39</v>
@@ -4832,32 +4851,32 @@
         <v>300</v>
       </c>
       <c r="D132" s="1" t="n">
-        <v>10023</v>
+        <v>10779</v>
       </c>
       <c r="E132" s="12" t="n">
         <f aca="false">D132/60.48</f>
-        <v>165.724206349206</v>
+        <v>178.224206349206</v>
       </c>
       <c r="F132" s="12" t="n">
-        <v>889</v>
+        <v>756</v>
       </c>
       <c r="G132" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H132" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$130,G132)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I132" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J132" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$142,I132)</f>
-        <v>15</v>
+        <f aca="false">_xlfn.DAYS($B$130,I132)</f>
+        <v>17</v>
       </c>
       <c r="K132" s="13" t="n">
         <f aca="false">$B$130+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L132" s="0"/>
       <c r="M132" s="0"/>
@@ -4874,32 +4893,32 @@
         <v>230</v>
       </c>
       <c r="D133" s="1" t="n">
-        <v>5982</v>
+        <v>6803</v>
       </c>
       <c r="E133" s="12" t="n">
         <f aca="false">D133/46.75</f>
-        <v>127.957219251337</v>
+        <v>145.51871657754</v>
       </c>
       <c r="F133" s="12" t="n">
-        <v>844</v>
+        <v>821</v>
       </c>
       <c r="G133" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H133" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$130,G133)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I133" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J133" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$142,I133)</f>
-        <v>4</v>
+        <f aca="false">_xlfn.DAYS($B$130,I133)</f>
+        <v>6</v>
       </c>
       <c r="K133" s="13" t="n">
         <f aca="false">$B$130+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L133" s="0"/>
       <c r="M133" s="0"/>
@@ -4916,32 +4935,32 @@
         <v>330</v>
       </c>
       <c r="D134" s="1" t="n">
-        <v>2314</v>
+        <v>2606</v>
       </c>
       <c r="E134" s="12" t="n">
         <f aca="false">D134/65.27</f>
-        <v>35.4527347939329</v>
+        <v>39.9264593228129</v>
       </c>
       <c r="F134" s="12" t="n">
-        <v>319</v>
+        <v>292</v>
       </c>
       <c r="G134" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H134" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$130,G134)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I134" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J134" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$142,I134)</f>
-        <v>3</v>
+        <f aca="false">_xlfn.DAYS($B$130,I134)</f>
+        <v>5</v>
       </c>
       <c r="K134" s="13" t="n">
         <f aca="false">$B$130+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L134" s="0"/>
       <c r="M134" s="0"/>
@@ -4958,25 +4977,25 @@
         <v>1660</v>
       </c>
       <c r="D135" s="1" t="n">
-        <v>2221</v>
+        <v>2583</v>
       </c>
       <c r="E135" s="12" t="n">
         <f aca="false">D135/331</f>
-        <v>6.70996978851964</v>
+        <v>7.8036253776435</v>
       </c>
       <c r="F135" s="12" t="n">
-        <v>525</v>
+        <v>363</v>
       </c>
       <c r="G135" s="13" t="n">
         <v>43917</v>
       </c>
       <c r="H135" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$130,G135)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I135" s="13" t="n">
         <f aca="false">$B$130+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="J135" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$130,I135)</f>
@@ -4984,7 +5003,7 @@
       </c>
       <c r="K135" s="13" t="n">
         <f aca="false">$B$130+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L135" s="0"/>
       <c r="M135" s="0"/>
@@ -5001,25 +5020,25 @@
         <v>330</v>
       </c>
       <c r="D136" s="1" t="n">
-        <v>1019</v>
+        <v>1228</v>
       </c>
       <c r="E136" s="12" t="n">
         <f aca="false">D136/67.79</f>
-        <v>15.0317155922702</v>
+        <v>18.1147661897035</v>
       </c>
       <c r="F136" s="12" t="n">
-        <v>260</v>
+        <v>209</v>
       </c>
       <c r="G136" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H136" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$130,G136)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I136" s="13" t="n">
         <f aca="false">$B$130+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="J136" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$130,I136)</f>
@@ -5027,7 +5046,7 @@
       </c>
       <c r="K136" s="13" t="n">
         <f aca="false">$B$130+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L136" s="0"/>
       <c r="M136" s="0"/>
@@ -5044,25 +5063,25 @@
         <v>414</v>
       </c>
       <c r="D137" s="1" t="n">
-        <v>433</v>
+        <v>541</v>
       </c>
       <c r="E137" s="12" t="n">
         <f aca="false">D137/83.784</f>
-        <v>5.16805117922276</v>
+        <v>6.457080110761</v>
       </c>
       <c r="F137" s="12" t="n">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="G137" s="13" t="n">
         <v>43918</v>
       </c>
       <c r="H137" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$130,G137)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I137" s="13" t="n">
         <f aca="false">$B$130+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="J137" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$130,I137)</f>
@@ -5070,7 +5089,7 @@
       </c>
       <c r="K137" s="13" t="n">
         <f aca="false">$B$130+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L137" s="0"/>
       <c r="M137" s="0"/>
@@ -5087,25 +5106,25 @@
         <v>50</v>
       </c>
       <c r="D138" s="12" t="n">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="E138" s="12" t="n">
         <f aca="false">D138/10.36</f>
-        <v>10.1351351351351</v>
+        <v>10.6177606177606</v>
       </c>
       <c r="F138" s="12" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G138" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H138" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$130,G138)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I138" s="13" t="n">
         <f aca="false">$B$130+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="J138" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$130,I138)</f>
@@ -5113,7 +5132,7 @@
       </c>
       <c r="K138" s="13" t="n">
         <f aca="false">$B$130+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="L138" s="0"/>
       <c r="M138" s="0"/>
@@ -5123,15 +5142,16 @@
       <c r="Q138" s="0"/>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C139" s="12"/>
-      <c r="D139" s="12"/>
-      <c r="E139" s="12"/>
-      <c r="F139" s="12"/>
-      <c r="G139" s="13"/>
+      <c r="B139" s="4"/>
+      <c r="C139" s="5"/>
+      <c r="D139" s="0"/>
+      <c r="E139" s="0"/>
+      <c r="F139" s="0"/>
+      <c r="G139" s="0"/>
       <c r="H139" s="0"/>
-      <c r="I139" s="13"/>
+      <c r="I139" s="0"/>
       <c r="J139" s="0"/>
-      <c r="K139" s="13"/>
+      <c r="K139" s="0"/>
       <c r="L139" s="0"/>
       <c r="M139" s="0"/>
       <c r="N139" s="0"/>
@@ -5176,11 +5196,10 @@
       <c r="P141" s="0"/>
       <c r="Q141" s="0"/>
     </row>
-    <row r="142" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B142" s="7" t="n">
-        <v>43917</v>
-      </c>
-      <c r="C142" s="0"/>
+        <v>43918</v>
+      </c>
       <c r="D142" s="8" t="s">
         <v>10</v>
       </c>
@@ -5203,10 +5222,14 @@
       <c r="K142" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="L142" s="8"/>
+      <c r="L142" s="0"/>
+      <c r="M142" s="0"/>
+      <c r="N142" s="0"/>
+      <c r="O142" s="0"/>
+      <c r="P142" s="0"/>
+      <c r="Q142" s="0"/>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="3"/>
       <c r="B143" s="9"/>
       <c r="C143" s="10" t="s">
         <v>38</v>
@@ -5235,7 +5258,7 @@
       <c r="K143" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="L143" s="8"/>
+      <c r="L143" s="0"/>
       <c r="M143" s="0"/>
       <c r="N143" s="0"/>
       <c r="O143" s="0"/>
@@ -5250,32 +5273,32 @@
         <v>300</v>
       </c>
       <c r="D144" s="1" t="n">
-        <v>9134</v>
+        <v>10023</v>
       </c>
       <c r="E144" s="12" t="n">
         <f aca="false">D144/60.48</f>
-        <v>151.025132275132</v>
+        <v>165.724206349206</v>
       </c>
       <c r="F144" s="12" t="n">
-        <v>919</v>
+        <v>889</v>
       </c>
       <c r="G144" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H144" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$142,G144)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I144" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J144" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$142,I144)</f>
+        <f aca="false">_xlfn.DAYS(B$154,I144)</f>
         <v>15</v>
       </c>
       <c r="K144" s="13" t="n">
         <f aca="false">$B$142+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L144" s="0"/>
       <c r="M144" s="0"/>
@@ -5292,32 +5315,32 @@
         <v>230</v>
       </c>
       <c r="D145" s="1" t="n">
-        <v>5138</v>
+        <v>5982</v>
       </c>
       <c r="E145" s="12" t="n">
         <f aca="false">D145/46.75</f>
-        <v>109.903743315508</v>
+        <v>127.957219251337</v>
       </c>
       <c r="F145" s="12" t="n">
-        <v>773</v>
+        <v>844</v>
       </c>
       <c r="G145" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H145" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$142,G145)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I145" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J145" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$142,I145)</f>
+        <f aca="false">_xlfn.DAYS(B$154,I145)</f>
         <v>4</v>
       </c>
       <c r="K145" s="13" t="n">
         <f aca="false">$B$142+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L145" s="0"/>
       <c r="M145" s="0"/>
@@ -5334,32 +5357,32 @@
         <v>330</v>
       </c>
       <c r="D146" s="1" t="n">
-        <v>1995</v>
+        <v>2314</v>
       </c>
       <c r="E146" s="12" t="n">
         <f aca="false">D146/65.27</f>
-        <v>30.5653439558756</v>
+        <v>35.4527347939329</v>
       </c>
       <c r="F146" s="12" t="n">
-        <v>299</v>
+        <v>319</v>
       </c>
       <c r="G146" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H146" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$142,G146)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I146" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J146" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$142,I146)</f>
+        <f aca="false">_xlfn.DAYS(B$154,I146)</f>
         <v>3</v>
       </c>
       <c r="K146" s="13" t="n">
         <f aca="false">$B$142+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L146" s="0"/>
       <c r="M146" s="0"/>
@@ -5376,34 +5399,33 @@
         <v>1660</v>
       </c>
       <c r="D147" s="1" t="n">
-        <v>1696</v>
+        <v>2221</v>
       </c>
       <c r="E147" s="12" t="n">
         <f aca="false">D147/331</f>
-        <v>5.12386706948641</v>
+        <v>6.70996978851964</v>
       </c>
       <c r="F147" s="12" t="n">
-        <v>400</v>
+        <v>525</v>
       </c>
       <c r="G147" s="13" t="n">
-        <f aca="false">$B$142</f>
         <v>43917</v>
       </c>
       <c r="H147" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$142,G147)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I147" s="13" t="n">
         <f aca="false">$B$142+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="J147" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$142,I147)</f>
+        <f aca="false">_xlfn.DAYS($B$142,I147)</f>
         <v>-1</v>
       </c>
       <c r="K147" s="13" t="n">
         <f aca="false">$B$142+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L147" s="0"/>
       <c r="M147" s="0"/>
@@ -5420,33 +5442,33 @@
         <v>330</v>
       </c>
       <c r="D148" s="1" t="n">
-        <v>759</v>
+        <v>1019</v>
       </c>
       <c r="E148" s="12" t="n">
         <f aca="false">D148/67.79</f>
-        <v>11.1963416433102</v>
+        <v>15.0317155922702</v>
       </c>
       <c r="F148" s="12" t="n">
-        <v>181</v>
+        <v>260</v>
       </c>
       <c r="G148" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H148" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$142,G148)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I148" s="13" t="n">
         <f aca="false">$B$142+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="J148" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$142,I148)</f>
+        <f aca="false">_xlfn.DAYS($B$142,I148)</f>
         <v>-1</v>
       </c>
       <c r="K148" s="13" t="n">
         <f aca="false">$B$142+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L148" s="0"/>
       <c r="M148" s="0"/>
@@ -5463,34 +5485,33 @@
         <v>414</v>
       </c>
       <c r="D149" s="1" t="n">
-        <v>351</v>
+        <v>433</v>
       </c>
       <c r="E149" s="12" t="n">
         <f aca="false">D149/83.784</f>
-        <v>4.18934402749928</v>
+        <v>5.16805117922276</v>
       </c>
       <c r="F149" s="12" t="n">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G149" s="13" t="n">
-        <f aca="false">$B$142+1</f>
         <v>43918</v>
       </c>
       <c r="H149" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$142,G149)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="I149" s="13" t="n">
         <f aca="false">$B$142+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="J149" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$142,I149)</f>
+        <f aca="false">_xlfn.DAYS($B$142,I149)</f>
         <v>-1</v>
       </c>
       <c r="K149" s="13" t="n">
         <f aca="false">$B$142+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L149" s="0"/>
       <c r="M149" s="0"/>
@@ -5514,26 +5535,26 @@
         <v>10.1351351351351</v>
       </c>
       <c r="F150" s="12" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="G150" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H150" s="1" t="n">
         <f aca="false">_xlfn.DAYS($B$142,G150)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I150" s="13" t="n">
         <f aca="false">$B$142+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="J150" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$142,I150)</f>
+        <f aca="false">_xlfn.DAYS($B$142,I150)</f>
         <v>-1</v>
       </c>
       <c r="K150" s="13" t="n">
         <f aca="false">$B$142+1</f>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="L150" s="0"/>
       <c r="M150" s="0"/>
@@ -5543,14 +5564,15 @@
       <c r="Q150" s="0"/>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D151" s="0"/>
-      <c r="E151" s="0"/>
-      <c r="F151" s="0"/>
-      <c r="G151" s="0"/>
+      <c r="C151" s="12"/>
+      <c r="D151" s="12"/>
+      <c r="E151" s="12"/>
+      <c r="F151" s="12"/>
+      <c r="G151" s="13"/>
       <c r="H151" s="0"/>
-      <c r="I151" s="0"/>
+      <c r="I151" s="13"/>
       <c r="J151" s="0"/>
-      <c r="K151" s="0"/>
+      <c r="K151" s="13"/>
       <c r="L151" s="0"/>
       <c r="M151" s="0"/>
       <c r="N151" s="0"/>
@@ -5559,6 +5581,8 @@
       <c r="Q151" s="0"/>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B152" s="4"/>
+      <c r="C152" s="5"/>
       <c r="D152" s="0"/>
       <c r="E152" s="0"/>
       <c r="F152" s="0"/>
@@ -5593,10 +5617,11 @@
       <c r="P153" s="0"/>
       <c r="Q153" s="0"/>
     </row>
-    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B154" s="7" t="n">
-        <v>43916</v>
-      </c>
+        <v>43917</v>
+      </c>
+      <c r="C154" s="0"/>
       <c r="D154" s="8" t="s">
         <v>10</v>
       </c>
@@ -5619,17 +5644,13 @@
       <c r="K154" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="L154" s="0"/>
-      <c r="M154" s="0"/>
-      <c r="N154" s="0"/>
-      <c r="O154" s="0"/>
-      <c r="P154" s="0"/>
-      <c r="Q154" s="0"/>
+      <c r="L154" s="8"/>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="3"/>
       <c r="B155" s="9"/>
       <c r="C155" s="10" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D155" s="10" t="s">
         <v>6</v>
@@ -5655,7 +5676,7 @@
       <c r="K155" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="L155" s="0"/>
+      <c r="L155" s="8"/>
       <c r="M155" s="0"/>
       <c r="N155" s="0"/>
       <c r="O155" s="0"/>
@@ -5670,32 +5691,32 @@
         <v>300</v>
       </c>
       <c r="D156" s="1" t="n">
-        <v>8215</v>
+        <v>9134</v>
       </c>
       <c r="E156" s="12" t="n">
         <f aca="false">D156/60.48</f>
-        <v>135.830026455026</v>
+        <v>151.025132275132</v>
       </c>
       <c r="F156" s="12" t="n">
-        <v>712</v>
+        <v>919</v>
       </c>
       <c r="G156" s="13" t="n">
         <v>43900</v>
       </c>
       <c r="H156" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$154,G156)</f>
-        <v>16</v>
+        <f aca="false">_xlfn.DAYS($B$154,G156)</f>
+        <v>17</v>
       </c>
       <c r="I156" s="13" t="n">
         <v>43902</v>
       </c>
       <c r="J156" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$154,I156)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K156" s="13" t="n">
-        <f aca="false">B$154+1</f>
-        <v>43917</v>
+        <f aca="false">$B$154+1</f>
+        <v>43918</v>
       </c>
       <c r="L156" s="0"/>
       <c r="M156" s="0"/>
@@ -5712,32 +5733,32 @@
         <v>230</v>
       </c>
       <c r="D157" s="1" t="n">
-        <v>4365</v>
+        <v>5138</v>
       </c>
       <c r="E157" s="12" t="n">
         <f aca="false">D157/46.75</f>
-        <v>93.3689839572193</v>
+        <v>109.903743315508</v>
       </c>
       <c r="F157" s="12" t="n">
-        <v>718</v>
+        <v>773</v>
       </c>
       <c r="G157" s="13" t="n">
         <v>43907</v>
       </c>
       <c r="H157" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$154,G157)</f>
-        <v>9</v>
+        <f aca="false">_xlfn.DAYS($B$154,G157)</f>
+        <v>10</v>
       </c>
       <c r="I157" s="13" t="n">
         <v>43913</v>
       </c>
       <c r="J157" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$154,I157)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K157" s="13" t="n">
-        <f aca="false">B$154+1</f>
-        <v>43917</v>
+        <f aca="false">$B$154+1</f>
+        <v>43918</v>
       </c>
       <c r="L157" s="0"/>
       <c r="M157" s="0"/>
@@ -5754,32 +5775,32 @@
         <v>330</v>
       </c>
       <c r="D158" s="1" t="n">
-        <v>1696</v>
+        <v>1995</v>
       </c>
       <c r="E158" s="12" t="n">
         <f aca="false">D158/65.27</f>
-        <v>25.9843726060978</v>
+        <v>30.5653439558756</v>
       </c>
       <c r="F158" s="12" t="n">
-        <v>365</v>
+        <v>299</v>
       </c>
       <c r="G158" s="13" t="n">
         <v>43912</v>
       </c>
       <c r="H158" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$154,G158)</f>
-        <v>4</v>
+        <f aca="false">_xlfn.DAYS($B$154,G158)</f>
+        <v>5</v>
       </c>
       <c r="I158" s="13" t="n">
         <v>43914</v>
       </c>
       <c r="J158" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$154,I158)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K158" s="13" t="n">
-        <f aca="false">B$154+1</f>
-        <v>43917</v>
+        <f aca="false">$B$154+1</f>
+        <v>43918</v>
       </c>
       <c r="L158" s="0"/>
       <c r="M158" s="0"/>
@@ -5796,33 +5817,34 @@
         <v>1660</v>
       </c>
       <c r="D159" s="1" t="n">
-        <v>1295</v>
+        <v>1696</v>
       </c>
       <c r="E159" s="12" t="n">
         <f aca="false">D159/331</f>
-        <v>3.91238670694864</v>
+        <v>5.12386706948641</v>
       </c>
       <c r="F159" s="12" t="n">
-        <v>268</v>
+        <v>400</v>
       </c>
       <c r="G159" s="13" t="n">
+        <f aca="false">$B$154</f>
         <v>43917</v>
       </c>
       <c r="H159" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$154,G159)</f>
+        <f aca="false">_xlfn.DAYS($B$154,G159)</f>
+        <v>0</v>
+      </c>
+      <c r="I159" s="13" t="n">
+        <f aca="false">$B$154+1</f>
+        <v>43918</v>
+      </c>
+      <c r="J159" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$154,I159)</f>
         <v>-1</v>
       </c>
-      <c r="I159" s="13" t="n">
-        <f aca="false">B$154+1</f>
-        <v>43917</v>
-      </c>
-      <c r="J159" s="1" t="n">
-        <f aca="false">_xlfn.DAYS($B$154,I159)</f>
-        <v>-1</v>
-      </c>
       <c r="K159" s="13" t="n">
-        <f aca="false">B$154+1</f>
-        <v>43917</v>
+        <f aca="false">$B$154+1</f>
+        <v>43918</v>
       </c>
       <c r="L159" s="0"/>
       <c r="M159" s="0"/>
@@ -5839,33 +5861,33 @@
         <v>330</v>
       </c>
       <c r="D160" s="1" t="n">
-        <v>578</v>
+        <v>759</v>
       </c>
       <c r="E160" s="12" t="n">
         <f aca="false">D160/67.79</f>
-        <v>8.52633131730344</v>
+        <v>11.1963416433102</v>
       </c>
       <c r="F160" s="12" t="n">
-        <v>115</v>
+        <v>181</v>
       </c>
       <c r="G160" s="13" t="n">
         <v>43916</v>
       </c>
       <c r="H160" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$154,G160)</f>
-        <v>0</v>
+        <f aca="false">_xlfn.DAYS($B$154,G160)</f>
+        <v>1</v>
       </c>
       <c r="I160" s="13" t="n">
-        <f aca="false">B$154+1</f>
-        <v>43917</v>
+        <f aca="false">$B$154+1</f>
+        <v>43918</v>
       </c>
       <c r="J160" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$154,I160)</f>
         <v>-1</v>
       </c>
       <c r="K160" s="13" t="n">
-        <f aca="false">B$154+1</f>
-        <v>43917</v>
+        <f aca="false">$B$154+1</f>
+        <v>43918</v>
       </c>
       <c r="L160" s="0"/>
       <c r="M160" s="0"/>
@@ -5882,33 +5904,34 @@
         <v>414</v>
       </c>
       <c r="D161" s="1" t="n">
-        <v>267</v>
+        <v>351</v>
       </c>
       <c r="E161" s="12" t="n">
         <f aca="false">D161/83.784</f>
-        <v>3.18676596963621</v>
+        <v>4.18934402749928</v>
       </c>
       <c r="F161" s="12" t="n">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="G161" s="13" t="n">
-        <v>43917</v>
+        <f aca="false">$B$154+1</f>
+        <v>43918</v>
       </c>
       <c r="H161" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$154,G161)</f>
+        <f aca="false">_xlfn.DAYS($B$154,G161)</f>
         <v>-1</v>
       </c>
       <c r="I161" s="13" t="n">
-        <f aca="false">B$154+1</f>
-        <v>43917</v>
+        <f aca="false">$B$154+1</f>
+        <v>43918</v>
       </c>
       <c r="J161" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$154,I161)</f>
         <v>-1</v>
       </c>
       <c r="K161" s="13" t="n">
-        <f aca="false">B$154+1</f>
-        <v>43917</v>
+        <f aca="false">$B$154+1</f>
+        <v>43918</v>
       </c>
       <c r="L161" s="0"/>
       <c r="M161" s="0"/>
@@ -5925,33 +5948,33 @@
         <v>50</v>
       </c>
       <c r="D162" s="12" t="n">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="E162" s="12" t="n">
         <f aca="false">D162/10.36</f>
-        <v>7.43243243243243</v>
+        <v>10.1351351351351</v>
       </c>
       <c r="F162" s="12" t="n">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="G162" s="13" t="n">
         <v>43915</v>
       </c>
       <c r="H162" s="1" t="n">
-        <f aca="false">_xlfn.DAYS(B$154,G162)</f>
-        <v>1</v>
+        <f aca="false">_xlfn.DAYS($B$154,G162)</f>
+        <v>2</v>
       </c>
       <c r="I162" s="13" t="n">
-        <f aca="false">B$154+1</f>
-        <v>43917</v>
+        <f aca="false">$B$154+1</f>
+        <v>43918</v>
       </c>
       <c r="J162" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B$154,I162)</f>
         <v>-1</v>
       </c>
       <c r="K162" s="13" t="n">
-        <f aca="false">B$154+1</f>
-        <v>43917</v>
+        <f aca="false">$B$154+1</f>
+        <v>43918</v>
       </c>
       <c r="L162" s="0"/>
       <c r="M162" s="0"/>
@@ -5959,6 +5982,424 @@
       <c r="O162" s="0"/>
       <c r="P162" s="0"/>
       <c r="Q162" s="0"/>
+    </row>
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D163" s="0"/>
+      <c r="E163" s="0"/>
+      <c r="F163" s="0"/>
+      <c r="G163" s="0"/>
+      <c r="H163" s="0"/>
+      <c r="I163" s="0"/>
+      <c r="J163" s="0"/>
+      <c r="K163" s="0"/>
+      <c r="L163" s="0"/>
+      <c r="M163" s="0"/>
+      <c r="N163" s="0"/>
+      <c r="O163" s="0"/>
+      <c r="P163" s="0"/>
+      <c r="Q163" s="0"/>
+    </row>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D164" s="0"/>
+      <c r="E164" s="0"/>
+      <c r="F164" s="0"/>
+      <c r="G164" s="0"/>
+      <c r="H164" s="0"/>
+      <c r="I164" s="0"/>
+      <c r="J164" s="0"/>
+      <c r="K164" s="0"/>
+      <c r="L164" s="0"/>
+      <c r="M164" s="0"/>
+      <c r="N164" s="0"/>
+      <c r="O164" s="0"/>
+      <c r="P164" s="0"/>
+      <c r="Q164" s="0"/>
+    </row>
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B165" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D165" s="0"/>
+      <c r="E165" s="0"/>
+      <c r="F165" s="0"/>
+      <c r="G165" s="0"/>
+      <c r="H165" s="0"/>
+      <c r="I165" s="0"/>
+      <c r="J165" s="0"/>
+      <c r="K165" s="0"/>
+      <c r="L165" s="0"/>
+      <c r="M165" s="0"/>
+      <c r="N165" s="0"/>
+      <c r="O165" s="0"/>
+      <c r="P165" s="0"/>
+      <c r="Q165" s="0"/>
+    </row>
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B166" s="7" t="n">
+        <v>43916</v>
+      </c>
+      <c r="D166" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E166" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F166" s="8"/>
+      <c r="G166" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H166" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I166" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J166" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="K166" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="L166" s="0"/>
+      <c r="M166" s="0"/>
+      <c r="N166" s="0"/>
+      <c r="O166" s="0"/>
+      <c r="P166" s="0"/>
+      <c r="Q166" s="0"/>
+    </row>
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B167" s="9"/>
+      <c r="C167" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D167" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E167" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F167" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G167" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H167" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I167" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="J167" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="K167" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="L167" s="0"/>
+      <c r="M167" s="0"/>
+      <c r="N167" s="0"/>
+      <c r="O167" s="0"/>
+      <c r="P167" s="0"/>
+      <c r="Q167" s="0"/>
+    </row>
+    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B168" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C168" s="12" t="n">
+        <v>300</v>
+      </c>
+      <c r="D168" s="1" t="n">
+        <v>8215</v>
+      </c>
+      <c r="E168" s="12" t="n">
+        <f aca="false">D168/60.48</f>
+        <v>135.830026455026</v>
+      </c>
+      <c r="F168" s="12" t="n">
+        <v>712</v>
+      </c>
+      <c r="G168" s="13" t="n">
+        <v>43900</v>
+      </c>
+      <c r="H168" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$166,G168)</f>
+        <v>16</v>
+      </c>
+      <c r="I168" s="13" t="n">
+        <v>43902</v>
+      </c>
+      <c r="J168" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$166,I168)</f>
+        <v>14</v>
+      </c>
+      <c r="K168" s="13" t="n">
+        <f aca="false">B$166+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L168" s="0"/>
+      <c r="M168" s="0"/>
+      <c r="N168" s="0"/>
+      <c r="O168" s="0"/>
+      <c r="P168" s="0"/>
+      <c r="Q168" s="0"/>
+    </row>
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B169" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C169" s="12" t="n">
+        <v>230</v>
+      </c>
+      <c r="D169" s="1" t="n">
+        <v>4365</v>
+      </c>
+      <c r="E169" s="12" t="n">
+        <f aca="false">D169/46.75</f>
+        <v>93.3689839572193</v>
+      </c>
+      <c r="F169" s="12" t="n">
+        <v>718</v>
+      </c>
+      <c r="G169" s="13" t="n">
+        <v>43907</v>
+      </c>
+      <c r="H169" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$166,G169)</f>
+        <v>9</v>
+      </c>
+      <c r="I169" s="13" t="n">
+        <v>43913</v>
+      </c>
+      <c r="J169" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$166,I169)</f>
+        <v>3</v>
+      </c>
+      <c r="K169" s="13" t="n">
+        <f aca="false">B$166+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L169" s="0"/>
+      <c r="M169" s="0"/>
+      <c r="N169" s="0"/>
+      <c r="O169" s="0"/>
+      <c r="P169" s="0"/>
+      <c r="Q169" s="0"/>
+    </row>
+    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B170" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C170" s="12" t="n">
+        <v>330</v>
+      </c>
+      <c r="D170" s="1" t="n">
+        <v>1696</v>
+      </c>
+      <c r="E170" s="12" t="n">
+        <f aca="false">D170/65.27</f>
+        <v>25.9843726060978</v>
+      </c>
+      <c r="F170" s="12" t="n">
+        <v>365</v>
+      </c>
+      <c r="G170" s="13" t="n">
+        <v>43912</v>
+      </c>
+      <c r="H170" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$166,G170)</f>
+        <v>4</v>
+      </c>
+      <c r="I170" s="13" t="n">
+        <v>43914</v>
+      </c>
+      <c r="J170" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$166,I170)</f>
+        <v>2</v>
+      </c>
+      <c r="K170" s="13" t="n">
+        <f aca="false">B$166+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L170" s="0"/>
+      <c r="M170" s="0"/>
+      <c r="N170" s="0"/>
+      <c r="O170" s="0"/>
+      <c r="P170" s="0"/>
+      <c r="Q170" s="0"/>
+    </row>
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B171" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C171" s="12" t="n">
+        <v>1660</v>
+      </c>
+      <c r="D171" s="1" t="n">
+        <v>1295</v>
+      </c>
+      <c r="E171" s="12" t="n">
+        <f aca="false">D171/331</f>
+        <v>3.91238670694864</v>
+      </c>
+      <c r="F171" s="12" t="n">
+        <v>268</v>
+      </c>
+      <c r="G171" s="13" t="n">
+        <v>43917</v>
+      </c>
+      <c r="H171" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$166,G171)</f>
+        <v>-1</v>
+      </c>
+      <c r="I171" s="13" t="n">
+        <f aca="false">B$166+1</f>
+        <v>43917</v>
+      </c>
+      <c r="J171" s="1" t="n">
+        <f aca="false">_xlfn.DAYS($B$166,I171)</f>
+        <v>-1</v>
+      </c>
+      <c r="K171" s="13" t="n">
+        <f aca="false">B$166+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L171" s="0"/>
+      <c r="M171" s="0"/>
+      <c r="N171" s="0"/>
+      <c r="O171" s="0"/>
+      <c r="P171" s="0"/>
+      <c r="Q171" s="0"/>
+    </row>
+    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B172" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C172" s="12" t="n">
+        <v>330</v>
+      </c>
+      <c r="D172" s="1" t="n">
+        <v>578</v>
+      </c>
+      <c r="E172" s="12" t="n">
+        <f aca="false">D172/67.79</f>
+        <v>8.52633131730344</v>
+      </c>
+      <c r="F172" s="12" t="n">
+        <v>115</v>
+      </c>
+      <c r="G172" s="13" t="n">
+        <v>43916</v>
+      </c>
+      <c r="H172" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$166,G172)</f>
+        <v>0</v>
+      </c>
+      <c r="I172" s="13" t="n">
+        <f aca="false">B$166+1</f>
+        <v>43917</v>
+      </c>
+      <c r="J172" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$166,I172)</f>
+        <v>-1</v>
+      </c>
+      <c r="K172" s="13" t="n">
+        <f aca="false">B$166+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L172" s="0"/>
+      <c r="M172" s="0"/>
+      <c r="N172" s="0"/>
+      <c r="O172" s="0"/>
+      <c r="P172" s="0"/>
+      <c r="Q172" s="0"/>
+    </row>
+    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B173" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C173" s="12" t="n">
+        <v>414</v>
+      </c>
+      <c r="D173" s="1" t="n">
+        <v>267</v>
+      </c>
+      <c r="E173" s="12" t="n">
+        <f aca="false">D173/83.784</f>
+        <v>3.18676596963621</v>
+      </c>
+      <c r="F173" s="12" t="n">
+        <v>61</v>
+      </c>
+      <c r="G173" s="13" t="n">
+        <v>43917</v>
+      </c>
+      <c r="H173" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$166,G173)</f>
+        <v>-1</v>
+      </c>
+      <c r="I173" s="13" t="n">
+        <f aca="false">B$166+1</f>
+        <v>43917</v>
+      </c>
+      <c r="J173" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$166,I173)</f>
+        <v>-1</v>
+      </c>
+      <c r="K173" s="13" t="n">
+        <f aca="false">B$166+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L173" s="0"/>
+      <c r="M173" s="0"/>
+      <c r="N173" s="0"/>
+      <c r="O173" s="0"/>
+      <c r="P173" s="0"/>
+      <c r="Q173" s="0"/>
+    </row>
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B174" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C174" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="D174" s="12" t="n">
+        <v>77</v>
+      </c>
+      <c r="E174" s="12" t="n">
+        <f aca="false">D174/10.36</f>
+        <v>7.43243243243243</v>
+      </c>
+      <c r="F174" s="12" t="n">
+        <v>15</v>
+      </c>
+      <c r="G174" s="13" t="n">
+        <v>43915</v>
+      </c>
+      <c r="H174" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$166,G174)</f>
+        <v>1</v>
+      </c>
+      <c r="I174" s="13" t="n">
+        <f aca="false">B$166+1</f>
+        <v>43917</v>
+      </c>
+      <c r="J174" s="1" t="n">
+        <f aca="false">_xlfn.DAYS(B$166,I174)</f>
+        <v>-1</v>
+      </c>
+      <c r="K174" s="13" t="n">
+        <f aca="false">B$166+1</f>
+        <v>43917</v>
+      </c>
+      <c r="L174" s="0"/>
+      <c r="M174" s="0"/>
+      <c r="N174" s="0"/>
+      <c r="O174" s="0"/>
+      <c r="P174" s="0"/>
+      <c r="Q174" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>